<commit_message>
chore: update revenue-data.xlsx and revenue-data.json with latest data
</commit_message>
<xml_diff>
--- a/data/revenue-data.xlsx
+++ b/data/revenue-data.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/Revenue_Performance_Analysis-2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F459F618-2AE8-FF45-8DB8-608F3CFC2927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61AC9EBD-220F-0E44-AB09-A40FDF321FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="21420" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="820" windowWidth="26800" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="223">
   <si>
     <t>Year</t>
   </si>
@@ -100,541 +100,595 @@
     <t>2025</t>
   </si>
   <si>
-    <t>4-MEDICAID – After Hours Zero-Balance Collection Dollar Impact decreased from avg -0.33 to -8.15; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00; 12-HUMANA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.28 to 0.00; 12-HUMANA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 0.78 to 0.00; 12-HUMANA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.12 to 0.00</t>
-  </si>
-  <si>
-    <t>12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00; 12-HUMANA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.28 to 0.00; 12-HUMANA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 0.78 to 0.00; 12-HUMANA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.12 to 0.00; 12-HUMANA – New E/M Codes Charge Billed Balance decreased from avg 0.44 to 0.00; 13-TRICARE – Existing E/M Code Charge Billed Balance decreased from avg 88.96 to 0.00</t>
-  </si>
-  <si>
-    <t>13-TRICARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 61.56 to -22.18; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00; 12-HUMANA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.28 to 0.00; 12-HUMANA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 0.78 to 0.00; 12-HUMANA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.12 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -145.36; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -150.00; 15-UNITED HEALTHCARE – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.95 to -3.89; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00; 12-HUMANA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.28 to 0.00; 12-HUMANA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 0.78 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00; 12-HUMANA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.28 to 0.00; 12-HUMANA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 0.78 to 0.00; 12-HUMANA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.12 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -122.59; 12-HUMANA – New E/M Codes Charge Billed Balance decreased from avg 0.44 to -250.00; 12-HUMANA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -6.89 to -225.56; 3-MEDICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -7.53 to -132.53; 12-HUMANA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg -12.86 to -180.04; 3-MEDICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 1.82 to -8.49</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance decreased from avg 63.06 to -53.44; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.50 to -2.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00; 12-HUMANA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.28 to 0.00</t>
-  </si>
-  <si>
-    <t>12-HUMANA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.12 to -4.07; 12-HUMANA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.28 to 0.00; 12-HUMANA – Existing E/M Code Zero Balance Collection Rate decreased from avg 0.38 to 0.00; 12-HUMANA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 0.78 to 0.00; 12-HUMANA – New E/M Codes Charge Billed Balance decreased from avg 0.44 to 0.00; 13-TRICARE – Existing E/M Code Charge Billed Balance decreased from avg 88.96 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -102.16; 3-MEDICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -7.53 to -101.04; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00; 12-HUMANA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.28 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Existing E/M Code Charge Billed Balance decreased from avg 88.96 to 0.00; 13-TRICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 33.42 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00; 12-HUMANA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.28 to 0.00; 12-HUMANA – Existing E/M Code Labs per Visit decreased from avg 1.20 to 0.00; 13-TRICARE – Existing E/M Code Charge Billed Balance decreased from avg 88.96 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 0.78 to 0.00; 12-HUMANA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.12 to 0.00; 12-HUMANA – New E/M Codes Charge Billed Balance decreased from avg 0.44 to 0.00; 13-TRICARE – Existing E/M Code Charge Billed Balance decreased from avg 88.96 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -60.44; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -106.22; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 70.81 to -13.32; 4-MEDICAID – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 70.72 to -12.78; 4-MEDICAID – Existing E/M Code Charge Billed Balance decreased from avg 214.26 to -4.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 3.46 to -3.92; 4-MEDICAID – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 162.82 to -5.10; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00; 12-HUMANA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.28 to 0.00; 12-HUMANA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 0.78 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -14.70; 3-MEDICARE – X-Ray CPT Codes Charge Billed Balance decreased from avg 3.31 to -4.99; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Existing E/M Code Charge Billed Balance decreased from avg 88.96 to 0.00; 13-TRICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 33.42 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.50 to -3.26; 1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00; 12-HUMANA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.28 to 0.00; 12-HUMANA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 0.78 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -20.77; 3-MEDICARE – Medications Charge Billed Balance decreased from avg 1.05 to -2.50; 3-MEDICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -7.53 to -25.87; 3-MEDICARE – New E/M Codes Charge Billed Balance decreased from avg 45.73 to -27.04; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -20.77; 3-MEDICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -7.53 to -24.20; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.50 to -11.73; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Existing E/M Code Charge Billed Balance decreased from avg 88.96 to 0.00; 13-TRICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 33.42 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -20.77; 1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – New E/M Codes Labs per Visit decreased from avg 0.86 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Lab/Test CPT Codes Charge Billed Balance decreased from avg 98.89 to 0.00; 13-TRICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 25.52 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Medications Payment per Visit decreased from avg 28.18 to 0.00; 1-SELF PAY – Medications Charge Amount decreased from avg 65.92 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 46.24 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount decreased from avg 116.93 to 0.00; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00</t>
-  </si>
-  <si>
-    <t>13-TRICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 33.42 to -204.76; 13-TRICARE – Existing E/M Code Charge Billed Balance decreased from avg 88.96 to -55.40; 13-TRICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 25.52 to -14.26; 13-TRICARE – Lab/Test CPT Codes Charge Billed Balance decreased from avg 98.89 to -1.94; 1-SELF PAY – Medications Payment per Visit decreased from avg 28.18 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – New E/M Codes Labs per Visit decreased from avg 1.32 to 0.00; 13-TRICARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.82 to 0.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.88 to 0.00; 18-CIGNA – X-Ray CPT Codes Labs per Visit decreased from avg 0.69 to 0.00; 4-MEDICAID – Medications Labs per Visit decreased from avg 1.26 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 12-HUMANA – New E/M Codes Labs per Visit decreased from avg 0.90 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00; 13-TRICARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.82 to 0.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.88 to 0.00; 3-MEDICARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.67 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.82 to 0.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.94 to 0.00; 3-MEDICARE – New E/M Codes Avg. Charge E/M Weight decreased from avg 3.50 to 0.00; 3-MEDICARE – New E/M Codes Payment per Visit decreased from avg 71.77 to 0.00; 5-COMMERCIAL – New E/M Codes Labs per Visit decreased from avg 1.75 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.93 to -329.00; 18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -33.96; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 25.96 to -463.00; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -116.80; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.20 to -46.03; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -383.59; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -313.71; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 25.96 to -122.70; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -208.13; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -0.54; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -70.00; 5-COMMERCIAL – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 41.75 to -11.64; 5-COMMERCIAL – New E/M Codes Charge Billed Balance decreased from avg 122.16 to -11.64; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00; 12-HUMANA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.28 to 0.00; 12-HUMANA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 0.78 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -150.00; 18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -47.43; 3-MEDICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -7.53 to -154.66; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.20 to -163.95; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -204.84; 5-COMMERCIAL – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 41.75 to -129.00</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -85.21; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -317.35; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -203.50; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 15.12 to -163.48; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.20 to -208.94; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -266.78</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -273.29; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -127.16; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.50 to -223.08; 5-COMMERCIAL – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 20.86 to -148.26; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 15.12 to -66.78; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 25.96 to -109.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -48.64; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -160.99; 18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -18.72; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 15.12 to -148.04; 3-MEDICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -7.53 to -50.26; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.20 to -118.28</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -15.53; 15-UNITED HEALTHCARE – Vaccines Charge Billed Balance decreased from avg -10.71 to -150.00; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -15.14; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -73.99; 1-SELF PAY – Existing E/M Code Avg. Charge E/M Weight decreased from avg 3.64 to 0.00; 1-SELF PAY – Existing E/M Code Payment per Visit decreased from avg 123.17 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -18.59; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -202.89; 3-MEDICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -7.53 to -50.26; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -152.09; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -11.65; 5-COMMERCIAL – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 41.75 to -33.36</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -92.15; 5-COMMERCIAL – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.93 to -39.70; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -135.15; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 15.12 to -117.84; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -51.44; 12-HUMANA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.28 to -5.51</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -293.19; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -166.67; 12-HUMANA – X-Ray CPT Codes Charge Billed Balance decreased from avg -1.21 to -25.51; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -133.31; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.20 to -300.32; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -243.09</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -54.03; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -110.00; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -61.14; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.20 to -108.07; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 2.76 to -5.18; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -103.32</t>
-  </si>
-  <si>
-    <t>12-HUMANA – New E/M Codes Charge Billed Balance decreased from avg 0.44 to -105.00; 12-HUMANA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -6.89 to -104.90; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -8.58; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -13.09; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 13.65 to -134.15; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 2.76 to -5.18; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 12.09 to -16.34; 5-COMMERCIAL – New E/M Codes Charge Billed Balance decreased from avg 122.16 to -30.00; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -5.95; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -0.11</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -88.35; 1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – Existing E/M Code Charge Billed Balance decreased from avg 10.28 to 0.00; 12-HUMANA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 1.28 to 0.00</t>
-  </si>
-  <si>
-    <t>12-HUMANA – New E/M Codes Charge Billed Balance decreased from avg 0.44 to -1.25; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -24.47; 4-MEDICAID – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 70.72 to -110.00; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 15.12 to -20.00; 4-MEDICAID – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 162.82 to -191.91; 5-COMMERCIAL – New E/M Codes Charge Billed Balance decreased from avg 122.16 to -75.00</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -164.28; 3-MEDICARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 13.65 to -110.54; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 15.12 to -90.00; 3-MEDICARE – New E/M Codes Charge Billed Balance decreased from avg 45.73 to -123.57; 5-COMMERCIAL – X-Ray CPT Codes Charge Billed Balance decreased from avg 17.35 to -35.00; 18-CIGNA – New E/M Codes Charge Billed Balance decreased from avg 61.06 to -90.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -209.42; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 25.96 to -137.70; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.20 to -106.83; 5-COMMERCIAL – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 41.75 to -126.43; 3-MEDICARE – Medications Charge Billed Balance decreased from avg 1.05 to -2.63; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 15.12 to -30.87</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -73.35; 3-MEDICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 1.82 to -11.46; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -40.52; 5-COMMERCIAL – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 41.75 to -52.21; 1-SELF PAY – Medications Payment per Visit decreased from avg 28.18 to 0.00; 1-SELF PAY – Medications Charge Amount decreased from avg 65.92 to 0.00</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – Self-pay physical &amp; No Charge Charge Billed Balance decreased from avg -11.50 to -61.00; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -14.10; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -25.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 4.07 to -5.11; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -20.00; 4-MEDICAID – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 162.82 to -9.27</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – DME Zero-Balance Collection Dollar Impact decreased from avg 6.87 to -93.40; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.20 to -71.17; 4-MEDICAID – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 70.72 to -24.31; 4-MEDICAID – Existing E/M Code Charge Billed Balance decreased from avg 214.26 to -20.00; 4-MEDICAID – New E/M Codes Charge Billed Balance decreased from avg 390.86 to -4.00; 1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg -0.06 to -150.00; 3-MEDICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 1.82 to -121.51; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -262.19; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -162.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 12-HUMANA – New E/M Codes Charge Billed Balance decreased from avg 0.44 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 46.24 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount decreased from avg 116.93 to 0.00; 12-HUMANA – Existing E/M Code Labs per Visit decreased from avg 1.20 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 12-HUMANA – New E/M Codes Labs per Visit decreased from avg 0.90 to 0.00; 13-TRICARE – Lab/Test CPT Codes Payment per Visit decreased from avg 56.50 to 0.00; 13-TRICARE – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 39.81 to 0.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.88 to 0.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.94 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 46.24 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount decreased from avg 116.93 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – New E/M Codes Payment per Visit decreased from avg 131.08 to 0.00; 13-TRICARE – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 39.81 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 225.00; 2-BCBS – After Hours Zero Balance Collection Rate increased from avg 0.01 to 0.15; 2-BCBS – After Hours Payment per Visit increased from avg 0.65 to 6.73; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 63.06 to 293.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg -36.34 to 82.60; 2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg -4.05 to 6.35</t>
-  </si>
-  <si>
-    <t>2-BCBS – Self-pay physical &amp; No Charge Zero Balance Collection Rate increased from avg 0.09 to 1.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 4.00; 18-CIGNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 12.20 to 54.56; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 3.00; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Zero Balance Collection Rate increased from avg 0.22 to 0.84; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 29.17 to 108.38</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit increased from avg 0.88 to 5.00; 1-SELF PAY – Existing E/M Code Labs per Visit increased from avg 0.91 to 2.88; 3-MEDICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.67 to 2.00; 5-COMMERCIAL – Lab/Test CPT Codes Charge Amount increased from avg 496.66 to 1371.00; 12-HUMANA – X-Ray CPT Codes Zero Balance Collection Rate increased from avg 0.24 to 0.65; 17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 5.00</t>
-  </si>
-  <si>
-    <t>12-HUMANA – Medications Labs per Visit increased from avg 0.96 to 5.00; 12-HUMANA – Lab/Test CPT Codes Charge Amount increased from avg 376.92 to 1799.00; 13-TRICARE – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.66 to 7.00; 5-COMMERCIAL – Lab/Test CPT Codes Charge Amount increased from avg 496.66 to 2073.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit increased from avg 0.39 to 1.50; 2-BCBS – DME Payment per Visit increased from avg 126.81 to 473.50</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 9.06 to 165.58; 1-SELF PAY – X-Ray CPT Codes Labs per Visit increased from avg 0.39 to 2.50; 15-UNITED HEALTHCARE – Medications Payment per Visit increased from avg 20.00 to 112.53; 17-AETNA – Medications Labs per Visit increased from avg 1.60 to 7.00; 15-UNITED HEALTHCARE – Medications Zero Balance Collection Rate increased from avg 0.14 to 0.52; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 2.50</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 0.55 to 7.38; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.39 to 5.00; 13-TRICARE – Medications Labs per Visit increased from avg 1.42 to 5.00; 12-HUMANA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 155.71 to 540.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit increased from avg 0.88 to 2.50; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 0.95 to 2.67</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg -16.11 to 55.28; 12-HUMANA – Medications Labs per Visit increased from avg 0.96 to 4.00; 17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 3.00; 15-UNITED HEALTHCARE – DME Payment per Visit increased from avg 55.83 to 181.96; 5-COMMERCIAL – After Hours Zero Balance Collection Rate increased from avg 0.21 to 0.62; 5-COMMERCIAL – After Hours Payment per Visit increased from avg 9.78 to 28.66</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg -0.06 to 49.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg 0.19 to 5.51; 1-SELF PAY – X-Ray CPT Codes Labs per Visit increased from avg 0.39 to 9.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 9.00; 12-HUMANA – Existing E/M Code Charge Billed Balance increased from avg 10.28 to 100.00; 5-COMMERCIAL – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 41.75 to 278.37</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 1.82 to 20.68; 18-CIGNA – X-Ray CPT Codes Labs per Visit increased from avg 0.69 to 3.00; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 4.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 4.80; 17-AETNA – Self-pay physical &amp; No Charge Payment per Visit increased from avg 1.33 to 4.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 2.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Labs per Visit increased from avg 1.60 to 9.00; 15-UNITED HEALTHCARE – Medications Labs per Visit increased from avg 1.45 to 7.00; 5-COMMERCIAL – After Hours Zero Balance Collection Rate increased from avg 0.21 to 0.62; 5-COMMERCIAL – After Hours Payment per Visit increased from avg 9.78 to 28.66; 5-COMMERCIAL – X-Ray CPT Codes Labs per Visit increased from avg 1.10 to 3.00; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 23.02 to 59.73</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Charge Billed Balance increased from avg 14.47 to 100.00; 17-AETNA – Medications Zero-Balance Collection Dollar Impact increased from avg 3.36 to 18.78; 1-SELF PAY – DME Charge Amount increased from avg 133.93 to 689.80; 13-TRICARE – Vaccines Labs per Visit increased from avg 0.50 to 2.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg 51.63 to 204.56; 17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 63.76 to 245.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Vaccines Labs per Visit increased from avg 0.10 to 2.00; 3-MEDICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.67 to 2.50; 17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 7.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.94 to 7.00; 5-COMMERCIAL – Medications Payment per Visit increased from avg 9.83 to 32.75; 5-COMMERCIAL – Medications Zero Balance Collection Rate increased from avg 0.11 to 0.35</t>
-  </si>
-  <si>
-    <t>2-BCBS – After Hours Payment per Visit increased from avg 0.65 to 2.43; 2-BCBS – After Hours Zero Balance Collection Rate increased from avg 0.01 to 0.05; 3-MEDICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.67 to 2.00; 13-TRICARE – New E/M Codes Labs per Visit increased from avg 1.32 to 3.50; 4-MEDICAID – Self-pay physical &amp; No Charge Payment per Visit increased from avg 15.32 to 40.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.67</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 76.76; 13-TRICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.82 to 6.00; 5-COMMERCIAL – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 20.86 to 135.79; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 15.12 to 90.65; 13-TRICARE – Medications Labs per Visit increased from avg 1.42 to 6.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero Balance Collection Rate increased from avg 0.16 to 0.66</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 160.00; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 284.35; 2-BCBS – After Hours Zero-Balance Collection Dollar Impact increased from avg 0.08 to 1.60; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg -16.11 to 96.94; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 364.54; 2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg -4.05 to 12.26</t>
-  </si>
-  <si>
-    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg -4.05 to 17.57; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 30.27; 2-BCBS – Self-pay physical &amp; No Charge Charge Amount increased from avg 15.08 to 52.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 46.24 to 155.00; 17-AETNA – DME Payment per Visit increased from avg 126.37 to 368.10; 18-CIGNA – New E/M Codes Labs per Visit increased from avg 1.98 to 5.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 9.06 to 186.19; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 23.95 to 135.81; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 15.12 to 72.48; 5-COMMERCIAL – Medications Labs per Visit increased from avg 1.73 to 5.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 2.00; 1-SELF PAY – DME Payment per Visit increased from avg 35.56 to 100.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Vaccines Labs per Visit increased from avg 0.57 to 8.00; 3-MEDICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 1.82 to 12.33; 17-AETNA – DME Payment per Visit increased from avg 126.37 to 529.98; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 116.93 to 415.00; 2-BCBS – Self-pay physical &amp; No Charge Charge Amount increased from avg 15.08 to 52.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.87 to 6.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 205.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 116.93 to 655.00; 1-SELF PAY – DME Charge Amount increased from avg 133.93 to 705.92; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg -36.34 to 65.97; 4-MEDICAID – DME Payment per Visit increased from avg 80.05 to 299.11; 2-BCBS – Self-pay physical &amp; No Charge Charge Amount increased from avg 15.08 to 52.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Vaccines Labs per Visit increased from avg 0.10 to 1.00; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 29.34; 3-MEDICARE – Medications Labs per Visit increased from avg 0.90 to 4.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 3.00; 17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 63.76 to 241.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact increased from avg 2.09 to 6.84</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg 1.93 to 167.50; 2-BCBS – DME Labs per Visit increased from avg 0.05 to 0.50; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 241.00; 5-COMMERCIAL – Lab/Test CPT Codes Charge Billed Balance increased from avg 74.50 to 293.00; 15-UNITED HEALTHCARE – DME Payment per Visit increased from avg 55.83 to 207.02; 1-SELF PAY – Medications Labs per Visit increased from avg 1.13 to 4.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 2.76 to 89.00; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 9.06 to 138.67; 2-BCBS – Vaccines Payment per Visit increased from avg 67.22 to 345.09; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance increased from avg 64.00 to 310.00; 4-MEDICAID – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 3.46 to 11.27; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 4.00</t>
-  </si>
-  <si>
-    <t>13-TRICARE – Existing E/M Code Labs per Visit increased from avg 1.42 to 7.00; 13-TRICARE – Medications Labs per Visit increased from avg 1.42 to 7.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 41.05 to 201.33; 13-TRICARE – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.66 to 7.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 2.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 174.38 to 504.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Self-pay physical &amp; No Charge Labs per Visit increased from avg 0.17 to 2.00; 2-BCBS – Self-pay physical &amp; No Charge Payment per Visit increased from avg 7.67 to 25.00; 2-BCBS – DME Charge Amount increased from avg 616.33 to 1680.52; 2-BCBS – Medications Labs per Visit increased from avg 1.33 to 3.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 0.95 to 2.00; 15-UNITED HEALTHCARE – Medications Labs per Visit increased from avg 1.45 to 3.00</t>
-  </si>
-  <si>
-    <t>18-CIGNA – X-Ray CPT Codes Labs per Visit increased from avg 0.69 to 2.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 2.14 to 6.00; 5-COMMERCIAL – New E/M Codes Payment per Visit increased from avg 142.42 to 342.70; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.75; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 3.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 1.67</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 20.86 to 567.00; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 230.61; 2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg -4.05 to 66.03; 4-MEDICAID – Vaccines Charge Billed Balance increased from avg 51.20 to 411.00; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 416.22; 5-COMMERCIAL – Lab/Test CPT Codes Charge Billed Balance increased from avg 74.50 to 525.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg -0.06 to 9.90; 2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 0.36 to 32.81; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 714.85; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 1243.38; 13-TRICARE – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 1.30 to 26.10; 13-TRICARE – Medications Zero-Balance Collection Dollar Impact increased from avg 2.17 to 21.77</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 31.40; 12-HUMANA – New E/M Codes Charge Billed Balance increased from avg 0.44 to 79.87; 17-AETNA – Medications Zero-Balance Collection Dollar Impact increased from avg 3.36 to 78.70; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 4.95 to 104.00; 12-HUMANA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -6.89 to 110.74; 4-MEDICAID – X-Ray CPT Codes Charge Billed Balance increased from avg 11.37 to 128.00</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – Medications Charge Billed Balance increased from avg 3.82 to 110.00; 4-MEDICAID – Medications Zero-Balance Collection Dollar Impact increased from avg 1.09 to 17.85; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 9.06 to 96.81; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance increased from avg 101.89 to 781.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 62.39 to 475.17; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 37.41</t>
+    <t>4-MEDICAID – After Hours Zero-Balance Collection Dollar Impact decreased from avg -0.33 to -8.15; 13-TRICARE – Lab/Test CPT Codes Visit Count increased from avg 2.59 to 9.00; 15-UNITED HEALTHCARE – Medications Payment per Visit increased from avg 21.82 to 69.82; 13-TRICARE – New E/M Codes Visit Count increased from avg 3.29 to 10.00; 13-TRICARE – New E/M Codes Charge Amount increased from avg 976.67 to 2950.00; 18-CIGNA – X-Ray CPT Codes Labs per Visit increased from avg 0.69 to 2.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 4.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 3.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 29.89 to 108.38; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Zero Balance Collection Rate increased from avg 0.27 to 0.84; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Collection Rate increased from avg 0.27 to 0.84; 3-MEDICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.67 to 2.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit increased from avg 0.88 to 5.00; 1-SELF PAY – Existing E/M Code Labs per Visit increased from avg 0.91 to 2.88; 3-MEDICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.67 to 2.00; 5-COMMERCIAL – Lab/Test CPT Codes Charge Amount increased from avg 496.66 to 1371.00; 12-HUMANA – X-Ray CPT Codes Zero Balance Collection Rate increased from avg 0.26 to 0.65; 12-HUMANA – X-Ray CPT Codes Collection Rate increased from avg 0.26 to 0.65</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -145.36; 12-HUMANA – Medications Labs per Visit increased from avg 0.96 to 5.00; 12-HUMANA – Lab/Test CPT Codes Charge Amount increased from avg 376.92 to 1799.00; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -150.00; 13-TRICARE – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.66 to 7.00; 5-COMMERCIAL – Lab/Test CPT Codes Charge Amount increased from avg 496.66 to 2073.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – X-Ray CPT Codes Labs per Visit increased from avg 0.39 to 2.50; 15-UNITED HEALTHCARE – Medications Payment per Visit increased from avg 21.82 to 112.53; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 2.50; 15-UNITED HEALTHCARE – Medications Collection Rate increased from avg 0.16 to 0.52; 18-CIGNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.94 to 6.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 50.76 to 155.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -122.59; 12-HUMANA – New E/M Codes Charge Billed Balance decreased from avg 0.44 to -250.00; 12-HUMANA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -7.37 to -225.56; 3-MEDICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -8.47 to -132.53; 12-HUMANA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg -15.00 to -180.04; 3-MEDICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 2.08 to -8.49</t>
+  </si>
+  <si>
+    <t>12-HUMANA – Medications Labs per Visit increased from avg 0.96 to 4.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance decreased from avg 63.06 to -53.44; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 2.00; 12-HUMANA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.51 to 4.00; 15-UNITED HEALTHCARE – DME Payment per Visit increased from avg 73.28 to 181.96; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 50.76 to 122.50</t>
+  </si>
+  <si>
+    <t>12-HUMANA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.13 to -4.07; 1-SELF PAY – X-Ray CPT Codes Labs per Visit increased from avg 0.39 to 9.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 9.00; 1-SELF PAY – New E/M Codes Labs per Visit increased from avg 0.86 to 3.50; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 0.95 to 3.67; 1-SELF PAY – Medications Labs per Visit increased from avg 1.13 to 4.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -102.16; 3-MEDICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -8.47 to -101.04; 18-CIGNA – X-Ray CPT Codes Labs per Visit increased from avg 0.69 to 3.00; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 4.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 2.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 1.43 to 4.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Medications Labs per Visit increased from avg 1.45 to 7.00; 5-COMMERCIAL – X-Ray CPT Codes Labs per Visit increased from avg 1.10 to 3.00; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 135.08 to 349.00; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 3.00; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 28.43 to 59.73; 4-MEDICAID – After Hours Labs per Visit increased from avg 2.04 to 4.20</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – DME Charge Amount increased from avg 133.93 to 689.80; 13-TRICARE – Vaccines Labs per Visit increased from avg 0.50 to 2.00; 3-MEDICARE – Medications Labs per Visit increased from avg 0.90 to 3.00; 13-TRICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.82 to 2.00; 4-MEDICAID – Self-pay physical &amp; No Charge Labs per Visit increased from avg 0.43 to 1.00; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.90 to 4.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.67 to 2.50; 18-CIGNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.94 to 7.00; 18-CIGNA – X-Ray CPT Codes Charge Amount increased from avg 240.79 to 607.00; 1-SELF PAY – Existing E/M Code Labs per Visit increased from avg 0.91 to 2.20; 4-MEDICAID – X-Ray CPT Codes Charge Amount increased from avg 339.20 to 769.00; 5-COMMERCIAL – Medications Payment per Visit increased from avg 14.74 to 32.75</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -60.44; 3-MEDICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.67 to 2.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -106.22; 13-TRICARE – New E/M Codes Labs per Visit increased from avg 1.32 to 3.50; 12-HUMANA – New E/M Codes Labs per Visit increased from avg 0.90 to 2.00; 1-SELF PAY – X-Ray CPT Codes Payment per Visit increased from avg 90.55 to 189.00</t>
+  </si>
+  <si>
+    <t>13-TRICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.82 to 6.00; 13-TRICARE – Medications Labs per Visit increased from avg 1.42 to 6.00; 5-COMMERCIAL – New E/M Codes Labs per Visit increased from avg 1.75 to 5.67; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 4.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.87 to 5.50; 5-COMMERCIAL – Medications Labs per Visit increased from avg 1.73 to 5.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 3.60 to -3.92; 5-COMMERCIAL – New E/M Codes Labs per Visit increased from avg 1.75 to 5.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.87 to 5.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit increased from avg 0.39 to 1.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 2.14 to 5.00; 3-MEDICARE – New E/M Codes Labs per Visit increased from avg 1.15 to 2.50</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -14.70; 3-MEDICARE – X-Ray CPT Codes Charge Billed Balance decreased from avg 3.31 to -4.99; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 50.76 to 155.00; 18-CIGNA – New E/M Codes Labs per Visit increased from avg 1.98 to 5.00; 1-SELF PAY – X-Ray CPT Codes Payment per Visit increased from avg 90.55 to 218.50; 3-MEDICARE – DME Charge Amount increased from avg 319.54 to 689.80</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 25.12 to 135.81; 5-COMMERCIAL – Medications Labs per Visit increased from avg 1.73 to 5.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 2.00; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 235.39 to 647.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.87 to 5.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 0.95 to 2.50</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -20.77; 15-UNITED HEALTHCARE – Vaccines Labs per Visit increased from avg 0.57 to 8.00; 3-MEDICARE – Medications Charge Billed Balance decreased from avg 1.05 to -2.50; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 116.93 to 415.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.87 to 6.00; 3-MEDICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -8.47 to -25.87</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -20.77; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 116.93 to 655.00; 1-SELF PAY – DME Charge Amount increased from avg 133.93 to 705.92; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 2.58 to 8.00; 15-UNITED HEALTHCARE – Self-pay physical &amp; No Charge Charge Amount increased from avg 17.33 to 52.00; 3-MEDICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -8.47 to -24.20</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -20.77; 3-MEDICARE – Medications Labs per Visit increased from avg 0.90 to 4.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 3.00; 1-SELF PAY – X-Ray CPT Codes Payment per Visit increased from avg 90.55 to 287.00; 13-TRICARE – Medications Labs per Visit increased from avg 1.42 to 4.00; 5-COMMERCIAL – New E/M Codes Labs per Visit increased from avg 1.75 to 4.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Medications Labs per Visit increased from avg 1.13 to 4.00; 15-UNITED HEALTHCARE – DME Payment per Visit increased from avg 73.28 to 207.02; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 135.08 to 360.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.87 to 4.20; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 2.33 to 5.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.94 to 4.00</t>
+  </si>
+  <si>
+    <t>13-TRICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 33.42 to -204.76; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 4.00; 1-SELF PAY – Medications Labs per Visit increased from avg 1.13 to 3.00; 13-TRICARE – Existing E/M Code Charge Billed Balance decreased from avg 88.96 to -55.40; 13-TRICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 28.64 to -14.26; 13-TRICARE – Existing E/M Code Labs per Visit increased from avg 1.42 to 3.33</t>
+  </si>
+  <si>
+    <t>13-TRICARE – Existing E/M Code Labs per Visit increased from avg 1.42 to 7.00; 13-TRICARE – Medications Labs per Visit increased from avg 1.42 to 7.00; 13-TRICARE – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.66 to 7.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 51.31 to 201.33; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 2.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 174.38 to 504.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 0.95 to 2.00; 15-UNITED HEALTHCARE – Medications Labs per Visit increased from avg 1.45 to 3.00; 3-MEDICARE – New E/M Codes Labs per Visit increased from avg 1.15 to 2.33; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes NRV Zero Balance decreased from avg 27.53 to 0.50; 13-TRICARE – New E/M Codes Labs per Visit increased from avg 1.32 to 2.50; 15-UNITED HEALTHCARE – DME NRV Zero Balance decreased from avg 73.88 to 8.38</t>
+  </si>
+  <si>
+    <t>18-CIGNA – X-Ray CPT Codes Labs per Visit increased from avg 0.69 to 2.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 2.14 to 6.00; 5-COMMERCIAL – New E/M Codes Payment per Visit increased from avg 142.42 to 342.70; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 3.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 1.67; 5-COMMERCIAL – Existing E/M Code Labs per Visit increased from avg 2.15 to 5.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 2.74 to -329.00; 18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -33.96; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 25.96 to -463.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 3.00; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -116.80; 5-COMMERCIAL – Existing E/M Code Payment per Visit increased from avg 115.74 to 409.50</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -383.59; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -313.71; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 25.96 to -122.70; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -208.13; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit increased from avg 0.88 to 4.00; 18-CIGNA – X-Ray CPT Codes Labs per Visit increased from avg 0.69 to 3.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -70.00; 1-SELF PAY – X-Ray CPT Codes Visit Count increased from avg 2.51 to 8.00; 1-SELF PAY – X-Ray CPT Codes Charge Amount increased from avg 235.81 to 735.00; 12-HUMANA – Existing E/M Code Labs per Visit increased from avg 1.20 to 3.00; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 3.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 1.67</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -150.00; 18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -47.43; 3-MEDICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -8.47 to -154.66; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.96 to -163.95; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -204.84; 5-COMMERCIAL – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 52.19 to -129.00</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -85.21; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -317.35; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -203.50; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 15.12 to -163.48; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.96 to -208.94; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -266.78</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -273.29; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -127.16; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.50 to -223.08; 5-COMMERCIAL – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 29.61 to -148.26; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 15.12 to -66.78; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 25.96 to -109.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -48.64; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -160.99; 15-UNITED HEALTHCARE – DME Labs per Visit increased from avg 0.10 to 2.00; 18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -18.72; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 15.12 to -148.04; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.96 to -118.28</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -15.53; 15-UNITED HEALTHCARE – Vaccines Charge Billed Balance decreased from avg -10.71 to -150.00; 15-UNITED HEALTHCARE – Vaccines Payment per Visit increased from avg 82.57 to 318.92; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -15.14; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -73.99; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Zero Balance Collection Rate increased from avg 0.35 to 1.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -18.59; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -202.89; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 25.12 to 166.19; 3-MEDICARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -8.47 to -50.26; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -152.09; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -11.65</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -92.15; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -135.15; 5-COMMERCIAL – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 2.74 to -39.70; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 15.12 to -117.84; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -51.44; 4-MEDICAID – Self-pay physical &amp; No Charge Labs per Visit increased from avg 0.43 to 3.00</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -293.19; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -166.67; 12-HUMANA – X-Ray CPT Codes Charge Billed Balance decreased from avg -1.21 to -25.51; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -133.31; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.96 to -300.32; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -243.09</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -54.03; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -110.00; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -61.14; 13-TRICARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 47.27 to 373.44; 13-TRICARE – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 200.53 to 1434.00; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.96 to -108.07</t>
+  </si>
+  <si>
+    <t>12-HUMANA – New E/M Codes Charge Billed Balance decreased from avg 0.44 to -105.00; 12-HUMANA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -7.37 to -104.90; 13-TRICARE – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 200.53 to 752.00; 12-HUMANA – Medications Charge Amount increased from avg 103.29 to 355.00; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -8.58; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 29.89 to 75.60</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 18.72 to -134.15; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 50.76 to 200.00; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 2.76 to -5.18; 18-CIGNA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 51.31 to 182.96; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 12.09 to -16.34; 3-MEDICARE – New E/M Codes Charge Amount increased from avg 667.84 to 1860.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -88.35; 12-HUMANA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 35.91 to 216.28; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 29.89 to 114.54; 18-CIGNA – Medications Charge Amount increased from avg 210.12 to 730.00; 12-HUMANA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 155.71 to 450.00; 12-HUMANA – Procedures &amp; Surgical CPT Codes Zero Balance Collection Rate increased from avg 0.18 to 0.48</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – Self-pay physical &amp; No Charge Charge Amount increased from avg 7.86 to 45.00; 12-HUMANA – New E/M Codes Charge Billed Balance decreased from avg 0.44 to -1.25; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -24.47; 4-MEDICAID – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 70.72 to -110.00; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 15.12 to -20.00; 4-MEDICAID – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 162.82 to -191.91</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -164.28; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 15.12 to -90.00; 3-MEDICARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 18.72 to -110.54; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 62.96 to 296.13; 3-MEDICARE – New E/M Codes Charge Billed Balance decreased from avg 45.73 to -123.57; 5-COMMERCIAL – X-Ray CPT Codes Charge Billed Balance decreased from avg 17.35 to -35.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -209.42; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 29.89 to 266.27; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 267.01 to 2000.00; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 25.96 to -137.70; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.96 to -106.83; 3-MEDICARE – Medications Charge Billed Balance decreased from avg 1.05 to -2.63</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -73.35; 3-MEDICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 2.08 to -11.46; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -40.52; 3-MEDICARE – New E/M Codes Charge Amount increased from avg 667.84 to 2170.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 0.95 to 3.00; 5-COMMERCIAL – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 52.19 to -52.21</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – Self-pay physical &amp; No Charge Charge Amount increased from avg 7.86 to 65.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Billed Balance decreased from avg -11.50 to -61.00; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 9.06 to -14.10; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -25.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 0.95 to 3.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 4.39 to -5.11</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – DME Zero-Balance Collection Dollar Impact decreased from avg 12.37 to -93.40; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -18.96 to -71.17; 5-COMMERCIAL – Lab/Test CPT Codes Collection Rate increased from avg 0.28 to 1.00; 1-SELF PAY – X-Ray CPT Codes Visit Count increased from avg 2.51 to 9.00; 1-SELF PAY – X-Ray CPT Codes Charge Amount increased from avg 235.81 to 800.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit increased from avg 0.88 to 3.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg -0.06 to -150.00; 3-MEDICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 2.08 to -121.51; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -262.19; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 62.96 to 381.15; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -36.34 to -162.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Payment per Visit increased from avg 30.24 to 100.00</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Vaccines Labs per Visit increased from avg 0.31 to 2.50; 1-SELF PAY – Vaccines Charge Amount increased from avg 296.43 to 1400.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 174.38 to 652.20; 18-CIGNA – Vaccines Charge Amount increased from avg 165.00 to 532.00; 1-SELF PAY – Vaccines Payment per Visit increased from avg 124.23 to 350.00; 18-CIGNA – Vaccines Payment per Visit increased from avg 81.62 to 206.84</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 28.43 to 230.73; 4-MEDICAID – DME Charge Amount increased from avg 682.71 to 2507.08; 4-MEDICAID – Medications Payment per Visit increased from avg 15.29 to 53.18; 4-MEDICAID – Medications Charge Amount increased from avg 201.17 to 690.00; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 135.08 to 450.00; 4-MEDICAID – DME Visit Count increased from avg 1.67 to 5.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Vaccines Charge Amount increased from avg 296.43 to 2145.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 267.01 to 1382.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 29.89 to 142.38; 1-SELF PAY – Vaccines Visit Count increased from avg 2.07 to 7.00; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 25.12 to 70.54; 13-TRICARE – New E/M Codes Labs per Visit increased from avg 1.32 to 3.67</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 225.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 63.06 to 293.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg -36.34 to 82.60; 2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg -4.05 to 6.35; 2-BCBS – After Hours NRV Zero Balance increased from avg 2.08 to 6.73; 15-UNITED HEALTHCARE – Medications NRV Zero Balance increased from avg 22.82 to 69.82</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 12.20 to 54.56; 4-MEDICAID – Procedures &amp; Surgical CPT Codes NRV Zero Balance increased from avg 43.58 to 108.38; 5-COMMERCIAL – Medications NRV Zero Balance increased from avg 15.12 to 33.64; 13-TRICARE – Procedures &amp; Surgical CPT Codes NRV Zero Balance increased from avg 45.55 to 100.28; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 15.12 to 32.15; 12-HUMANA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -7.37 to 0.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – Medications NRV Zero Balance increased from avg 16.26 to 33.86; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -7.37 to 0.00; 12-HUMANA – New E/M Codes Labs per Visit decreased from avg 0.90 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg -36.34 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – DME NRV Zero Balance increased from avg 140.68 to 473.50; 12-HUMANA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -7.37 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg -36.34 to 0.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.88 to 0.00; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 0.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 9.06 to 165.58; 15-UNITED HEALTHCARE – Medications NRV Zero Balance increased from avg 22.82 to 112.53; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance increased from avg 64.00 to 199.00; 1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 12-HUMANA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -7.37 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 0.72 to 7.38; 3-MEDICARE – X-Ray CPT Codes NRV Zero Balance increased from avg 30.60 to 61.21; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.82 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg -36.34 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg -16.11 to 55.28; 15-UNITED HEALTHCARE – DME NRV Zero Balance increased from avg 73.88 to 181.96; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg -0.06 to 49.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg 0.26 to 5.51; 12-HUMANA – Existing E/M Code Charge Billed Balance increased from avg 10.28 to 100.00; 5-COMMERCIAL – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 52.19 to 278.37; 5-COMMERCIAL – New E/M Codes Charge Billed Balance increased from avg 122.16 to 287.00; 12-HUMANA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -7.37 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 2.08 to 20.68; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – Existing E/M Code Labs per Visit decreased from avg 1.20 to 0.00; 13-TRICARE – New E/M Codes Labs per Visit decreased from avg 1.32 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Procedures &amp; Surgical CPT Codes NRV Zero Balance increased from avg 28.43 to 59.73; 1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Medications Charge Billed Balance increased from avg 14.47 to 100.00; 17-AETNA – Medications Zero-Balance Collection Dollar Impact increased from avg 4.43 to 18.78; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg 51.63 to 204.56; 17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 63.76 to 245.00; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Medications NRV Zero Balance increased from avg 15.12 to 32.75; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -7.37 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00; 13-TRICARE – New E/M Codes Labs per Visit decreased from avg 1.32 to 0.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -7.37 to 0.00; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 0.00; 18-CIGNA – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg -18.96 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 76.76; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 15.12 to 90.65; 5-COMMERCIAL – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 29.61 to 135.79; 17-AETNA – Procedures &amp; Surgical CPT Codes NRV Zero Balance increased from avg 34.92 to 150.69; 5-COMMERCIAL – Lab/Test CPT Codes Charge Billed Balance increased from avg 74.50 to 293.00; 5-COMMERCIAL – New E/M Codes Charge Billed Balance increased from avg 122.16 to 310.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 160.00; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 284.35; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg -16.11 to 96.94; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 364.54; 2-BCBS – After Hours Zero-Balance Collection Dollar Impact increased from avg 0.27 to 1.60; 2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg -4.05 to 12.26</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg -4.05 to 17.57; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 30.27; 17-AETNA – DME NRV Zero Balance increased from avg 179.12 to 368.10; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 9.06 to 186.19; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes NRV Zero Balance increased from avg 27.53 to 135.81; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 15.12 to 72.48; 1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 2.08 to 12.33; 17-AETNA – Procedures &amp; Surgical CPT Codes NRV Zero Balance increased from avg 34.92 to 137.69; 17-AETNA – DME NRV Zero Balance increased from avg 179.12 to 529.98; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.66 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 205.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg -36.34 to 65.97; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 9.06 to 21.94; 4-MEDICAID – DME NRV Zero Balance increased from avg 137.19 to 299.11; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 29.34; 17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 63.76 to 241.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact increased from avg 2.30 to 6.84; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg 51.63 to 143.36; 1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – New E/M Codes Labs per Visit decreased from avg 0.86 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg 2.74 to 167.50; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 241.00; 5-COMMERCIAL – Lab/Test CPT Codes Charge Billed Balance increased from avg 74.50 to 293.00; 15-UNITED HEALTHCARE – DME NRV Zero Balance increased from avg 73.88 to 207.02; 1-SELF PAY – Medications Charge Amount decreased from avg 65.92 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 2.76 to 89.00; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 9.06 to 138.67; 2-BCBS – Vaccines NRV Zero Balance increased from avg 69.01 to 345.09; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance increased from avg 64.00 to 310.00; 4-MEDICAID – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 3.60 to 11.27; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Procedures &amp; Surgical CPT Codes NRV Zero Balance increased from avg 49.02 to 201.33; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – New E/M Codes Labs per Visit decreased from avg 1.32 to 0.00; 13-TRICARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.82 to 0.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.88 to 0.00; 18-CIGNA – X-Ray CPT Codes Labs per Visit decreased from avg 0.69 to 0.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 12-HUMANA – New E/M Codes Labs per Visit decreased from avg 0.90 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00; 13-TRICARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.82 to 0.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.88 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – New E/M Codes NRV Zero Balance increased from avg 161.13 to 342.70; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.82 to 0.00; 17-AETNA – New E/M Codes Labs per Visit decreased from avg 1.59 to 0.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.94 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 230.61; 5-COMMERCIAL – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 29.61 to 567.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg -4.05 to 66.03; 4-MEDICAID – Vaccines Charge Billed Balance increased from avg 51.20 to 411.00; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 416.22; 5-COMMERCIAL – Lab/Test CPT Codes Charge Billed Balance increased from avg 74.50 to 525.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg -0.06 to 9.90; 2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 0.36 to 32.81; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 714.85; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 1243.38; 13-TRICARE – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 1.45 to 26.10; 13-TRICARE – Medications Zero-Balance Collection Dollar Impact increased from avg 2.63 to 21.77</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 31.40; 12-HUMANA – New E/M Codes Charge Billed Balance increased from avg 0.44 to 79.87; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 4.95 to 104.00; 17-AETNA – Medications Zero-Balance Collection Dollar Impact increased from avg 4.43 to 78.70; 12-HUMANA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -7.37 to 110.74; 4-MEDICAID – X-Ray CPT Codes Charge Billed Balance increased from avg 11.37 to 128.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – Medications Charge Billed Balance increased from avg 3.82 to 110.00; 4-MEDICAID – Medications Zero-Balance Collection Dollar Impact increased from avg 1.28 to 17.85; 15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 9.06 to 96.81; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance increased from avg 101.89 to 781.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 62.39 to 475.17; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 37.41</t>
   </si>
   <si>
     <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 148.79; 13-TRICARE – Existing E/M Code Charge Billed Balance increased from avg 88.96 to 735.00; 13-TRICARE – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg 33.42 to 274.20; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 23.63 to 158.72; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 23.50 to 140.31; 18-CIGNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 12.20 to 69.21</t>
   </si>
   <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 205.00; 12-HUMANA – New E/M Codes Charge Billed Balance increased from avg 0.44 to 55.00; 13-TRICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 25.52 to 491.52; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 159.50; 13-TRICARE – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg 33.42 to 321.00; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 446.33</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – DME Labs per Visit increased from avg 0.10 to 2.00; 4-MEDICAID – Medications Zero-Balance Collection Dollar Impact increased from avg 1.09 to 20.93; 17-AETNA – DME Zero-Balance Collection Dollar Impact increased from avg 10.48 to 188.61; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg 5.70 to 66.02; 4-MEDICAID – Medications Charge Billed Balance increased from avg 3.82 to 40.00; 4-MEDICAID – Lab/Test CPT Codes Charge Billed Balance increased from avg 231.39 to 1782.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 213.84; 18-CIGNA – X-Ray CPT Codes Charge Billed Balance increased from avg 6.24 to 115.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 5.67 to 98.76; 18-CIGNA – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 2.18 to 31.18; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 12.09 to 152.00; 5-COMMERCIAL – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 41.75 to 480.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg 1.93 to 63.81; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 96.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 23.50 to 202.12; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 220.00; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 15.12 to 111.96; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 62.39 to 457.11</t>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 205.00; 12-HUMANA – New E/M Codes Charge Billed Balance increased from avg 0.44 to 55.00; 13-TRICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 28.64 to 491.52; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 159.50; 13-TRICARE – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg 33.42 to 321.00; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 446.33</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – Medications Zero-Balance Collection Dollar Impact increased from avg 1.28 to 20.93; 17-AETNA – DME Zero-Balance Collection Dollar Impact increased from avg 15.72 to 188.61; 4-MEDICAID – Medications Charge Billed Balance increased from avg 3.82 to 40.00; 4-MEDICAID – Lab/Test CPT Codes Charge Billed Balance increased from avg 231.39 to 1782.00; 4-MEDICAID – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 70.81 to 527.27; 13-TRICARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 98.89 to 690.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 213.84; 18-CIGNA – X-Ray CPT Codes Charge Billed Balance increased from avg 6.24 to 115.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 6.18 to 98.76; 18-CIGNA – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 2.39 to 31.18; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 12.09 to 152.00; 5-COMMERCIAL – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 52.19 to 480.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 96.00; 5-COMMERCIAL – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg 2.74 to 63.81; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 23.50 to 202.12; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 220.00; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 15.12 to 111.96; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 62.39 to 457.11</t>
   </si>
   <si>
     <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 462.26; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg -16.11 to 371.95; 12-HUMANA – Existing E/M Code Charge Billed Balance increased from avg 10.28 to 195.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg -4.05 to 25.65; 13-TRICARE – Existing E/M Code Charge Billed Balance increased from avg 88.96 to 735.00; 13-TRICARE – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg 33.42 to 267.60</t>
   </si>
   <si>
-    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 358.55; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 125.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 17.97 to 436.00; 5-COMMERCIAL – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 3.19 to 63.75; 2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg -4.05 to 68.99; 18-CIGNA – Vaccines Charge Billed Balance increased from avg 7.00 to 131.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg 1.93 to 98.94; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg 5.70 to 98.69; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 436.00; 3-MEDICARE – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 13.65 to 156.59; 5-COMMERCIAL – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 41.75 to 452.62; 4-MEDICAID – X-Ray CPT Codes Charge Billed Balance increased from avg 11.37 to 123.00</t>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 358.55; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 125.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 17.97 to 436.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg -4.05 to 68.99; 18-CIGNA – Vaccines Charge Billed Balance increased from avg 7.00 to 131.00; 5-COMMERCIAL – X-Ray CPT Codes Charge Billed Balance increased from avg 17.35 to 246.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Existing E/M Code Zero-Balance Collection Dollar Impact increased from avg 2.74 to 98.94; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 436.00; 4-MEDICAID – X-Ray CPT Codes Charge Billed Balance increased from avg 11.37 to 123.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg 9.69 to 98.69; 4-MEDICAID – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 3.60 to 35.69; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 98.28 to 861.07</t>
   </si>
   <si>
     <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 245.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 160.00; 13-TRICARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 45.89 to 752.00; 17-AETNA – Medications Charge Billed Balance increased from avg 14.47 to 192.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg -4.05 to 34.11; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 90.70</t>
   </si>
   <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 145.00; 3-MEDICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 1.82 to 185.94; 3-MEDICARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 9.57 to 450.00; 2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 0.36 to 14.87; 15-UNITED HEALTHCARE – Medications Zero-Balance Collection Dollar Impact increased from avg 2.95 to 67.66; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 149.46</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg -0.06 to 89.00; 15-UNITED HEALTHCARE – DME Zero-Balance Collection Dollar Impact increased from avg 0.92 to 19.38; 17-AETNA – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 11.15 to 78.65; 12-HUMANA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 30.78 to 216.28; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 49.67; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 136.00</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg -0.05 to 6.53; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 110.85; 12-HUMANA – Medications Charge Billed Balance increased from avg 2.86 to 40.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 63.06 to 736.00; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 210.00; 3-MEDICARE – DME Charge Billed Balance increased from avg 8.62 to 69.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 9.06 to 407.68; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 192.67; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 63.06 to 841.78; 13-TRICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 25.52 to 337.34; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance increased from avg 64.00 to 814.36; 2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 0.36 to 3.57</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 20.27; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 167.92; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg 4.07 to 98.43; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 20.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 12.09 to 208.00; 4-MEDICAID – X-Ray CPT Codes Charge Billed Balance increased from avg 11.37 to 163.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 20.27; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 585.00; 3-MEDICARE – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 13.65 to 288.42; 2-BCBS – DME Labs per Visit increased from avg 0.05 to 1.00; 3-MEDICARE – X-Ray CPT Codes Charge Billed Balance increased from avg 3.31 to 36.46; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 15.12 to 140.44</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 46.18; 17-AETNA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 56.31 to 997.19; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 98.67; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 211.52 to 2187.00; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 15.12 to 151.96; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 245.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 0.36 to 76.94; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 123.00; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 88.71; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 267.63; 15-UNITED HEALTHCARE – Medications Charge Billed Balance increased from avg 3.48 to 110.00; 18-CIGNA – Medications Zero-Balance Collection Dollar Impact increased from avg 0.76 to 18.26</t>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 145.00; 3-MEDICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 2.08 to 185.94; 3-MEDICARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 9.57 to 450.00; 2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 0.36 to 14.87; 15-UNITED HEALTHCARE – Medications Zero-Balance Collection Dollar Impact increased from avg 3.67 to 67.66; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 149.46</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg -0.06 to 89.00; 15-UNITED HEALTHCARE – DME Zero-Balance Collection Dollar Impact increased from avg 1.21 to 19.38; 12-HUMANA – Procedures &amp; Surgical CPT Codes NRV Zero Balance increased from avg 30.05 to 216.28; 17-AETNA – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 11.49 to 78.65; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 49.67; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 136.00</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg -0.06 to 6.53; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 110.85; 12-HUMANA – Medications Charge Billed Balance increased from avg 2.86 to 40.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 63.06 to 736.00; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 210.00; 3-MEDICARE – DME Charge Billed Balance increased from avg 8.62 to 69.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 9.06 to 407.68; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 192.67; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 63.06 to 841.78; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance increased from avg 64.00 to 814.36; 13-TRICARE – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact increased from avg 28.64 to 337.34; 2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 0.36 to 3.57</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 20.27; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 167.92; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact increased from avg 4.39 to 98.43; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 20.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 12.09 to 208.00; 4-MEDICAID – X-Ray CPT Codes Charge Billed Balance increased from avg 11.37 to 163.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 20.27; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 585.00; 3-MEDICARE – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 18.72 to 288.42; 3-MEDICARE – X-Ray CPT Codes Charge Billed Balance increased from avg 3.31 to 36.46; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 15.12 to 140.44; 3-MEDICARE – New E/M Codes Charge Billed Balance increased from avg 45.73 to 290.71</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 46.18; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 98.67; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 15.12 to 151.96; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 245.00; 5-COMMERCIAL – X-Ray CPT Codes Charge Billed Balance increased from avg 17.35 to 123.00; 18-CIGNA – New E/M Codes Charge Billed Balance increased from avg 61.06 to 310.98</t>
+  </si>
+  <si>
+    <t>2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact increased from avg 0.36 to 76.94; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 123.00; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 88.71; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 267.63; 15-UNITED HEALTHCARE – Medications Charge Billed Balance increased from avg 3.48 to 110.00; 18-CIGNA – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg 15.12 to 298.92</t>
   </si>
   <si>
     <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 40.54; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact increased from avg -11.19 to 340.70; 2-BCBS – Medications Charge Billed Balance increased from avg 3.79 to 70.60; 18-CIGNA – X-Ray CPT Codes Charge Billed Balance increased from avg 6.24 to 72.00; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 35.52; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 520.17</t>
   </si>
   <si>
-    <t>18-CIGNA – Vaccines Labs per Visit increased from avg 0.31 to 2.50; 1-SELF PAY – Vaccines Charge Amount increased from avg 296.43 to 1400.00; 2-BCBS – Self-pay physical &amp; No Charge Payment per Visit increased from avg 7.67 to 35.00; 4-MEDICAID – Self-pay physical &amp; No Charge Payment per Visit increased from avg 15.32 to 65.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 174.38 to 652.20; 18-CIGNA – Vaccines Charge Amount increased from avg 165.00 to 532.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 23.02 to 230.73; 4-MEDICAID – Medications Payment per Visit increased from avg 14.20 to 53.18; 4-MEDICAID – DME Charge Amount increased from avg 682.71 to 2507.08; 4-MEDICAID – Medications Charge Amount increased from avg 201.17 to 690.00; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 135.08 to 450.00; 4-MEDICAID – DME Visit Count increased from avg 1.67 to 5.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Vaccines Charge Amount increased from avg 296.43 to 2145.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 267.01 to 1382.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 29.17 to 142.38; 1-SELF PAY – Vaccines Visit Count increased from avg 2.07 to 7.00; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 23.95 to 70.54; 13-TRICARE – New E/M Codes Labs per Visit increased from avg 1.32 to 3.67</t>
+    <t>18-CIGNA – Procedures &amp; Surgical CPT Codes NRV Zero Balance increased from avg 49.02 to 159.70; 17-AETNA – X-Ray CPT Codes NRV Zero Balance increased from avg 54.42 to 141.77; 15-UNITED HEALTHCARE – Lab/Test CPT Codes NRV Zero Balance increased from avg 34.40 to 76.25; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount decreased from avg 116.93 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Procedures &amp; Surgical CPT Codes NRV Zero Balance increased from avg 28.43 to 230.73; 2-BCBS – Medications NRV Zero Balance increased from avg 18.08 to 67.53; 4-MEDICAID – Medications NRV Zero Balance increased from avg 16.26 to 53.18; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance increased from avg 45.56 to 98.08; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 12-HUMANA – New E/M Codes Labs per Visit decreased from avg 0.90 to 0.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – Procedures &amp; Surgical CPT Codes NRV Zero Balance increased from avg 43.58 to 410.81; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes NRV Zero Balance increased from avg 27.53 to 65.24; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount decreased from avg 116.93 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.90 to 0.00</t>
   </si>
   <si>
     <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to 0.00</t>
   </si>
   <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Existing E/M Code Labs per Visit decreased from avg 1.75 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance decreased from avg 22.59 to 0.00; 17-AETNA – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 11.15 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – After Hours Labs per Visit decreased from avg 2.15 to 0.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to -37.05; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 5.70 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance decreased from avg 22.59 to 0.00; 17-AETNA – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 11.15 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to -177.97; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero Balance Collection Rate decreased from avg 0.16 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – New E/M Codes Visit Count decreased from avg 8.71 to 2.00; 17-AETNA – New E/M Codes Charge Amount decreased from avg 2631.41 to 620.00; 17-AETNA – Existing E/M Code Charge Amount decreased from avg 1291.98 to 405.00; 17-AETNA – New E/M Codes Labs per Visit decreased from avg 1.59 to 0.50; 17-AETNA – Lab/Test CPT Codes Charge Amount decreased from avg 1570.78 to 555.00; 17-AETNA – Existing E/M Code Visit Count decreased from avg 5.52 to 2.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – New E/M Codes Visit Count decreased from avg 8.71 to 2.00; 17-AETNA – New E/M Codes Charge Amount decreased from avg 2631.41 to 620.00; 17-AETNA – Existing E/M Code Charge Amount decreased from avg 1291.98 to 650.00; 17-AETNA – Lab/Test CPT Codes Visit Count decreased from avg 7.50 to 4.00; 17-AETNA – Existing E/M Code Visit Count decreased from avg 5.52 to 3.00; 17-AETNA – Lab/Test CPT Codes Charge Amount decreased from avg 1570.78 to 911.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – New E/M Codes Labs per Visit decreased from avg 1.59 to 0.00; 17-AETNA – Medications Labs per Visit decreased from avg 1.60 to 0.00; 17-AETNA – X-Ray CPT Codes Labs per Visit decreased from avg 0.80 to 0.00; 17-AETNA – New E/M Codes Visit Count decreased from avg 8.71 to 2.00; 17-AETNA – New E/M Codes Charge Amount decreased from avg 2631.41 to 620.00; 17-AETNA – X-Ray CPT Codes Charge Amount decreased from avg 292.71 to 123.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -3.54; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – DME Charge Billed Balance decreased from avg 149.25 to 0.00; 17-AETNA – DME Zero-Balance Collection Dollar Impact decreased from avg 10.48 to 0.00; 17-AETNA – DME Zero Balance Collection Rate decreased from avg 0.38 to 0.10; 17-AETNA – DME Payment per Visit decreased from avg 126.37 to 75.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to -15.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -1.02; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 5.70 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00; 17-AETNA – Medications Zero-Balance Collection Dollar Impact decreased from avg 3.36 to 0.00; 17-AETNA – Medications Labs per Visit decreased from avg 1.60 to 0.00; 17-AETNA – X-Ray CPT Codes Payment per Visit decreased from avg 49.48 to 25.20; 17-AETNA – Medications Visit Count decreased from avg 1.48 to 1.00; 17-AETNA – Medications Charge Amount decreased from avg 135.48 to 94.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to -0.26; 17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00; 17-AETNA – Medications Zero-Balance Collection Dollar Impact decreased from avg 3.36 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 5.70 to 0.00; 17-AETNA – Vaccines Zero Balance Collection Rate decreased from avg 0.54 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -222.20; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to -132.51; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to -63.72; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -70.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to -6.56; 17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00; 17-AETNA – Medications Zero-Balance Collection Dollar Impact decreased from avg 3.36 to 0.00; 17-AETNA – Medications Zero Balance Collection Rate decreased from avg 0.15 to 0.00; 17-AETNA – Medications Payment per Visit decreased from avg 14.32 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to 0.00; 17-AETNA – New E/M Codes Labs per Visit decreased from avg 1.59 to 1.00; 17-AETNA – Lab/Test CPT Codes Charge Amount decreased from avg 1570.78 to 1102.00; 17-AETNA – New E/M Codes Visit Count decreased from avg 8.71 to 7.00; 17-AETNA – Lab/Test CPT Codes Labs per Visit decreased from avg 2.95 to 2.43</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00; 17-AETNA – Medications Zero-Balance Collection Dollar Impact decreased from avg 3.36 to 0.00; 17-AETNA – Medications Zero Balance Collection Rate decreased from avg 0.15 to 0.00; 17-AETNA – Medications Payment per Visit decreased from avg 14.32 to 0.00</t>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 211.52 to 565.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 1.56 to 4.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 5.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Medications Labs per Visit increased from avg 1.60 to 7.00; 17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 3.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.67; 17-AETNA – Medications Charge Amount increased from avg 135.48 to 305.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 211.52 to 464.00; 17-AETNA – Medications Visit Count increased from avg 1.48 to 3.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 5.00; 17-AETNA – Existing E/M Code Labs per Visit increased from avg 1.75 to 4.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Medications Labs per Visit increased from avg 1.60 to 9.00; 17-AETNA – Lab/Test CPT Codes Labs per Visit increased from avg 2.95 to 6.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance decreased from avg 22.59 to 0.00; 17-AETNA – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 11.49 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 7.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – New E/M Codes Labs per Visit increased from avg 1.59 to 3.50; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Zero Balance Collection Rate increased from avg 0.27 to 0.66; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Rate increased from avg 0.30 to 0.66; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to -37.05; 17-AETNA – After Hours Labs per Visit increased from avg 2.15 to 5.00; 17-AETNA – Existing E/M Code Labs per Visit increased from avg 1.75 to 4.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 4.00; 17-AETNA – DME Payment per Visit increased from avg 174.97 to 368.10; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance decreased from avg 22.59 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – DME Payment per Visit increased from avg 174.97 to 529.98; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Medications Charge Amount increased from avg 135.48 to 334.00; 17-AETNA – Medications Visit Count increased from avg 1.48 to 3.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to -177.97; 17-AETNA – New E/M Codes Labs per Visit increased from avg 1.59 to 5.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Rate increased from avg 0.30 to 0.50</t>
+  </si>
+  <si>
+    <t>17-AETNA – Medications Visit Count increased from avg 1.48 to 3.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Labs per Visit increased from avg 1.75 to 2.50; 17-AETNA – After Hours Payment per Visit increased from avg 5.52 to 7.60; 17-AETNA – Existing E/M Code NRV Zero Balance decreased from avg 150.29 to 114.30; 17-AETNA – Lab/Test CPT Codes NRV Zero Balance decreased from avg 86.49 to 73.89; 17-AETNA – New E/M Codes NRV Zero Balance decreased from avg 213.66 to 204.75; 17-AETNA – New E/M Codes Avg. Charge E/M Weight increased from avg 3.89 to 4.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Labs per Visit increased from avg 1.75 to 2.67; 17-AETNA – Existing E/M Code NRV Zero Balance decreased from avg 150.29 to 121.34; 17-AETNA – Lab/Test CPT Codes Payment per Visit increased from avg 79.57 to 91.06; 17-AETNA – After Hours NRV Zero Balance decreased from avg 5.52 to 5.07; 17-AETNA – New E/M Codes NRV Zero Balance decreased from avg 213.66 to 205.00; 17-AETNA – New E/M Codes Avg. Charge E/M Weight increased from avg 3.89 to 4.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Labs per Visit increased from avg 1.75 to 3.33; 17-AETNA – After Hours Charge Amount increased from avg 170.58 to 322.00; 17-AETNA – After Hours Visit Count increased from avg 3.75 to 7.00; 17-AETNA – Lab/Test CPT Codes Labs per Visit increased from avg 2.95 to 4.00; 17-AETNA – X-Ray CPT Codes NRV Zero Balance decreased from avg 54.42 to 39.91; 17-AETNA – Lab/Test CPT Codes NRV Zero Balance decreased from avg 86.49 to 68.61</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 6.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Lab/Test CPT Codes Charge Amount increased from avg 1570.78 to 4744.00; 17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.33; 17-AETNA – X-Ray CPT Codes Visit Count increased from avg 2.12 to 6.00; 17-AETNA – X-Ray CPT Codes Charge Amount increased from avg 292.71 to 760.00; 17-AETNA – Lab/Test CPT Codes Visit Count increased from avg 7.50 to 18.00; 17-AETNA – New E/M Codes Visit Count increased from avg 8.71 to 18.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Medications Zero Balance Collection Rate increased from avg 0.19 to 0.67; 17-AETNA – X-Ray CPT Codes Payment per Visit increased from avg 50.98 to 159.11; 17-AETNA – Medications Payment per Visit increased from avg 18.88 to 51.89; 17-AETNA – Medications Charge Amount increased from avg 135.48 to 350.00; 17-AETNA – Medications Collection Rate increased from avg 0.18 to 0.44; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to -15.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Lab/Test CPT Codes Visit Count increased from avg 7.50 to 21.00; 17-AETNA – Lab/Test CPT Codes Charge Amount increased from avg 1570.78 to 4359.00; 17-AETNA – New E/M Codes Charge Amount increased from avg 2631.41 to 6745.00; 17-AETNA – New E/M Codes Visit Count increased from avg 8.71 to 22.00; 17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.00; 17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Lab/Test CPT Codes Charge Amount increased from avg 1570.78 to 4470.00; 17-AETNA – New E/M Codes Charge Amount increased from avg 2631.41 to 7365.00; 17-AETNA – New E/M Codes Visit Count increased from avg 8.71 to 24.00; 17-AETNA – Lab/Test CPT Codes Visit Count increased from avg 7.50 to 19.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to -0.26; 17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -222.20; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to -132.51; 17-AETNA – Lab/Test CPT Codes Charge Amount increased from avg 1570.78 to 4615.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to -63.72; 17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.00; 17-AETNA – Lab/Test CPT Codes Visit Count increased from avg 7.50 to 18.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -70.00; 17-AETNA – X-Ray CPT Codes Collection Rate increased from avg 0.36 to 1.00; 17-AETNA – X-Ray CPT Codes Payment per Visit increased from avg 50.98 to 131.50; 17-AETNA – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 1.56 to 4.00; 17-AETNA – X-Ray CPT Codes Zero Balance Collection Rate increased from avg 0.39 to 1.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero Balance Collection Rate increased from avg 0.27 to 0.63</t>
+  </si>
+  <si>
+    <t>17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.42 to 0.76; 17-AETNA – Lab/Test CPT Codes Collection Rate increased from avg 0.38 to 0.60; 17-AETNA – New E/M Codes Payment per Visit increased from avg 205.14 to 271.21; 17-AETNA – New E/M Codes Collection Rate increased from avg 0.68 to 0.87</t>
+  </si>
+  <si>
+    <t>17-AETNA – Medications Labs per Visit increased from avg 1.60 to 4.00; 17-AETNA – X-Ray CPT Codes Charge Amount increased from avg 292.71 to 650.00; 17-AETNA – X-Ray CPT Codes Payment per Visit increased from avg 50.98 to 103.03; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00</t>
   </si>
   <si>
     <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -14.56; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to 0.00; 17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00</t>
   </si>
   <si>
-    <t>17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00; 17-AETNA – Medications Zero-Balance Collection Dollar Impact decreased from avg 3.36 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 56.31 to 5.92; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Amount decreased from avg 211.52 to 61.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 56.31 to 11.77; 17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.89 to 0.50; 17-AETNA – X-Ray CPT Codes Payment per Visit decreased from avg 49.48 to 20.04; 17-AETNA – Lab/Test CPT Codes Payment per Visit decreased from avg 79.57 to 35.52; 17-AETNA – New E/M Codes Labs per Visit decreased from avg 1.59 to 1.17; 17-AETNA – Lab/Test CPT Codes Labs per Visit decreased from avg 2.95 to 2.18</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Zero-Balance Collection Dollar Impact decreased from avg 3.36 to 0.00; 17-AETNA – Medications Zero Balance Collection Rate decreased from avg 0.15 to 0.00; 17-AETNA – Medications Labs per Visit decreased from avg 1.60 to 0.00; 17-AETNA – Medications Payment per Visit decreased from avg 14.32 to 0.00; 17-AETNA – DME Zero-Balance Collection Dollar Impact decreased from avg 10.48 to 0.00; 17-AETNA – DME Zero Balance Collection Rate decreased from avg 0.38 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Zero-Balance Collection Dollar Impact decreased from avg 3.36 to 0.00; 17-AETNA – Medications Zero Balance Collection Rate decreased from avg 0.15 to 0.00; 17-AETNA – Medications Labs per Visit decreased from avg 1.60 to 0.00; 17-AETNA – Medications Payment per Visit decreased from avg 14.32 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero Balance Collection Rate decreased from avg 0.16 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00; 17-AETNA – Medications Zero-Balance Collection Dollar Impact decreased from avg 3.36 to 0.00; 17-AETNA – Medications Zero Balance Collection Rate decreased from avg 0.15 to 0.00; 17-AETNA – Medications Payment per Visit decreased from avg 14.32 to 0.00; 17-AETNA – Medications Charge Amount decreased from avg 135.48 to 0.00; 17-AETNA – DME Zero-Balance Collection Dollar Impact decreased from avg 10.48 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to -108.32; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to -45.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to -11.97; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to -3.10; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 5.70 to 0.00</t>
+    <t>17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00; 17-AETNA – Medications Zero-Balance Collection Dollar Impact decreased from avg 4.43 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 9.69 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes NRV Zero Balance decreased from avg 34.92 to 5.92; 17-AETNA – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.42 to 0.64</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 211.52 to 540.00; 17-AETNA – Existing E/M Code Charge Amount increased from avg 1291.98 to 1960.00; 17-AETNA – Lab/Test CPT Codes Visit Count increased from avg 7.50 to 11.00; 17-AETNA – Existing E/M Code Visit Count increased from avg 5.52 to 8.00; 17-AETNA – New E/M Codes Charge Amount increased from avg 2631.41 to 3720.00; 17-AETNA – New E/M Codes Visit Count increased from avg 8.71 to 12.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – DME Charge Billed Balance decreased from avg 149.25 to 25.00; 17-AETNA – Medications Charge Amount increased from avg 135.48 to 192.00; 17-AETNA – X-Ray CPT Codes Visit Count increased from avg 2.12 to 3.00; 17-AETNA – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.42 to 0.58; 17-AETNA – Medications Visit Count increased from avg 1.48 to 2.00; 17-AETNA – X-Ray CPT Codes NRV Zero Balance decreased from avg 54.42 to 35.65</t>
+  </si>
+  <si>
+    <t>17-AETNA – Lab/Test CPT Codes NRV Zero Balance decreased from avg 86.49 to 30.07; 17-AETNA – DME Charge Amount increased from avg 429.55 to 630.92; 17-AETNA – Existing E/M Code Visit Count increased from avg 5.52 to 8.00; 17-AETNA – X-Ray CPT Codes Visit Count increased from avg 2.12 to 3.00; 17-AETNA – X-Ray CPT Codes Charge Amount increased from avg 292.71 to 414.00; 17-AETNA – New E/M Codes Charge Amount increased from avg 2631.41 to 3720.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 2.88; 17-AETNA – X-Ray CPT Codes Visit Count increased from avg 2.12 to 4.00; 17-AETNA – Medications Labs per Visit increased from avg 1.60 to 3.00; 17-AETNA – X-Ray CPT Codes Charge Amount increased from avg 292.71 to 505.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 17.37</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Collection Rate increased from avg 0.30 to 1.01; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to -108.32; 17-AETNA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 76.58 to 229.10; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to -45.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to -11.97; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to -3.10</t>
   </si>
   <si>
     <t>17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to -190.76; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -210.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to 0.00</t>
   </si>
   <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 74.00; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to 75.45</t>
-  </si>
-  <si>
-    <t>17-AETNA – X-Ray CPT Codes Charge Billed Balance decreased from avg 22.59 to 0.00; 17-AETNA – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Labs per Visit decreased from avg 0.80 to 0.00; 17-AETNA – Lab/Test CPT Codes Visit Count decreased from avg 7.50 to 3.00; 17-AETNA – X-Ray CPT Codes Charge Amount decreased from avg 292.71 to 123.00; 17-AETNA – Existing E/M Code Labs per Visit decreased from avg 1.75 to 0.75</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -64.56; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to -11.31; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg 98.28 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -40.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.89 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance decreased from avg 22.59 to 0.00; 17-AETNA – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 11.15 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero Balance Collection Rate decreased from avg 0.16 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.89 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 2.12; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Amount decreased from avg 211.52 to 20.72; 17-AETNA – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 56.31 to 8.50</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Labs per Visit decreased from avg 1.60 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.89 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 56.31 to 0.00; 17-AETNA – X-Ray CPT Codes Labs per Visit decreased from avg 0.80 to 0.00; 17-AETNA – New E/M Codes Labs per Visit decreased from avg 1.59 to 0.33; 17-AETNA – Lab/Test CPT Codes Payment per Visit decreased from avg 79.57 to 36.20</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Labs per Visit decreased from avg 1.60 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.89 to 0.00; 17-AETNA – New E/M Codes Labs per Visit decreased from avg 1.59 to 0.22; 17-AETNA – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 56.31 to 11.19; 17-AETNA – Lab/Test CPT Codes Labs per Visit decreased from avg 2.95 to 1.33; 17-AETNA – Lab/Test CPT Codes Charge Amount decreased from avg 1570.78 to 777.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – X-Ray CPT Codes Labs per Visit decreased from avg 0.80 to 0.00; 17-AETNA – DME Payment per Visit decreased from avg 126.37 to 0.00; 17-AETNA – Existing E/M Code Labs per Visit decreased from avg 1.75 to 0.29; 17-AETNA – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 56.31 to 12.82; 17-AETNA – Lab/Test CPT Codes Charge Amount decreased from avg 1570.78 to 397.00; 17-AETNA – Lab/Test CPT Codes Visit Count decreased from avg 7.50 to 3.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to -50.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to -2.77; 2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.08 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.08 to 0.00; 2-BCBS – After Hours Zero Balance Collection Rate decreased from avg 0.01 to 0.00; 2-BCBS – After Hours Payment per Visit decreased from avg 0.65 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -118.35; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -130.33; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to -20.62; 2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.08 to 0.00; 2-BCBS – After Hours Zero Balance Collection Rate decreased from avg 0.01 to 0.00; 2-BCBS – After Hours Payment per Visit decreased from avg 0.65 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.08 to 0.00; 2-BCBS – After Hours Zero Balance Collection Rate decreased from avg 0.01 to 0.00; 2-BCBS – After Hours Payment per Visit decreased from avg 0.65 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.08 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to -2.48; 2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.08 to 0.00; 2-BCBS – After Hours Zero Balance Collection Rate decreased from avg 0.01 to 0.00; 2-BCBS – After Hours Payment per Visit decreased from avg 0.65 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.09 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -150.46; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -179.32; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to -7.93; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to -13.57; 2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.08 to 0.00; 2-BCBS – After Hours Zero Balance Collection Rate decreased from avg 0.01 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to -355.92; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -82.30; 2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.08 to 0.00; 2-BCBS – After Hours Zero Balance Collection Rate decreased from avg 0.01 to 0.00; 2-BCBS – After Hours Payment per Visit decreased from avg 0.65 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.08 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.09 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to -2.48; 2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.08 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.09 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – Vaccines Labs per Visit decreased from avg 0.10 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -107.62; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -37.97; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.09 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.09 to 0.00; 2-BCBS – Medications Labs per Visit decreased from avg 1.33 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.08 to 0.00; 2-BCBS – After Hours Zero Balance Collection Rate decreased from avg 0.01 to 0.00; 2-BCBS – After Hours Labs per Visit decreased from avg 1.97 to 0.00; 2-BCBS – After Hours Payment per Visit decreased from avg 0.65 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.08 to 0.00; 2-BCBS – After Hours Zero Balance Collection Rate decreased from avg 0.01 to 0.00; 2-BCBS – After Hours Payment per Visit decreased from avg 0.65 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -50.00; 2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.08 to 0.00; 2-BCBS – After Hours Zero Balance Collection Rate decreased from avg 0.01 to 0.00; 2-BCBS – After Hours Labs per Visit decreased from avg 1.97 to 0.00; 2-BCBS – After Hours Payment per Visit decreased from avg 0.65 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – Vaccines Labs per Visit decreased from avg 0.10 to 0.00; 2-BCBS – Self-pay physical &amp; No Charge Labs per Visit decreased from avg 0.17 to 0.00; 2-BCBS – Self-pay physical &amp; No Charge Payment per Visit decreased from avg 7.67 to 0.00; 2-BCBS – Self-pay physical &amp; No Charge Charge Amount decreased from avg 15.08 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 45.90 to 3.72</t>
-  </si>
-  <si>
-    <t>2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – X-Ray CPT Codes Labs per Visit decreased from avg 0.78 to 0.00; 2-BCBS – Self-pay physical &amp; No Charge Charge Amount decreased from avg 15.08 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 45.90 to 9.26; 2-BCBS – Medications Charge Amount decreased from avg 363.59 to 150.00; 2-BCBS – Medications Visit Count decreased from avg 3.91 to 2.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – Vaccines Labs per Visit decreased from avg 0.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 45.90 to 4.65; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Amount decreased from avg 571.38 to 179.00; 2-BCBS – Lab/Test CPT Codes Charge Amount decreased from avg 6412.32 to 3957.00; 2-BCBS – New E/M Codes Charge Amount decreased from avg 8921.72 to 5599.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -62.32; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -71.07; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.56 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00; 2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.36 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -204.90; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -256.10; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.09 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -560.87; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -457.10; 2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.36 to -8.56; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -268.05; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -10.22; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00</t>
+    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00; 17-AETNA – Existing E/M Code Charge Amount increased from avg 1291.98 to 2205.00; 17-AETNA – Existing E/M Code Visit Count increased from avg 5.52 to 9.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – X-Ray CPT Codes Charge Billed Balance decreased from avg 22.59 to 0.00; 17-AETNA – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 11.49 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.42 to 0.56; 17-AETNA – X-Ray CPT Codes NRV Zero Balance decreased from avg 54.42 to 39.91; 17-AETNA – New E/M Codes Zero Balance Collection Rate increased from avg 0.71 to 0.77; 17-AETNA – Existing E/M Code Zero Balance Collection Rate increased from avg 0.65 to 0.70</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 76.58 to 997.19; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 211.52 to 2187.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -64.56; 17-AETNA – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg 51.63 to -11.31; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 62.39 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -40.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 9.69 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance decreased from avg 22.59 to 0.00; 17-AETNA – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 11.49 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 31.17</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 2.12; 17-AETNA – Lab/Test CPT Codes Charge Amount increased from avg 1570.78 to 2385.00; 17-AETNA – New E/M Codes Charge Amount increased from avg 2631.41 to 3955.00; 17-AETNA – New E/M Codes Visit Count increased from avg 8.71 to 13.00; 17-AETNA – Lab/Test CPT Codes Visit Count increased from avg 7.50 to 11.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Rate increased from avg 0.30 to 0.41</t>
+  </si>
+  <si>
+    <t>17-AETNA – X-Ray CPT Codes Payment per Visit increased from avg 50.98 to 141.77; 17-AETNA – X-Ray CPT Codes Charge Amount increased from avg 292.71 to 480.00; 17-AETNA – Lab/Test CPT Codes NRV Zero Balance decreased from avg 86.49 to 56.77; 17-AETNA – Existing E/M Code Charge Amount increased from avg 1291.98 to 1715.00; 17-AETNA – Existing E/M Code Visit Count increased from avg 5.52 to 7.00; 17-AETNA – Medications NRV Zero Balance decreased from avg 19.97 to 14.90</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes NRV Zero Balance decreased from avg 34.92 to 22.38; 17-AETNA – Lab/Test CPT Codes NRV Zero Balance decreased from avg 86.49 to 59.94; 17-AETNA – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 1.56 to 2.00; 17-AETNA – Medications Payment per Visit increased from avg 18.88 to 21.84; 17-AETNA – New E/M Codes Payment per Visit increased from avg 205.14 to 226.96; 17-AETNA – Existing E/M Code Payment per Visit increased from avg 141.04 to 149.41</t>
+  </si>
+  <si>
+    <t>17-AETNA – DME Charge Amount increased from avg 429.55 to 1055.13; 17-AETNA – X-Ray CPT Codes Visit Count increased from avg 2.12 to 4.00; 17-AETNA – X-Ray CPT Codes Charge Amount increased from avg 292.71 to 529.00; 17-AETNA – DME Visit Count increased from avg 1.17 to 2.00; 17-AETNA – Procedures &amp; Surgical CPT Codes NRV Zero Balance decreased from avg 34.92 to 12.82; 17-AETNA – Lab/Test CPT Codes NRV Zero Balance decreased from avg 86.49 to 33.29</t>
+  </si>
+  <si>
+    <t>2-BCBS – Medications Labs per Visit increased from avg 1.33 to 4.50; 2-BCBS – After Hours Collection Rate increased from avg 0.05 to 0.15; 2-BCBS – After Hours Zero Balance Collection Rate increased from avg 0.05 to 0.15; 2-BCBS – After Hours Payment per Visit increased from avg 2.07 to 6.73; 2-BCBS – X-Ray CPT Codes Charge Amount increased from avg 655.56 to 1783.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to -50.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 571.38 to 1782.00; 2-BCBS – Self-pay physical &amp; No Charge Zero Balance Collection Rate increased from avg 0.38 to 1.00; 2-BCBS – Self-pay physical &amp; No Charge Collection Rate increased from avg 0.38 to 1.00; 2-BCBS – X-Ray CPT Codes Charge Amount increased from avg 655.56 to 1401.00; 2-BCBS – Medications Labs per Visit increased from avg 1.33 to 2.75; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -118.35; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -130.33; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to -20.62; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – DME Payment per Visit increased from avg 145.60 to 473.50; 2-BCBS – Medications Charge Amount increased from avg 363.59 to 766.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 571.38 to 1552.00; 2-BCBS – Medications Visit Count increased from avg 3.91 to 10.00; 2-BCBS – Medications Charge Amount increased from avg 363.59 to 893.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 5.06 to 12.00; 2-BCBS – X-Ray CPT Codes Visit Count increased from avg 5.04 to 11.00; 2-BCBS – X-Ray CPT Codes Charge Amount increased from avg 655.56 to 1414.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 1.60; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to -2.48; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Medications Visit Count increased from avg 3.91 to 9.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 4.80; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -150.46; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -179.32; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.71; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to -7.93; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to -13.57; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to -355.92; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -82.30; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Vaccines Labs per Visit increased from avg 0.10 to 2.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.50; 2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.27 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.67; 2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.27 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to -2.48; 2-BCBS – Medications Charge Amount increased from avg 363.59 to 756.00; 2-BCBS – Medications Visit Count increased from avg 3.91 to 8.00; 2-BCBS – X-Ray CPT Codes Charge Amount increased from avg 655.56 to 1338.00; 2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.27 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 5.06 to 14.00; 2-BCBS – Medications Visit Count increased from avg 3.91 to 10.00; 2-BCBS – Medications Charge Amount increased from avg 363.59 to 925.00; 2-BCBS – DME Charge Amount increased from avg 616.33 to 1466.85; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Self-pay physical &amp; No Charge Charge Amount increased from avg 15.08 to 52.00; 2-BCBS – Vaccines Visit Count increased from avg 1.31 to 3.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -107.62; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -37.97; 2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 1.67; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Self-pay physical &amp; No Charge Charge Amount increased from avg 15.08 to 52.00; 2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 2.00; 2-BCBS – Vaccines Visit Count increased from avg 1.31 to 3.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Self-pay physical &amp; No Charge Charge Amount increased from avg 15.08 to 52.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Vaccines Labs per Visit increased from avg 0.10 to 1.00; 2-BCBS – Medications Labs per Visit increased from avg 1.33 to 3.20; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – DME Labs per Visit increased from avg 0.05 to 0.50; 2-BCBS – DME Charge Amount increased from avg 616.33 to 1482.97; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -50.00; 2-BCBS – Vaccines Payment per Visit increased from avg 69.62 to 345.09; 2-BCBS – Vaccines Zero Balance Collection Rate increased from avg 0.64 to 1.64; 2-BCBS – Vaccines Collection Rate increased from avg 0.64 to 1.64; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.80; 2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 1.56; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance decreased from avg 45.56 to 3.72; 2-BCBS – X-Ray CPT Codes Visit Count increased from avg 5.04 to 9.00; 2-BCBS – X-Ray CPT Codes Charge Amount increased from avg 655.56 to 1038.00; 2-BCBS – DME Charge Amount increased from avg 616.33 to 965.66</t>
+  </si>
+  <si>
+    <t>2-BCBS – Self-pay physical &amp; No Charge Labs per Visit increased from avg 0.17 to 2.00; 2-BCBS – DME Charge Amount increased from avg 616.33 to 1680.52; 2-BCBS – Medications Labs per Visit increased from avg 1.33 to 3.00; 2-BCBS – DME Visit Count increased from avg 1.61 to 3.00; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance decreased from avg 45.56 to 11.57; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 2.60</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.75; 2-BCBS – Vaccines Visit Count increased from avg 1.31 to 3.00; 2-BCBS – Vaccines Charge Amount increased from avg 137.31 to 275.05; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance decreased from avg 45.56 to 4.65; 2-BCBS – X-Ray CPT Codes Visit Count increased from avg 5.04 to 9.00; 2-BCBS – X-Ray CPT Codes Charge Amount increased from avg 655.56 to 1150.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -62.32; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -71.07; 2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 2.33; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00; 2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.36 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -204.90; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -256.10; 2-BCBS – X-Ray CPT Codes Charge Amount increased from avg 655.56 to 1508.00; 2-BCBS – X-Ray CPT Codes Visit Count increased from avg 5.04 to 11.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -560.87; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -457.10; 2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.36 to -8.56; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -268.05; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 231.76; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -10.22</t>
   </si>
   <si>
     <t>2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg -4.05 to -290.82; 2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.36 to -9.77; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -83.00; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -170.34; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -177.00; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -232.60</t>
   </si>
   <si>
-    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -87.98; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.09 to 0.00; 2-BCBS – Medications Labs per Visit decreased from avg 1.33 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.56 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -90.00; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -72.37; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.09 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – Vaccines Labs per Visit decreased from avg 0.10 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -201.15; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -329.34; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -22.08; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.09 to -1.65; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.36 to -50.99; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to -40.25; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -372.10; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -305.12; 2-BCBS – After Hours Zero-Balance Collection Dollar Impact decreased from avg 0.08 to 0.00; 2-BCBS – After Hours Zero Balance Collection Rate decreased from avg 0.01 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -222.92; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -306.29; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.09 to 0.00; 2-BCBS – Medications Zero Balance Collection Rate decreased from avg 0.16 to 0.00; 2-BCBS – Medications Payment per Visit decreased from avg 15.88 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.36 to -19.11; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.56 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Amount decreased from avg 655.56 to 220.00; 2-BCBS – X-Ray CPT Codes Visit Count decreased from avg 5.04 to 2.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -195.15; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -252.85; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.09 to 0.00; 2-BCBS – Medications Zero Balance Collection Rate decreased from avg 0.16 to 0.00; 2-BCBS – Medications Labs per Visit decreased from avg 1.33 to 0.00</t>
+    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -87.98; 2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 3.50; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 118.42; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -90.00; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -72.37; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -201.15; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -329.34; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -22.08; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to -1.65; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.36 to -50.99; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to -40.25; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -372.10; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -305.12; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 316.71; 2-BCBS – DME Charge Amount increased from avg 616.33 to 1507.97</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -222.92; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -306.29; 2-BCBS – Medications Labs per Visit increased from avg 1.33 to 3.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.36 to -19.11; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 86.31; 2-BCBS – Procedures &amp; Surgical CPT Codes Zero Balance Collection Rate increased from avg 0.31 to 0.59; 2-BCBS – Procedures &amp; Surgical CPT Codes Collection Rate increased from avg 0.31 to 0.56</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -195.15; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -252.85; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 571.38 to 1493.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Vaccines NRV Zero Balance decreased from avg 69.01 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00</t>
   </si>
   <si>
     <t>2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.36 to -22.39; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -195.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to -29.00; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -150.97; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -183.77; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00</t>
   </si>
   <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -297.48; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -256.81; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Zero Balance Collection Rate decreased from avg 0.31 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – DME Payment per Visit decreased from avg 126.81 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -13.16; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.56 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -164.83; 2-BCBS – Vaccines Charge Billed Balance decreased from avg -0.69 to -20.00; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -167.31; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -80.61; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -65.54; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -757.42; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -129.48; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -776.79; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -152.16; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to -2.04; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -147.63; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -314.63; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.09 to -17.33; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -153.13; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -269.24; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -68.29; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -74.02; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -47.06; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -148.28; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -85.52; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Labs per Visit decreased from avg 1.33 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 10.54</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -86.67; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.09 to -2.09; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Zero Balance Collection Rate decreased from avg 0.31 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – DME Payment per Visit decreased from avg 126.81 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg -4.05 to -235.56; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -94.32; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.56 to 0.25</t>
-  </si>
-  <si>
-    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.56 to 0.00; 2-BCBS – Self-pay physical &amp; No Charge Labs per Visit decreased from avg 0.17 to 0.00; 2-BCBS – Self-pay physical &amp; No Charge Charge Amount decreased from avg 15.08 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Amount decreased from avg 6412.32 to 1624.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit decreased from avg 45.90 to 12.25; 2-BCBS – X-Ray CPT Codes Visit Count decreased from avg 5.04 to 2.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Vaccines Labs per Visit decreased from avg 0.10 to 0.00; 2-BCBS – X-Ray CPT Codes Labs per Visit decreased from avg 0.78 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Amount decreased from avg 655.56 to 75.00; 2-BCBS – X-Ray CPT Codes Visit Count decreased from avg 5.04 to 1.00; 2-BCBS – Medications Labs per Visit decreased from avg 1.33 to 0.50; 2-BCBS – Lab/Test CPT Codes Charge Amount decreased from avg 6412.32 to 3010.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – DME Payment per Visit decreased from avg 126.81 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.56 to 0.00; 2-BCBS – Vaccines Labs per Visit decreased from avg 0.10 to 0.00; 2-BCBS – X-Ray CPT Codes Labs per Visit decreased from avg 0.78 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Amount decreased from avg 571.38 to 104.00</t>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -297.48; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -256.81; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00; 2-BCBS – X-Ray CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 0.36 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -13.16; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00; 2-BCBS – Medications Payment per Visit increased from avg 16.62 to 32.67; 2-BCBS – Medications Charge Amount increased from avg 363.59 to 580.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -164.83; 2-BCBS – Vaccines Charge Billed Balance decreased from avg -0.69 to -20.00; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -167.31; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -80.61; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -65.54; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -757.42; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -129.48; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -776.79; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -152.16; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 155.60; 2-BCBS – Lab/Test CPT Codes Zero-Balance Collection Dollar Impact decreased from avg 23.63 to -2.04</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -147.63; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -314.63; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to -17.33; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -153.13; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -269.24; 2-BCBS – Procedures &amp; Surgical CPT Codes Collection Rate increased from avg 0.31 to 0.66</t>
+  </si>
+  <si>
+    <t>2-BCBS – DME Labs per Visit increased from avg 0.05 to 1.00; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -68.29; 2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -74.02; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -47.06; 2-BCBS – DME Zero Balance Collection Rate increased from avg 0.36 to 1.00; 2-BCBS – DME Collection Rate increased from avg 0.37 to 1.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -148.28; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -85.52; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 10.54; 2-BCBS – Medications Payment per Visit increased from avg 16.62 to 26.58</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Zero-Balance Collection Dollar Impact decreased from avg -11.19 to -86.67; 2-BCBS – Medications Zero-Balance Collection Dollar Impact decreased from avg 2.30 to -2.09; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance decreased from avg 45.56 to 16.79; 2-BCBS – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.21 to 0.33</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Zero-Balance Collection Dollar Impact decreased from avg -4.05 to -235.56; 2-BCBS – Existing E/M Code Zero-Balance Collection Dollar Impact decreased from avg -16.11 to -94.32; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 110.22; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 571.38 to 929.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Self-pay physical &amp; No Charge Payment per Visit increased from avg 18.42 to 35.00; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance decreased from avg 45.56 to 18.37; 2-BCBS – Lab/Test CPT Codes NRV Zero Balance decreased from avg 42.48 to 29.62; 2-BCBS – X-Ray CPT Codes Payment per Visit increased from avg 49.59 to 55.13; 2-BCBS – Existing E/M Code NRV Zero Balance decreased from avg 141.16 to 129.00; 2-BCBS – X-Ray CPT Codes NRV Zero Balance decreased from avg 49.50 to 45.92</t>
+  </si>
+  <si>
+    <t>2-BCBS – Medications Payment per Visit increased from avg 16.62 to 33.77; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 69.12; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 571.38 to 793.00; 2-BCBS – X-Ray CPT Codes NRV Zero Balance decreased from avg 49.50 to 33.96; 2-BCBS – Lab/Test CPT Codes NRV Zero Balance decreased from avg 42.48 to 29.32; 2-BCBS – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 5.06 to 6.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance decreased from avg 45.56 to 22.38; 2-BCBS – X-Ray CPT Codes Payment per Visit increased from avg 49.59 to 57.81; 2-BCBS – Medications Payment per Visit increased from avg 16.62 to 18.27; 2-BCBS – Vaccines Payment per Visit increased from avg 69.62 to 75.59; 2-BCBS – Lab/Test CPT Codes NRV Zero Balance decreased from avg 42.48 to 39.54; 2-BCBS – Existing E/M Code NRV Zero Balance decreased from avg 141.16 to 133.45</t>
   </si>
 </sst>
 </file>
@@ -1004,13 +1058,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
@@ -1118,7 +1172,7 @@
         <v>516</v>
       </c>
       <c r="D2">
-        <v>1.253202724113714</v>
+        <v>3.82556621045239</v>
       </c>
       <c r="E2">
         <v>104157.77</v>
@@ -1127,34 +1181,34 @@
         <v>28.068965517241381</v>
       </c>
       <c r="G2">
-        <v>10.380272712947029</v>
+        <v>10.56238276054259</v>
       </c>
       <c r="H2">
-        <v>74.128161888585552</v>
+        <v>75.428655956806338</v>
       </c>
       <c r="I2">
-        <v>74.846835094815503</v>
+        <v>76.159937464899969</v>
       </c>
       <c r="J2">
-        <v>0.43554057061271179</v>
+        <v>0.44318163325504012</v>
       </c>
       <c r="K2">
-        <v>0.43219024906774861</v>
+        <v>0.43977253413911249</v>
       </c>
       <c r="L2">
-        <v>1.7064900923255379</v>
+        <v>1.7064900923255391</v>
       </c>
       <c r="M2">
         <v>47000.03</v>
       </c>
       <c r="N2">
-        <v>46556.644687299733</v>
+        <v>46527.012242774057</v>
       </c>
       <c r="O2">
-        <v>443.38531270026579</v>
+        <v>473.01775722593447</v>
       </c>
       <c r="P2">
-        <v>0.95235667363549847</v>
+        <v>1.016651906977752</v>
       </c>
       <c r="Q2" t="s">
         <v>23</v>
@@ -1169,7 +1223,7 @@
         <v>126</v>
       </c>
       <c r="U2" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -1192,28 +1246,28 @@
         <v>405</v>
       </c>
       <c r="D3">
-        <v>1.2298199659108879</v>
+        <v>3.8124418943237521</v>
       </c>
       <c r="E3">
-        <v>74188.039999999994</v>
+        <v>74188.040000000008</v>
       </c>
       <c r="F3">
         <v>1.0717741935483871</v>
       </c>
       <c r="G3">
-        <v>1.3986195842805811</v>
+        <v>1.445240237089934</v>
       </c>
       <c r="H3">
-        <v>60.855900084682347</v>
+        <v>62.884430087505081</v>
       </c>
       <c r="I3">
-        <v>60.975322767734063</v>
+        <v>63.007833526658523</v>
       </c>
       <c r="J3">
-        <v>0.3910519848391012</v>
+        <v>0.4040870510004046</v>
       </c>
       <c r="K3">
-        <v>0.39040717986268331</v>
+        <v>0.40342075252477277</v>
       </c>
       <c r="L3">
         <v>2.0372369923982832</v>
@@ -1222,13 +1276,13 @@
         <v>31610.29</v>
       </c>
       <c r="N3">
-        <v>31952.259489398039</v>
+        <v>31649.551966696061</v>
       </c>
       <c r="O3">
-        <v>341.96948939804503</v>
+        <v>39.261966696059972</v>
       </c>
       <c r="P3">
-        <v>-1.070251352682938</v>
+        <v>-0.1240522037638139</v>
       </c>
       <c r="Q3" t="s">
         <v>23</v>
@@ -1240,10 +1294,10 @@
         <v>77</v>
       </c>
       <c r="T3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U3" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -1266,7 +1320,7 @@
         <v>365</v>
       </c>
       <c r="D4">
-        <v>1.2859633774052781</v>
+        <v>3.793591963345571</v>
       </c>
       <c r="E4">
         <v>69928.02</v>
@@ -1275,37 +1329,37 @@
         <v>-1.581864406779661</v>
       </c>
       <c r="G4">
-        <v>-2.731451537033657</v>
+        <v>-2.8777792979461752</v>
       </c>
       <c r="H4">
-        <v>62.284351393328507</v>
+        <v>65.621013075113979</v>
       </c>
       <c r="I4">
-        <v>62.275780491918617</v>
+        <v>65.611983018271417</v>
       </c>
       <c r="J4">
-        <v>0.37714646618905717</v>
+        <v>0.39735074116347102</v>
       </c>
       <c r="K4">
-        <v>0.37805783430400219</v>
+        <v>0.39831093257028799</v>
       </c>
       <c r="L4">
-        <v>2.010170209492244</v>
+        <v>2.0101702094922431</v>
       </c>
       <c r="M4">
-        <v>29340.77</v>
+        <v>29340.76999999999</v>
       </c>
       <c r="N4">
-        <v>30155.365174374721</v>
+        <v>30025.184761716431</v>
       </c>
       <c r="O4">
-        <v>814.59517437472095</v>
+        <v>684.41476171643808</v>
       </c>
       <c r="P4">
-        <v>-2.701327507275368</v>
+        <v>-2.279468942982493</v>
       </c>
       <c r="Q4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R4" t="s">
         <v>28</v>
@@ -1314,19 +1368,19 @@
         <v>78</v>
       </c>
       <c r="T4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="U4" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="V4">
         <v>0</v>
       </c>
       <c r="W4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -1340,7 +1394,7 @@
         <v>484</v>
       </c>
       <c r="D5">
-        <v>1.15900644973155</v>
+        <v>3.7088206391409599</v>
       </c>
       <c r="E5">
         <v>86214.87</v>
@@ -1349,19 +1403,19 @@
         <v>-2.34375</v>
       </c>
       <c r="G5">
-        <v>-2.2665139462432822</v>
+        <v>-2.4176148759928342</v>
       </c>
       <c r="H5">
-        <v>73.230221894345817</v>
+        <v>78.1122366873022</v>
       </c>
       <c r="I5">
-        <v>73.038728658415081</v>
+        <v>77.907977235642747</v>
       </c>
       <c r="J5">
-        <v>0.40710054272929108</v>
+        <v>0.43424057891124379</v>
       </c>
       <c r="K5">
-        <v>0.40797139153978151</v>
+        <v>0.4351694843091003</v>
       </c>
       <c r="L5">
         <v>1.9650903784599929</v>
@@ -1370,13 +1424,13 @@
         <v>37248.69</v>
       </c>
       <c r="N5">
-        <v>38218.384590934147</v>
+        <v>38457.874123281319</v>
       </c>
       <c r="O5">
-        <v>969.69459093415207</v>
+        <v>1209.1841232813169</v>
       </c>
       <c r="P5">
-        <v>-2.537246409844792</v>
+        <v>-3.1441782751826901</v>
       </c>
       <c r="Q5" t="s">
         <v>22</v>
@@ -1391,7 +1445,7 @@
         <v>126</v>
       </c>
       <c r="U5" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -1414,10 +1468,10 @@
         <v>449</v>
       </c>
       <c r="D6">
-        <v>1.139301896373244</v>
+        <v>3.7343784381123002</v>
       </c>
       <c r="E6">
-        <v>80847.569999999992</v>
+        <v>80847.570000000007</v>
       </c>
       <c r="F6">
         <v>3.3728813559322028</v>
@@ -1426,16 +1480,16 @@
         <v>3.4235838205977678</v>
       </c>
       <c r="H6">
-        <v>75.241478926577713</v>
+        <v>75.241478926577699</v>
       </c>
       <c r="I6">
-        <v>75.73258644194371</v>
+        <v>75.732586441943695</v>
       </c>
       <c r="J6">
         <v>0.41799365526023818</v>
       </c>
       <c r="K6">
-        <v>0.41599673970426382</v>
+        <v>0.41599673970426371</v>
       </c>
       <c r="L6">
         <v>2.105482066881033</v>
@@ -1444,13 +1498,13 @@
         <v>35962.17</v>
       </c>
       <c r="N6">
-        <v>35937.765052657021</v>
+        <v>35543.509047541433</v>
       </c>
       <c r="O6">
-        <v>24.404947342976811</v>
+        <v>418.66095245856559</v>
       </c>
       <c r="P6">
-        <v>6.7908917839542893E-2</v>
+        <v>1.177883005019519</v>
       </c>
       <c r="Q6" t="s">
         <v>23</v>
@@ -1462,10 +1516,10 @@
         <v>80</v>
       </c>
       <c r="T6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="U6" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -1488,43 +1542,43 @@
         <v>458</v>
       </c>
       <c r="D7">
-        <v>1.081621252742208</v>
+        <v>3.5693501340492859</v>
       </c>
       <c r="E7">
-        <v>80800.289999999994</v>
+        <v>80800.290000000008</v>
       </c>
       <c r="F7">
         <v>-6.122727272727273</v>
       </c>
       <c r="G7">
-        <v>-8.8161484447929723</v>
+        <v>-9.8621321585819715</v>
       </c>
       <c r="H7">
-        <v>58.287775045025988</v>
+        <v>65.2032737791816</v>
       </c>
       <c r="I7">
-        <v>56.308621004621948</v>
+        <v>62.989304852627932</v>
       </c>
       <c r="J7">
-        <v>0.37505150148533772</v>
+        <v>0.41954913725478438</v>
       </c>
       <c r="K7">
-        <v>0.38475762478133002</v>
+        <v>0.43040683450114869</v>
       </c>
       <c r="L7">
-        <v>1.758785969985432</v>
+        <v>1.7587859699854309</v>
       </c>
       <c r="M7">
-        <v>35947.040000000001</v>
+        <v>35947.040000000008</v>
       </c>
       <c r="N7">
-        <v>34540.057642502958</v>
+        <v>35058.865794566373</v>
       </c>
       <c r="O7">
-        <v>1406.982357497043</v>
+        <v>888.17420543363551</v>
       </c>
       <c r="P7">
-        <v>4.073480050495613</v>
+        <v>2.533379746618301</v>
       </c>
       <c r="Q7" t="s">
         <v>21</v>
@@ -1536,10 +1590,10 @@
         <v>81</v>
       </c>
       <c r="T7" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="U7" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="V7">
         <v>1</v>
@@ -1562,7 +1616,7 @@
         <v>433</v>
       </c>
       <c r="D8">
-        <v>1.1615245150653219</v>
+        <v>3.667972152837859</v>
       </c>
       <c r="E8">
         <v>80246.880000000005</v>
@@ -1571,19 +1625,19 @@
         <v>-0.93199999999999994</v>
       </c>
       <c r="G8">
-        <v>0.9267667444415032</v>
+        <v>0.97554394151737178</v>
       </c>
       <c r="H8">
-        <v>70.534963987566016</v>
+        <v>74.247330513227382</v>
       </c>
       <c r="I8">
-        <v>70.511629723753785</v>
+        <v>74.222768130267156</v>
       </c>
       <c r="J8">
-        <v>0.40884719062614611</v>
+        <v>0.43036546381699592</v>
       </c>
       <c r="K8">
-        <v>0.40872056796538969</v>
+        <v>0.43023217680567333</v>
       </c>
       <c r="L8">
         <v>1.7829461936215529</v>
@@ -1592,13 +1646,13 @@
         <v>35708.6</v>
       </c>
       <c r="N8">
-        <v>35653.184344629582</v>
+        <v>35775.293697167079</v>
       </c>
       <c r="O8">
-        <v>55.415655370416061</v>
+        <v>66.693697167080245</v>
       </c>
       <c r="P8">
-        <v>0.1554297502146208</v>
+        <v>-0.18642389837979581</v>
       </c>
       <c r="Q8" t="s">
         <v>23</v>
@@ -1610,10 +1664,10 @@
         <v>82</v>
       </c>
       <c r="T8" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="U8" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -1636,43 +1690,43 @@
         <v>482</v>
       </c>
       <c r="D9">
-        <v>1.1361799973619859</v>
+        <v>3.6925849914264561</v>
       </c>
       <c r="E9">
-        <v>85608.46</v>
+        <v>85608.459999999992</v>
       </c>
       <c r="F9">
         <v>8.1075384615384625</v>
       </c>
       <c r="G9">
-        <v>6.2027120346512428</v>
+        <v>6.7196047042055129</v>
       </c>
       <c r="H9">
-        <v>64.268090330463721</v>
+        <v>68.482391335740033</v>
       </c>
       <c r="I9">
-        <v>67.252731356104746</v>
+        <v>72.85712563578015</v>
       </c>
       <c r="J9">
-        <v>0.39304507048026849</v>
+        <v>0.42579882635362432</v>
       </c>
       <c r="K9">
-        <v>0.38385653796249608</v>
+        <v>0.40902745848462702</v>
       </c>
       <c r="L9">
         <v>2.063387612369934</v>
       </c>
       <c r="M9">
-        <v>36306.25</v>
+        <v>36306.250000000007</v>
       </c>
       <c r="N9">
-        <v>37017.191384552643</v>
+        <v>37210.529267743063</v>
       </c>
       <c r="O9">
-        <v>710.94138455263601</v>
+        <v>904.27926774305524</v>
       </c>
       <c r="P9">
-        <v>-1.9205708427930961</v>
+        <v>-2.4301703994491519</v>
       </c>
       <c r="Q9" t="s">
         <v>23</v>
@@ -1684,10 +1738,10 @@
         <v>83</v>
       </c>
       <c r="T9" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="U9" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -1710,28 +1764,28 @@
         <v>381</v>
       </c>
       <c r="D10">
-        <v>1.204956056291437</v>
+        <v>3.681810172001613</v>
       </c>
       <c r="E10">
-        <v>66856.55</v>
+        <v>66856.549999999988</v>
       </c>
       <c r="F10">
         <v>-1.857454545454545</v>
       </c>
       <c r="G10">
-        <v>-1.4609900577216131</v>
+        <v>-1.639886799483443</v>
       </c>
       <c r="H10">
-        <v>61.330828851926441</v>
+        <v>67.463911737119091</v>
       </c>
       <c r="I10">
-        <v>61.162184407482002</v>
+        <v>67.278402848230201</v>
       </c>
       <c r="J10">
-        <v>0.37509439988830962</v>
+        <v>0.42102432640524529</v>
       </c>
       <c r="K10">
-        <v>0.37616902179437611</v>
+        <v>0.42223053466715682</v>
       </c>
       <c r="L10">
         <v>1.8241555858179901</v>
@@ -1740,13 +1794,13 @@
         <v>29620.74</v>
       </c>
       <c r="N10">
-        <v>28970.076607561179</v>
+        <v>29196.135995283141</v>
       </c>
       <c r="O10">
-        <v>650.66339243882612</v>
+        <v>424.6040047168608</v>
       </c>
       <c r="P10">
-        <v>2.2459843695028519</v>
+        <v>1.454315751870243</v>
       </c>
       <c r="Q10" t="s">
         <v>23</v>
@@ -1758,10 +1812,10 @@
         <v>84</v>
       </c>
       <c r="T10" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="U10" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -1784,7 +1838,7 @@
         <v>318</v>
       </c>
       <c r="D11">
-        <v>1.144050105235729</v>
+        <v>3.6228253332464759</v>
       </c>
       <c r="E11">
         <v>55533.57</v>
@@ -1793,19 +1847,19 @@
         <v>4.7738596491228069</v>
       </c>
       <c r="G11">
-        <v>-0.12741990692780261</v>
+        <v>-0.1424104842134262</v>
       </c>
       <c r="H11">
-        <v>59.154214432617763</v>
+        <v>66.113533777631616</v>
       </c>
       <c r="I11">
-        <v>59.332440455058872</v>
+        <v>66.312727567418747</v>
       </c>
       <c r="J11">
-        <v>0.39626663368211512</v>
+        <v>0.4428862376447168</v>
       </c>
       <c r="K11">
-        <v>0.39558006271018431</v>
+        <v>0.44211889361726481</v>
       </c>
       <c r="L11">
         <v>1.817865433530254</v>
@@ -1814,13 +1868,13 @@
         <v>24459.74</v>
       </c>
       <c r="N11">
-        <v>23972.559960628801</v>
+        <v>24545.232877674989</v>
       </c>
       <c r="O11">
-        <v>487.18003937120011</v>
+        <v>85.49287767498754</v>
       </c>
       <c r="P11">
-        <v>2.032240362194599</v>
+        <v>-0.34830746198683338</v>
       </c>
       <c r="Q11" t="s">
         <v>23</v>
@@ -1832,10 +1886,10 @@
         <v>85</v>
       </c>
       <c r="T11" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="U11" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="V11">
         <v>0</v>
@@ -1858,28 +1912,28 @@
         <v>333</v>
       </c>
       <c r="D12">
-        <v>0.99279076969045799</v>
+        <v>3.7229653863392169</v>
       </c>
       <c r="E12">
-        <v>61681.71</v>
+        <v>61681.710000000006</v>
       </c>
       <c r="F12">
         <v>24.263333333333328</v>
       </c>
       <c r="G12">
-        <v>2.9184704594486441</v>
+        <v>3.4334946581748751</v>
       </c>
       <c r="H12">
-        <v>58.571108450868117</v>
+        <v>68.907186412786032</v>
       </c>
       <c r="I12">
-        <v>59.709998376623368</v>
+        <v>70.247056913674555</v>
       </c>
       <c r="J12">
-        <v>0.38947725700267027</v>
+        <v>0.45820853765020031</v>
       </c>
       <c r="K12">
-        <v>0.36968452087901149</v>
+        <v>0.43492296574001349</v>
       </c>
       <c r="L12">
         <v>1.3034723191981259</v>
@@ -1888,13 +1942,13 @@
         <v>27164.76</v>
       </c>
       <c r="N12">
-        <v>26793.35338295978</v>
+        <v>27736.95384146737</v>
       </c>
       <c r="O12">
-        <v>371.40661704021841</v>
+        <v>572.19384146737502</v>
       </c>
       <c r="P12">
-        <v>1.386189372161337</v>
+        <v>-2.0629296379760791</v>
       </c>
       <c r="Q12" t="s">
         <v>23</v>
@@ -1906,10 +1960,10 @@
         <v>86</v>
       </c>
       <c r="T12" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="U12" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="V12">
         <v>0</v>
@@ -1932,7 +1986,7 @@
         <v>396</v>
       </c>
       <c r="D13">
-        <v>1.1337402610096361</v>
+        <v>3.75924402334774</v>
       </c>
       <c r="E13">
         <v>68290.27</v>
@@ -1944,16 +1998,16 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>56.963165118095837</v>
+        <v>58.830809876066184</v>
       </c>
       <c r="I13">
-        <v>56.963165118095837</v>
+        <v>58.830809876066184</v>
       </c>
       <c r="J13">
-        <v>0.37231401242102452</v>
+        <v>0.39092971304207569</v>
       </c>
       <c r="K13">
-        <v>0.37231401242102452</v>
+        <v>0.39092971304207569</v>
       </c>
       <c r="L13">
         <v>1.700802207390782</v>
@@ -1962,13 +2016,13 @@
         <v>27476.09</v>
       </c>
       <c r="N13">
-        <v>29287.266268868789</v>
+        <v>28698.70182474234</v>
       </c>
       <c r="O13">
-        <v>1811.176268868792</v>
+        <v>1222.611824742344</v>
       </c>
       <c r="P13">
-        <v>-6.184176605086563</v>
+        <v>-4.2601642130316826</v>
       </c>
       <c r="Q13" t="s">
         <v>22</v>
@@ -1980,10 +2034,10 @@
         <v>87</v>
       </c>
       <c r="T13" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="U13" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -2006,7 +2060,7 @@
         <v>272</v>
       </c>
       <c r="D14">
-        <v>1.1988269996426839</v>
+        <v>3.6595771568039819</v>
       </c>
       <c r="E14">
         <v>44036.04</v>
@@ -2015,19 +2069,19 @@
         <v>-1.042068965517241</v>
       </c>
       <c r="G14">
-        <v>-1.831465517241379</v>
+        <v>-2.0427884615384611</v>
       </c>
       <c r="H14">
-        <v>62.509995294934953</v>
+        <v>67.140365316781995</v>
       </c>
       <c r="I14">
-        <v>62.143702191486668</v>
+        <v>66.74693939085607</v>
       </c>
       <c r="J14">
-        <v>0.38067347744513969</v>
+        <v>0.42459734022727119</v>
       </c>
       <c r="K14">
-        <v>0.38216855133676531</v>
+        <v>0.42626492264485361</v>
       </c>
       <c r="L14">
         <v>1.5194035849208261</v>
@@ -2036,13 +2090,13 @@
         <v>20575.77</v>
       </c>
       <c r="N14">
-        <v>19715.428977304819</v>
+        <v>19528.593183724559</v>
       </c>
       <c r="O14">
-        <v>860.34102269517825</v>
+        <v>1047.176816275442</v>
       </c>
       <c r="P14">
-        <v>4.3637956023455002</v>
+        <v>5.3622747241628002</v>
       </c>
       <c r="Q14" t="s">
         <v>21</v>
@@ -2054,10 +2108,10 @@
         <v>88</v>
       </c>
       <c r="T14" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="U14" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="V14">
         <v>1</v>
@@ -2080,7 +2134,7 @@
         <v>352</v>
       </c>
       <c r="D15">
-        <v>1.086238134629872</v>
+        <v>3.7160778289969292</v>
       </c>
       <c r="E15">
         <v>65324.84</v>
@@ -2089,19 +2143,19 @@
         <v>20.452000000000002</v>
       </c>
       <c r="G15">
-        <v>15.4439160123069</v>
+        <v>16.456631816392601</v>
       </c>
       <c r="H15">
-        <v>62.361885862143552</v>
+        <v>66.451189853103784</v>
       </c>
       <c r="I15">
-        <v>64.154895198135208</v>
+        <v>68.361773571783417</v>
       </c>
       <c r="J15">
-        <v>0.38511082223696552</v>
+        <v>0.41036399090824188</v>
       </c>
       <c r="K15">
-        <v>0.35547939568990322</v>
+        <v>0.37878951999743782</v>
       </c>
       <c r="L15">
         <v>2.1240479890479889</v>
@@ -2110,13 +2164,13 @@
         <v>26750.36</v>
       </c>
       <c r="N15">
-        <v>27840.963727131952</v>
+        <v>27636.29684884744</v>
       </c>
       <c r="O15">
-        <v>1090.603727131951</v>
+        <v>885.93684884743561</v>
       </c>
       <c r="P15">
-        <v>-3.9172628426979381</v>
+        <v>-3.2057002922386229</v>
       </c>
       <c r="Q15" t="s">
         <v>22</v>
@@ -2128,10 +2182,10 @@
         <v>89</v>
       </c>
       <c r="T15" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="U15" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="V15">
         <v>0</v>
@@ -2154,7 +2208,7 @@
         <v>342</v>
       </c>
       <c r="D16">
-        <v>1.162272358512012</v>
+        <v>3.6703337637221418</v>
       </c>
       <c r="E16">
         <v>62627.59</v>
@@ -2163,19 +2217,19 @@
         <v>21.016999999999999</v>
       </c>
       <c r="G16">
-        <v>18.090776730173939</v>
+        <v>19.3829750680435</v>
       </c>
       <c r="H16">
-        <v>65.706060458058289</v>
+        <v>69.16427416637714</v>
       </c>
       <c r="I16">
-        <v>66.189816147135119</v>
+        <v>70.917660157644761</v>
       </c>
       <c r="J16">
-        <v>0.40046228918097532</v>
+        <v>0.42906673840818782</v>
       </c>
       <c r="K16">
-        <v>0.39381004736879133</v>
+        <v>0.41453689196714871</v>
       </c>
       <c r="L16">
         <v>1.687856337441241</v>
@@ -2184,13 +2238,13 @@
         <v>27416.39</v>
       </c>
       <c r="N16">
-        <v>27844.135748454199</v>
+        <v>27595.47037888004</v>
       </c>
       <c r="O16">
-        <v>427.74574845420278</v>
+        <v>179.08037888004401</v>
       </c>
       <c r="P16">
-        <v>-1.5362148508342539</v>
+        <v>-0.64894845574765658</v>
       </c>
       <c r="Q16" t="s">
         <v>23</v>
@@ -2205,7 +2259,7 @@
         <v>126</v>
       </c>
       <c r="U16" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="V16">
         <v>0</v>
@@ -2228,7 +2282,7 @@
         <v>259</v>
       </c>
       <c r="D17">
-        <v>1.182957255430434</v>
+        <v>3.6145916138152172</v>
       </c>
       <c r="E17">
         <v>47318.98</v>
@@ -2237,19 +2291,19 @@
         <v>1.380727272727273</v>
       </c>
       <c r="G17">
-        <v>2.5459443957386498</v>
+        <v>2.745626309129916</v>
       </c>
       <c r="H17">
-        <v>76.97282452298434</v>
+        <v>81.41356439931036</v>
       </c>
       <c r="I17">
-        <v>77.14790950413223</v>
+        <v>83.19872593582889</v>
       </c>
       <c r="J17">
-        <v>0.42677508341890968</v>
+        <v>0.46024763898117721</v>
       </c>
       <c r="K17">
-        <v>0.42982202630710098</v>
+        <v>0.45461945090174138</v>
       </c>
       <c r="L17">
         <v>1.5674812713082511</v>
@@ -2258,13 +2312,13 @@
         <v>21838.43</v>
       </c>
       <c r="N17">
-        <v>22461.26205708972</v>
+        <v>22781.840765286699</v>
       </c>
       <c r="O17">
-        <v>622.83205708971946</v>
+        <v>943.4107652866951</v>
       </c>
       <c r="P17">
-        <v>-2.772916568564443</v>
+        <v>-4.1410646971257714</v>
       </c>
       <c r="Q17" t="s">
         <v>22</v>
@@ -2276,10 +2330,10 @@
         <v>91</v>
       </c>
       <c r="T17" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="U17" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="V17">
         <v>0</v>
@@ -2302,7 +2356,7 @@
         <v>320</v>
       </c>
       <c r="D18">
-        <v>1.1839270815587699</v>
+        <v>3.749102424936106</v>
       </c>
       <c r="E18">
         <v>59745.47</v>
@@ -2311,19 +2365,19 @@
         <v>1.6964912280701749</v>
       </c>
       <c r="G18">
-        <v>4.0986353953204278</v>
+        <v>4.2476766824229886</v>
       </c>
       <c r="H18">
-        <v>66.636289642461549</v>
+        <v>67.826223386076919</v>
       </c>
       <c r="I18">
-        <v>67.158275831111311</v>
+        <v>69.600394952242624</v>
       </c>
       <c r="J18">
-        <v>0.42946444959717672</v>
+        <v>0.44508133867343758</v>
       </c>
       <c r="K18">
-        <v>0.43068969322622958</v>
+        <v>0.43838058060526952</v>
       </c>
       <c r="L18">
         <v>1.8141773996612709</v>
@@ -2332,13 +2386,13 @@
         <v>25951.37</v>
       </c>
       <c r="N18">
-        <v>26707.053324308239</v>
+        <v>26739.63237118892</v>
       </c>
       <c r="O18">
-        <v>755.68332430823648</v>
+        <v>788.26237118892095</v>
       </c>
       <c r="P18">
-        <v>-2.829527148247494</v>
+        <v>-2.947917758354254</v>
       </c>
       <c r="Q18" t="s">
         <v>22</v>
@@ -2350,10 +2404,10 @@
         <v>92</v>
       </c>
       <c r="T18" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="U18" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="V18">
         <v>0</v>
@@ -2376,7 +2430,7 @@
         <v>275</v>
       </c>
       <c r="D19">
-        <v>1.1704715005345001</v>
+        <v>3.696225791161579</v>
       </c>
       <c r="E19">
         <v>52579.07</v>
@@ -2385,19 +2439,19 @@
         <v>-0.83850000000000002</v>
       </c>
       <c r="G19">
-        <v>-0.22568829810416161</v>
+        <v>-0.24180889082588741</v>
       </c>
       <c r="H19">
-        <v>72.53632329059829</v>
+        <v>75.037575817860301</v>
       </c>
       <c r="I19">
-        <v>71.826820512820504</v>
+        <v>76.957307692307694</v>
       </c>
       <c r="J19">
-        <v>0.40421591002322649</v>
+        <v>0.43308847502488562</v>
       </c>
       <c r="K19">
-        <v>0.41542760182525179</v>
+        <v>0.42975269154336398</v>
       </c>
       <c r="L19">
         <v>1.954093452843453</v>
@@ -2406,16 +2460,16 @@
         <v>24325.55</v>
       </c>
       <c r="N19">
-        <v>23582.63640458904</v>
+        <v>23935.172238873591</v>
       </c>
       <c r="O19">
-        <v>742.91359541095517</v>
+        <v>390.37776112641592</v>
       </c>
       <c r="P19">
-        <v>3.1502567510492101</v>
+        <v>1.630979536016856</v>
       </c>
       <c r="Q19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="R19" t="s">
         <v>43</v>
@@ -2424,19 +2478,19 @@
         <v>93</v>
       </c>
       <c r="T19" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="U19" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="V19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W19">
         <v>0</v>
       </c>
       <c r="X19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
@@ -2450,7 +2504,7 @@
         <v>313</v>
       </c>
       <c r="D20">
-        <v>1.1909634735829631</v>
+        <v>3.713003770582179</v>
       </c>
       <c r="E20">
         <v>54834.27</v>
@@ -2459,19 +2513,19 @@
         <v>25.965094339622642</v>
       </c>
       <c r="G20">
-        <v>10.553342839782211</v>
+        <v>10.967199421734451</v>
       </c>
       <c r="H20">
-        <v>64.454446960611222</v>
+        <v>66.982072331615583</v>
       </c>
       <c r="I20">
-        <v>65.318366068448753</v>
+        <v>67.87987062015263</v>
       </c>
       <c r="J20">
-        <v>0.39908161985568141</v>
+        <v>0.41473187945786499</v>
       </c>
       <c r="K20">
-        <v>0.38992811943512989</v>
+        <v>0.40521941823650759</v>
       </c>
       <c r="L20">
         <v>1.4569887644110731</v>
@@ -2480,16 +2534,16 @@
         <v>24475.18</v>
       </c>
       <c r="N20">
-        <v>24700.730845011771</v>
+        <v>23859.66039302506</v>
       </c>
       <c r="O20">
-        <v>225.55084501177041</v>
+        <v>615.51960697493632</v>
       </c>
       <c r="P20">
-        <v>-0.91313429722796913</v>
+        <v>2.5797500753819289</v>
       </c>
       <c r="Q20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R20" t="s">
         <v>44</v>
@@ -2498,19 +2552,19 @@
         <v>94</v>
       </c>
       <c r="T20" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="U20" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="V20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20">
         <v>0</v>
       </c>
       <c r="X20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
@@ -2524,7 +2578,7 @@
         <v>310</v>
       </c>
       <c r="D21">
-        <v>1.1521351222843981</v>
+        <v>3.727495983861286</v>
       </c>
       <c r="E21">
         <v>54324.62</v>
@@ -2533,19 +2587,19 @@
         <v>10.13709090909091</v>
       </c>
       <c r="G21">
-        <v>1.842176099961776</v>
+        <v>2.0263937099579539</v>
       </c>
       <c r="H21">
-        <v>63.713785577694757</v>
+        <v>67.389580899484841</v>
       </c>
       <c r="I21">
-        <v>62.527732513015941</v>
+        <v>68.780505764317525</v>
       </c>
       <c r="J21">
-        <v>0.39365316216850499</v>
+        <v>0.43301847838535562</v>
       </c>
       <c r="K21">
-        <v>0.41088880916204679</v>
+        <v>0.43459393276754948</v>
       </c>
       <c r="L21">
         <v>1.7529160276583931</v>
@@ -2554,16 +2608,16 @@
         <v>24504.18</v>
       </c>
       <c r="N21">
-        <v>23876.782904222251</v>
+        <v>24095.853925189451</v>
       </c>
       <c r="O21">
-        <v>627.3970957777492</v>
+        <v>408.32607481054953</v>
       </c>
       <c r="P21">
-        <v>2.6276450152202182</v>
+        <v>1.694590596698843</v>
       </c>
       <c r="Q21" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="R21" t="s">
         <v>45</v>
@@ -2572,19 +2626,19 @@
         <v>95</v>
       </c>
       <c r="T21" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="U21" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="V21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W21">
         <v>0</v>
       </c>
       <c r="X21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
@@ -2598,28 +2652,28 @@
         <v>301</v>
       </c>
       <c r="D22">
-        <v>1.275564913149448</v>
+        <v>3.8266947394483419</v>
       </c>
       <c r="E22">
-        <v>55277.99</v>
+        <v>55277.989999999991</v>
       </c>
       <c r="F22">
         <v>17.07017543859649</v>
       </c>
       <c r="G22">
-        <v>5.2717314094462688</v>
+        <v>6.1324222518048437</v>
       </c>
       <c r="H22">
-        <v>64.686398808087972</v>
+        <v>75.247443511449276</v>
       </c>
       <c r="I22">
-        <v>65.475113897722565</v>
+        <v>76.164928411636453</v>
       </c>
       <c r="J22">
-        <v>0.35380968355378162</v>
+        <v>0.41157452984827658</v>
       </c>
       <c r="K22">
-        <v>0.3495537218135259</v>
+        <v>0.40662371721165258</v>
       </c>
       <c r="L22">
         <v>1.564564126158329</v>
@@ -2628,13 +2682,13 @@
         <v>24780.58</v>
       </c>
       <c r="N22">
-        <v>24466.901109315218</v>
+        <v>24757.876640269529</v>
       </c>
       <c r="O22">
-        <v>313.67889068477598</v>
+        <v>22.70335973046895</v>
       </c>
       <c r="P22">
-        <v>1.282054025899299</v>
+        <v>9.1701562538449508E-2</v>
       </c>
       <c r="Q22" t="s">
         <v>23</v>
@@ -2646,10 +2700,10 @@
         <v>96</v>
       </c>
       <c r="T22" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="U22" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="V22">
         <v>0</v>
@@ -2672,7 +2726,7 @@
         <v>288</v>
       </c>
       <c r="D23">
-        <v>1.1682313575401719</v>
+        <v>3.642133055860536</v>
       </c>
       <c r="E23">
         <v>50183.360000000001</v>
@@ -2681,19 +2735,19 @@
         <v>6.993584905660378</v>
       </c>
       <c r="G23">
-        <v>-1.370561015230094</v>
+        <v>-1.5455262512169139</v>
       </c>
       <c r="H23">
-        <v>70.395292712528573</v>
+        <v>79.38192582476627</v>
       </c>
       <c r="I23">
-        <v>69.30942797349401</v>
+        <v>78.157440055216654</v>
       </c>
       <c r="J23">
-        <v>0.41199924075065852</v>
+        <v>0.46459488850606168</v>
       </c>
       <c r="K23">
-        <v>0.41842843169512589</v>
+        <v>0.47184482723067378</v>
       </c>
       <c r="L23">
         <v>1.5389817729440369</v>
@@ -2702,16 +2756,16 @@
         <v>23883.61</v>
       </c>
       <c r="N23">
-        <v>23064.518047241669</v>
+        <v>23831.875574299749</v>
       </c>
       <c r="O23">
-        <v>819.09195275832826</v>
+        <v>51.734425700247812</v>
       </c>
       <c r="P23">
-        <v>3.5513074718519211</v>
+        <v>0.21708079810570219</v>
       </c>
       <c r="Q23" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="R23" t="s">
         <v>47</v>
@@ -2723,16 +2777,16 @@
         <v>126</v>
       </c>
       <c r="U23" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="V23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W23">
         <v>0</v>
       </c>
       <c r="X23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
@@ -2746,7 +2800,7 @@
         <v>302</v>
       </c>
       <c r="D24">
-        <v>1.07826416370989</v>
+        <v>3.7140210083340661</v>
       </c>
       <c r="E24">
         <v>49683.519999999997</v>
@@ -2755,19 +2809,19 @@
         <v>3.9087096774193548</v>
       </c>
       <c r="G24">
-        <v>4.3370817849698566</v>
+        <v>4.7175275555812473</v>
       </c>
       <c r="H24">
-        <v>63.553452056337612</v>
+        <v>65.671900458215546</v>
       </c>
       <c r="I24">
-        <v>61.371347284694423</v>
+        <v>66.754798800895699</v>
       </c>
       <c r="J24">
-        <v>0.40522242115019169</v>
+        <v>0.44076824756687522</v>
       </c>
       <c r="K24">
-        <v>0.41507614249141372</v>
+        <v>0.4289120139077941</v>
       </c>
       <c r="L24">
         <v>1.897552587092435</v>
@@ -2776,13 +2830,13 @@
         <v>23209.87</v>
       </c>
       <c r="N24">
-        <v>21738.611652546719</v>
+        <v>21730.26890132319</v>
       </c>
       <c r="O24">
-        <v>1471.2583474532839</v>
+        <v>1479.601098676816</v>
       </c>
       <c r="P24">
-        <v>6.7679499085256598</v>
+        <v>6.8089405860353667</v>
       </c>
       <c r="Q24" t="s">
         <v>21</v>
@@ -2794,10 +2848,10 @@
         <v>98</v>
       </c>
       <c r="T24" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="U24" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="V24">
         <v>1</v>
@@ -2820,46 +2874,46 @@
         <v>275</v>
       </c>
       <c r="D25">
-        <v>1.2229871772613949</v>
+        <v>3.7409019539760311</v>
       </c>
       <c r="E25">
         <v>47268.62</v>
       </c>
       <c r="F25">
-        <v>0.59692307692307567</v>
+        <v>0.59692307692307511</v>
       </c>
       <c r="G25">
-        <v>13.147978172027759</v>
+        <v>13.95295642745803</v>
       </c>
       <c r="H25">
-        <v>63.133984274272727</v>
+        <v>65.659343645243638</v>
       </c>
       <c r="I25">
-        <v>64.558535585141357</v>
+        <v>67.140877008547008</v>
       </c>
       <c r="J25">
-        <v>0.39419291586758742</v>
+        <v>0.41832717602274572</v>
       </c>
       <c r="K25">
-        <v>0.37887013738784192</v>
+        <v>0.40206626824832198</v>
       </c>
       <c r="L25">
-        <v>1.443130800823109</v>
+        <v>1.4431308008231081</v>
       </c>
       <c r="M25">
         <v>21325.84</v>
       </c>
       <c r="N25">
-        <v>21507.454482786179</v>
+        <v>20766.711134083711</v>
       </c>
       <c r="O25">
-        <v>181.61448278618261</v>
+        <v>559.12886591628921</v>
       </c>
       <c r="P25">
-        <v>-0.84442574518309699</v>
+        <v>2.6924285810409789</v>
       </c>
       <c r="Q25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R25" t="s">
         <v>49</v>
@@ -2868,19 +2922,19 @@
         <v>99</v>
       </c>
       <c r="T25" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="U25" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="V25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W25">
         <v>0</v>
       </c>
       <c r="X25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
@@ -2894,7 +2948,7 @@
         <v>299</v>
       </c>
       <c r="D26">
-        <v>1.1703227388668931</v>
+        <v>3.7573519510989741</v>
       </c>
       <c r="E26">
         <v>47751.199999999997</v>
@@ -2903,34 +2957,34 @@
         <v>11.8072131147541</v>
       </c>
       <c r="G26">
-        <v>12.93610144784177</v>
+        <v>13.374613361327929</v>
       </c>
       <c r="H26">
-        <v>72.162809424445754</v>
+        <v>74.609006354087981</v>
       </c>
       <c r="I26">
-        <v>71.002147886721659</v>
+        <v>73.409000357457984</v>
       </c>
       <c r="J26">
-        <v>0.43604511160892712</v>
+        <v>0.45082630183295858</v>
       </c>
       <c r="K26">
-        <v>0.42896740542880191</v>
+        <v>0.44350867340943922</v>
       </c>
       <c r="L26">
-        <v>1.7118116290765131</v>
+        <v>1.711811629076512</v>
       </c>
       <c r="M26">
         <v>22153.67</v>
       </c>
       <c r="N26">
-        <v>22350.667312942121</v>
+        <v>21734.916627067931</v>
       </c>
       <c r="O26">
-        <v>196.99731294211961</v>
+        <v>418.75337293207491</v>
       </c>
       <c r="P26">
-        <v>-0.88139342858926017</v>
+        <v>1.926638965849879</v>
       </c>
       <c r="Q26" t="s">
         <v>23</v>
@@ -2942,10 +2996,10 @@
         <v>100</v>
       </c>
       <c r="T26" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="U26" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="V26">
         <v>0</v>
@@ -2968,28 +3022,28 @@
         <v>230</v>
       </c>
       <c r="D27">
-        <v>1.4910826560894459</v>
+        <v>3.8933824909002208</v>
       </c>
       <c r="E27">
         <v>48561.61</v>
       </c>
       <c r="F27">
-        <v>63.726382978723407</v>
+        <v>63.7263829787234</v>
       </c>
       <c r="G27">
-        <v>20.202819184631998</v>
+        <v>22.082151201807068</v>
       </c>
       <c r="H27">
-        <v>82.630307899534429</v>
+        <v>86.302766028402615</v>
       </c>
       <c r="I27">
-        <v>79.093718829043297</v>
+        <v>86.451274068954291</v>
       </c>
       <c r="J27">
-        <v>0.43159956620585838</v>
+        <v>0.47174836306221729</v>
       </c>
       <c r="K27">
-        <v>0.44028085115136062</v>
+        <v>0.45984888898031001</v>
       </c>
       <c r="L27">
         <v>1.875067866915693</v>
@@ -2998,13 +3052,13 @@
         <v>21848.21</v>
       </c>
       <c r="N27">
-        <v>23475.571997481911</v>
+        <v>23177.022480609368</v>
       </c>
       <c r="O27">
-        <v>1627.361997481908</v>
+        <v>1328.812480609366</v>
       </c>
       <c r="P27">
-        <v>-6.9321505676473674</v>
+        <v>-5.7333183402703787</v>
       </c>
       <c r="Q27" t="s">
         <v>22</v>
@@ -3016,10 +3070,10 @@
         <v>101</v>
       </c>
       <c r="T27" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="U27" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="V27">
         <v>0</v>
@@ -3042,7 +3096,7 @@
         <v>400</v>
       </c>
       <c r="D28">
-        <v>1.2703455129227821</v>
+        <v>3.881611289486278</v>
       </c>
       <c r="E28">
         <v>87649.02</v>
@@ -3051,16 +3105,16 @@
         <v>43.781999999999996</v>
       </c>
       <c r="G28">
-        <v>30.816942789128639</v>
+        <v>33.898637068041502</v>
       </c>
       <c r="H28">
-        <v>78.831537716120224</v>
+        <v>78.831537716120252</v>
       </c>
       <c r="I28">
-        <v>76.047174390760745</v>
+        <v>83.651891829836828</v>
       </c>
       <c r="J28">
-        <v>0.38224566220163841</v>
+        <v>0.42047022842180232</v>
       </c>
       <c r="K28">
         <v>0.40293408730727981</v>
@@ -3072,13 +3126,13 @@
         <v>38653.370000000003</v>
       </c>
       <c r="N28">
-        <v>39264.45658881795</v>
+        <v>39333.798454200158</v>
       </c>
       <c r="O28">
-        <v>611.0865888179469</v>
+        <v>680.4284542001551</v>
       </c>
       <c r="P28">
-        <v>-1.5563352759910021</v>
+        <v>-1.7298823936173831</v>
       </c>
       <c r="Q28" t="s">
         <v>23</v>
@@ -3090,10 +3144,10 @@
         <v>102</v>
       </c>
       <c r="T28" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="U28" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="V28">
         <v>0</v>
@@ -3116,28 +3170,28 @@
         <v>373</v>
       </c>
       <c r="D29">
-        <v>1.4758199891283841</v>
+        <v>3.9614115497656619</v>
       </c>
       <c r="E29">
-        <v>80813.460000000006</v>
+        <v>80813.459999999992</v>
       </c>
       <c r="F29">
         <v>81.304901960784321</v>
       </c>
       <c r="G29">
-        <v>15.302489285715129</v>
+        <v>17.736976217533439</v>
       </c>
       <c r="H29">
-        <v>77.179067508678926</v>
+        <v>83.747498786013296</v>
       </c>
       <c r="I29">
-        <v>78.43631950069026</v>
+        <v>90.914824875800079</v>
       </c>
       <c r="J29">
-        <v>0.44736356747456879</v>
+        <v>0.51853504411825024</v>
       </c>
       <c r="K29">
-        <v>0.43932485587444892</v>
+        <v>0.47671420531057218</v>
       </c>
       <c r="L29">
         <v>1.4220969821832989</v>
@@ -3146,13 +3200,13 @@
         <v>37610.19</v>
       </c>
       <c r="N29">
-        <v>37435.333620335368</v>
+        <v>38066.032535421102</v>
       </c>
       <c r="O29">
-        <v>174.85637966463401</v>
+        <v>455.84253542110667</v>
       </c>
       <c r="P29">
-        <v>0.46708914481170732</v>
+        <v>-1.197504717616519</v>
       </c>
       <c r="Q29" t="s">
         <v>23</v>
@@ -3164,10 +3218,10 @@
         <v>103</v>
       </c>
       <c r="T29" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="U29" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="V29">
         <v>0</v>
@@ -3190,7 +3244,7 @@
         <v>454</v>
       </c>
       <c r="D30">
-        <v>1.501809316409815</v>
+        <v>3.952129780025829</v>
       </c>
       <c r="E30">
         <v>95882.49</v>
@@ -3199,37 +3253,37 @@
         <v>111.6844</v>
       </c>
       <c r="G30">
-        <v>17.97222970897694</v>
+        <v>18.721072613517649</v>
       </c>
       <c r="H30">
-        <v>70.371641905433123</v>
+        <v>71.807797862686854</v>
       </c>
       <c r="I30">
-        <v>71.17269827051075</v>
+        <v>72.625202316847705</v>
       </c>
       <c r="J30">
-        <v>0.38425927700347368</v>
+        <v>0.40027008021195182</v>
       </c>
       <c r="K30">
-        <v>0.38919163453208189</v>
+        <v>0.40540795263758528</v>
       </c>
       <c r="L30">
         <v>1.489966456210964</v>
       </c>
       <c r="M30">
-        <v>40645.57</v>
+        <v>40645.569999999992</v>
       </c>
       <c r="N30">
-        <v>42734.801405546947</v>
+        <v>41563.891931192193</v>
       </c>
       <c r="O30">
-        <v>2089.2314055469542</v>
+        <v>918.32193119219301</v>
       </c>
       <c r="P30">
-        <v>-4.8888290967365373</v>
+        <v>-2.209422382082141</v>
       </c>
       <c r="Q30" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R30" t="s">
         <v>54</v>
@@ -3238,19 +3292,19 @@
         <v>104</v>
       </c>
       <c r="T30" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="U30" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="V30">
         <v>0</v>
       </c>
       <c r="W30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
@@ -3264,7 +3318,7 @@
         <v>397</v>
       </c>
       <c r="D31">
-        <v>1.522344668267041</v>
+        <v>3.9260467760571052</v>
       </c>
       <c r="E31">
         <v>90558</v>
@@ -3273,19 +3327,19 @@
         <v>58.00938775510204</v>
       </c>
       <c r="G31">
-        <v>11.24411029242291</v>
+        <v>12.52185009838005</v>
       </c>
       <c r="H31">
-        <v>78.851795307277627</v>
+        <v>82.207190852268155</v>
       </c>
       <c r="I31">
-        <v>77.619174332754312</v>
+        <v>86.439535052385494</v>
       </c>
       <c r="J31">
-        <v>0.39943777312480422</v>
+        <v>0.44482842916171372</v>
       </c>
       <c r="K31">
-        <v>0.41016157832396422</v>
+        <v>0.42761526250796261</v>
       </c>
       <c r="L31">
         <v>1.5812402632504361</v>
@@ -3294,13 +3348,13 @@
         <v>43466.07</v>
       </c>
       <c r="N31">
-        <v>41164.250757557747</v>
+        <v>41278.343799426642</v>
       </c>
       <c r="O31">
-        <v>2301.819242442245</v>
+        <v>2187.7262005733569</v>
       </c>
       <c r="P31">
-        <v>5.5917919070095818</v>
+        <v>5.2999369625962194</v>
       </c>
       <c r="Q31" t="s">
         <v>21</v>
@@ -3312,10 +3366,10 @@
         <v>105</v>
       </c>
       <c r="T31" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="U31" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="V31">
         <v>1</v>
@@ -3338,7 +3392,7 @@
         <v>462</v>
       </c>
       <c r="D32">
-        <v>1.510700610517</v>
+        <v>3.85228655681835</v>
       </c>
       <c r="E32">
         <v>102359.21</v>
@@ -3347,19 +3401,19 @@
         <v>53.269019607843141</v>
       </c>
       <c r="G32">
-        <v>16.504345705237931</v>
+        <v>17.908970871641149</v>
       </c>
       <c r="H32">
-        <v>83.108836762014093</v>
+        <v>84.771013497254387</v>
       </c>
       <c r="I32">
-        <v>82.66368993746714</v>
+        <v>89.698897591719671</v>
       </c>
       <c r="J32">
-        <v>0.40664288758695621</v>
+        <v>0.44125079291350572</v>
       </c>
       <c r="K32">
-        <v>0.42572012934758058</v>
+        <v>0.43423453193453232</v>
       </c>
       <c r="L32">
         <v>1.3808061834359411</v>
@@ -3368,13 +3422,13 @@
         <v>46804.33</v>
       </c>
       <c r="N32">
-        <v>46961.445061774481</v>
+        <v>46916.620696260063</v>
       </c>
       <c r="O32">
-        <v>157.11506177447879</v>
+        <v>112.2906962600609</v>
       </c>
       <c r="P32">
-        <v>-0.33456181249917882</v>
+        <v>-0.2393409725458171</v>
       </c>
       <c r="Q32" t="s">
         <v>23</v>
@@ -3386,10 +3440,10 @@
         <v>106</v>
       </c>
       <c r="T32" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="U32" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="V32">
         <v>0</v>
@@ -3412,43 +3466,43 @@
         <v>414</v>
       </c>
       <c r="D33">
-        <v>1.4965295523380651</v>
+        <v>3.9907454729015068</v>
       </c>
       <c r="E33">
-        <v>91703.8</v>
+        <v>91703.799999999988</v>
       </c>
       <c r="F33">
         <v>164.3133333333333</v>
       </c>
       <c r="G33">
-        <v>57.880351783259357</v>
+        <v>66.148973466582135</v>
       </c>
       <c r="H33">
-        <v>82.871078942577427</v>
+        <v>86.474169331385141</v>
       </c>
       <c r="I33">
-        <v>83.009055074022754</v>
+        <v>94.867491513168872</v>
       </c>
       <c r="J33">
-        <v>0.43983697038692587</v>
+        <v>0.50267082329934387</v>
       </c>
       <c r="K33">
-        <v>0.43365756059724508</v>
+        <v>0.45251223714495148</v>
       </c>
       <c r="L33">
         <v>1.433169152353416</v>
       </c>
       <c r="M33">
-        <v>44343.99</v>
+        <v>44343.990000000013</v>
       </c>
       <c r="N33">
-        <v>42570.071491996343</v>
+        <v>42154.857504999687</v>
       </c>
       <c r="O33">
-        <v>1773.9185080036621</v>
+        <v>2189.1324950003182</v>
       </c>
       <c r="P33">
-        <v>4.167055505972499</v>
+        <v>5.1930729329133198</v>
       </c>
       <c r="Q33" t="s">
         <v>21</v>
@@ -3460,10 +3514,10 @@
         <v>107</v>
       </c>
       <c r="T33" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="U33" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="V33">
         <v>1</v>
@@ -3486,46 +3540,46 @@
         <v>348</v>
       </c>
       <c r="D34">
-        <v>1.283018867924528</v>
+        <v>4</v>
       </c>
       <c r="E34">
-        <v>76798.98</v>
+        <v>76798.98000000001</v>
       </c>
       <c r="F34">
         <v>111.21528301886789</v>
       </c>
       <c r="G34">
-        <v>44.159960558921227</v>
+        <v>53.192679764155109</v>
       </c>
       <c r="H34">
-        <v>85.000565628908021</v>
+        <v>97.935434311567946</v>
       </c>
       <c r="I34">
-        <v>85.617329137057908</v>
+        <v>103.1299646423652</v>
       </c>
       <c r="J34">
-        <v>0.43411008734746098</v>
+        <v>0.52290533248671422</v>
       </c>
       <c r="K34">
-        <v>0.42273944805075259</v>
+        <v>0.48706936405847578</v>
       </c>
       <c r="L34">
         <v>1.1003059032470801</v>
       </c>
       <c r="M34">
-        <v>35643.440000000002</v>
+        <v>35643.44000000001</v>
       </c>
       <c r="N34">
-        <v>36400.092767666938</v>
+        <v>37593.723655914277</v>
       </c>
       <c r="O34">
-        <v>756.65276766693569</v>
+        <v>1950.283655914267</v>
       </c>
       <c r="P34">
-        <v>-2.0787110969646938</v>
+        <v>-5.187790583781255</v>
       </c>
       <c r="Q34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R34" t="s">
         <v>58</v>
@@ -3534,19 +3588,19 @@
         <v>108</v>
       </c>
       <c r="T34" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="U34" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="V34">
         <v>0</v>
       </c>
       <c r="W34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
@@ -3560,7 +3614,7 @@
         <v>329</v>
       </c>
       <c r="D35">
-        <v>1.3713942307692311</v>
+        <v>3.9618055555555549</v>
       </c>
       <c r="E35">
         <v>67499.05</v>
@@ -3569,19 +3623,19 @@
         <v>54.782115384615388</v>
       </c>
       <c r="G35">
-        <v>22.106366787717899</v>
+        <v>24.45810793534746</v>
       </c>
       <c r="H35">
-        <v>87.367589633061385</v>
+        <v>92.716625733044737</v>
       </c>
       <c r="I35">
-        <v>86.617297164209816</v>
+        <v>95.831903245508741</v>
       </c>
       <c r="J35">
-        <v>0.46225101059142049</v>
+        <v>0.5114266500160396</v>
       </c>
       <c r="K35">
-        <v>0.45680898739835879</v>
+        <v>0.48477688458601348</v>
       </c>
       <c r="L35">
         <v>1.398052712623856</v>
@@ -3590,16 +3644,16 @@
         <v>33771.230000000003</v>
       </c>
       <c r="N35">
-        <v>32709.435645284921</v>
+        <v>32994.112280849957</v>
       </c>
       <c r="O35">
-        <v>1061.794354715079</v>
+        <v>777.11771915003192</v>
       </c>
       <c r="P35">
-        <v>3.2461408574260648</v>
+        <v>2.3553224058132241</v>
       </c>
       <c r="Q35" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="R35" t="s">
         <v>59</v>
@@ -3608,19 +3662,19 @@
         <v>109</v>
       </c>
       <c r="T35" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="U35" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="V35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W35">
         <v>0</v>
       </c>
       <c r="X35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
@@ -3634,7 +3688,7 @@
         <v>346</v>
       </c>
       <c r="D36">
-        <v>1.416866454845193</v>
+        <v>3.967226073566541</v>
       </c>
       <c r="E36">
         <v>69660.75</v>
@@ -3643,19 +3697,19 @@
         <v>114.07125000000001</v>
       </c>
       <c r="G36">
-        <v>35.516243531495327</v>
+        <v>42.317226335398693</v>
       </c>
       <c r="H36">
-        <v>65.107630552648416</v>
+        <v>74.408720631598186</v>
       </c>
       <c r="I36">
-        <v>70.195598262288783</v>
+        <v>83.637308567833458</v>
       </c>
       <c r="J36">
-        <v>0.40881465477223589</v>
+        <v>0.48709831206904702</v>
       </c>
       <c r="K36">
-        <v>0.39456028995332149</v>
+        <v>0.45092604566093891</v>
       </c>
       <c r="L36">
         <v>1.0919104209282779</v>
@@ -3664,13 +3718,13 @@
         <v>31989.18</v>
       </c>
       <c r="N36">
-        <v>31895.627230307789</v>
+        <v>32112.86813309462</v>
       </c>
       <c r="O36">
-        <v>93.552769692207221</v>
+        <v>123.68813309461621</v>
       </c>
       <c r="P36">
-        <v>0.29330907655991068</v>
+        <v>-0.38516688257797399</v>
       </c>
       <c r="Q36" t="s">
         <v>23</v>
@@ -3682,10 +3736,10 @@
         <v>110</v>
       </c>
       <c r="T36" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="U36" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="V36">
         <v>0</v>
@@ -3708,7 +3762,7 @@
         <v>305</v>
       </c>
       <c r="D37">
-        <v>1.373106281989976</v>
+        <v>3.9747813426025611</v>
       </c>
       <c r="E37">
         <v>64071.94</v>
@@ -3717,19 +3771,19 @@
         <v>84.962909090909093</v>
       </c>
       <c r="G37">
-        <v>15.520853368755461</v>
+        <v>19.85225430887326</v>
       </c>
       <c r="H37">
-        <v>76.95787919340944</v>
+        <v>84.653667112750412</v>
       </c>
       <c r="I37">
-        <v>71.030670179315635</v>
+        <v>90.853182787496735</v>
       </c>
       <c r="J37">
-        <v>0.36323560275095429</v>
+        <v>0.46460367793726731</v>
       </c>
       <c r="K37">
-        <v>0.40541799550322521</v>
+        <v>0.44595979505354771</v>
       </c>
       <c r="L37">
         <v>0.80705564455029088</v>
@@ -3738,13 +3792,13 @@
         <v>30141.74</v>
       </c>
       <c r="N37">
-        <v>30169.168804838471</v>
+        <v>30585.472343267451</v>
       </c>
       <c r="O37">
-        <v>27.428804838476939</v>
+        <v>443.73234326745302</v>
       </c>
       <c r="P37">
-        <v>-9.0916673959137898E-2</v>
+        <v>-1.4507944761727001</v>
       </c>
       <c r="Q37" t="s">
         <v>23</v>
@@ -3756,10 +3810,10 @@
         <v>111</v>
       </c>
       <c r="T37" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="U37" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="V37">
         <v>0</v>
@@ -3782,7 +3836,7 @@
         <v>322</v>
       </c>
       <c r="D38">
-        <v>1.378564994647576</v>
+        <v>3.990582879242984</v>
       </c>
       <c r="E38">
         <v>64744.55</v>
@@ -3791,34 +3845,34 @@
         <v>122.14472727272729</v>
       </c>
       <c r="G38">
-        <v>50.39502716869157</v>
+        <v>56.565846822000744</v>
       </c>
       <c r="H38">
-        <v>75.699033526055047</v>
+        <v>80.066285460250526</v>
       </c>
       <c r="I38">
-        <v>81.206509863873492</v>
+        <v>91.15016413291923</v>
       </c>
       <c r="J38">
-        <v>0.43595580333021289</v>
+        <v>0.48933814659513708</v>
       </c>
       <c r="K38">
-        <v>0.41902299572663371</v>
+        <v>0.44319739932624719</v>
       </c>
       <c r="L38">
-        <v>0.78116826578056531</v>
+        <v>0.78116826578056542</v>
       </c>
       <c r="M38">
         <v>30871.119999999999</v>
       </c>
       <c r="N38">
-        <v>31292.652441857452</v>
+        <v>30635.44539314121</v>
       </c>
       <c r="O38">
-        <v>421.53244185744921</v>
+        <v>235.67460685879271</v>
       </c>
       <c r="P38">
-        <v>-1.3470652340534801</v>
+        <v>0.76928735271972415</v>
       </c>
       <c r="Q38" t="s">
         <v>23</v>
@@ -3830,10 +3884,10 @@
         <v>112</v>
       </c>
       <c r="T38" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="U38" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="V38">
         <v>0</v>
@@ -3856,7 +3910,7 @@
         <v>317</v>
       </c>
       <c r="D39">
-        <v>1.407407407407407</v>
+        <v>4</v>
       </c>
       <c r="E39">
         <v>63840.13</v>
@@ -3865,34 +3919,34 @@
         <v>188.5224074074074</v>
       </c>
       <c r="G39">
-        <v>49.476227491376527</v>
+        <v>63.612292488912693</v>
       </c>
       <c r="H39">
-        <v>63.278602952852403</v>
+        <v>77.660103623955223</v>
       </c>
       <c r="I39">
-        <v>67.804647062069947</v>
+        <v>87.177403365518487</v>
       </c>
       <c r="J39">
-        <v>0.38504079037710082</v>
+        <v>0.49505244477055821</v>
       </c>
       <c r="K39">
-        <v>0.36007370559774998</v>
+        <v>0.44190863868814778</v>
       </c>
       <c r="L39">
-        <v>0.75050874540375145</v>
+        <v>0.75050874540375134</v>
       </c>
       <c r="M39">
         <v>28055.05</v>
       </c>
       <c r="N39">
-        <v>29348.170653975711</v>
+        <v>29350.405406639351</v>
       </c>
       <c r="O39">
-        <v>1293.1206539757079</v>
+        <v>1295.3554066393519</v>
       </c>
       <c r="P39">
-        <v>-4.406137163443721</v>
+        <v>-4.4134157218364329</v>
       </c>
       <c r="Q39" t="s">
         <v>22</v>
@@ -3904,10 +3958,10 @@
         <v>113</v>
       </c>
       <c r="T39" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="U39" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="V39">
         <v>0</v>
@@ -3930,28 +3984,28 @@
         <v>327</v>
       </c>
       <c r="D40">
-        <v>1.1940779236163781</v>
+        <v>3.933433160148069</v>
       </c>
       <c r="E40">
         <v>65306.92</v>
       </c>
       <c r="F40">
-        <v>166.39517857142849</v>
+        <v>166.3951785714286</v>
       </c>
       <c r="G40">
-        <v>54.471954781321678</v>
+        <v>72.629273041762232</v>
       </c>
       <c r="H40">
-        <v>63.821466043290748</v>
+        <v>68.730809585082341</v>
       </c>
       <c r="I40">
-        <v>58.807250530883863</v>
+        <v>78.409667374511812</v>
       </c>
       <c r="J40">
-        <v>0.34851764920152828</v>
+        <v>0.46469019893537111</v>
       </c>
       <c r="K40">
-        <v>0.36690235560670481</v>
+        <v>0.39512561373029742</v>
       </c>
       <c r="L40">
         <v>0.78448032551647395</v>
@@ -3960,16 +4014,16 @@
         <v>28477.45</v>
       </c>
       <c r="N40">
-        <v>29377.714127608218</v>
+        <v>28748.100787845779</v>
       </c>
       <c r="O40">
-        <v>900.26412760821768</v>
+        <v>270.65078784578151</v>
       </c>
       <c r="P40">
-        <v>-3.064445803025154</v>
+        <v>-0.94145623685933399</v>
       </c>
       <c r="Q40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R40" t="s">
         <v>64</v>
@@ -3978,19 +4032,19 @@
         <v>114</v>
       </c>
       <c r="T40" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="U40" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="V40">
         <v>0</v>
       </c>
       <c r="W40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X40">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
@@ -4004,7 +4058,7 @@
         <v>303</v>
       </c>
       <c r="D41">
-        <v>1.43301416661443</v>
+        <v>3.9973553068718299</v>
       </c>
       <c r="E41">
         <v>67191.94</v>
@@ -4013,19 +4067,19 @@
         <v>60.524339622641513</v>
       </c>
       <c r="G41">
-        <v>10.54693528781225</v>
+        <v>12.15190370117498</v>
       </c>
       <c r="H41">
-        <v>79.478040003745576</v>
+        <v>84.246722403970296</v>
       </c>
       <c r="I41">
-        <v>74.156768430234663</v>
+        <v>85.441494060922537</v>
       </c>
       <c r="J41">
-        <v>0.36143203021261577</v>
+        <v>0.41643255654931821</v>
       </c>
       <c r="K41">
-        <v>0.40972349831556037</v>
+        <v>0.43430690821449403</v>
       </c>
       <c r="L41">
         <v>0.84139516557590044</v>
@@ -4034,13 +4088,13 @@
         <v>30479.26</v>
       </c>
       <c r="N41">
-        <v>31733.15190278539</v>
+        <v>31596.14107927322</v>
       </c>
       <c r="O41">
-        <v>1253.8919027853881</v>
+        <v>1116.8810792732179</v>
       </c>
       <c r="P41">
-        <v>-3.9513626211058082</v>
+        <v>-3.5348654649661699</v>
       </c>
       <c r="Q41" t="s">
         <v>22</v>
@@ -4052,10 +4106,10 @@
         <v>115</v>
       </c>
       <c r="T41" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="U41" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="V41">
         <v>0</v>
@@ -4078,7 +4132,7 @@
         <v>227</v>
       </c>
       <c r="D42">
-        <v>1.43906976744186</v>
+        <v>3.9974160206718339</v>
       </c>
       <c r="E42">
         <v>50059.35</v>
@@ -4087,19 +4141,19 @@
         <v>34.5946</v>
       </c>
       <c r="G42">
-        <v>-4.2107188507570648</v>
+        <v>-5.3983575009705946</v>
       </c>
       <c r="H42">
-        <v>69.153674634920634</v>
+        <v>73.56773897331982</v>
       </c>
       <c r="I42">
-        <v>58.994585753184012</v>
+        <v>75.634084298953866</v>
       </c>
       <c r="J42">
-        <v>0.33382923818802379</v>
+        <v>0.42798620280515881</v>
       </c>
       <c r="K42">
-        <v>0.38141885726410452</v>
+        <v>0.40576474177032401</v>
       </c>
       <c r="L42">
         <v>0.98196703296703292</v>
@@ -4108,13 +4162,13 @@
         <v>22660.3</v>
       </c>
       <c r="N42">
-        <v>23152.994246500009</v>
+        <v>22991.60941403174</v>
       </c>
       <c r="O42">
-        <v>492.69424650001019</v>
+        <v>331.30941403173711</v>
       </c>
       <c r="P42">
-        <v>-2.1279936463271469</v>
+        <v>-1.441001402144295</v>
       </c>
       <c r="Q42" t="s">
         <v>23</v>
@@ -4126,10 +4180,10 @@
         <v>116</v>
       </c>
       <c r="T42" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="U42" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="V42">
         <v>0</v>
@@ -4152,7 +4206,7 @@
         <v>359</v>
       </c>
       <c r="D43">
-        <v>1.474485255761147</v>
+        <v>3.9578288444114982</v>
       </c>
       <c r="E43">
         <v>76741.75</v>
@@ -4161,19 +4215,19 @@
         <v>86.680196078431379</v>
       </c>
       <c r="G43">
-        <v>6.7097767327903961</v>
+        <v>8.1475860326740523</v>
       </c>
       <c r="H43">
-        <v>83.465733936952972</v>
+        <v>86.872498587440845</v>
       </c>
       <c r="I43">
-        <v>69.768834575152994</v>
+        <v>84.719299126971492</v>
       </c>
       <c r="J43">
-        <v>0.35030460832695071</v>
+        <v>0.42536988153986871</v>
       </c>
       <c r="K43">
-        <v>0.42035235074505439</v>
+        <v>0.43750958955097502</v>
       </c>
       <c r="L43">
         <v>1.0177159916882159</v>
@@ -4182,16 +4236,16 @@
         <v>36644.300000000003</v>
       </c>
       <c r="N43">
-        <v>35791.188347260453</v>
+        <v>35293.024701944829</v>
       </c>
       <c r="O43">
-        <v>853.11165273954975</v>
+        <v>1351.2752980551741</v>
       </c>
       <c r="P43">
-        <v>2.3835801272154442</v>
+        <v>3.828731907981556</v>
       </c>
       <c r="Q43" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R43" t="s">
         <v>67</v>
@@ -4200,19 +4254,19 @@
         <v>117</v>
       </c>
       <c r="T43" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="U43" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="V43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W43">
         <v>0</v>
       </c>
       <c r="X43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.2">
@@ -4226,7 +4280,7 @@
         <v>351</v>
       </c>
       <c r="D44">
-        <v>1.393947673780819</v>
+        <v>3.888380353178075</v>
       </c>
       <c r="E44">
         <v>72034.86</v>
@@ -4235,19 +4289,19 @@
         <v>13.43660377358491</v>
       </c>
       <c r="G44">
-        <v>1.788876255402204</v>
+        <v>2.0610965551373228</v>
       </c>
       <c r="H44">
-        <v>77.193985874773219</v>
+        <v>80.221201007117273</v>
       </c>
       <c r="I44">
-        <v>76.756525241871415</v>
+        <v>88.43686603954751</v>
       </c>
       <c r="J44">
-        <v>0.40756443400743247</v>
+        <v>0.46958510874769388</v>
       </c>
       <c r="K44">
-        <v>0.42598876437141509</v>
+        <v>0.44269420611147059</v>
       </c>
       <c r="L44">
         <v>0.84694928517251544</v>
@@ -4256,13 +4310,13 @@
         <v>33799.46</v>
       </c>
       <c r="N44">
-        <v>34133.441030239257</v>
+        <v>34339.754775460278</v>
       </c>
       <c r="O44">
-        <v>333.98103023925802</v>
+        <v>540.2947754602792</v>
       </c>
       <c r="P44">
-        <v>-0.9784569623185071</v>
+        <v>-1.573379830441836</v>
       </c>
       <c r="Q44" t="s">
         <v>23</v>
@@ -4274,10 +4328,10 @@
         <v>118</v>
       </c>
       <c r="T44" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="U44" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="V44">
         <v>0</v>
@@ -4300,7 +4354,7 @@
         <v>293</v>
       </c>
       <c r="D45">
-        <v>1.5329031633806749</v>
+        <v>3.9417509915503062</v>
       </c>
       <c r="E45">
         <v>58133.5</v>
@@ -4309,19 +4363,19 @@
         <v>67.030185185185189</v>
       </c>
       <c r="G45">
-        <v>23.744458037407149</v>
+        <v>28.493349644888578</v>
       </c>
       <c r="H45">
-        <v>64.582084837789964</v>
+        <v>72.654845442513704</v>
       </c>
       <c r="I45">
-        <v>67.455270992855247</v>
+        <v>80.946325191426297</v>
       </c>
       <c r="J45">
-        <v>0.40257005583278122</v>
+        <v>0.48308406699933742</v>
       </c>
       <c r="K45">
-        <v>0.39754206470739151</v>
+        <v>0.44723482279581539</v>
       </c>
       <c r="L45">
         <v>1.1043983617877779</v>
@@ -4330,13 +4384,13 @@
         <v>27433.96</v>
       </c>
       <c r="N45">
-        <v>27139.920012803359</v>
+        <v>27212.84970694191</v>
       </c>
       <c r="O45">
-        <v>294.0399871966365</v>
+        <v>221.11029305808921</v>
       </c>
       <c r="P45">
-        <v>1.0834224531904371</v>
+        <v>0.8125216412071854</v>
       </c>
       <c r="Q45" t="s">
         <v>23</v>
@@ -4348,10 +4402,10 @@
         <v>119</v>
       </c>
       <c r="T45" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="U45" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="V45">
         <v>0</v>
@@ -4374,7 +4428,7 @@
         <v>300</v>
       </c>
       <c r="D46">
-        <v>1.6188950998827529</v>
+        <v>3.9194302418214009</v>
       </c>
       <c r="E46">
         <v>60882.64</v>
@@ -4383,37 +4437,37 @@
         <v>38.998260869565222</v>
       </c>
       <c r="G46">
-        <v>10.624715768717181</v>
+        <v>14.374615451793829</v>
       </c>
       <c r="H46">
-        <v>94.973018681978715</v>
+        <v>104.0180680802624</v>
       </c>
       <c r="I46">
-        <v>63.293950136326643</v>
+        <v>85.632991360912499</v>
       </c>
       <c r="J46">
-        <v>0.36733139845649249</v>
+        <v>0.49697777438231339</v>
       </c>
       <c r="K46">
-        <v>0.43064467775201187</v>
+        <v>0.47165845658553679</v>
       </c>
       <c r="L46">
-        <v>0.86826743872779677</v>
+        <v>0.86826743872779688</v>
       </c>
       <c r="M46">
-        <v>29872.15</v>
+        <v>29872.149999999991</v>
       </c>
       <c r="N46">
-        <v>30794.031152391799</v>
+        <v>29784.50357140402</v>
       </c>
       <c r="O46">
-        <v>921.88115239180115</v>
+        <v>87.646428595973703</v>
       </c>
       <c r="P46">
-        <v>-2.993700785160756</v>
+        <v>0.29426855608270958</v>
       </c>
       <c r="Q46" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R46" t="s">
         <v>70</v>
@@ -4422,19 +4476,19 @@
         <v>120</v>
       </c>
       <c r="T46" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="U46" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="V46">
         <v>0</v>
       </c>
       <c r="W46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.2">
@@ -4448,28 +4502,28 @@
         <v>334</v>
       </c>
       <c r="D47">
-        <v>1.350694990374167</v>
+        <v>3.980995761102808</v>
       </c>
       <c r="E47">
-        <v>65073.93</v>
+        <v>65073.930000000008</v>
       </c>
       <c r="F47">
         <v>53.702500000000001</v>
       </c>
       <c r="G47">
-        <v>14.732341883579171</v>
+        <v>19.6431225114389</v>
       </c>
       <c r="H47">
-        <v>65.640004033664752</v>
+        <v>76.580004705942216</v>
       </c>
       <c r="I47">
-        <v>59.848024992864268</v>
+        <v>79.797366657152367</v>
       </c>
       <c r="J47">
-        <v>0.32978202883673241</v>
+        <v>0.43970937178230968</v>
       </c>
       <c r="K47">
-        <v>0.36408858586749299</v>
+        <v>0.42477001684540849</v>
       </c>
       <c r="L47">
         <v>1.1934800318728891</v>
@@ -4478,13 +4532,13 @@
         <v>31500.77</v>
       </c>
       <c r="N47">
-        <v>29079.525220155541</v>
+        <v>29722.915441554709</v>
       </c>
       <c r="O47">
-        <v>2421.2447798444591</v>
+        <v>1777.8545584452911</v>
       </c>
       <c r="P47">
-        <v>8.326287178052862</v>
+        <v>5.981427232268496</v>
       </c>
       <c r="Q47" t="s">
         <v>21</v>
@@ -4496,10 +4550,10 @@
         <v>121</v>
       </c>
       <c r="T47" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="U47" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="V47">
         <v>1</v>
@@ -4522,43 +4576,43 @@
         <v>325</v>
       </c>
       <c r="D48">
-        <v>1.445744943193676</v>
+        <v>3.956775634003745</v>
       </c>
       <c r="E48">
         <v>67860.05</v>
       </c>
       <c r="F48">
-        <v>80.667307692307688</v>
+        <v>80.667307692307702</v>
       </c>
       <c r="G48">
-        <v>30.18389349671509</v>
+        <v>36.501452600678718</v>
       </c>
       <c r="H48">
-        <v>87.596123339863325</v>
+        <v>91.099968273457847</v>
       </c>
       <c r="I48">
-        <v>73.296876155910397</v>
+        <v>88.638082793193973</v>
       </c>
       <c r="J48">
-        <v>0.39102662974449548</v>
+        <v>0.47286941271427368</v>
       </c>
       <c r="K48">
-        <v>0.44870700298664618</v>
+        <v>0.46665528310611187</v>
       </c>
       <c r="L48">
         <v>1.028220732806618</v>
       </c>
       <c r="M48">
-        <v>32899.29</v>
+        <v>32899.289999999994</v>
       </c>
       <c r="N48">
-        <v>32868.687133479652</v>
+        <v>32437.811180017568</v>
       </c>
       <c r="O48">
-        <v>30.602866520348471</v>
+        <v>461.47881998242519</v>
       </c>
       <c r="P48">
-        <v>9.310644625406031E-2</v>
+        <v>1.4226570881166809</v>
       </c>
       <c r="Q48" t="s">
         <v>23</v>
@@ -4570,10 +4624,10 @@
         <v>122</v>
       </c>
       <c r="T48" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="U48" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="V48">
         <v>0</v>
@@ -4596,7 +4650,7 @@
         <v>284</v>
       </c>
       <c r="D49">
-        <v>1.537888302174016</v>
+        <v>3.9661329898172002</v>
       </c>
       <c r="E49">
         <v>55908.05</v>
@@ -4605,19 +4659,19 @@
         <v>103.9604081632653</v>
       </c>
       <c r="G49">
-        <v>39.874045281746277</v>
+        <v>50.098159456553027</v>
       </c>
       <c r="H49">
-        <v>79.373578580433175</v>
+        <v>84.550116313939682</v>
       </c>
       <c r="I49">
-        <v>82.014847310552597</v>
+        <v>103.0442953388994</v>
       </c>
       <c r="J49">
-        <v>0.3892603964860844</v>
+        <v>0.48907075455943938</v>
       </c>
       <c r="K49">
-        <v>0.37624017424414002</v>
+        <v>0.41899473949915578</v>
       </c>
       <c r="L49">
         <v>1.0153909865644559</v>
@@ -4626,16 +4680,16 @@
         <v>27868.52</v>
       </c>
       <c r="N49">
-        <v>27367.951061219679</v>
+        <v>27136.907931097841</v>
       </c>
       <c r="O49">
-        <v>500.56893878032503</v>
+        <v>731.61206890215908</v>
       </c>
       <c r="P49">
-        <v>1.8290333012529749</v>
+        <v>2.6960037995477011</v>
       </c>
       <c r="Q49" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R49" t="s">
         <v>73</v>
@@ -4644,19 +4698,19 @@
         <v>123</v>
       </c>
       <c r="T49" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="U49" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="V49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W49">
         <v>0</v>
       </c>
       <c r="X49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.2">
@@ -4670,28 +4724,28 @@
         <v>345</v>
       </c>
       <c r="D50">
-        <v>1.4241974314036749</v>
+        <v>3.9727612560207781</v>
       </c>
       <c r="E50">
         <v>66632.08</v>
       </c>
       <c r="F50">
-        <v>98.717924528301893</v>
+        <v>98.717924528301879</v>
       </c>
       <c r="G50">
-        <v>23.04172755207399</v>
+        <v>32.137146322629498</v>
       </c>
       <c r="H50">
-        <v>73.687212416341609</v>
+        <v>88.759596774229678</v>
       </c>
       <c r="I50">
-        <v>67.26649199056294</v>
+        <v>93.819054618416729</v>
       </c>
       <c r="J50">
-        <v>0.37933068850215718</v>
+        <v>0.52906648659511391</v>
       </c>
       <c r="K50">
-        <v>0.40333492842649937</v>
+        <v>0.48583525469555622</v>
       </c>
       <c r="L50">
         <v>0.77387011432965125</v>
@@ -4700,16 +4754,16 @@
         <v>32220.68</v>
       </c>
       <c r="N50">
-        <v>31431.423734747859</v>
+        <v>32477.661961722151</v>
       </c>
       <c r="O50">
-        <v>789.25626525213738</v>
+        <v>256.98196172215103</v>
       </c>
       <c r="P50">
-        <v>2.5110420447789128</v>
+        <v>-0.79125757890154591</v>
       </c>
       <c r="Q50" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="R50" t="s">
         <v>74</v>
@@ -4718,19 +4772,19 @@
         <v>124</v>
       </c>
       <c r="T50" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="U50" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="V50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W50">
         <v>0</v>
       </c>
       <c r="X50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.2">
@@ -4744,28 +4798,28 @@
         <v>310</v>
       </c>
       <c r="D51">
-        <v>1.3824615172382331</v>
+        <v>3.8563400217698089</v>
       </c>
       <c r="E51">
         <v>61719.87</v>
       </c>
       <c r="F51">
-        <v>164.7150943396226</v>
+        <v>164.71509433962271</v>
       </c>
       <c r="G51">
-        <v>55.00957401599787</v>
+        <v>72.887685571197181</v>
       </c>
       <c r="H51">
-        <v>69.898937654406481</v>
+        <v>80.53573251485966</v>
       </c>
       <c r="I51">
-        <v>78.56616835994194</v>
+        <v>104.1001730769231</v>
       </c>
       <c r="J51">
-        <v>0.35082835750762631</v>
+        <v>0.46484757369760482</v>
       </c>
       <c r="K51">
-        <v>0.33023278213026602</v>
+        <v>0.3889408322867578</v>
       </c>
       <c r="L51">
         <v>1.0371377640225059</v>
@@ -4774,13 +4828,13 @@
         <v>28842.07</v>
       </c>
       <c r="N51">
-        <v>28376.136209669159</v>
+        <v>28654.780410976098</v>
       </c>
       <c r="O51">
-        <v>465.93379033084062</v>
+        <v>187.28958902389789</v>
       </c>
       <c r="P51">
-        <v>1.641991661190553</v>
+        <v>0.65360678510786052</v>
       </c>
       <c r="Q51" t="s">
         <v>23</v>
@@ -4792,10 +4846,10 @@
         <v>125</v>
       </c>
       <c r="T51" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="U51" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="V51">
         <v>0</v>

</xml_diff>

<commit_message>
chore: update revenue-data.xlsx with latest local changes
</commit_message>
<xml_diff>
--- a/data/revenue-data.xlsx
+++ b/data/revenue-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/Revenue_Performance_Analysis-2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61AC9EBD-220F-0E44-AB09-A40FDF321FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938D0AF0-C104-7D42-A58A-7623088E67D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="820" windowWidth="26800" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1480" windowWidth="25800" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -1058,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
chore: update revenue-data.xlsx and revenue-data.json with latest uploaded data
</commit_message>
<xml_diff>
--- a/data/revenue-data.xlsx
+++ b/data/revenue-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/Revenue_Performance_Analysis-2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DA868D9-5081-7D44-BA9E-5E0F5BB4F57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBF62DE9-AD94-DF4E-A8BB-71BE738FAABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="21660" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="22460" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="234">
   <si>
     <t>Year</t>
   </si>
@@ -124,7 +124,7 @@
     <t>2025</t>
   </si>
   <si>
-    <t>4-MEDICAID – After Hours Upfront Collections Efficiency decreased from avg -0.33 to -8.15; 15-UNITED HEALTHCARE – Medications Payment Amount* increased from avg 46.29 to 209.45; 13-TRICARE – Lab/Test CPT Codes Visit Count increased from avg 2.59 to 9.00; 13-TRICARE – New E/M Codes Payment Amount* increased from avg 298.18 to 1024.98; 15-UNITED HEALTHCARE – Medications Payment per Visit increased from avg 21.82 to 69.82; 15-UNITED HEALTHCARE – Medications NRV Zero Balance* increased from avg 22.82 to 69.82</t>
+    <t>4-MEDICAID – After Hours Collection Efficiency increased from avg -0.33 to -8.15; 15-UNITED HEALTHCARE – Medications Payment Amount* increased from avg 46.29 to 209.45; 13-TRICARE – Lab/Test CPT Codes Visit Count increased from avg 2.59 to 9.00; 13-TRICARE – New E/M Codes Payment Amount* increased from avg 298.18 to 1024.98; 15-UNITED HEALTHCARE – Medications Payment per Visit increased from avg 21.82 to 69.82; 15-UNITED HEALTHCARE – Medications NRV Zero Balance* increased from avg 22.82 to 69.82</t>
   </si>
   <si>
     <t>4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 4.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 3.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 29.89 to 108.38; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 68.64 to 216.76; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Zero Balance Collection Rate increased from avg 0.27 to 0.84; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Collection Rate* increased from avg 0.27 to 0.84</t>
@@ -133,22 +133,22 @@
     <t>15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit increased from avg 0.88 to 5.00; 1-SELF PAY – Existing E/M Code Labs per Visit increased from avg 0.91 to 2.88; 3-MEDICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.67 to 2.00; 5-COMMERCIAL – Lab/Test CPT Codes Charge Amount increased from avg 496.66 to 1371.00; 12-HUMANA – X-Ray CPT Codes Zero Balance Collection Rate increased from avg 0.26 to 0.65; 12-HUMANA – X-Ray CPT Codes Collection Rate* increased from avg 0.26 to 0.65</t>
   </si>
   <si>
-    <t>15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency decreased from avg 9.06 to -145.36; 12-HUMANA – Medications Labs per Visit increased from avg 0.96 to 5.00; 12-HUMANA – Lab/Test CPT Codes Charge Amount increased from avg 376.92 to 1799.00; 5-COMMERCIAL – Lab/Test CPT Codes Payment Amount* increased from avg 150.59 to 659.65; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -150.00; 13-TRICARE – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.66 to 7.00</t>
+    <t>15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency increased from avg 9.06 to -145.36; 12-HUMANA – Medications Labs per Visit increased from avg 0.96 to 5.00; 12-HUMANA – Lab/Test CPT Codes Charge Amount increased from avg 376.92 to 1799.00; 5-COMMERCIAL – Lab/Test CPT Codes Payment Amount* increased from avg 150.59 to 659.65; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance increased from avg 64.00 to -150.00; 13-TRICARE – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.66 to 7.00</t>
   </si>
   <si>
     <t>15-UNITED HEALTHCARE – Medications Payment Amount* increased from avg 46.29 to 337.58; 1-SELF PAY – X-Ray CPT Codes Labs per Visit increased from avg 0.39 to 2.50; 15-UNITED HEALTHCARE – Medications Payment per Visit increased from avg 21.82 to 112.53; 15-UNITED HEALTHCARE – Medications NRV Zero Balance* increased from avg 22.82 to 112.53; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 2.50; 15-UNITED HEALTHCARE – Medications Collection Rate* increased from avg 0.16 to 0.52</t>
   </si>
   <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -122.59; 12-HUMANA – New E/M Codes Charge Billed Balance decreased from avg 0.44 to -250.00; 12-HUMANA – New E/M Codes Upfront Collections Efficiency decreased from avg -6.89 to -225.56; 3-MEDICARE – Existing E/M Code Upfront Collections Efficiency decreased from avg -7.53 to -132.53; 12-HUMANA – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency decreased from avg -12.86 to -180.04; 3-MEDICARE – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 1.82 to -8.49</t>
-  </si>
-  <si>
-    <t>12-HUMANA – Medications Labs per Visit increased from avg 0.96 to 4.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance decreased from avg 63.06 to -53.44; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 2.00; 12-HUMANA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.51 to 4.00; 15-UNITED HEALTHCARE – DME Payment per Visit increased from avg 73.28 to 181.96; 15-UNITED HEALTHCARE – DME NRV Zero Balance* increased from avg 73.88 to 181.96</t>
-  </si>
-  <si>
-    <t>12-HUMANA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 0.12 to -4.07; 1-SELF PAY – X-Ray CPT Codes Labs per Visit increased from avg 0.39 to 9.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 9.00; 1-SELF PAY – New E/M Codes Labs per Visit increased from avg 0.86 to 3.50; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 0.95 to 3.67; 1-SELF PAY – Medications Labs per Visit increased from avg 1.13 to 4.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -102.16; 3-MEDICARE – Existing E/M Code Upfront Collections Efficiency decreased from avg -7.53 to -101.04; 18-CIGNA – X-Ray CPT Codes Labs per Visit increased from avg 0.69 to 3.00; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 4.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 2.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 1.43 to 4.00</t>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to -122.59; 12-HUMANA – New E/M Codes Charge Billed Balance increased from avg 0.44 to -250.00; 12-HUMANA – New E/M Codes Collection Efficiency increased from avg -6.89 to -225.56; 3-MEDICARE – Existing E/M Code Collection Efficiency increased from avg -7.53 to -132.53; 12-HUMANA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg -12.86 to -180.04; 3-MEDICARE – Lab/Test CPT Codes Collection Efficiency increased from avg 1.82 to -8.49</t>
+  </si>
+  <si>
+    <t>12-HUMANA – Medications Labs per Visit increased from avg 0.96 to 4.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 63.06 to -53.44; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 2.00; 12-HUMANA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.51 to 4.00; 15-UNITED HEALTHCARE – DME Payment per Visit increased from avg 73.28 to 181.96; 15-UNITED HEALTHCARE – DME NRV Zero Balance* increased from avg 73.88 to 181.96</t>
+  </si>
+  <si>
+    <t>12-HUMANA – Lab/Test CPT Codes Collection Efficiency increased from avg 0.12 to -4.07; 1-SELF PAY – X-Ray CPT Codes Labs per Visit increased from avg 0.39 to 9.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 9.00; 1-SELF PAY – New E/M Codes Labs per Visit increased from avg 0.86 to 3.50; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 0.95 to 3.67; 1-SELF PAY – Medications Labs per Visit increased from avg 1.13 to 4.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to -102.16; 3-MEDICARE – Existing E/M Code Collection Efficiency increased from avg -7.53 to -101.04; 18-CIGNA – X-Ray CPT Codes Labs per Visit increased from avg 0.69 to 3.00; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 4.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 2.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 1.43 to 4.00</t>
   </si>
   <si>
     <t>15-UNITED HEALTHCARE – Medications Labs per Visit increased from avg 1.45 to 7.00; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 36.72 to 119.46; 5-COMMERCIAL – X-Ray CPT Codes Labs per Visit increased from avg 1.10 to 3.00; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 135.08 to 349.00; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 3.00; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 28.43 to 59.73</t>
@@ -160,34 +160,34 @@
     <t>3-MEDICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.67 to 2.50; 18-CIGNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.94 to 7.00; 18-CIGNA – X-Ray CPT Codes Charge Amount increased from avg 240.79 to 607.00; 1-SELF PAY – Existing E/M Code Labs per Visit increased from avg 0.91 to 2.20; 4-MEDICAID – X-Ray CPT Codes Charge Amount increased from avg 339.20 to 769.00; 4-MEDICAID – X-Ray CPT Codes Payment Amount* increased from avg 68.53 to 152.74</t>
   </si>
   <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -60.44; 3-MEDICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.67 to 2.00; 15-UNITED HEALTHCARE – Existing E/M Code Upfront Collections Efficiency decreased from avg -36.34 to -106.22; 13-TRICARE – New E/M Codes Labs per Visit increased from avg 1.32 to 3.50; 12-HUMANA – New E/M Codes Labs per Visit increased from avg 0.90 to 2.00; 12-HUMANA – Existing E/M Code Payment Amount* increased from avg 205.83 to 451.23</t>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to -60.44; 3-MEDICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.67 to 2.00; 15-UNITED HEALTHCARE – Existing E/M Code Collection Efficiency increased from avg -36.34 to -106.22; 13-TRICARE – New E/M Codes Labs per Visit increased from avg 1.32 to 3.50; 12-HUMANA – New E/M Codes Labs per Visit increased from avg 0.90 to 2.00; 12-HUMANA – Existing E/M Code Payment Amount* increased from avg 205.83 to 451.23</t>
   </si>
   <si>
     <t>13-TRICARE – X-Ray CPT Codes Labs per Visit increased from avg 0.82 to 6.00; 13-TRICARE – Medications Labs per Visit increased from avg 1.42 to 6.00; 5-COMMERCIAL – New E/M Codes Labs per Visit increased from avg 1.75 to 5.67; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 4.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.87 to 5.50; 5-COMMERCIAL – Medications Labs per Visit increased from avg 1.73 to 5.00</t>
   </si>
   <si>
-    <t>4-MEDICAID – X-Ray CPT Codes Upfront Collections Efficiency decreased from avg 3.46 to -3.92; 5-COMMERCIAL – New E/M Codes Labs per Visit increased from avg 1.75 to 5.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.87 to 5.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit increased from avg 0.39 to 1.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 2.14 to 5.00; 13-TRICARE – New E/M Codes Payment Amount* increased from avg 298.18 to 678.62</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -14.70; 3-MEDICARE – X-Ray CPT Codes Charge Billed Balance decreased from avg 3.31 to -4.99; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 50.76 to 155.00; 18-CIGNA – New E/M Codes Labs per Visit increased from avg 1.98 to 5.00; 1-SELF PAY – X-Ray CPT Codes Payment per Visit increased from avg 90.55 to 218.50; 3-MEDICARE – DME Charge Amount increased from avg 319.54 to 689.80</t>
+    <t>4-MEDICAID – X-Ray CPT Codes Collection Efficiency increased from avg 3.46 to -3.92; 5-COMMERCIAL – New E/M Codes Labs per Visit increased from avg 1.75 to 5.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.87 to 5.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit increased from avg 0.39 to 1.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 2.14 to 5.00; 13-TRICARE – New E/M Codes Payment Amount* increased from avg 298.18 to 678.62</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to -14.70; 3-MEDICARE – X-Ray CPT Codes Charge Billed Balance increased from avg 3.31 to -4.99; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 50.76 to 155.00; 18-CIGNA – New E/M Codes Labs per Visit increased from avg 1.98 to 5.00; 1-SELF PAY – X-Ray CPT Codes Payment per Visit increased from avg 90.55 to 218.50; 3-MEDICARE – DME Charge Amount increased from avg 319.54 to 689.80</t>
   </si>
   <si>
     <t>15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 25.12 to 135.81; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 54.50 to 271.61; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 27.53 to 135.81; 5-COMMERCIAL – Medications Labs per Visit increased from avg 1.73 to 5.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 2.00; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 235.39 to 647.00</t>
   </si>
   <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -20.77; 15-UNITED HEALTHCARE – Vaccines Labs per Visit increased from avg 0.57 to 8.00; 3-MEDICARE – Medications Charge Billed Balance decreased from avg 1.05 to -2.50; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 116.93 to 415.00; 3-MEDICARE – Existing E/M Code Upfront Collections Efficiency decreased from avg -7.53 to -25.87; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.87 to 6.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -20.77; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 116.93 to 655.00; 1-SELF PAY – DME Charge Amount increased from avg 133.93 to 705.92; 3-MEDICARE – Existing E/M Code Upfront Collections Efficiency decreased from avg -7.53 to -24.20; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 2.58 to 8.00; 15-UNITED HEALTHCARE – Self-pay physical &amp; No Charge Charge Amount increased from avg 17.33 to 52.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -20.77; 3-MEDICARE – Medications Labs per Visit increased from avg 0.90 to 4.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 3.00; 1-SELF PAY – X-Ray CPT Codes Payment per Visit increased from avg 90.55 to 287.00; 13-TRICARE – Medications Labs per Visit increased from avg 1.42 to 4.00; 5-COMMERCIAL – New E/M Codes Labs per Visit increased from avg 1.75 to 4.00</t>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to -20.77; 15-UNITED HEALTHCARE – Vaccines Labs per Visit increased from avg 0.57 to 8.00; 3-MEDICARE – Medications Charge Billed Balance increased from avg 1.05 to -2.50; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 116.93 to 415.00; 3-MEDICARE – Existing E/M Code Collection Efficiency increased from avg -7.53 to -25.87; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.87 to 6.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to -20.77; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 116.93 to 655.00; 1-SELF PAY – DME Charge Amount increased from avg 133.93 to 705.92; 3-MEDICARE – Existing E/M Code Collection Efficiency increased from avg -7.53 to -24.20; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 2.58 to 8.00; 15-UNITED HEALTHCARE – Self-pay physical &amp; No Charge Charge Amount increased from avg 17.33 to 52.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to -20.77; 3-MEDICARE – Medications Labs per Visit increased from avg 0.90 to 4.00; 1-SELF PAY – Vaccines Labs per Visit increased from avg 0.68 to 3.00; 1-SELF PAY – X-Ray CPT Codes Payment per Visit increased from avg 90.55 to 287.00; 13-TRICARE – Medications Labs per Visit increased from avg 1.42 to 4.00; 5-COMMERCIAL – New E/M Codes Labs per Visit increased from avg 1.75 to 4.00</t>
   </si>
   <si>
     <t>1-SELF PAY – Medications Labs per Visit increased from avg 1.13 to 4.00; 15-UNITED HEALTHCARE – DME Payment per Visit increased from avg 73.28 to 207.02; 15-UNITED HEALTHCARE – DME NRV Zero Balance* increased from avg 73.88 to 207.02; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 135.08 to 360.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.87 to 4.20; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 2.33 to 5.00</t>
   </si>
   <si>
-    <t>13-TRICARE – Existing E/M Code Upfront Collections Efficiency decreased from avg 33.42 to -204.76; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 4.00; 1-SELF PAY – Medications Labs per Visit increased from avg 1.13 to 3.00; 13-TRICARE – Existing E/M Code Charge Billed Balance decreased from avg 88.96 to -55.40; 13-TRICARE – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 25.52 to -14.26; 13-TRICARE – Existing E/M Code Labs per Visit increased from avg 1.42 to 3.33</t>
+    <t>13-TRICARE – Existing E/M Code Collection Efficiency increased from avg 33.42 to -204.76; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 4.00; 1-SELF PAY – Medications Labs per Visit increased from avg 1.13 to 3.00; 13-TRICARE – Existing E/M Code Charge Billed Balance increased from avg 88.96 to -55.40; 13-TRICARE – Lab/Test CPT Codes Collection Efficiency increased from avg 25.52 to -14.26; 13-TRICARE – Existing E/M Code Labs per Visit increased from avg 1.42 to 3.33</t>
   </si>
   <si>
     <t>13-TRICARE – Existing E/M Code Labs per Visit increased from avg 1.42 to 7.00; 13-TRICARE – Medications Labs per Visit increased from avg 1.42 to 7.00; 13-TRICARE – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.66 to 7.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 49.02 to 201.33; 18-CIGNA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 51.31 to 201.33; 3-MEDICARE – New E/M Codes Payment Amount* increased from avg 273.10 to 869.67</t>
@@ -199,70 +199,70 @@
     <t>18-CIGNA – X-Ray CPT Codes Labs per Visit increased from avg 0.69 to 2.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 2.14 to 6.00; 5-COMMERCIAL – New E/M Codes Payment per Visit increased from avg 142.42 to 342.70; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 3.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 1.67; 5-COMMERCIAL – Existing E/M Code Labs per Visit increased from avg 2.15 to 5.00</t>
   </si>
   <si>
-    <t>5-COMMERCIAL – Existing E/M Code Upfront Collections Efficiency decreased from avg 1.93 to -329.00; 18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -33.96; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 25.96 to -463.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 3.00; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -116.80; 5-COMMERCIAL – Existing E/M Code Payment per Visit increased from avg 115.74 to 409.50</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -383.59; 15-UNITED HEALTHCARE – Existing E/M Code Upfront Collections Efficiency decreased from avg -36.34 to -313.71; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 25.96 to -122.70; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -208.13; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit increased from avg 0.88 to 4.00; 18-CIGNA – X-Ray CPT Codes Labs per Visit increased from avg 0.69 to 3.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -70.00; 1-SELF PAY – X-Ray CPT Codes Visit Count increased from avg 2.51 to 8.00; 1-SELF PAY – X-Ray CPT Codes Charge Amount increased from avg 235.81 to 735.00; 12-HUMANA – Existing E/M Code Labs per Visit increased from avg 1.20 to 3.00; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 3.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 1.67</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -150.00; 18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -47.43; 3-MEDICARE – Existing E/M Code Upfront Collections Efficiency decreased from avg -7.53 to -154.66; 18-CIGNA – Existing E/M Code Upfront Collections Efficiency decreased from avg -18.20 to -163.95; 15-UNITED HEALTHCARE – Existing E/M Code Upfront Collections Efficiency decreased from avg -36.34 to -204.84; 5-COMMERCIAL – New E/M Codes Upfront Collections Efficiency decreased from avg 41.75 to -129.00</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -85.21; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -317.35; 15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency decreased from avg 9.06 to -203.50; 18-CIGNA – New E/M Codes Upfront Collections Efficiency decreased from avg 15.12 to -163.48; 18-CIGNA – Existing E/M Code Upfront Collections Efficiency decreased from avg -18.20 to -208.94; 15-UNITED HEALTHCARE – Existing E/M Code Upfront Collections Efficiency decreased from avg -36.34 to -266.78</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -273.29; 15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency decreased from avg 9.06 to -127.16; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 23.50 to -223.08; 5-COMMERCIAL – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 20.86 to -148.26; 18-CIGNA – New E/M Codes Upfront Collections Efficiency decreased from avg 15.12 to -66.78; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 25.96 to -109.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -48.64; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -160.99; 15-UNITED HEALTHCARE – DME Labs per Visit increased from avg 0.10 to 2.00; 18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -18.72; 18-CIGNA – New E/M Codes Upfront Collections Efficiency decreased from avg 15.12 to -148.04; 3-MEDICARE – Existing E/M Code Upfront Collections Efficiency decreased from avg -7.53 to -50.26</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -15.53; 15-UNITED HEALTHCARE – Vaccines Charge Billed Balance decreased from avg -10.71 to -150.00; 15-UNITED HEALTHCARE – Vaccines Payment per Visit increased from avg 82.57 to 318.92; 15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency decreased from avg 9.06 to -15.14; 15-UNITED HEALTHCARE – Vaccines Payment Amount* increased from avg 90.91 to 318.92; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decreased from avg 64.00 to -73.99</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 0.15 to -18.59; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -202.89; 3-MEDICARE – Existing E/M Code Upfront Collections Efficiency decreased from avg -7.53 to -50.26; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 25.12 to 166.19; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 54.50 to 332.39; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 27.53 to 166.19</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -92.15; 5-COMMERCIAL – Existing E/M Code Upfront Collections Efficiency decreased from avg 1.93 to -39.70; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -135.15; 18-CIGNA – New E/M Codes Upfront Collections Efficiency decreased from avg 15.12 to -117.84; 15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency decreased from avg 9.06 to -51.44; 4-MEDICAID – Self-pay physical &amp; No Charge Labs per Visit increased from avg 0.43 to 3.00</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -293.19; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -166.67; 12-HUMANA – X-Ray CPT Codes Charge Billed Balance decreased from avg -1.21 to -25.51; 15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency decreased from avg 9.06 to -133.31; 18-CIGNA – Existing E/M Code Upfront Collections Efficiency decreased from avg -18.20 to -300.32; 15-UNITED HEALTHCARE – Existing E/M Code Upfront Collections Efficiency decreased from avg -36.34 to -243.09</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -54.03; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -110.00; 15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency decreased from avg 9.06 to -61.14; 13-TRICARE – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 45.55 to 373.44; 13-TRICARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 47.27 to 373.44; 13-TRICARE – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 48.14 to 373.44</t>
-  </si>
-  <si>
-    <t>12-HUMANA – New E/M Codes Charge Billed Balance decreased from avg 0.44 to -105.00; 12-HUMANA – New E/M Codes Upfront Collections Efficiency decreased from avg -6.89 to -104.90; 13-TRICARE – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 200.53 to 752.00; 12-HUMANA – Medications Charge Amount increased from avg 103.29 to 355.00; 12-HUMANA – Medications Payment Amount* increased from avg 12.94 to 40.91; 15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency decreased from avg 9.06 to -8.58</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – New E/M Codes Upfront Collections Efficiency decreased from avg 13.65 to -134.15; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 50.76 to 200.00; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 2.76 to -5.18; 18-CIGNA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 51.31 to 182.96; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 12.09 to -16.34; 3-MEDICARE – New E/M Codes Charge Amount increased from avg 667.84 to 1860.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency decreased from avg 9.06 to -88.35; 12-HUMANA – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 30.05 to 216.28; 12-HUMANA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 35.91 to 216.28; 12-HUMANA – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 53.34 to 216.28; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 29.89 to 114.54; 18-CIGNA – Medications Charge Amount increased from avg 210.12 to 730.00</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – Self-pay physical &amp; No Charge Charge Amount increased from avg 7.86 to 45.00; 12-HUMANA – New E/M Codes Charge Billed Balance decreased from avg 0.44 to -1.25; 15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency decreased from avg 9.06 to -24.47; 4-MEDICAID – Existing E/M Code Upfront Collections Efficiency decreased from avg 70.72 to -110.00; 18-CIGNA – New E/M Codes Upfront Collections Efficiency decreased from avg 15.12 to -20.00; 4-MEDICAID – New E/M Codes Upfront Collections Efficiency decreased from avg 162.82 to -191.91</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg -1.08 to -164.28; 3-MEDICARE – New E/M Codes Upfront Collections Efficiency decreased from avg 13.65 to -110.54; 18-CIGNA – New E/M Codes Upfront Collections Efficiency decreased from avg 15.12 to -90.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 62.96 to 296.13; 3-MEDICARE – New E/M Codes Charge Billed Balance decreased from avg 45.73 to -123.57; 5-COMMERCIAL – X-Ray CPT Codes Charge Billed Balance decreased from avg 17.35 to -35.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency decreased from avg 9.06 to -209.42; 4-MEDICAID – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 43.58 to 532.54; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 29.89 to 266.27; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 68.64 to 532.54; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 267.01 to 2000.00; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 25.96 to -137.70</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency decreased from avg 9.06 to -73.35; 3-MEDICARE – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 1.82 to -11.46; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -40.52; 5-COMMERCIAL – New E/M Codes Upfront Collections Efficiency decreased from avg 41.75 to -52.21; 3-MEDICARE – New E/M Codes Charge Amount increased from avg 667.84 to 2170.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 0.95 to 3.00</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – Self-pay physical &amp; No Charge Charge Amount increased from avg 7.86 to 65.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Billed Balance decreased from avg -11.50 to -61.00; 15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency decreased from avg 9.06 to -14.10; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -25.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency decreased from avg 4.07 to -5.11; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 0.95 to 3.00</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – DME Upfront Collections Efficiency decreased from avg 6.87 to -93.40; 18-CIGNA – Existing E/M Code Upfront Collections Efficiency decreased from avg -18.20 to -71.17; 5-COMMERCIAL – Lab/Test CPT Codes Collection Rate* increased from avg 0.28 to 1.00; 1-SELF PAY – X-Ray CPT Codes Visit Count increased from avg 2.51 to 9.00; 1-SELF PAY – X-Ray CPT Codes Charge Amount increased from avg 235.81 to 800.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit increased from avg 0.88 to 3.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg -0.06 to -150.00; 3-MEDICARE – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 1.82 to -121.51; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg -7.36 to -262.19; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 62.96 to 381.15; 15-UNITED HEALTHCARE – Existing E/M Code Upfront Collections Efficiency decreased from avg -36.34 to -162.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 95.70 to 381.15</t>
+    <t>5-COMMERCIAL – Existing E/M Code Collection Efficiency increased from avg 1.93 to -329.00; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to -33.96; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to -463.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 3.00; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance increased from avg 64.00 to -116.80; 5-COMMERCIAL – Existing E/M Code Payment per Visit increased from avg 115.74 to 409.50</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to -383.59; 15-UNITED HEALTHCARE – Existing E/M Code Collection Efficiency increased from avg -36.34 to -313.71; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to -122.70; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance increased from avg 64.00 to -208.13; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit increased from avg 0.88 to 4.00; 18-CIGNA – X-Ray CPT Codes Labs per Visit increased from avg 0.69 to 3.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to -70.00; 1-SELF PAY – X-Ray CPT Codes Visit Count increased from avg 2.51 to 8.00; 1-SELF PAY – X-Ray CPT Codes Charge Amount increased from avg 235.81 to 735.00; 12-HUMANA – Existing E/M Code Labs per Visit increased from avg 1.20 to 3.00; 4-MEDICAID – Medications Labs per Visit increased from avg 1.26 to 3.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit increased from avg 0.71 to 1.67</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to -150.00; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to -47.43; 3-MEDICARE – Existing E/M Code Collection Efficiency increased from avg -7.53 to -154.66; 18-CIGNA – Existing E/M Code Collection Efficiency increased from avg -18.20 to -163.95; 15-UNITED HEALTHCARE – Existing E/M Code Collection Efficiency increased from avg -36.34 to -204.84; 5-COMMERCIAL – New E/M Codes Collection Efficiency increased from avg 41.75 to -129.00</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to -85.21; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to -317.35; 15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency increased from avg 9.06 to -203.50; 18-CIGNA – New E/M Codes Collection Efficiency increased from avg 15.12 to -163.48; 18-CIGNA – Existing E/M Code Collection Efficiency increased from avg -18.20 to -208.94; 15-UNITED HEALTHCARE – Existing E/M Code Collection Efficiency increased from avg -36.34 to -266.78</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to -273.29; 15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency increased from avg 9.06 to -127.16; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Collection Efficiency increased from avg 23.50 to -223.08; 5-COMMERCIAL – Lab/Test CPT Codes Collection Efficiency increased from avg 20.86 to -148.26; 18-CIGNA – New E/M Codes Collection Efficiency increased from avg 15.12 to -66.78; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to -109.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to -48.64; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to -160.99; 15-UNITED HEALTHCARE – DME Labs per Visit increased from avg 0.10 to 2.00; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to -18.72; 18-CIGNA – New E/M Codes Collection Efficiency increased from avg 15.12 to -148.04; 3-MEDICARE – Existing E/M Code Collection Efficiency increased from avg -7.53 to -50.26</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to -15.53; 15-UNITED HEALTHCARE – Vaccines Charge Billed Balance increased from avg -10.71 to -150.00; 15-UNITED HEALTHCARE – Vaccines Payment per Visit increased from avg 82.57 to 318.92; 15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency increased from avg 9.06 to -15.14; 15-UNITED HEALTHCARE – Vaccines Payment Amount* increased from avg 90.91 to 318.92; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance increased from avg 64.00 to -73.99</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to -18.59; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to -202.89; 3-MEDICARE – Existing E/M Code Collection Efficiency increased from avg -7.53 to -50.26; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 25.12 to 166.19; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 54.50 to 332.39; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 27.53 to 166.19</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to -92.15; 5-COMMERCIAL – Existing E/M Code Collection Efficiency increased from avg 1.93 to -39.70; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to -135.15; 18-CIGNA – New E/M Codes Collection Efficiency increased from avg 15.12 to -117.84; 15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency increased from avg 9.06 to -51.44; 4-MEDICAID – Self-pay physical &amp; No Charge Labs per Visit increased from avg 0.43 to 3.00</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to -293.19; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to -166.67; 12-HUMANA – X-Ray CPT Codes Charge Billed Balance increased from avg -1.21 to -25.51; 15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency increased from avg 9.06 to -133.31; 18-CIGNA – Existing E/M Code Collection Efficiency increased from avg -18.20 to -300.32; 15-UNITED HEALTHCARE – Existing E/M Code Collection Efficiency increased from avg -36.34 to -243.09</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to -54.03; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to -110.00; 15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency increased from avg 9.06 to -61.14; 13-TRICARE – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 45.55 to 373.44; 13-TRICARE – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 47.27 to 373.44; 13-TRICARE – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 48.14 to 373.44</t>
+  </si>
+  <si>
+    <t>12-HUMANA – New E/M Codes Charge Billed Balance increased from avg 0.44 to -105.00; 12-HUMANA – New E/M Codes Collection Efficiency increased from avg -6.89 to -104.90; 13-TRICARE – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 200.53 to 752.00; 12-HUMANA – Medications Charge Amount increased from avg 103.29 to 355.00; 12-HUMANA – Medications Payment Amount* increased from avg 12.94 to 40.91; 15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency increased from avg 9.06 to -8.58</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – New E/M Codes Collection Efficiency increased from avg 13.65 to -134.15; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 50.76 to 200.00; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 2.76 to -5.18; 18-CIGNA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 51.31 to 182.96; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 12.09 to -16.34; 3-MEDICARE – New E/M Codes Charge Amount increased from avg 667.84 to 1860.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency increased from avg 9.06 to -88.35; 12-HUMANA – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 30.05 to 216.28; 12-HUMANA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 35.91 to 216.28; 12-HUMANA – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 53.34 to 216.28; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 29.89 to 114.54; 18-CIGNA – Medications Charge Amount increased from avg 210.12 to 730.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – Self-pay physical &amp; No Charge Charge Amount increased from avg 7.86 to 45.00; 12-HUMANA – New E/M Codes Charge Billed Balance increased from avg 0.44 to -1.25; 15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency increased from avg 9.06 to -24.47; 4-MEDICAID – Existing E/M Code Collection Efficiency increased from avg 70.72 to -110.00; 18-CIGNA – New E/M Codes Collection Efficiency increased from avg 15.12 to -20.00; 4-MEDICAID – New E/M Codes Collection Efficiency increased from avg 162.82 to -191.91</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to -164.28; 3-MEDICARE – New E/M Codes Collection Efficiency increased from avg 13.65 to -110.54; 18-CIGNA – New E/M Codes Collection Efficiency increased from avg 15.12 to -90.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 62.96 to 296.13; 3-MEDICARE – New E/M Codes Charge Billed Balance increased from avg 45.73 to -123.57; 5-COMMERCIAL – X-Ray CPT Codes Charge Billed Balance increased from avg 17.35 to -35.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency increased from avg 9.06 to -209.42; 4-MEDICAID – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 43.58 to 532.54; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 29.89 to 266.27; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 68.64 to 532.54; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 267.01 to 2000.00; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to -137.70</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency increased from avg 9.06 to -73.35; 3-MEDICARE – Lab/Test CPT Codes Collection Efficiency increased from avg 1.82 to -11.46; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to -40.52; 5-COMMERCIAL – New E/M Codes Collection Efficiency increased from avg 41.75 to -52.21; 3-MEDICARE – New E/M Codes Charge Amount increased from avg 667.84 to 2170.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 0.95 to 3.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – Self-pay physical &amp; No Charge Charge Amount increased from avg 7.86 to 65.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Billed Balance increased from avg -11.50 to -61.00; 15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency increased from avg 9.06 to -14.10; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to -25.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 4.07 to -5.11; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 0.95 to 3.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – DME Collection Efficiency increased from avg 6.87 to -93.40; 18-CIGNA – Existing E/M Code Collection Efficiency increased from avg -18.20 to -71.17; 5-COMMERCIAL – Lab/Test CPT Codes Collection Rate* increased from avg 0.28 to 1.00; 1-SELF PAY – X-Ray CPT Codes Visit Count increased from avg 2.51 to 9.00; 1-SELF PAY – X-Ray CPT Codes Charge Amount increased from avg 235.81 to 800.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit increased from avg 0.88 to 3.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg -0.06 to -150.00; 3-MEDICARE – Lab/Test CPT Codes Collection Efficiency increased from avg 1.82 to -121.51; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to -262.19; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 62.96 to 381.15; 15-UNITED HEALTHCARE – Existing E/M Code Collection Efficiency increased from avg -36.34 to -162.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 95.70 to 381.15</t>
   </si>
   <si>
     <t>18-CIGNA – Vaccines Labs per Visit increased from avg 0.31 to 2.50; 1-SELF PAY – Vaccines Charge Amount increased from avg 296.43 to 1400.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 174.38 to 652.20; 18-CIGNA – Vaccines Payment Amount* increased from avg 111.17 to 413.69; 18-CIGNA – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 70.38 to 235.34; 18-CIGNA – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 49.02 to 159.70</t>
@@ -274,211 +274,214 @@
     <t>4-MEDICAID – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 43.58 to 410.81; 1-SELF PAY – Vaccines Charge Amount increased from avg 296.43 to 2145.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 68.64 to 427.15; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 267.01 to 1382.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 29.89 to 142.38; 1-SELF PAY – Vaccines Visit Count increased from avg 2.07 to 7.00</t>
   </si>
   <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 225.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 63.06 to 293.00; 15-UNITED HEALTHCARE – Existing E/M Code Upfront Collections Efficiency increased from avg -36.34 to 82.60; 2-BCBS – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency increased from avg -4.05 to 6.35; 13-TRICARE – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 25.52 to 76.73; 13-TRICARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 98.89 to 230.00</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 12.20 to 54.56; 18-CIGNA – New E/M Codes Upfront Collections Efficiency increased from avg 15.12 to 32.15; 12-HUMANA – New E/M Codes Upfront Collections Efficiency increased from avg -6.89 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Upfront Collections Efficiency increased from avg -36.34 to 0.00; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – New E/M Codes Upfront Collections Efficiency increased from avg -6.89 to 0.00; 12-HUMANA – New E/M Codes Labs per Visit decreased from avg 0.90 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Upfront Collections Efficiency increased from avg -36.34 to 0.00; 15-UNITED HEALTHCARE – Medications Labs per Visit decreased from avg 1.45 to 0.00</t>
-  </si>
-  <si>
-    <t>12-HUMANA – New E/M Codes Upfront Collections Efficiency increased from avg -6.89 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Upfront Collections Efficiency increased from avg -36.34 to 0.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.88 to 0.00; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 0.00; 18-CIGNA – Existing E/M Code Upfront Collections Efficiency increased from avg -18.20 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency increased from avg 9.06 to 165.58; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance increased from avg 64.00 to 199.00; 1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 12-HUMANA – New E/M Codes Upfront Collections Efficiency increased from avg -6.89 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – X-Ray CPT Codes Upfront Collections Efficiency increased from avg 0.55 to 7.38; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.82 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Upfront Collections Efficiency increased from avg -36.34 to 0.00; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Upfront Collections Efficiency increased from avg -16.11 to 55.28; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg -0.06 to 49.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency increased from avg 0.19 to 5.51; 12-HUMANA – Existing E/M Code Charge Billed Balance increased from avg 10.28 to 100.00; 5-COMMERCIAL – New E/M Codes Upfront Collections Efficiency increased from avg 41.75 to 278.37; 5-COMMERCIAL – New E/M Codes Charge Billed Balance increased from avg 122.16 to 287.00; 12-HUMANA – New E/M Codes Upfront Collections Efficiency increased from avg -6.89 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 1.82 to 20.68; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – Existing E/M Code Labs per Visit decreased from avg 1.20 to 0.00; 13-TRICARE – New E/M Codes Labs per Visit decreased from avg 1.32 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Upfront Collections Efficiency increased from avg -36.34 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Charge Billed Balance increased from avg 14.47 to 100.00; 17-AETNA – Medications Upfront Collections Efficiency increased from avg 3.36 to 18.78; 17-AETNA – Existing E/M Code Upfront Collections Efficiency increased from avg 51.63 to 204.56; 17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 63.76 to 245.00; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – New E/M Codes Upfront Collections Efficiency increased from avg -6.89 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00; 13-TRICARE – New E/M Codes Labs per Visit decreased from avg 1.32 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – New E/M Codes Upfront Collections Efficiency increased from avg -6.89 to 0.00; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 0.00; 18-CIGNA – Existing E/M Code Upfront Collections Efficiency increased from avg -18.20 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Upfront Collections Efficiency increased from avg -11.19 to 76.76; 5-COMMERCIAL – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 20.86 to 135.79; 18-CIGNA – New E/M Codes Upfront Collections Efficiency increased from avg 15.12 to 90.65; 5-COMMERCIAL – Lab/Test CPT Codes Charge Billed Balance increased from avg 74.50 to 293.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency increased from avg 0.19 to 0.64; 5-COMMERCIAL – New E/M Codes Charge Billed Balance increased from avg 122.16 to 310.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 160.00; 2-BCBS – New E/M Codes Upfront Collections Efficiency increased from avg -11.19 to 284.35; 2-BCBS – After Hours Upfront Collections Efficiency increased from avg 0.08 to 1.60; 2-BCBS – Existing E/M Code Upfront Collections Efficiency increased from avg -16.11 to 96.94; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 364.54; 2-BCBS – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency increased from avg -4.05 to 12.26</t>
-  </si>
-  <si>
-    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency increased from avg -4.05 to 17.57; 2-BCBS – New E/M Codes Upfront Collections Efficiency increased from avg -11.19 to 30.27; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00; 13-TRICARE – New E/M Codes Labs per Visit decreased from avg 1.32 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency increased from avg 9.06 to 186.19; 18-CIGNA – New E/M Codes Upfront Collections Efficiency increased from avg 15.12 to 72.48; 1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00; 13-TRICARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.82 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 1.82 to 12.33; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.66 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Upfront Collections Efficiency increased from avg -36.34 to 0.00; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 205.00; 15-UNITED HEALTHCARE – Existing E/M Code Upfront Collections Efficiency increased from avg -36.34 to 65.97; 15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency increased from avg 9.06 to 21.94; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.88 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Upfront Collections Efficiency increased from avg -11.19 to 29.34; 17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 63.76 to 241.00; 2-BCBS – Medications Upfront Collections Efficiency increased from avg 2.09 to 6.84; 17-AETNA – Existing E/M Code Upfront Collections Efficiency increased from avg 51.63 to 143.36; 1-SELF PAY – Medications Labs per Visit decreased from avg 1.13 to 0.00; 1-SELF PAY – New E/M Codes Labs per Visit decreased from avg 0.86 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Existing E/M Code Upfront Collections Efficiency increased from avg 1.93 to 167.50; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 241.00; 5-COMMERCIAL – Lab/Test CPT Codes Charge Billed Balance increased from avg 74.50 to 293.00; 1-SELF PAY – Medications Charge Amount decreased from avg 65.92 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount decreased from avg 116.93 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 2.76 to 89.00; 15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency increased from avg 9.06 to 138.67; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance increased from avg 64.00 to 310.00; 4-MEDICAID – X-Ray CPT Codes Upfront Collections Efficiency increased from avg 3.46 to 11.27; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 12-HUMANA – New E/M Codes Upfront Collections Efficiency increased from avg -6.89 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – New E/M Codes Labs per Visit decreased from avg 1.32 to 0.00; 13-TRICARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.82 to 0.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.88 to 0.00; 18-CIGNA – X-Ray CPT Codes Labs per Visit decreased from avg 0.69 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 12-HUMANA – New E/M Codes Labs per Visit decreased from avg 0.90 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00; 13-TRICARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.82 to 0.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.88 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 13-TRICARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.82 to 0.00; 17-AETNA – New E/M Codes Labs per Visit decreased from avg 1.59 to 0.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.94 to 0.00; 2-BCBS – DME Labs per Visit decreased from avg 0.05 to 0.00; 2-BCBS – Vaccines Labs per Visit decreased from avg 0.10 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 20.86 to 567.00; 2-BCBS – New E/M Codes Upfront Collections Efficiency increased from avg -11.19 to 230.61; 2-BCBS – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency increased from avg -4.05 to 66.03; 4-MEDICAID – Vaccines Charge Billed Balance increased from avg 51.20 to 411.00; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 416.22; 5-COMMERCIAL – Lab/Test CPT Codes Charge Billed Balance increased from avg 74.50 to 525.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg -0.06 to 9.90; 2-BCBS – X-Ray CPT Codes Upfront Collections Efficiency increased from avg 0.36 to 32.81; 2-BCBS – New E/M Codes Upfront Collections Efficiency increased from avg -11.19 to 714.85; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 1243.38; 13-TRICARE – X-Ray CPT Codes Upfront Collections Efficiency increased from avg 1.30 to 26.10; 13-TRICARE – Medications Upfront Collections Efficiency increased from avg 2.17 to 21.77</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 31.40; 12-HUMANA – New E/M Codes Charge Billed Balance increased from avg 0.44 to 79.87; 17-AETNA – Medications Upfront Collections Efficiency increased from avg 3.36 to 78.70; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 4.95 to 104.00; 12-HUMANA – New E/M Codes Upfront Collections Efficiency increased from avg -6.89 to 110.74; 4-MEDICAID – X-Ray CPT Codes Charge Billed Balance increased from avg 11.37 to 128.00</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – Medications Charge Billed Balance increased from avg 3.82 to 110.00; 4-MEDICAID – Medications Upfront Collections Efficiency increased from avg 1.09 to 17.85; 15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency increased from avg 9.06 to 96.81; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance increased from avg 101.89 to 781.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 62.39 to 475.17; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 37.41</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 148.79; 13-TRICARE – Existing E/M Code Charge Billed Balance increased from avg 88.96 to 735.00; 13-TRICARE – Existing E/M Code Upfront Collections Efficiency increased from avg 33.42 to 274.20; 2-BCBS – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 23.63 to 158.72; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 23.50 to 140.31; 18-CIGNA – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 12.20 to 69.21</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 205.00; 12-HUMANA – New E/M Codes Charge Billed Balance increased from avg 0.44 to 55.00; 13-TRICARE – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 25.52 to 491.52; 2-BCBS – New E/M Codes Upfront Collections Efficiency increased from avg -11.19 to 159.50; 13-TRICARE – Existing E/M Code Upfront Collections Efficiency increased from avg 33.42 to 321.00; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 446.33</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – Medications Upfront Collections Efficiency increased from avg 1.09 to 20.93; 17-AETNA – DME Upfront Collections Efficiency increased from avg 10.48 to 188.61; 17-AETNA – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency increased from avg 5.70 to 66.02; 4-MEDICAID – Medications Charge Billed Balance increased from avg 3.82 to 40.00; 4-MEDICAID – Lab/Test CPT Codes Charge Billed Balance increased from avg 231.39 to 1782.00; 4-MEDICAID – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 70.81 to 527.27</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 213.84; 18-CIGNA – X-Ray CPT Codes Charge Billed Balance increased from avg 6.24 to 115.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Upfront Collections Efficiency increased from avg 5.67 to 98.76; 18-CIGNA – X-Ray CPT Codes Upfront Collections Efficiency increased from avg 2.18 to 31.18; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 12.09 to 152.00; 5-COMMERCIAL – New E/M Codes Upfront Collections Efficiency increased from avg 41.75 to 480.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Existing E/M Code Upfront Collections Efficiency increased from avg 1.93 to 63.81; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 96.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 23.50 to 202.12; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 220.00; 18-CIGNA – New E/M Codes Upfront Collections Efficiency increased from avg 15.12 to 111.96; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 62.39 to 457.11</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 462.26; 2-BCBS – Existing E/M Code Upfront Collections Efficiency increased from avg -16.11 to 371.95; 12-HUMANA – Existing E/M Code Charge Billed Balance increased from avg 10.28 to 195.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency increased from avg -4.05 to 25.65; 13-TRICARE – Existing E/M Code Charge Billed Balance increased from avg 88.96 to 735.00; 13-TRICARE – Existing E/M Code Upfront Collections Efficiency increased from avg 33.42 to 267.60</t>
-  </si>
-  <si>
-    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 358.55; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 125.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 17.97 to 436.00; 5-COMMERCIAL – X-Ray CPT Codes Upfront Collections Efficiency increased from avg 3.19 to 63.75; 2-BCBS – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency increased from avg -4.05 to 68.99; 18-CIGNA – Vaccines Charge Billed Balance increased from avg 7.00 to 131.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Existing E/M Code Upfront Collections Efficiency increased from avg 1.93 to 98.94; 17-AETNA – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency increased from avg 5.70 to 98.69; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 436.00; 3-MEDICARE – New E/M Codes Upfront Collections Efficiency increased from avg 13.65 to 156.59; 5-COMMERCIAL – New E/M Codes Upfront Collections Efficiency increased from avg 41.75 to 452.62; 4-MEDICAID – X-Ray CPT Codes Charge Billed Balance increased from avg 11.37 to 123.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 245.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 160.00; 13-TRICARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 45.89 to 752.00; 17-AETNA – Medications Charge Billed Balance increased from avg 14.47 to 192.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency increased from avg -4.05 to 34.11; 2-BCBS – New E/M Codes Upfront Collections Efficiency increased from avg -11.19 to 90.70</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 145.00; 3-MEDICARE – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 1.82 to 185.94; 3-MEDICARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 9.57 to 450.00; 2-BCBS – X-Ray CPT Codes Upfront Collections Efficiency increased from avg 0.36 to 14.87; 15-UNITED HEALTHCARE – Medications Upfront Collections Efficiency increased from avg 2.95 to 67.66; 2-BCBS – New E/M Codes Upfront Collections Efficiency increased from avg -11.19 to 149.46</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg -0.06 to 89.00; 15-UNITED HEALTHCARE – DME Upfront Collections Efficiency increased from avg 0.92 to 19.38; 17-AETNA – X-Ray CPT Codes Upfront Collections Efficiency increased from avg 11.15 to 78.65; 2-BCBS – New E/M Codes Upfront Collections Efficiency increased from avg -11.19 to 49.67; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 136.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 63.06 to 368.00</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency increased from avg -0.05 to 6.53; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 110.85; 12-HUMANA – Medications Charge Billed Balance increased from avg 2.86 to 40.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 63.06 to 736.00; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 210.00; 3-MEDICARE – DME Charge Billed Balance increased from avg 8.62 to 69.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Codes Upfront Collections Efficiency increased from avg 9.06 to 407.68; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 192.67; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance increased from avg 63.06 to 841.78; 13-TRICARE – Lab/Test CPT Codes Upfront Collections Efficiency increased from avg 25.52 to 337.34; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance increased from avg 64.00 to 814.36; 2-BCBS – X-Ray CPT Codes Upfront Collections Efficiency increased from avg 0.36 to 3.57</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 20.27; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg -7.36 to 167.92; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency increased from avg 4.07 to 98.43; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 20.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 12.09 to 208.00; 4-MEDICAID – X-Ray CPT Codes Charge Billed Balance increased from avg 11.37 to 163.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 20.27; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 585.00; 3-MEDICARE – New E/M Codes Upfront Collections Efficiency increased from avg 13.65 to 288.42; 3-MEDICARE – X-Ray CPT Codes Charge Billed Balance increased from avg 3.31 to 36.46; 18-CIGNA – New E/M Codes Upfront Collections Efficiency increased from avg 15.12 to 140.44; 3-MEDICARE – New E/M Codes Charge Billed Balance increased from avg 45.73 to 290.71</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 46.18; 2-BCBS – New E/M Codes Upfront Collections Efficiency increased from avg -11.19 to 98.67; 18-CIGNA – New E/M Codes Upfront Collections Efficiency increased from avg 15.12 to 151.96; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 25.96 to 245.00; 5-COMMERCIAL – X-Ray CPT Codes Charge Billed Balance increased from avg 17.35 to 123.00; 17-AETNA – X-Ray CPT Codes Upfront Collections Efficiency increased from avg 11.15 to 58.02</t>
-  </si>
-  <si>
-    <t>2-BCBS – X-Ray CPT Codes Upfront Collections Efficiency increased from avg 0.36 to 76.94; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 123.00; 18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg -1.08 to 88.71; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 267.63; 15-UNITED HEALTHCARE – Medications Charge Billed Balance increased from avg 3.48 to 110.00; 18-CIGNA – Medications Upfront Collections Efficiency increased from avg 0.76 to 18.26</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 0.15 to 40.54; 2-BCBS – New E/M Codes Upfront Collections Efficiency increased from avg -11.19 to 340.70; 2-BCBS – Medications Charge Billed Balance increased from avg 3.79 to 70.60; 18-CIGNA – X-Ray CPT Codes Charge Billed Balance increased from avg 6.24 to 72.00; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to 35.52; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 520.17</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.91 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount decreased from avg 116.93 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 12-HUMANA – Existing E/M Code Labs per Visit decreased from avg 1.20 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 1.42 to 0.00; 13-TRICARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.82 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 12-HUMANA – New E/M Codes Labs per Visit decreased from avg 0.90 to 0.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.88 to 0.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.94 to 0.00; 18-CIGNA – Vaccines Labs per Visit decreased from avg 0.31 to 0.00; 18-CIGNA – X-Ray CPT Codes Labs per Visit decreased from avg 0.69 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Procedures &amp; Surgical CPT Codes Charge Amount decreased from avg 116.93 to 0.00; 1-SELF PAY – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 0.95 to 0.00; 1-SELF PAY – X-Ray CPT Codes Labs per Visit decreased from avg 0.39 to 0.00; 15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Labs per Visit decreased from avg 1.90 to 0.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Labs per Visit decreased from avg 0.88 to 0.00; 18-CIGNA – X-Ray CPT Codes Labs per Visit decreased from avg 0.69 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Upfront Collections Efficiency decreased from avg 98.28 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 211.52 to 565.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 1.56 to 4.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 5.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Labs per Visit increased from avg 1.60 to 7.00; 17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 3.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.67; 17-AETNA – Medications Charge Amount increased from avg 135.48 to 305.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 211.52 to 464.00; 17-AETNA – Medications Visit Count increased from avg 1.48 to 3.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 5.00; 17-AETNA – Existing E/M Code Labs per Visit increased from avg 1.75 to 4.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Labs per Visit increased from avg 1.60 to 9.00; 17-AETNA – Lab/Test CPT Codes Labs per Visit increased from avg 2.95 to 6.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Upfront Collections Efficiency decreased from avg 98.28 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance decreased from avg 22.59 to 0.00; 17-AETNA – X-Ray CPT Codes Upfront Collections Efficiency decreased from avg 11.15 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 7.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – New E/M Codes Labs per Visit increased from avg 1.59 to 3.50; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 34.92 to 150.69; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero Balance Collection Rate increased from avg 0.27 to 0.66; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Rate* increased from avg 0.30 to 0.66; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to -37.05; 17-AETNA – After Hours Labs per Visit increased from avg 2.15 to 5.00; 17-AETNA – Existing E/M Code Labs per Visit increased from avg 1.75 to 4.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 4.00; 17-AETNA – DME Payment per Visit increased from avg 174.97 to 368.10; 17-AETNA – DME NRV Zero Balance* increased from avg 179.12 to 368.10</t>
-  </si>
-  <si>
-    <t>17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance decreased from avg 22.59 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 34.92 to 137.69; 17-AETNA – DME Payment per Visit increased from avg 174.97 to 529.98; 17-AETNA – DME NRV Zero Balance* increased from avg 179.12 to 529.98; 17-AETNA – DME Payment Amount* increased from avg 200.73 to 529.98; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Charge Amount increased from avg 135.48 to 334.00; 17-AETNA – Medications Visit Count increased from avg 1.48 to 3.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to -177.97; 17-AETNA – New E/M Codes Labs per Visit increased from avg 1.59 to 5.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Upfront Collections Efficiency decreased from avg 98.28 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency decreased from avg 5.70 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Visit Count increased from avg 1.48 to 3.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decrease from avg -7.36 to 225.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance decrease from avg 63.06 to 293.00; 15-UNITED HEALTHCARE – Existing E/M Code Collection Efficiency decrease from avg -36.34 to 82.60; 2-BCBS – Procedures &amp; Surgical CPT Codes Collection Efficiency decrease from avg -4.05 to 6.35; 13-TRICARE – Lab/Test CPT Codes Collection Efficiency decrease from avg 25.52 to 76.73; 13-TRICARE – Lab/Test CPT Codes Charge Billed Balance decrease from avg 98.89 to 230.00</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Lab/Test CPT Codes Collection Efficiency decrease from avg 12.20 to 54.56; 18-CIGNA – New E/M Codes Collection Efficiency decrease from avg 15.12 to 32.15; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 4-MEDICAID – After Hours Collection Efficiency decrease from avg -0.33 to 0.00; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Labs per Visit decrease from avg 1.39 to 0.00; 3-MEDICARE – Existing E/M Code Labs per Visit decrease from avg 1.41 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 4-MEDICAID – After Hours Collection Efficiency decrease from avg -0.33 to 0.00; 3-MEDICARE – Existing E/M Code Collection Efficiency decrease from avg -7.53 to 0.00; 2-BCBS – Vaccines Labs per Visit decrease from avg 0.10 to 0.00; 2-BCBS – Vaccines Charge Billed Balance decrease from avg -0.69 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Collection Efficiency decrease from avg -4.05 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 5-COMMERCIAL – Medications Labs per Visit decrease from avg 1.73 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Billed Balance decrease from avg -11.50 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Amount decrease from avg 7.86 to 0.00; 4-MEDICAID – Medications Labs per Visit decrease from avg 1.26 to 0.00; 4-MEDICAID – After Hours Collection Efficiency decrease from avg -0.33 to 0.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency decrease from avg 9.06 to 165.58; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decrease from avg 64.00 to 199.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 4-MEDICAID – After Hours Collection Efficiency decrease from avg -0.33 to 0.00; 3-MEDICARE – X-Ray CPT Codes Labs per Visit decrease from avg 0.67 to 0.00; 2-BCBS – Vaccines Labs per Visit decrease from avg 0.10 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – X-Ray CPT Codes Collection Efficiency decrease from avg 0.55 to 7.38; 5-COMMERCIAL – X-Ray CPT Codes Labs per Visit decrease from avg 1.10 to 0.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Labs per Visit decrease from avg 2.14 to 0.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 5-COMMERCIAL – Existing E/M Code Labs per Visit decrease from avg 2.15 to 0.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit decrease from avg 0.71 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Collection Efficiency decrease from avg -16.11 to 55.28; 5-COMMERCIAL – X-Ray CPT Codes Labs per Visit decrease from avg 1.10 to 0.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 5-COMMERCIAL – After Hours Labs per Visit decrease from avg 2.12 to 0.00; 4-MEDICAID – After Hours Collection Efficiency decrease from avg -0.33 to 0.00; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Labs per Visit decrease from avg 1.39 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 49.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Collection Efficiency decrease from avg 0.19 to 5.51; 12-HUMANA – Existing E/M Code Charge Billed Balance decrease from avg 10.28 to 100.00; 5-COMMERCIAL – New E/M Codes Collection Efficiency decrease from avg 41.75 to 278.37; 5-COMMERCIAL – New E/M Codes Charge Billed Balance decrease from avg 122.16 to 287.00; 5-COMMERCIAL – Medications Labs per Visit decrease from avg 1.73 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Lab/Test CPT Codes Collection Efficiency decrease from avg 1.82 to 20.68; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit decrease from avg 0.71 to 0.00; 4-MEDICAID – After Hours Collection Efficiency decrease from avg -0.33 to 0.00; 2-BCBS – Vaccines Labs per Visit decrease from avg 0.10 to 0.00; 2-BCBS – Vaccines Charge Billed Balance decrease from avg -0.69 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 5-COMMERCIAL – New E/M Codes Labs per Visit decrease from avg 1.75 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Labs per Visit decrease from avg 0.43 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Billed Balance decrease from avg -11.50 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Amount decrease from avg 7.86 to 0.00; 4-MEDICAID – Medications Charge Amount decrease from avg 201.17 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Medications Charge Billed Balance decrease from avg 14.47 to 100.00; 17-AETNA – Medications Collection Efficiency decrease from avg 3.36 to 18.78; 17-AETNA – Existing E/M Code Collection Efficiency decrease from avg 51.63 to 204.56; 17-AETNA – Existing E/M Code Charge Billed Balance decrease from avg 63.76 to 245.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit decrease from avg 0.71 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Billed Balance decrease from avg -11.50 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 5-COMMERCIAL – Medications Labs per Visit decrease from avg 1.73 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Labs per Visit decrease from avg 0.43 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Billed Balance decrease from avg -11.50 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Amount decrease from avg 7.86 to 0.00; 4-MEDICAID – Medications Labs per Visit decrease from avg 1.26 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – X-Ray CPT Codes Labs per Visit decrease from avg 1.10 to 0.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 5-COMMERCIAL – After Hours Labs per Visit decrease from avg 2.12 to 0.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit decrease from avg 0.71 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Labs per Visit decrease from avg 0.43 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Billed Balance decrease from avg -11.50 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Collection Efficiency decrease from avg -11.19 to 76.76; 5-COMMERCIAL – Lab/Test CPT Codes Collection Efficiency decrease from avg 20.86 to 135.79; 18-CIGNA – New E/M Codes Collection Efficiency decrease from avg 15.12 to 90.65; 5-COMMERCIAL – Lab/Test CPT Codes Charge Billed Balance decrease from avg 74.50 to 293.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Collection Efficiency decrease from avg 0.19 to 0.64; 5-COMMERCIAL – New E/M Codes Charge Billed Balance decrease from avg 122.16 to 310.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance decrease from avg -4.13 to 160.00; 2-BCBS – New E/M Codes Collection Efficiency decrease from avg -11.19 to 284.35; 2-BCBS – After Hours Collection Efficiency decrease from avg 0.08 to 1.60; 2-BCBS – Existing E/M Code Collection Efficiency decrease from avg -16.11 to 96.94; 2-BCBS – New E/M Codes Charge Billed Balance decrease from avg 52.44 to 364.54; 2-BCBS – Procedures &amp; Surgical CPT Codes Collection Efficiency decrease from avg -4.05 to 12.26</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Collection Efficiency decrease from avg -4.05 to 17.57; 2-BCBS – New E/M Codes Collection Efficiency decrease from avg -11.19 to 30.27; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit decrease from avg 0.71 to 0.00; 4-MEDICAID – After Hours Collection Efficiency decrease from avg -0.33 to 0.00; 3-MEDICARE – X-Ray CPT Codes Labs per Visit decrease from avg 0.67 to 0.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency decrease from avg 9.06 to 186.19; 18-CIGNA – New E/M Codes Collection Efficiency decrease from avg 15.12 to 72.48; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 4-MEDICAID – After Hours Collection Efficiency decrease from avg -0.33 to 0.00; 3-MEDICARE – X-Ray CPT Codes Labs per Visit decrease from avg 0.67 to 0.00; 3-MEDICARE – Medications Labs per Visit decrease from avg 0.90 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Lab/Test CPT Codes Collection Efficiency decrease from avg 1.82 to 12.33; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 5-COMMERCIAL – Medications Labs per Visit decrease from avg 1.73 to 0.00; 4-MEDICAID – After Hours Collection Efficiency decrease from avg -0.33 to 0.00; 2-BCBS – Vaccines Labs per Visit decrease from avg 0.10 to 0.00; 2-BCBS – Vaccines Charge Billed Balance decrease from avg -0.69 to 0.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decrease from avg -7.36 to 205.00; 15-UNITED HEALTHCARE – Existing E/M Code Collection Efficiency decrease from avg -36.34 to 65.97; 15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency decrease from avg 9.06 to 21.94; 5-COMMERCIAL – X-Ray CPT Codes Labs per Visit decrease from avg 1.10 to 0.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 5-COMMERCIAL – Medications Labs per Visit decrease from avg 1.73 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Collection Efficiency decrease from avg -11.19 to 29.34; 17-AETNA – Existing E/M Code Charge Billed Balance decrease from avg 63.76 to 241.00; 2-BCBS – Medications Collection Efficiency decrease from avg 2.09 to 6.84; 17-AETNA – Existing E/M Code Collection Efficiency decrease from avg 51.63 to 143.36; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit decrease from avg 0.71 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Existing E/M Code Collection Efficiency decrease from avg 1.93 to 167.50; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decrease from avg 25.96 to 241.00; 5-COMMERCIAL – Lab/Test CPT Codes Charge Billed Balance decrease from avg 74.50 to 293.00; 5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 0.00; 4-MEDICAID – After Hours Collection Efficiency decrease from avg -0.33 to 0.00; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Labs per Visit decrease from avg 1.39 to 0.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg 2.76 to 89.00; 15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency decrease from avg 9.06 to 138.67; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decrease from avg 64.00 to 310.00; 4-MEDICAID – X-Ray CPT Codes Collection Efficiency decrease from avg 3.46 to 11.27; 5-COMMERCIAL – New E/M Codes Labs per Visit decrease from avg 1.75 to 0.00; 4-MEDICAID – After Hours Collection Efficiency decrease from avg -0.33 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Medications Charge Amount decrease from avg 69.73 to 0.00; 4-MEDICAID – Medications Labs per Visit decrease from avg 1.26 to 0.00; 2-BCBS – Vaccines Labs per Visit decrease from avg 0.10 to 0.00; 2-BCBS – Self-pay physical &amp; No Charge Labs per Visit decrease from avg 0.17 to 0.00; 2-BCBS – Self-pay physical &amp; No Charge Charge Amount decrease from avg 15.08 to 0.00; 2-BCBS – DME Labs per Visit decrease from avg 0.05 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Labs per Visit decrease from avg 2.14 to 0.00; 5-COMMERCIAL – New E/M Codes Labs per Visit decrease from avg 1.75 to 0.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit decrease from avg 0.71 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Labs per Visit decrease from avg 0.43 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Amount decrease from avg 7.86 to 0.00; 4-MEDICAID – Medications Labs per Visit decrease from avg 1.26 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – New E/M Codes Labs per Visit decrease from avg 1.75 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Labs per Visit decrease from avg 0.43 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Amount decrease from avg 7.86 to 0.00; 2-BCBS – Vaccines Labs per Visit decrease from avg 0.10 to 0.00; 2-BCBS – DME Labs per Visit decrease from avg 0.05 to 0.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Labs per Visit decrease from avg 1.94 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Lab/Test CPT Codes Collection Efficiency decrease from avg 20.86 to 567.00; 2-BCBS – New E/M Codes Collection Efficiency decrease from avg -11.19 to 230.61; 2-BCBS – Procedures &amp; Surgical CPT Codes Collection Efficiency decrease from avg -4.05 to 66.03; 4-MEDICAID – Vaccines Charge Billed Balance decrease from avg 51.20 to 411.00; 2-BCBS – New E/M Codes Charge Billed Balance decrease from avg 52.44 to 416.22; 5-COMMERCIAL – Lab/Test CPT Codes Charge Billed Balance decrease from avg 74.50 to 525.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 9.90; 2-BCBS – X-Ray CPT Codes Collection Efficiency decrease from avg 0.36 to 32.81; 2-BCBS – New E/M Codes Collection Efficiency decrease from avg -11.19 to 714.85; 2-BCBS – New E/M Codes Charge Billed Balance decrease from avg 52.44 to 1243.38; 13-TRICARE – X-Ray CPT Codes Collection Efficiency decrease from avg 1.30 to 26.10; 13-TRICARE – Medications Collection Efficiency decrease from avg 2.17 to 21.77</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decrease from avg 0.15 to 31.40; 12-HUMANA – New E/M Codes Charge Billed Balance decrease from avg 0.44 to 79.87; 17-AETNA – Medications Collection Efficiency decrease from avg 3.36 to 78.70; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg 4.95 to 104.00; 12-HUMANA – New E/M Codes Collection Efficiency decrease from avg -6.89 to 110.74; 4-MEDICAID – X-Ray CPT Codes Charge Billed Balance decrease from avg 11.37 to 128.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – Medications Charge Billed Balance decrease from avg 3.82 to 110.00; 4-MEDICAID – Medications Collection Efficiency decrease from avg 1.09 to 17.85; 15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency decrease from avg 9.06 to 96.81; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decrease from avg 101.89 to 781.00; 17-AETNA – Lab/Test CPT Codes Collection Efficiency decrease from avg 62.39 to 475.17; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decrease from avg -7.36 to 37.41</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance decrease from avg -4.13 to 148.79; 13-TRICARE – Existing E/M Code Charge Billed Balance decrease from avg 88.96 to 735.00; 13-TRICARE – Existing E/M Code Collection Efficiency decrease from avg 33.42 to 274.20; 2-BCBS – Lab/Test CPT Codes Collection Efficiency decrease from avg 23.63 to 158.72; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Collection Efficiency decrease from avg 23.50 to 140.31; 18-CIGNA – Lab/Test CPT Codes Collection Efficiency decrease from avg 12.20 to 69.21</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decrease from avg -1.08 to 205.00; 12-HUMANA – New E/M Codes Charge Billed Balance decrease from avg 0.44 to 55.00; 13-TRICARE – Lab/Test CPT Codes Collection Efficiency decrease from avg 25.52 to 491.52; 2-BCBS – New E/M Codes Collection Efficiency decrease from avg -11.19 to 159.50; 13-TRICARE – Existing E/M Code Collection Efficiency decrease from avg 33.42 to 321.00; 2-BCBS – New E/M Codes Charge Billed Balance decrease from avg 52.44 to 446.33</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – Medications Collection Efficiency decrease from avg 1.09 to 20.93; 17-AETNA – DME Collection Efficiency decrease from avg 10.48 to 188.61; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency decrease from avg 5.70 to 66.02; 4-MEDICAID – Medications Charge Billed Balance decrease from avg 3.82 to 40.00; 4-MEDICAID – Lab/Test CPT Codes Charge Billed Balance decrease from avg 231.39 to 1782.00; 4-MEDICAID – Lab/Test CPT Codes Collection Efficiency decrease from avg 70.81 to 527.27</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decrease from avg -7.36 to 213.84; 18-CIGNA – X-Ray CPT Codes Charge Billed Balance decrease from avg 6.24 to 115.00; 15-UNITED HEALTHCARE – X-Ray CPT Codes Collection Efficiency decrease from avg 5.67 to 98.76; 18-CIGNA – X-Ray CPT Codes Collection Efficiency decrease from avg 2.18 to 31.18; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg 12.09 to 152.00; 5-COMMERCIAL – New E/M Codes Collection Efficiency decrease from avg 41.75 to 480.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Existing E/M Code Collection Efficiency decrease from avg 1.93 to 63.81; 2-BCBS – Existing E/M Code Charge Billed Balance decrease from avg -4.13 to 96.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Collection Efficiency decrease from avg 23.50 to 202.12; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decrease from avg 25.96 to 220.00; 18-CIGNA – New E/M Codes Collection Efficiency decrease from avg 15.12 to 111.96; 17-AETNA – Lab/Test CPT Codes Collection Efficiency decrease from avg 62.39 to 457.11</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance decrease from avg -4.13 to 462.26; 2-BCBS – Existing E/M Code Collection Efficiency decrease from avg -16.11 to 371.95; 12-HUMANA – Existing E/M Code Charge Billed Balance decrease from avg 10.28 to 195.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Collection Efficiency decrease from avg -4.05 to 25.65; 13-TRICARE – Existing E/M Code Charge Billed Balance decrease from avg 88.96 to 735.00; 13-TRICARE – Existing E/M Code Collection Efficiency decrease from avg 33.42 to 267.60</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg 8.81 to 358.55; 2-BCBS – Existing E/M Code Charge Billed Balance decrease from avg -4.13 to 125.00; 18-CIGNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg 17.97 to 436.00; 5-COMMERCIAL – X-Ray CPT Codes Collection Efficiency decrease from avg 3.19 to 63.75; 2-BCBS – Procedures &amp; Surgical CPT Codes Collection Efficiency decrease from avg -4.05 to 68.99; 18-CIGNA – Vaccines Charge Billed Balance decrease from avg 7.00 to 131.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Existing E/M Code Collection Efficiency decrease from avg 1.93 to 98.94; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency decrease from avg 5.70 to 98.69; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg 29.14 to 436.00; 3-MEDICARE – New E/M Codes Collection Efficiency decrease from avg 13.65 to 156.59; 5-COMMERCIAL – New E/M Codes Collection Efficiency decrease from avg 41.75 to 452.62; 4-MEDICAID – X-Ray CPT Codes Charge Billed Balance decrease from avg 11.37 to 123.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decrease from avg 0.15 to 245.00; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decrease from avg -7.36 to 160.00; 13-TRICARE – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg 45.89 to 752.00; 17-AETNA – Medications Charge Billed Balance decrease from avg 14.47 to 192.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Collection Efficiency decrease from avg -4.05 to 34.11; 2-BCBS – New E/M Codes Collection Efficiency decrease from avg -11.19 to 90.70</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance decrease from avg -1.08 to 145.00; 3-MEDICARE – Lab/Test CPT Codes Collection Efficiency decrease from avg 1.82 to 185.94; 3-MEDICARE – Lab/Test CPT Codes Charge Billed Balance decrease from avg 9.57 to 450.00; 2-BCBS – X-Ray CPT Codes Collection Efficiency decrease from avg 0.36 to 14.87; 15-UNITED HEALTHCARE – Medications Collection Efficiency decrease from avg 2.95 to 67.66; 2-BCBS – New E/M Codes Collection Efficiency decrease from avg -11.19 to 149.46</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg -0.06 to 89.00; 15-UNITED HEALTHCARE – DME Collection Efficiency decrease from avg 0.92 to 19.38; 17-AETNA – X-Ray CPT Codes Collection Efficiency decrease from avg 11.15 to 78.65; 2-BCBS – New E/M Codes Collection Efficiency decrease from avg -11.19 to 49.67; 17-AETNA – X-Ray CPT Codes Charge Billed Balance decrease from avg 22.59 to 136.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance decrease from avg 63.06 to 368.00</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Procedures &amp; Surgical CPT Codes Collection Efficiency decrease from avg -0.05 to 6.53; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decrease from avg -7.36 to 110.85; 12-HUMANA – Medications Charge Billed Balance decrease from avg 2.86 to 40.00; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance decrease from avg 63.06 to 736.00; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decrease from avg 25.96 to 210.00; 3-MEDICARE – DME Charge Billed Balance decrease from avg 8.62 to 69.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Codes Collection Efficiency decrease from avg 9.06 to 407.68; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decrease from avg -7.36 to 192.67; 15-UNITED HEALTHCARE – Lab/Test CPT Codes Charge Billed Balance decrease from avg 63.06 to 841.78; 13-TRICARE – Lab/Test CPT Codes Collection Efficiency decrease from avg 25.52 to 337.34; 15-UNITED HEALTHCARE – New E/M Codes Charge Billed Balance decrease from avg 64.00 to 814.36; 2-BCBS – X-Ray CPT Codes Collection Efficiency decrease from avg 0.36 to 3.57</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decrease from avg 0.15 to 20.27; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decrease from avg -7.36 to 167.92; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Collection Efficiency decrease from avg 4.07 to 98.43; 18-CIGNA – Existing E/M Code Charge Billed Balance decrease from avg -1.08 to 20.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Charge Billed Balance decrease from avg 12.09 to 208.00; 4-MEDICAID – X-Ray CPT Codes Charge Billed Balance decrease from avg 11.37 to 163.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decrease from avg 0.15 to 20.27; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decrease from avg 25.96 to 585.00; 3-MEDICARE – New E/M Codes Collection Efficiency decrease from avg 13.65 to 288.42; 3-MEDICARE – X-Ray CPT Codes Charge Billed Balance decrease from avg 3.31 to 36.46; 18-CIGNA – New E/M Codes Collection Efficiency decrease from avg 15.12 to 140.44; 3-MEDICARE – New E/M Codes Charge Billed Balance decrease from avg 45.73 to 290.71</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decrease from avg 0.15 to 46.18; 2-BCBS – New E/M Codes Collection Efficiency decrease from avg -11.19 to 98.67; 18-CIGNA – New E/M Codes Collection Efficiency decrease from avg 15.12 to 151.96; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decrease from avg 25.96 to 245.00; 5-COMMERCIAL – X-Ray CPT Codes Charge Billed Balance decrease from avg 17.35 to 123.00; 17-AETNA – X-Ray CPT Codes Collection Efficiency decrease from avg 11.15 to 58.02</t>
+  </si>
+  <si>
+    <t>2-BCBS – X-Ray CPT Codes Collection Efficiency decrease from avg 0.36 to 76.94; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decrease from avg 1.10 to 123.00; 18-CIGNA – Existing E/M Code Charge Billed Balance decrease from avg -1.08 to 88.71; 2-BCBS – Existing E/M Code Charge Billed Balance decrease from avg -4.13 to 267.63; 15-UNITED HEALTHCARE – Medications Charge Billed Balance decrease from avg 3.48 to 110.00; 18-CIGNA – Medications Collection Efficiency decrease from avg 0.76 to 18.26</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decrease from avg 0.15 to 40.54; 2-BCBS – New E/M Codes Collection Efficiency decrease from avg -11.19 to 340.70; 2-BCBS – Medications Charge Billed Balance decrease from avg 3.79 to 70.60; 18-CIGNA – X-Ray CPT Codes Charge Billed Balance decrease from avg 6.24 to 72.00; 2-BCBS – Existing E/M Code Charge Billed Balance decrease from avg -4.13 to 35.52; 2-BCBS – New E/M Codes Charge Billed Balance decrease from avg 52.44 to 520.17</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – New E/M Codes Labs per Visit decrease from avg 1.75 to 0.00; 4-MEDICAID – X-Ray CPT Codes Labs per Visit decrease from avg 0.71 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Labs per Visit decrease from avg 0.43 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Amount decrease from avg 7.86 to 0.00; 3-MEDICARE – New E/M Codes Labs per Visit decrease from avg 1.15 to 0.00; 2-BCBS – Self-pay physical &amp; No Charge Labs per Visit decrease from avg 0.17 to 0.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – X-Ray CPT Codes Labs per Visit decrease from avg 0.71 to 0.00; 4-MEDICAID – Medications Labs per Visit decrease from avg 1.26 to 0.00; 3-MEDICARE – X-Ray CPT Codes Labs per Visit decrease from avg 0.67 to 0.00; 3-MEDICARE – Procedures &amp; Surgical CPT Codes Labs per Visit decrease from avg 1.39 to 0.00; 3-MEDICARE – New E/M Codes Labs per Visit decrease from avg 1.15 to 0.00; 3-MEDICARE – Medications Labs per Visit decrease from avg 0.90 to 0.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – X-Ray CPT Codes Labs per Visit decrease from avg 0.71 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Labs per Visit decrease from avg 0.43 to 0.00; 4-MEDICAID – Self-pay physical &amp; No Charge Charge Amount decrease from avg 7.86 to 0.00; 4-MEDICAID – Procedures &amp; Surgical CPT Codes Labs per Visit decrease from avg 1.87 to 0.00; 4-MEDICAID – Medications Labs per Visit decrease from avg 1.26 to 0.00; 3-MEDICARE – X-Ray CPT Codes Labs per Visit decrease from avg 0.67 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance increased from avg 130.16 to 0.00; 17-AETNA – Lab/Test CPT Codes Collection Efficiency increased from avg 62.39 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance increased from avg 101.89 to 0.00; 17-AETNA – Existing E/M Code Collection Efficiency increased from avg 51.63 to 0.00; 17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 63.76 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 211.52 to 565.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 1.56 to 4.00; 17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 5.00; 17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance increased from avg 130.16 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Medications Labs per Visit increased from avg 1.60 to 7.00; 17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.00; 17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.00; 17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance increased from avg 130.16 to 0.00; 17-AETNA – Medications Collection Efficiency increased from avg 3.36 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 3.00; 17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance increased from avg 130.16 to 0.00; 17-AETNA – Medications Collection Efficiency increased from avg 3.36 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.67; 17-AETNA – Medications Charge Amount increased from avg 135.48 to 305.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 211.52 to 464.00; 17-AETNA – Medications Visit Count increased from avg 1.48 to 3.00; 17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 5.00; 17-AETNA – Existing E/M Code Labs per Visit increased from avg 1.75 to 4.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance increased from avg 130.16 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Medications Labs per Visit increased from avg 1.60 to 9.00; 17-AETNA – Lab/Test CPT Codes Labs per Visit increased from avg 2.95 to 6.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance increased from avg 130.16 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance increased from avg 130.16 to 0.00; 17-AETNA – Lab/Test CPT Codes Collection Efficiency increased from avg 62.39 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance increased from avg 101.89 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 7.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance increased from avg 130.16 to 0.00; 17-AETNA – Lab/Test CPT Codes Collection Efficiency increased from avg 62.39 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – New E/M Codes Labs per Visit increased from avg 1.59 to 3.50; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance increased from avg 130.16 to 0.00; 17-AETNA – Medications Collection Efficiency increased from avg 3.36 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 34.92 to 150.69; 17-AETNA – Procedures &amp; Surgical CPT Codes Zero Balance Collection Rate increased from avg 0.27 to 0.66; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Rate* increased from avg 0.30 to 0.66; 17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Collection Efficiency increased from avg 51.63 to -37.05; 17-AETNA – After Hours Labs per Visit increased from avg 2.15 to 5.00; 17-AETNA – Existing E/M Code Labs per Visit increased from avg 1.75 to 4.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 4.00; 17-AETNA – DME Payment per Visit increased from avg 174.97 to 368.10; 17-AETNA – DME NRV Zero Balance* increased from avg 179.12 to 368.10</t>
+  </si>
+  <si>
+    <t>17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.00; 17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – Lab/Test CPT Codes Collection Efficiency increased from avg 62.39 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance increased from avg 101.89 to 0.00; 17-AETNA – Existing E/M Code Collection Efficiency increased from avg 51.63 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 34.92 to 137.69; 17-AETNA – DME Payment per Visit increased from avg 174.97 to 529.98; 17-AETNA – DME NRV Zero Balance* increased from avg 179.12 to 529.98; 17-AETNA – DME Payment Amount* increased from avg 200.73 to 529.98; 17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Medications Charge Amount increased from avg 135.48 to 334.00; 17-AETNA – Medications Visit Count increased from avg 1.48 to 3.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance increased from avg 130.16 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Lab/Test CPT Codes Collection Efficiency increased from avg 62.39 to -177.97; 17-AETNA – New E/M Codes Labs per Visit increased from avg 1.59 to 5.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance increased from avg 130.16 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Medications Visit Count increased from avg 1.48 to 3.00; 17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance increased from avg 130.16 to 0.00; 17-AETNA – Medications Collection Efficiency increased from avg 3.36 to 0.00</t>
   </si>
   <si>
     <t>17-AETNA – Existing E/M Code Labs per Visit increased from avg 1.75 to 2.50; 17-AETNA – After Hours Payment per Visit increased from avg 5.52 to 7.60; 17-AETNA – After Hours NRV Zero Balance* increased from avg 5.52 to 7.60; 17-AETNA – New E/M Codes Avg. Charge E/M Weight increased from avg 3.89 to 4.00</t>
@@ -490,7 +493,7 @@
     <t>17-AETNA – After Hours Payment Amount* increased from avg 18.58 to 46.40; 17-AETNA – Existing E/M Code Labs per Visit increased from avg 1.75 to 3.33; 17-AETNA – After Hours Charge Amount increased from avg 170.58 to 322.00; 17-AETNA – After Hours Visit Count increased from avg 3.75 to 7.00; 17-AETNA – Lab/Test CPT Codes Labs per Visit increased from avg 2.95 to 4.00; 17-AETNA – After Hours Payment per Visit increased from avg 5.52 to 6.63</t>
   </si>
   <si>
-    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 6.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00</t>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.89 to 6.00; 17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00</t>
   </si>
   <si>
     <t>17-AETNA – Lab/Test CPT Codes Payment Amount* increased from avg 641.96 to 2015.22; 17-AETNA – Lab/Test CPT Codes Charge Amount increased from avg 1570.78 to 4744.00; 17-AETNA – X-Ray CPT Codes Labs per Visit increased from avg 0.80 to 2.33; 17-AETNA – X-Ray CPT Codes Visit Count increased from avg 2.12 to 6.00; 17-AETNA – X-Ray CPT Codes Charge Amount increased from avg 292.71 to 760.00; 17-AETNA – Lab/Test CPT Codes Visit Count increased from avg 7.50 to 18.00</t>
@@ -505,55 +508,55 @@
     <t>17-AETNA – Lab/Test CPT Codes Payment Amount* increased from avg 641.96 to 2402.40; 17-AETNA – New E/M Codes Payment Amount* increased from avg 1816.92 to 5807.42; 17-AETNA – Lab/Test CPT Codes Charge Amount increased from avg 1570.78 to 4470.00; 17-AETNA – New E/M Codes Charge Amount increased from avg 2631.41 to 7365.00; 17-AETNA – New E/M Codes Visit Count increased from avg 8.71 to 24.00; 17-AETNA – Lab/Test CPT Codes Visit Count increased from avg 7.50 to 19.00</t>
   </si>
   <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -222.20; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to -132.51; 17-AETNA – Lab/Test CPT Codes Payment Amount* increased from avg 641.96 to 2380.16; 17-AETNA – Lab/Test CPT Codes Charge Amount increased from avg 1570.78 to 4615.00; 17-AETNA – Existing E/M Code Payment Amount* increased from avg 810.88 to 2183.16; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to -63.72</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -70.00; 17-AETNA – X-Ray CPT Codes Collection Rate* increased from avg 0.36 to 1.00; 17-AETNA – Lab/Test CPT Codes Payment Amount* increased from avg 641.96 to 1664.38; 17-AETNA – X-Ray CPT Codes Payment per Visit increased from avg 50.98 to 131.50; 17-AETNA – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 1.56 to 4.00; 17-AETNA – X-Ray CPT Codes Zero Balance Collection Rate increased from avg 0.39 to 1.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Upfront Collections Efficiency decreased from avg 98.28 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.42 to 0.76; 17-AETNA – Lab/Test CPT Codes Collection Rate* increased from avg 0.38 to 0.60; 17-AETNA – New E/M Codes Payment per Visit increased from avg 205.14 to 271.21; 17-AETNA – New E/M Codes Collection Rate* increased from avg 0.68 to 0.87</t>
+    <t>17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 63.76 to -222.20; 17-AETNA – Existing E/M Code Collection Efficiency increased from avg 51.63 to -132.51; 17-AETNA – Lab/Test CPT Codes Payment Amount* increased from avg 641.96 to 2380.16; 17-AETNA – Lab/Test CPT Codes Charge Amount increased from avg 1570.78 to 4615.00; 17-AETNA – Existing E/M Code Payment Amount* increased from avg 810.88 to 2183.16; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance increased from avg 101.89 to -63.72</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 63.76 to -70.00; 17-AETNA – X-Ray CPT Codes Collection Rate* increased from avg 0.36 to 1.00; 17-AETNA – Lab/Test CPT Codes Payment Amount* increased from avg 641.96 to 1664.38; 17-AETNA – X-Ray CPT Codes Payment per Visit increased from avg 50.98 to 131.50; 17-AETNA – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 1.56 to 4.00; 17-AETNA – X-Ray CPT Codes Zero Balance Collection Rate increased from avg 0.39 to 1.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance increased from avg 130.16 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.42 to 0.76; 17-AETNA – Lab/Test CPT Codes Collection Rate* increased from avg 0.38 to 0.60; 17-AETNA – New E/M Codes Payment per Visit increased from avg 205.14 to 271.21; 17-AETNA – New E/M Codes Collection Rate* increased from avg 0.68 to 0.87</t>
   </si>
   <si>
     <t>17-AETNA – X-Ray CPT Codes Payment Amount* increased from avg 106.71 to 412.14; 17-AETNA – Medications Labs per Visit increased from avg 1.60 to 4.00; 17-AETNA – Lab/Test CPT Codes Payment Amount* increased from avg 641.96 to 1496.15; 17-AETNA – X-Ray CPT Codes Charge Amount increased from avg 292.71 to 650.00; 17-AETNA – Lab/Test CPT Codes NRV Zero Balance* increased from avg 86.49 to 187.02; 17-AETNA – Existing E/M Code Payment Amount* increased from avg 810.88 to 1641.88</t>
   </si>
   <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -14.56; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Upfront Collections Efficiency decreased from avg 98.28 to 0.00; 17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00; 17-AETNA – Medications Upfront Collections Efficiency decreased from avg 3.36 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency decreased from avg 5.70 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.42 to 0.64; 17-AETNA – Existing E/M Code Payment Amount* increased from avg 810.88 to 1154.83</t>
+    <t>17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 63.76 to -14.56; 17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00; 17-AETNA – Medications Collection Efficiency increased from avg 3.36 to 0.00; 17-AETNA – Medications Charge Billed Balance increased from avg 14.47 to 0.00; 17-AETNA – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.42 to 0.64; 17-AETNA – Existing E/M Code Payment Amount* increased from avg 810.88 to 1154.83</t>
   </si>
   <si>
     <t>17-AETNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 211.52 to 540.00; 17-AETNA – Existing E/M Code Charge Amount increased from avg 1291.98 to 1960.00; 17-AETNA – Lab/Test CPT Codes Visit Count increased from avg 7.50 to 11.00; 17-AETNA – Existing E/M Code Payment Amount* increased from avg 810.88 to 1182.88; 17-AETNA – Existing E/M Code Visit Count increased from avg 5.52 to 8.00; 17-AETNA – New E/M Codes Charge Amount increased from avg 2631.41 to 3720.00</t>
   </si>
   <si>
-    <t>17-AETNA – Medications Upfront Collections Efficiency decreased from avg 3.36 to 0.00; 17-AETNA – DME Upfront Collections Efficiency decreased from avg 10.48 to 0.00; 17-AETNA – DME Charge Billed Balance decreased from avg 149.25 to 25.00; 17-AETNA – Medications Charge Amount increased from avg 135.48 to 192.00; 17-AETNA – X-Ray CPT Codes Visit Count increased from avg 2.12 to 3.00; 17-AETNA – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.42 to 0.58</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Upfront Collections Efficiency decreased from avg 3.36 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency decreased from avg 5.70 to 0.00; 17-AETNA – DME Upfront Collections Efficiency decreased from avg 10.48 to 0.00; 17-AETNA – DME Charge Amount increased from avg 429.55 to 630.92; 17-AETNA – Existing E/M Code Visit Count increased from avg 5.52 to 8.00; 17-AETNA – X-Ray CPT Codes Visit Count increased from avg 2.12 to 3.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Medications Charge Billed Balance decreased from avg 14.47 to 0.00; 17-AETNA – Medications Upfront Collections Efficiency decreased from avg 3.36 to 0.00; 17-AETNA – DME Upfront Collections Efficiency decreased from avg 10.48 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 2.88; 17-AETNA – X-Ray CPT Codes Visit Count increased from avg 2.12 to 4.00; 17-AETNA – Medications Labs per Visit increased from avg 1.60 to 3.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Collection Rate* increased from avg 0.30 to 1.01; 17-AETNA – New E/M Codes Upfront Collections Efficiency decreased from avg 98.28 to -108.32; 17-AETNA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 76.58 to 229.10; 17-AETNA – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 94.17 to 229.10; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to -45.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to -11.97</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to -190.76; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -210.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00; 17-AETNA – New E/M Codes Charge Billed Balance decreased from avg 130.16 to 0.00; 17-AETNA – New E/M Codes Upfront Collections Efficiency decreased from avg 98.28 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 0.00; 17-AETNA – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 62.39 to 0.00; 17-AETNA – Existing E/M Code Payment Amount* increased from avg 810.88 to 1459.20; 17-AETNA – Existing E/M Code Charge Amount increased from avg 1291.98 to 2205.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – X-Ray CPT Codes Charge Billed Balance decreased from avg 22.59 to 0.00; 17-AETNA – X-Ray CPT Codes Upfront Collections Efficiency decreased from avg 11.15 to 0.00; 17-AETNA – Lab/Test CPT Codes NRV Zero Balance* increased from avg 86.49 to 152.69; 17-AETNA – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.42 to 0.56; 17-AETNA – Existing E/M Code NRV Zero Balance* increased from avg 150.29 to 172.35; 17-AETNA – New E/M Codes NRV Zero Balance* increased from avg 213.66 to 237.89</t>
-  </si>
-  <si>
-    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 76.58 to 997.19; 17-AETNA – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 94.17 to 997.19; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 211.52 to 2187.00; 17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -64.56; 17-AETNA – DME Payment Amount* increased from avg 200.73 to 460.13; 17-AETNA – Existing E/M Code Upfront Collections Efficiency decreased from avg 51.63 to -11.31</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Charge Billed Balance decreased from avg 63.76 to -40.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency decreased from avg 5.70 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance decreased from avg 22.59 to 0.00; 17-AETNA – X-Ray CPT Codes Upfront Collections Efficiency decreased from avg 11.15 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance decreased from avg 101.89 to 31.17</t>
-  </si>
-  <si>
-    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency decreased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 29.14 to 2.12; 17-AETNA – Lab/Test CPT Codes Charge Amount increased from avg 1570.78 to 2385.00; 17-AETNA – New E/M Codes Charge Amount increased from avg 2631.41 to 3955.00; 17-AETNA – New E/M Codes Visit Count increased from avg 8.71 to 13.00; 17-AETNA – Lab/Test CPT Codes Visit Count increased from avg 7.50 to 11.00</t>
+    <t>17-AETNA – Medications Collection Efficiency increased from avg 3.36 to 0.00; 17-AETNA – DME Collection Efficiency increased from avg 10.48 to 0.00; 17-AETNA – DME Charge Billed Balance increased from avg 149.25 to 25.00; 17-AETNA – Medications Charge Amount increased from avg 135.48 to 192.00; 17-AETNA – X-Ray CPT Codes Visit Count increased from avg 2.12 to 3.00; 17-AETNA – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.42 to 0.58</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Medications Collection Efficiency increased from avg 3.36 to 0.00; 17-AETNA – DME Collection Efficiency increased from avg 10.48 to 0.00; 17-AETNA – DME Charge Amount increased from avg 429.55 to 630.92; 17-AETNA – Existing E/M Code Visit Count increased from avg 5.52 to 8.00; 17-AETNA – X-Ray CPT Codes Visit Count increased from avg 2.12 to 3.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Medications Collection Efficiency increased from avg 3.36 to 0.00; 17-AETNA – Medications Charge Billed Balance increased from avg 14.47 to 0.00; 17-AETNA – DME Collection Efficiency increased from avg 10.48 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance increased from avg 101.89 to 2.88; 17-AETNA – X-Ray CPT Codes Visit Count increased from avg 2.12 to 4.00; 17-AETNA – Medications Labs per Visit increased from avg 1.60 to 3.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Collection Rate* increased from avg 0.30 to 1.01; 17-AETNA – New E/M Codes Collection Efficiency increased from avg 98.28 to -108.32; 17-AETNA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 76.58 to 229.10; 17-AETNA – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 94.17 to 229.10; 17-AETNA – New E/M Codes Charge Billed Balance increased from avg 130.16 to -45.00; 17-AETNA – Lab/Test CPT Codes Collection Efficiency increased from avg 62.39 to -11.97</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Collection Efficiency increased from avg 51.63 to -190.76; 17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 63.76 to -210.00; 17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Lab/Test CPT Codes Collection Efficiency increased from avg 62.39 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance increased from avg 101.89 to 0.00; 17-AETNA – Existing E/M Code Collection Efficiency increased from avg 51.63 to 0.00; 17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 63.76 to 0.00; 17-AETNA – Existing E/M Code Payment Amount* increased from avg 810.88 to 1459.20; 17-AETNA – Existing E/M Code Charge Amount increased from avg 1291.98 to 2205.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – Lab/Test CPT Codes NRV Zero Balance* increased from avg 86.49 to 152.69; 17-AETNA – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.42 to 0.56; 17-AETNA – Existing E/M Code NRV Zero Balance* increased from avg 150.29 to 172.35; 17-AETNA – New E/M Codes NRV Zero Balance* increased from avg 213.66 to 237.89</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 76.58 to 997.19; 17-AETNA – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 94.17 to 997.19; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 211.52 to 2187.00; 17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 63.76 to -64.56; 17-AETNA – DME Payment Amount* increased from avg 200.73 to 460.13; 17-AETNA – Existing E/M Code Collection Efficiency increased from avg 51.63 to -11.31</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 63.76 to -40.00; 17-AETNA – X-Ray CPT Codes Collection Efficiency increased from avg 11.15 to 0.00; 17-AETNA – X-Ray CPT Codes Charge Billed Balance increased from avg 22.59 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 0.00; 17-AETNA – Lab/Test CPT Codes Charge Billed Balance increased from avg 101.89 to 31.17</t>
+  </si>
+  <si>
+    <t>17-AETNA – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg 5.70 to 0.00; 17-AETNA – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 29.14 to 2.12; 17-AETNA – Lab/Test CPT Codes Charge Amount increased from avg 1570.78 to 2385.00; 17-AETNA – New E/M Codes Charge Amount increased from avg 2631.41 to 3955.00; 17-AETNA – New E/M Codes Visit Count increased from avg 8.71 to 13.00; 17-AETNA – Lab/Test CPT Codes Visit Count increased from avg 7.50 to 11.00</t>
   </si>
   <si>
     <t>17-AETNA – X-Ray CPT Codes Payment per Visit increased from avg 50.98 to 141.77; 17-AETNA – X-Ray CPT Codes NRV Zero Balance* increased from avg 54.42 to 141.77; 17-AETNA – X-Ray CPT Codes Charge Amount increased from avg 292.71 to 480.00; 17-AETNA – X-Ray CPT Codes Payment Amount* increased from avg 106.71 to 141.77; 17-AETNA – Existing E/M Code Charge Amount increased from avg 1291.98 to 1715.00; 17-AETNA – Existing E/M Code Visit Count increased from avg 5.52 to 7.00</t>
@@ -571,64 +574,64 @@
     <t>2-BCBS – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 571.38 to 1782.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 205.41 to 592.27; 2-BCBS – Self-pay physical &amp; No Charge Zero Balance Collection Rate increased from avg 0.38 to 1.00; 2-BCBS – Self-pay physical &amp; No Charge Collection Rate* increased from avg 0.38 to 1.00; 2-BCBS – X-Ray CPT Codes Charge Amount increased from avg 655.56 to 1401.00; 2-BCBS – Medications Labs per Visit increased from avg 1.33 to 2.75</t>
   </si>
   <si>
-    <t>2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -118.35; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -130.33; 2-BCBS – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 23.63 to -20.62; 2-BCBS – After Hours Upfront Collections Efficiency decreased from avg 0.08 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – DME NRV Zero Balance* increased from avg 140.68 to 473.50; 2-BCBS – DME Payment per Visit increased from avg 145.60 to 473.50; 2-BCBS – Medications Charge Amount increased from avg 363.59 to 766.00; 2-BCBS – After Hours Upfront Collections Efficiency decreased from avg 0.08 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00</t>
+    <t>2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -118.35; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to -130.33; 2-BCBS – Lab/Test CPT Codes Collection Efficiency increased from avg 23.63 to -20.62; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – DME NRV Zero Balance* increased from avg 140.68 to 473.50; 2-BCBS – DME Payment per Visit increased from avg 145.60 to 473.50; 2-BCBS – Medications Charge Amount increased from avg 363.59 to 766.00; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00</t>
   </si>
   <si>
     <t>2-BCBS – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 205.41 to 731.66; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 571.38 to 1552.00; 2-BCBS – Medications Visit Count increased from avg 3.91 to 10.00; 2-BCBS – Medications Charge Amount increased from avg 363.59 to 893.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 5.06 to 12.00; 2-BCBS – Medications Payment Amount* increased from avg 67.30 to 156.57</t>
   </si>
   <si>
-    <t>2-BCBS – After Hours Upfront Collections Efficiency decreased from avg 0.08 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Upfront Collections Efficiency decreased from avg 2.09 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 1.60; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to -2.48; 2-BCBS – After Hours Upfront Collections Efficiency decreased from avg 0.08 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Upfront Collections Efficiency decreased from avg 2.09 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Medications Visit Count increased from avg 3.91 to 9.00; 2-BCBS – After Hours Upfront Collections Efficiency decreased from avg 0.08 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Upfront Collections Efficiency decreased from avg 2.09 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 4.80; 2-BCBS – After Hours Upfront Collections Efficiency decreased from avg 0.08 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -150.46; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -179.32; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.71; 2-BCBS – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 23.63 to -7.93; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to -13.57; 2-BCBS – After Hours Upfront Collections Efficiency decreased from avg 0.08 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 23.63 to -355.92; 2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -82.30; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 205.41 to 469.56; 2-BCBS – After Hours Upfront Collections Efficiency decreased from avg 0.08 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Vaccines Labs per Visit increased from avg 0.10 to 2.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.50; 2-BCBS – After Hours Upfront Collections Efficiency decreased from avg 0.08 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.67; 2-BCBS – After Hours Upfront Collections Efficiency decreased from avg 0.08 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Upfront Collections Efficiency decreased from avg 2.09 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 23.63 to -2.48; 2-BCBS – Medications Charge Amount increased from avg 363.59 to 756.00; 2-BCBS – Medications Visit Count increased from avg 3.91 to 8.00; 2-BCBS – X-Ray CPT Codes Charge Amount increased from avg 655.56 to 1338.00; 2-BCBS – After Hours Upfront Collections Efficiency decreased from avg 0.08 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00</t>
+    <t>2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 0.00; 2-BCBS – Medications Collection Efficiency increased from avg 2.09 to 0.00; 2-BCBS – Medications Charge Billed Balance increased from avg 3.79 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 1.60; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance increased from avg 71.92 to -2.48; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Medications Visit Count increased from avg 3.91 to 9.00; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 0.00; 2-BCBS – Medications Collection Efficiency increased from avg 2.09 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 4.80; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 0.00; 2-BCBS – Medications Collection Efficiency increased from avg 2.09 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -150.46; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to -179.32; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.71; 2-BCBS – Lab/Test CPT Codes Collection Efficiency increased from avg 23.63 to -7.93; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance increased from avg 71.92 to -13.57; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Lab/Test CPT Codes Collection Efficiency increased from avg 23.63 to -355.92; 2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -82.30; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 205.41 to 469.56; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Vaccines Labs per Visit increased from avg 0.10 to 2.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.50; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.67; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 0.00; 2-BCBS – Medications Collection Efficiency increased from avg 2.09 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Lab/Test CPT Codes Collection Efficiency increased from avg 23.63 to -2.48; 2-BCBS – Medications Charge Amount increased from avg 363.59 to 756.00; 2-BCBS – Medications Visit Count increased from avg 3.91 to 8.00; 2-BCBS – X-Ray CPT Codes Charge Amount increased from avg 655.56 to 1338.00; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00</t>
   </si>
   <si>
     <t>2-BCBS – Procedures &amp; Surgical CPT Codes Visit Count increased from avg 5.06 to 14.00; 2-BCBS – Medications Payment Amount* increased from avg 67.30 to 181.65; 2-BCBS – Medications Visit Count increased from avg 3.91 to 10.00; 2-BCBS – Medications Charge Amount increased from avg 363.59 to 925.00; 2-BCBS – DME Charge Amount increased from avg 616.33 to 1466.85; 2-BCBS – X-Ray CPT Codes Payment Amount* increased from avg 256.59 to 599.09</t>
   </si>
   <si>
-    <t>2-BCBS – Self-pay physical &amp; No Charge Charge Amount increased from avg 15.08 to 52.00; 2-BCBS – Vaccines Visit Count increased from avg 1.31 to 3.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Upfront Collections Efficiency decreased from avg 2.09 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -107.62; 2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -37.97; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 205.41 to 466.34; 2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 1.67; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Self-pay physical &amp; No Charge Charge Amount increased from avg 15.08 to 52.00; 2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 2.00; 2-BCBS – Vaccines Visit Count increased from avg 1.31 to 3.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Self-pay physical &amp; No Charge Charge Amount increased from avg 15.08 to 52.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Lab/Test CPT Codes Upfront Collections Efficiency decreased from avg 23.63 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Upfront Collections Efficiency decreased from avg 2.09 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Vaccines Labs per Visit increased from avg 0.10 to 1.00; 2-BCBS – Medications Labs per Visit increased from avg 1.33 to 3.20; 2-BCBS – After Hours Upfront Collections Efficiency decreased from avg 0.08 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – DME Labs per Visit increased from avg 0.05 to 0.50; 2-BCBS – DME Charge Amount increased from avg 616.33 to 1482.97; 2-BCBS – DME Payment Amount* increased from avg 258.71 to 517.86; 2-BCBS – After Hours Upfront Collections Efficiency decreased from avg 0.08 to 0.00; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -50.00; 2-BCBS – Vaccines NRV Zero Balance* increased from avg 69.01 to 345.09; 2-BCBS – Vaccines Payment per Visit increased from avg 69.62 to 345.09; 2-BCBS – Vaccines Payment Amount* increased from avg 88.21 to 345.09; 2-BCBS – Vaccines Zero Balance Collection Rate increased from avg 0.64 to 1.64; 2-BCBS – Vaccines Collection Rate* increased from avg 0.64 to 1.64</t>
+    <t>2-BCBS – Self-pay physical &amp; No Charge Charge Amount increased from avg 15.08 to 52.00; 2-BCBS – Vaccines Visit Count increased from avg 1.31 to 3.00; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – Medications Collection Efficiency increased from avg 2.09 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to -107.62; 2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -37.97; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 205.41 to 466.34; 2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 1.67; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Self-pay physical &amp; No Charge Charge Amount increased from avg 15.08 to 52.00; 2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 2.00; 2-BCBS – Vaccines Visit Count increased from avg 1.31 to 3.00; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Self-pay physical &amp; No Charge Charge Amount increased from avg 15.08 to 52.00; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to 0.00; 2-BCBS – Medications Collection Efficiency increased from avg 2.09 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Vaccines Labs per Visit increased from avg 0.10 to 1.00; 2-BCBS – Medications Labs per Visit increased from avg 1.33 to 3.20; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – Medications Charge Billed Balance increased from avg 3.79 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – DME Labs per Visit increased from avg 0.05 to 0.50; 2-BCBS – DME Charge Amount increased from avg 616.33 to 1482.97; 2-BCBS – DME Payment Amount* increased from avg 258.71 to 517.86; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -50.00; 2-BCBS – Vaccines NRV Zero Balance* increased from avg 69.01 to 345.09; 2-BCBS – Vaccines Payment per Visit increased from avg 69.62 to 345.09; 2-BCBS – Vaccines Payment Amount* increased from avg 88.21 to 345.09; 2-BCBS – Vaccines Zero Balance Collection Rate increased from avg 0.64 to 1.64; 2-BCBS – Vaccines Collection Rate* increased from avg 0.64 to 1.64</t>
   </si>
   <si>
     <t>2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.80; 2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 1.56; 2-BCBS – X-Ray CPT Codes Visit Count increased from avg 5.04 to 9.00; 2-BCBS – X-Ray CPT Codes Payment Amount* increased from avg 256.59 to 438.71; 2-BCBS – X-Ray CPT Codes Charge Amount increased from avg 655.56 to 1038.00; 2-BCBS – DME Charge Amount increased from avg 616.33 to 965.66</t>
@@ -640,70 +643,70 @@
     <t>2-BCBS – Procedures &amp; Surgical CPT Codes Labs per Visit increased from avg 1.56 to 3.75; 2-BCBS – Vaccines Visit Count increased from avg 1.31 to 3.00; 2-BCBS – X-Ray CPT Codes Payment Amount* increased from avg 256.59 to 574.75; 2-BCBS – Vaccines Charge Amount increased from avg 137.31 to 275.05; 2-BCBS – Vaccines Payment Amount* increased from avg 88.21 to 159.70; 2-BCBS – X-Ray CPT Codes Visit Count increased from avg 5.04 to 9.00</t>
   </si>
   <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -62.32; 2-BCBS – Existing E/M Code Upfront Collections Efficiency decreased from avg -16.11 to -71.07; 2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 2.33; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00; 2-BCBS – X-Ray CPT Codes Upfront Collections Efficiency decreased from avg 0.36 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -204.90; 2-BCBS – Existing E/M Code Upfront Collections Efficiency decreased from avg -16.11 to -256.10; 2-BCBS – X-Ray CPT Codes Charge Amount increased from avg 655.56 to 1508.00; 2-BCBS – X-Ray CPT Codes Visit Count increased from avg 5.04 to 11.00; 2-BCBS – X-Ray CPT Codes Payment Amount* increased from avg 256.59 to 527.57; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -560.87; 2-BCBS – Existing E/M Code Upfront Collections Efficiency decreased from avg -16.11 to -457.10; 2-BCBS – X-Ray CPT Codes Upfront Collections Efficiency decreased from avg 0.36 to -8.56; 2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -268.05; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 45.56 to 231.76; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 231.76</t>
-  </si>
-  <si>
-    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency decreased from avg -4.05 to -290.82; 2-BCBS – X-Ray CPT Codes Upfront Collections Efficiency decreased from avg 0.36 to -9.77; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -83.00; 2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -170.34; 2-BCBS – Existing E/M Code Upfront Collections Efficiency decreased from avg -16.11 to -177.00; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -232.60</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -87.98; 2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 3.50; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 45.56 to 118.42; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 118.42; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 205.41 to 473.70; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -90.00; 2-BCBS – Existing E/M Code Upfront Collections Efficiency decreased from avg -16.11 to -72.37; 2-BCBS – Lab/Test CPT Codes Payment Amount* increased from avg 1282.57 to 2648.14; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Upfront Collections Efficiency decreased from avg 2.09 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -201.15; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -329.34; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -22.08; 2-BCBS – Medications Upfront Collections Efficiency decreased from avg 2.09 to -1.65; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – X-Ray CPT Codes Upfront Collections Efficiency decreased from avg 0.36 to -50.99; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to -40.25; 2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -372.10; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -305.12; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 45.56 to 316.71; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 316.71</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -222.92; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -306.29; 2-BCBS – Medications Labs per Visit increased from avg 1.33 to 3.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Upfront Collections Efficiency decreased from avg 2.09 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – X-Ray CPT Codes Upfront Collections Efficiency decreased from avg 0.36 to -19.11; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 205.41 to 517.88; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 45.56 to 90.76; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 86.31</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -195.15; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -252.85; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 571.38 to 1493.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Upfront Collections Efficiency decreased from avg 2.09 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – X-Ray CPT Codes Upfront Collections Efficiency decreased from avg 0.36 to -22.39; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -195.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to -29.00; 2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -150.97; 2-BCBS – Existing E/M Code Upfront Collections Efficiency decreased from avg -16.11 to -183.77; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -297.48; 2-BCBS – Existing E/M Code Upfront Collections Efficiency decreased from avg -16.11 to -256.81; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00; 2-BCBS – X-Ray CPT Codes Upfront Collections Efficiency decreased from avg 0.36 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -13.16; 2-BCBS – Medications NRV Zero Balance* increased from avg 18.08 to 39.74; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00; 2-BCBS – Medications Payment per Visit increased from avg 16.62 to 32.67</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -164.83; 2-BCBS – Vaccines Charge Billed Balance decreased from avg -0.69 to -20.00; 2-BCBS – Existing E/M Code Upfront Collections Efficiency decreased from avg -16.11 to -167.31; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Upfront Collections Efficiency decreased from avg 2.09 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -80.61; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -65.54; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 0.00; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Medications Upfront Collections Efficiency decreased from avg 2.09 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -757.42; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -129.48; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -776.79; 2-BCBS – Existing E/M Code Upfront Collections Efficiency decreased from avg -16.11 to -152.16; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 45.56 to 155.60; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 155.60</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -147.63; 2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -314.63; 2-BCBS – Medications Upfront Collections Efficiency decreased from avg 2.09 to -17.33; 2-BCBS – Existing E/M Code Upfront Collections Efficiency decreased from avg -16.11 to -153.13; 2-BCBS – New E/M Codes Charge Billed Balance decreased from avg 52.44 to -269.24; 2-BCBS – Procedures &amp; Surgical CPT Codes Collection Rate* increased from avg 0.31 to 0.66</t>
-  </si>
-  <si>
-    <t>2-BCBS – DME Labs per Visit increased from avg 0.05 to 1.00; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -68.29; 2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -74.02; 2-BCBS – Existing E/M Code Upfront Collections Efficiency decreased from avg -16.11 to -47.06; 2-BCBS – DME Zero Balance Collection Rate increased from avg 0.36 to 1.00; 2-BCBS – DME Collection Rate* increased from avg 0.37 to 1.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg -4.13 to -148.28; 2-BCBS – Existing E/M Code Upfront Collections Efficiency decreased from avg -16.11 to -85.52; 2-BCBS – Medications Charge Billed Balance decreased from avg 3.79 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance decreased from avg 71.92 to 10.54; 2-BCBS – Medications Payment per Visit increased from avg 16.62 to 26.58</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Codes Upfront Collections Efficiency decreased from avg -11.19 to -86.67; 2-BCBS – Medications Upfront Collections Efficiency decreased from avg 2.09 to -2.09; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance decreased from avg 8.81 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.21 to 0.33; 2-BCBS – X-Ray CPT Codes Zero Balance Collection Rate increased from avg 0.39 to 0.63</t>
-  </si>
-  <si>
-    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Upfront Collections Efficiency decreased from avg -4.05 to -235.56; 2-BCBS – Existing E/M Code Upfront Collections Efficiency decreased from avg -16.11 to -94.32; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 110.22; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 205.41 to 440.86; 2-BCBS – DME Charge Billed Balance decreased from avg 6.55 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance decreased from avg 1.10 to 0.00</t>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -62.32; 2-BCBS – Existing E/M Code Collection Efficiency increased from avg -16.11 to -71.07; 2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 2.33; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -204.90; 2-BCBS – Existing E/M Code Collection Efficiency increased from avg -16.11 to -256.10; 2-BCBS – X-Ray CPT Codes Charge Amount increased from avg 655.56 to 1508.00; 2-BCBS – X-Ray CPT Codes Visit Count increased from avg 5.04 to 11.00; 2-BCBS – X-Ray CPT Codes Payment Amount* increased from avg 256.59 to 527.57; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -560.87; 2-BCBS – Existing E/M Code Collection Efficiency increased from avg -16.11 to -457.10; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to -8.56; 2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -268.05; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 45.56 to 231.76; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 231.76</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg -4.05 to -290.82; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to -9.77; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -83.00; 2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -170.34; 2-BCBS – Existing E/M Code Collection Efficiency increased from avg -16.11 to -177.00; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to -232.60</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -87.98; 2-BCBS – X-Ray CPT Codes Labs per Visit increased from avg 0.78 to 3.50; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 45.56 to 118.42; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 118.42; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 205.41 to 473.70; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -90.00; 2-BCBS – Existing E/M Code Collection Efficiency increased from avg -16.11 to -72.37; 2-BCBS – Lab/Test CPT Codes Payment Amount* increased from avg 1282.57 to 2648.14; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -201.15; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to -329.34; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -22.08; 2-BCBS – Medications Collection Efficiency increased from avg 2.09 to -1.65; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to -50.99; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to -40.25; 2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -372.10; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to -305.12; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 45.56 to 316.71; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 316.71</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -222.92; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to -306.29; 2-BCBS – Medications Labs per Visit increased from avg 1.33 to 3.00; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to -19.11; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 205.41 to 517.88; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 45.56 to 90.76; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 86.31</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -195.15; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to -252.85; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Amount increased from avg 571.38 to 1493.00; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Medications Collection Efficiency increased from avg 2.09 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to -22.39; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -195.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to -29.00; 2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -150.97; 2-BCBS – Existing E/M Code Collection Efficiency increased from avg -16.11 to -183.77; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -297.48; 2-BCBS – Existing E/M Code Collection Efficiency increased from avg -16.11 to -256.81; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – DME Charge Billed Balance increased from avg 6.55 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -13.16; 2-BCBS – Medications NRV Zero Balance* increased from avg 18.08 to 39.74; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – DME Charge Billed Balance increased from avg 6.55 to 0.00; 2-BCBS – Medications Payment per Visit increased from avg 16.62 to 32.67</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -164.83; 2-BCBS – Vaccines Charge Billed Balance increased from avg -0.69 to -20.00; 2-BCBS – Existing E/M Code Collection Efficiency increased from avg -16.11 to -167.31; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -80.61; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to -65.54; 2-BCBS – X-Ray CPT Codes Collection Efficiency increased from avg 0.36 to 0.00; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – Medications Collection Efficiency increased from avg 2.09 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -757.42; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -129.48; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to -776.79; 2-BCBS – Existing E/M Code Collection Efficiency increased from avg -16.11 to -152.16; 2-BCBS – Procedures &amp; Surgical CPT Codes NRV Zero Balance* increased from avg 45.56 to 155.60; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 155.60</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -147.63; 2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -314.63; 2-BCBS – Medications Collection Efficiency increased from avg 2.09 to -17.33; 2-BCBS – Existing E/M Code Collection Efficiency increased from avg -16.11 to -153.13; 2-BCBS – New E/M Codes Charge Billed Balance increased from avg 52.44 to -269.24; 2-BCBS – Procedures &amp; Surgical CPT Codes Collection Rate* increased from avg 0.31 to 0.66</t>
+  </si>
+  <si>
+    <t>2-BCBS – DME Labs per Visit increased from avg 0.05 to 1.00; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -68.29; 2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -74.02; 2-BCBS – Existing E/M Code Collection Efficiency increased from avg -16.11 to -47.06; 2-BCBS – DME Zero Balance Collection Rate increased from avg 0.36 to 1.00; 2-BCBS – DME Collection Rate* increased from avg 0.37 to 1.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Charge Billed Balance increased from avg -4.13 to -148.28; 2-BCBS – Existing E/M Code Collection Efficiency increased from avg -16.11 to -85.52; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – Medications Charge Billed Balance increased from avg 3.79 to 0.00; 2-BCBS – Lab/Test CPT Codes Charge Billed Balance increased from avg 71.92 to 10.54; 2-BCBS – Medications Payment per Visit increased from avg 16.62 to 26.58</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Codes Collection Efficiency increased from avg -11.19 to -86.67; 2-BCBS – Medications Collection Efficiency increased from avg 2.09 to -2.09; 2-BCBS – Procedures &amp; Surgical CPT Codes Charge Billed Balance increased from avg 8.81 to 0.00; 2-BCBS – DME Charge Billed Balance increased from avg 6.55 to 0.00; 2-BCBS – Lab/Test CPT Codes Zero Balance Collection Rate increased from avg 0.21 to 0.33; 2-BCBS – X-Ray CPT Codes Zero Balance Collection Rate increased from avg 0.39 to 0.63</t>
+  </si>
+  <si>
+    <t>2-BCBS – Procedures &amp; Surgical CPT Codes Collection Efficiency increased from avg -4.05 to -235.56; 2-BCBS – Existing E/M Code Collection Efficiency increased from avg -16.11 to -94.32; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment per Visit increased from avg 45.90 to 110.22; 2-BCBS – Procedures &amp; Surgical CPT Codes Payment Amount* increased from avg 205.41 to 440.86; 2-BCBS – X-Ray CPT Codes Charge Billed Balance increased from avg 1.10 to 0.00; 2-BCBS – DME Charge Billed Balance increased from avg 6.55 to 0.00</t>
   </si>
   <si>
     <t>2-BCBS – Self-pay physical &amp; No Charge Payment per Visit increased from avg 18.42 to 35.00; 2-BCBS – Self-pay physical &amp; No Charge Payment Amount* increased from avg 18.42 to 35.00; 2-BCBS – X-Ray CPT Codes Payment per Visit increased from avg 49.59 to 55.13; 2-BCBS – Existing E/M Code Avg. Charge E/M Weight increased from avg 3.86 to 3.91; 2-BCBS – New E/M Codes Avg. Charge E/M Weight increased from avg 3.83 to 3.85</t>
@@ -715,7 +718,7 @@
     <t>2-BCBS – X-Ray CPT Codes NRV Zero Balance* increased from avg 49.50 to 59.11; 2-BCBS – X-Ray CPT Codes Payment per Visit increased from avg 49.59 to 57.81; 2-BCBS – Medications Payment per Visit increased from avg 16.62 to 18.27; 2-BCBS – Vaccines NRV Zero Balance* increased from avg 69.01 to 75.59; 2-BCBS – Vaccines Payment per Visit increased from avg 69.62 to 75.59; 2-BCBS – New E/M Codes Avg. Charge E/M Weight increased from avg 3.83 to 3.92</t>
   </si>
   <si>
-    <t>Improved Upfront Collections Efficiency; Investigate Billing Timeliness or Collections</t>
+    <t>Improved Collections Efficiency</t>
   </si>
   <si>
     <t>Investigate Billing Timeliness or Collections</t>
@@ -1089,7 +1092,7 @@
   <dimension ref="A1:AF51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="A1:XFD1048576"/>
+      <selection activeCell="S1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1121,7 +1124,7 @@
     <col min="29" max="29" width="13.5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="66" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.2">
@@ -1260,7 +1263,7 @@
         <v>1.7064900923255391</v>
       </c>
       <c r="M2">
-        <v>824.56192982456139</v>
+        <v>47000.03</v>
       </c>
       <c r="N2">
         <v>135.4441272696294</v>
@@ -1281,13 +1284,13 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <v>843.19958217169221</v>
+        <v>47253.204146801218</v>
       </c>
       <c r="U2">
-        <v>18.637652347130821</v>
+        <v>253.17414680122599</v>
       </c>
       <c r="V2">
-        <v>-2.2103488594158041</v>
+        <v>-0.53578196732372163</v>
       </c>
       <c r="W2" t="s">
         <v>30</v>
@@ -1302,7 +1305,10 @@
         <v>134</v>
       </c>
       <c r="AA2" t="s">
-        <v>181</v>
+        <v>182</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -1314,7 +1320,7 @@
         <v>1</v>
       </c>
       <c r="AF2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
@@ -1355,7 +1361,7 @@
         <v>2.0372369923982832</v>
       </c>
       <c r="M3">
-        <v>526.83816666666667</v>
+        <v>31610.29</v>
       </c>
       <c r="N3">
         <v>113.9756474206349</v>
@@ -1376,13 +1382,13 @@
         <v>0</v>
       </c>
       <c r="T3">
-        <v>536.19271532359926</v>
+        <v>31612.778858942671</v>
       </c>
       <c r="U3">
-        <v>9.3545486569325931</v>
+        <v>2.4888589426700491</v>
       </c>
       <c r="V3">
-        <v>-1.7446243467308209</v>
+        <v>-7.8729521177983916E-3</v>
       </c>
       <c r="W3" t="s">
         <v>30</v>
@@ -1397,7 +1403,10 @@
         <v>135</v>
       </c>
       <c r="AA3" t="s">
-        <v>182</v>
+        <v>183</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
       </c>
       <c r="AC3">
         <v>0</v>
@@ -1450,7 +1459,7 @@
         <v>2.0101702094922431</v>
       </c>
       <c r="M4">
-        <v>523.94232142857129</v>
+        <v>29340.76999999999</v>
       </c>
       <c r="N4">
         <v>109.3878281928357</v>
@@ -1471,16 +1480,16 @@
         <v>1</v>
       </c>
       <c r="T4">
-        <v>544.51892202591705</v>
+        <v>29932.692475377709</v>
       </c>
       <c r="U4">
-        <v>20.57660059734576</v>
+        <v>591.92247537771982</v>
       </c>
       <c r="V4">
-        <v>-3.778858688838437</v>
+        <v>-1.9775116316870871</v>
       </c>
       <c r="W4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X4" t="s">
         <v>36</v>
@@ -1492,16 +1501,19 @@
         <v>136</v>
       </c>
       <c r="AA4" t="s">
-        <v>183</v>
+        <v>184</v>
+      </c>
+      <c r="AB4">
+        <v>1</v>
       </c>
       <c r="AC4">
         <v>0</v>
       </c>
       <c r="AD4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF4" t="s">
         <v>232</v>
@@ -1545,7 +1557,7 @@
         <v>1.9650903784599929</v>
       </c>
       <c r="M5">
-        <v>620.81150000000002</v>
+        <v>37248.69</v>
       </c>
       <c r="N5">
         <v>118.5630511866635</v>
@@ -1566,16 +1578,16 @@
         <v>1</v>
       </c>
       <c r="T5">
-        <v>646.84248435960183</v>
+        <v>37737.270591595538</v>
       </c>
       <c r="U5">
-        <v>26.030984359601799</v>
+        <v>488.5805915955425</v>
       </c>
       <c r="V5">
-        <v>-4.0243158093385656</v>
+        <v>-1.294689795886707</v>
       </c>
       <c r="W5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X5" t="s">
         <v>37</v>
@@ -1584,22 +1596,25 @@
         <v>87</v>
       </c>
       <c r="Z5" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="AA5" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
       </c>
       <c r="AC5">
         <v>0</v>
       </c>
       <c r="AD5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
@@ -1640,7 +1655,7 @@
         <v>2.105482066881033</v>
       </c>
       <c r="M6">
-        <v>609.52830508474574</v>
+        <v>35962.17</v>
       </c>
       <c r="N6">
         <v>123.9179285332069</v>
@@ -1661,13 +1676,13 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>612.45154278298912</v>
+        <v>35762.233322253778</v>
       </c>
       <c r="U6">
-        <v>2.923237698243383</v>
+        <v>199.93667774622011</v>
       </c>
       <c r="V6">
-        <v>-0.47730105878420143</v>
+        <v>0.5590721248994408</v>
       </c>
       <c r="W6" t="s">
         <v>30</v>
@@ -1679,10 +1694,13 @@
         <v>88</v>
       </c>
       <c r="Z6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AA6" t="s">
-        <v>185</v>
+        <v>186</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
       </c>
       <c r="AC6">
         <v>0</v>
@@ -1735,7 +1753,7 @@
         <v>1.7587859699854309</v>
       </c>
       <c r="M7">
-        <v>609.27186440677986</v>
+        <v>35947.040000000008</v>
       </c>
       <c r="N7">
         <v>119.6763499847375</v>
@@ -1756,13 +1774,13 @@
         <v>1</v>
       </c>
       <c r="T7">
-        <v>607.6272692557983</v>
+        <v>35280.434786203587</v>
       </c>
       <c r="U7">
-        <v>1.6445951509815591</v>
+        <v>666.60521379641432</v>
       </c>
       <c r="V7">
-        <v>0.27065854911281451</v>
+        <v>1.8894472753410909</v>
       </c>
       <c r="W7" t="s">
         <v>30</v>
@@ -1774,10 +1792,13 @@
         <v>89</v>
       </c>
       <c r="Z7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AA7" t="s">
-        <v>186</v>
+        <v>187</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
       </c>
       <c r="AC7">
         <v>0</v>
@@ -1789,7 +1810,7 @@
         <v>1</v>
       </c>
       <c r="AF7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
@@ -1830,7 +1851,7 @@
         <v>1.7829461936215529</v>
       </c>
       <c r="M8">
-        <v>626.4666666666667</v>
+        <v>35708.6</v>
       </c>
       <c r="N8">
         <v>116.33640368773951</v>
@@ -1851,13 +1872,13 @@
         <v>1</v>
       </c>
       <c r="T8">
-        <v>640.74467285882088</v>
+        <v>35815.182435012539</v>
       </c>
       <c r="U8">
-        <v>14.27800619215418</v>
+        <v>106.5824350125404</v>
       </c>
       <c r="V8">
-        <v>-2.2283456729261228</v>
+        <v>-0.29759009382665191</v>
       </c>
       <c r="W8" t="s">
         <v>30</v>
@@ -1869,10 +1890,13 @@
         <v>90</v>
       </c>
       <c r="Z8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AA8" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
       </c>
       <c r="AC8">
         <v>0</v>
@@ -1925,7 +1949,7 @@
         <v>2.063387612369934</v>
       </c>
       <c r="M9">
-        <v>595.18442622950829</v>
+        <v>36306.250000000007</v>
       </c>
       <c r="N9">
         <v>110.4131975619791</v>
@@ -1946,13 +1970,13 @@
         <v>0</v>
       </c>
       <c r="T9">
-        <v>651.70226066660587</v>
+        <v>37257.176753906133</v>
       </c>
       <c r="U9">
-        <v>56.517834437097576</v>
+        <v>950.92675390612567</v>
       </c>
       <c r="V9">
-        <v>-8.6723397858536284</v>
+        <v>-2.5523317566096262</v>
       </c>
       <c r="W9" t="s">
         <v>29</v>
@@ -1964,10 +1988,13 @@
         <v>91</v>
       </c>
       <c r="Z9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AA9" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -1979,7 +2006,7 @@
         <v>0</v>
       </c>
       <c r="AF9" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
@@ -2020,7 +2047,7 @@
         <v>1.8241555858179901</v>
       </c>
       <c r="M10">
-        <v>592.41480000000001</v>
+        <v>29620.74</v>
       </c>
       <c r="N10">
         <v>117.0283045815296</v>
@@ -2041,16 +2068,16 @@
         <v>1</v>
       </c>
       <c r="T10">
-        <v>516.84662865134044</v>
+        <v>29318.357654446008</v>
       </c>
       <c r="U10">
-        <v>75.568171348659575</v>
+        <v>302.38234555399322</v>
       </c>
       <c r="V10">
-        <v>14.62100498669154</v>
+        <v>1.0313754580592549</v>
       </c>
       <c r="W10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X10" t="s">
         <v>42</v>
@@ -2059,22 +2086,25 @@
         <v>92</v>
       </c>
       <c r="Z10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AA10" t="s">
-        <v>189</v>
+        <v>190</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
       </c>
       <c r="AC10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD10">
         <v>0</v>
       </c>
       <c r="AE10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF10" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
@@ -2115,7 +2145,7 @@
         <v>1.817865433530254</v>
       </c>
       <c r="M11">
-        <v>479.60274509803918</v>
+        <v>24459.74</v>
       </c>
       <c r="N11">
         <v>117.4611144654728</v>
@@ -2136,16 +2166,16 @@
         <v>0</v>
       </c>
       <c r="T11">
-        <v>460.54582718997801</v>
+        <v>24670.121359227411</v>
       </c>
       <c r="U11">
-        <v>19.05691790806117</v>
+        <v>210.38135922740909</v>
       </c>
       <c r="V11">
-        <v>4.1378982900218677</v>
+        <v>-0.85277796636667058</v>
       </c>
       <c r="W11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X11" t="s">
         <v>43</v>
@@ -2154,19 +2184,22 @@
         <v>93</v>
       </c>
       <c r="Z11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AA11" t="s">
-        <v>190</v>
+        <v>191</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
       </c>
       <c r="AC11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD11">
         <v>0</v>
       </c>
       <c r="AE11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF11" t="s">
         <v>232</v>
@@ -2210,7 +2243,7 @@
         <v>1.3034723191981259</v>
       </c>
       <c r="M12">
-        <v>532.64235294117645</v>
+        <v>27164.76</v>
       </c>
       <c r="N12">
         <v>124.0415157527657</v>
@@ -2231,13 +2264,13 @@
         <v>0</v>
       </c>
       <c r="T12">
-        <v>541.42171847944303</v>
+        <v>27496.243064165599</v>
       </c>
       <c r="U12">
-        <v>8.7793655382665747</v>
+        <v>331.48306416560439</v>
       </c>
       <c r="V12">
-        <v>-1.6215392250837299</v>
+        <v>-1.205557658884711</v>
       </c>
       <c r="W12" t="s">
         <v>30</v>
@@ -2249,10 +2282,13 @@
         <v>94</v>
       </c>
       <c r="Z12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AA12" t="s">
-        <v>191</v>
+        <v>192</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
       </c>
       <c r="AC12">
         <v>0</v>
@@ -2305,7 +2341,7 @@
         <v>1.700802207390782</v>
       </c>
       <c r="M13">
-        <v>450.4277049180327</v>
+        <v>27476.09</v>
       </c>
       <c r="N13">
         <v>117.9692355990783</v>
@@ -2326,16 +2362,16 @@
         <v>0</v>
       </c>
       <c r="T13">
-        <v>459.73180829151158</v>
+        <v>28401.3463234345</v>
       </c>
       <c r="U13">
-        <v>9.304103373478938</v>
+        <v>925.25632343449979</v>
       </c>
       <c r="V13">
-        <v>-2.023811101532329</v>
+        <v>-3.2577903628147831</v>
       </c>
       <c r="W13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X13" t="s">
         <v>45</v>
@@ -2344,19 +2380,22 @@
         <v>95</v>
       </c>
       <c r="Z13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AA13" t="s">
-        <v>192</v>
+        <v>193</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
       </c>
       <c r="AC13">
         <v>0</v>
       </c>
       <c r="AD13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF13" t="s">
         <v>232</v>
@@ -2400,7 +2439,7 @@
         <v>1.5194035849208261</v>
       </c>
       <c r="M14">
-        <v>381.03277777777782</v>
+        <v>20575.77</v>
       </c>
       <c r="N14">
         <v>118.857144047619</v>
@@ -2421,13 +2460,13 @@
         <v>1</v>
       </c>
       <c r="T14">
-        <v>370.56628233835397</v>
+        <v>19514.698300410859</v>
       </c>
       <c r="U14">
-        <v>10.466495439423801</v>
+        <v>1061.0716995891451</v>
       </c>
       <c r="V14">
-        <v>2.8244597358879839</v>
+        <v>5.4372949212686823</v>
       </c>
       <c r="W14" t="s">
         <v>28</v>
@@ -2439,10 +2478,13 @@
         <v>96</v>
       </c>
       <c r="Z14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AA14" t="s">
-        <v>193</v>
+        <v>194</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
       </c>
       <c r="AC14">
         <v>1</v>
@@ -2454,7 +2496,7 @@
         <v>0</v>
       </c>
       <c r="AF14" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
@@ -2495,7 +2537,7 @@
         <v>2.1240479890479889</v>
       </c>
       <c r="M15">
-        <v>438.53049180327872</v>
+        <v>26750.36</v>
       </c>
       <c r="N15">
         <v>117.7685198051948</v>
@@ -2516,16 +2558,16 @@
         <v>0</v>
       </c>
       <c r="T15">
-        <v>471.73506695636672</v>
+        <v>27157.781893207099</v>
       </c>
       <c r="U15">
-        <v>33.204575153088001</v>
+        <v>407.42189320710168</v>
       </c>
       <c r="V15">
-        <v>-7.0388184977054653</v>
+        <v>-1.500203127078684</v>
       </c>
       <c r="W15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X15" t="s">
         <v>47</v>
@@ -2534,22 +2576,25 @@
         <v>97</v>
       </c>
       <c r="Z15" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AA15" t="s">
-        <v>194</v>
+        <v>195</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
       </c>
       <c r="AC15">
         <v>0</v>
       </c>
       <c r="AD15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF15" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
@@ -2590,7 +2635,7 @@
         <v>1.687856337441241</v>
       </c>
       <c r="M16">
-        <v>480.98929824561401</v>
+        <v>27416.39</v>
       </c>
       <c r="N16">
         <v>112.2565775456774</v>
@@ -2611,13 +2656,13 @@
         <v>0</v>
       </c>
       <c r="T16">
-        <v>486.30717850283293</v>
+        <v>27307.74398893808</v>
       </c>
       <c r="U16">
-        <v>5.3178802572189738</v>
+        <v>108.6460110619191</v>
       </c>
       <c r="V16">
-        <v>-1.0935228786033631</v>
+        <v>0.39785787909074383</v>
       </c>
       <c r="W16" t="s">
         <v>30</v>
@@ -2629,10 +2674,13 @@
         <v>98</v>
       </c>
       <c r="Z16" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="AA16" t="s">
-        <v>195</v>
+        <v>196</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
       </c>
       <c r="AC16">
         <v>0</v>
@@ -2644,7 +2692,7 @@
         <v>1</v>
       </c>
       <c r="AF16" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.2">
@@ -2685,7 +2733,7 @@
         <v>1.5674812713082511</v>
       </c>
       <c r="M17">
-        <v>419.96980769230771</v>
+        <v>21838.43</v>
       </c>
       <c r="N17">
         <v>123.21825</v>
@@ -2706,13 +2754,13 @@
         <v>0</v>
       </c>
       <c r="T17">
-        <v>460.75509215263889</v>
+        <v>22651.966039408999</v>
       </c>
       <c r="U17">
-        <v>40.785284460331177</v>
+        <v>813.53603940899484</v>
       </c>
       <c r="V17">
-        <v>-8.8518358570456854</v>
+        <v>-3.5914588517113128</v>
       </c>
       <c r="W17" t="s">
         <v>29</v>
@@ -2724,10 +2772,13 @@
         <v>99</v>
       </c>
       <c r="Z17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AA17" t="s">
-        <v>196</v>
+        <v>197</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
       </c>
       <c r="AC17">
         <v>0</v>
@@ -2780,7 +2831,7 @@
         <v>1.8141773996612709</v>
       </c>
       <c r="M18">
-        <v>463.41732142857143</v>
+        <v>25951.37</v>
       </c>
       <c r="N18">
         <v>113.8683702764977</v>
@@ -2801,16 +2852,16 @@
         <v>0</v>
       </c>
       <c r="T18">
-        <v>479.03239702523382</v>
+        <v>26313.290939277231</v>
       </c>
       <c r="U18">
-        <v>15.61507559666234</v>
+        <v>361.92093927723539</v>
       </c>
       <c r="V18">
-        <v>-3.2597118052205118</v>
+        <v>-1.3754301585173621</v>
       </c>
       <c r="W18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X18" t="s">
         <v>50</v>
@@ -2819,19 +2870,22 @@
         <v>100</v>
       </c>
       <c r="Z18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AA18" t="s">
-        <v>197</v>
+        <v>198</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
       </c>
       <c r="AC18">
         <v>0</v>
       </c>
       <c r="AD18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF18" t="s">
         <v>232</v>
@@ -2875,7 +2929,7 @@
         <v>1.954093452843453</v>
       </c>
       <c r="M19">
-        <v>419.40603448275868</v>
+        <v>24325.55</v>
       </c>
       <c r="N19">
         <v>115.7116204545455</v>
@@ -2896,16 +2950,16 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <v>468.37674858222391</v>
+        <v>23845.643835502451</v>
       </c>
       <c r="U19">
-        <v>48.970714099465233</v>
+        <v>479.9061644975518</v>
       </c>
       <c r="V19">
-        <v>-10.45541100144265</v>
+        <v>2.0125527656462201</v>
       </c>
       <c r="W19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X19" t="s">
         <v>51</v>
@@ -2914,22 +2968,25 @@
         <v>101</v>
       </c>
       <c r="Z19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA19" t="s">
-        <v>198</v>
+        <v>199</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
       </c>
       <c r="AC19">
         <v>0</v>
       </c>
       <c r="AD19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF19" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.2">
@@ -2970,7 +3027,7 @@
         <v>1.4569887644110731</v>
       </c>
       <c r="M20">
-        <v>479.90549019607852</v>
+        <v>24475.18</v>
       </c>
       <c r="N20">
         <v>116.34891610803859</v>
@@ -2991,13 +3048,13 @@
         <v>0</v>
       </c>
       <c r="T20">
-        <v>471.58649911860653</v>
+        <v>24826.902848934769</v>
       </c>
       <c r="U20">
-        <v>8.318991077471992</v>
+        <v>351.72284893476899</v>
       </c>
       <c r="V20">
-        <v>1.7640435196979041</v>
+        <v>-1.4167004683383619</v>
       </c>
       <c r="W20" t="s">
         <v>30</v>
@@ -3009,10 +3066,13 @@
         <v>102</v>
       </c>
       <c r="Z20" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AA20" t="s">
-        <v>199</v>
+        <v>200</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
       </c>
       <c r="AC20">
         <v>0</v>
@@ -3024,7 +3084,7 @@
         <v>1</v>
       </c>
       <c r="AF20" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.2">
@@ -3065,7 +3125,7 @@
         <v>1.7529160276583931</v>
       </c>
       <c r="M21">
-        <v>471.23423076923092</v>
+        <v>24504.18</v>
       </c>
       <c r="N21">
         <v>120.900096874182</v>
@@ -3086,13 +3146,13 @@
         <v>0</v>
       </c>
       <c r="T21">
-        <v>462.66209917955229</v>
+        <v>24970.077785854901</v>
       </c>
       <c r="U21">
-        <v>8.57213158967852</v>
+        <v>465.8977858548933</v>
       </c>
       <c r="V21">
-        <v>1.852784484590297</v>
+        <v>-1.8658243272226249</v>
       </c>
       <c r="W21" t="s">
         <v>30</v>
@@ -3104,10 +3164,13 @@
         <v>103</v>
       </c>
       <c r="Z21" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AA21" t="s">
-        <v>200</v>
+        <v>201</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
       </c>
       <c r="AC21">
         <v>0</v>
@@ -3160,7 +3223,7 @@
         <v>1.564564126158329</v>
       </c>
       <c r="M22">
-        <v>505.72612244897971</v>
+        <v>24780.58</v>
       </c>
       <c r="N22">
         <v>114.711094916034</v>
@@ -3181,13 +3244,13 @@
         <v>0</v>
       </c>
       <c r="T22">
-        <v>497.26620496787899</v>
+        <v>25253.949886098992</v>
       </c>
       <c r="U22">
-        <v>8.4599174811006037</v>
+        <v>473.36988609898981</v>
       </c>
       <c r="V22">
-        <v>1.7012854275200691</v>
+        <v>-1.8744390015581509</v>
       </c>
       <c r="W22" t="s">
         <v>30</v>
@@ -3199,10 +3262,13 @@
         <v>104</v>
       </c>
       <c r="Z22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AA22" t="s">
-        <v>201</v>
+        <v>202</v>
+      </c>
+      <c r="AB22">
+        <v>0</v>
       </c>
       <c r="AC22">
         <v>0</v>
@@ -3255,7 +3321,7 @@
         <v>1.5389817729440369</v>
       </c>
       <c r="M23">
-        <v>508.16191489361711</v>
+        <v>23883.61</v>
       </c>
       <c r="N23">
         <v>140.24368777056279</v>
@@ -3276,16 +3342,16 @@
         <v>1</v>
       </c>
       <c r="T23">
-        <v>468.54965353951332</v>
+        <v>24048.665214311892</v>
       </c>
       <c r="U23">
-        <v>39.612261354103786</v>
+        <v>165.05521431189121</v>
       </c>
       <c r="V23">
-        <v>8.4542291419629123</v>
+        <v>-0.68633835949307975</v>
       </c>
       <c r="W23" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X23" t="s">
         <v>55</v>
@@ -3294,22 +3360,25 @@
         <v>105</v>
       </c>
       <c r="Z23" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="AA23" t="s">
-        <v>202</v>
+        <v>203</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
       </c>
       <c r="AC23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD23">
         <v>0</v>
       </c>
       <c r="AE23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF23" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.2">
@@ -3350,7 +3419,7 @@
         <v>1.897552587092435</v>
       </c>
       <c r="M24">
-        <v>386.83116666666672</v>
+        <v>23209.87</v>
       </c>
       <c r="N24">
         <v>124.4409357371795</v>
@@ -3371,16 +3440,16 @@
         <v>0</v>
       </c>
       <c r="T24">
-        <v>388.20087009726808</v>
+        <v>22138.43206772126</v>
       </c>
       <c r="U24">
-        <v>1.3697034306014191</v>
+        <v>1071.4379322787429</v>
       </c>
       <c r="V24">
-        <v>-0.35283368382410479</v>
+        <v>4.839719131875392</v>
       </c>
       <c r="W24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X24" t="s">
         <v>56</v>
@@ -3389,19 +3458,25 @@
         <v>106</v>
       </c>
       <c r="Z24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AA24" t="s">
-        <v>203</v>
+        <v>204</v>
+      </c>
+      <c r="AB24">
+        <v>0</v>
       </c>
       <c r="AC24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD24">
         <v>0</v>
       </c>
       <c r="AE24">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.2">
@@ -3442,7 +3517,7 @@
         <v>1.4431308008231081</v>
       </c>
       <c r="M25">
-        <v>426.5168000000001</v>
+        <v>21325.84</v>
       </c>
       <c r="N25">
         <v>110.7009294594295</v>
@@ -3463,13 +3538,13 @@
         <v>0</v>
       </c>
       <c r="T25">
-        <v>360.40514911672841</v>
+        <v>20491.057524434909</v>
       </c>
       <c r="U25">
-        <v>66.11165088327175</v>
+        <v>834.78247556509814</v>
       </c>
       <c r="V25">
-        <v>18.343703203269008</v>
+        <v>4.0738867409339301</v>
       </c>
       <c r="W25" t="s">
         <v>28</v>
@@ -3481,10 +3556,13 @@
         <v>107</v>
       </c>
       <c r="Z25" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AA25" t="s">
-        <v>204</v>
+        <v>205</v>
+      </c>
+      <c r="AB25">
+        <v>0</v>
       </c>
       <c r="AC25">
         <v>1</v>
@@ -3494,6 +3572,9 @@
       </c>
       <c r="AE25">
         <v>0</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.2">
@@ -3534,7 +3615,7 @@
         <v>1.711811629076512</v>
       </c>
       <c r="M26">
-        <v>375.48593220338978</v>
+        <v>22153.67</v>
       </c>
       <c r="N26">
         <v>128.2202876421824</v>
@@ -3555,13 +3636,13 @@
         <v>1</v>
       </c>
       <c r="T26">
-        <v>364.75399214930701</v>
+        <v>21171.329234802011</v>
       </c>
       <c r="U26">
-        <v>10.73194005408288</v>
+        <v>982.34076519799055</v>
       </c>
       <c r="V26">
-        <v>2.942240601904067</v>
+        <v>4.6399579086569203</v>
       </c>
       <c r="W26" t="s">
         <v>28</v>
@@ -3573,10 +3654,13 @@
         <v>108</v>
       </c>
       <c r="Z26" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AA26" t="s">
-        <v>205</v>
+        <v>206</v>
+      </c>
+      <c r="AB26">
+        <v>0</v>
       </c>
       <c r="AC26">
         <v>1</v>
@@ -3586,6 +3670,9 @@
       </c>
       <c r="AE26">
         <v>0</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.2">
@@ -3626,7 +3713,7 @@
         <v>1.875067866915693</v>
       </c>
       <c r="M27">
-        <v>485.51577777777783</v>
+        <v>21848.21</v>
       </c>
       <c r="N27">
         <v>140.40672752787339</v>
@@ -3647,16 +3734,16 @@
         <v>0</v>
       </c>
       <c r="T27">
-        <v>485.47100600739282</v>
+        <v>22690.597292529499</v>
       </c>
       <c r="U27">
-        <v>4.4771770385011678E-2</v>
+        <v>842.38729252949634</v>
       </c>
       <c r="V27">
-        <v>9.2223366238126884E-3</v>
+        <v>-3.7124950113448021</v>
       </c>
       <c r="W27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X27" t="s">
         <v>59</v>
@@ -3665,22 +3752,25 @@
         <v>109</v>
       </c>
       <c r="Z27" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AA27" t="s">
-        <v>206</v>
+        <v>207</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
       </c>
       <c r="AC27">
         <v>0</v>
       </c>
       <c r="AD27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF27" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.2">
@@ -3721,7 +3811,7 @@
         <v>1.8164579919252031</v>
       </c>
       <c r="M28">
-        <v>702.78854545454556</v>
+        <v>38653.370000000003</v>
       </c>
       <c r="N28">
         <v>133.91088395922961</v>
@@ -3742,13 +3832,13 @@
         <v>0</v>
       </c>
       <c r="T28">
-        <v>698.3836370446196</v>
+        <v>38796.276212906829</v>
       </c>
       <c r="U28">
-        <v>4.4049084099259517</v>
+        <v>142.90621290682611</v>
       </c>
       <c r="V28">
-        <v>0.63072904006834896</v>
+        <v>-0.36835033373456538</v>
       </c>
       <c r="W28" t="s">
         <v>30</v>
@@ -3760,10 +3850,13 @@
         <v>110</v>
       </c>
       <c r="Z28" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AA28" t="s">
-        <v>207</v>
+        <v>208</v>
+      </c>
+      <c r="AB28">
+        <v>0</v>
       </c>
       <c r="AC28">
         <v>0</v>
@@ -3775,7 +3868,7 @@
         <v>1</v>
       </c>
       <c r="AF28" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.2">
@@ -3816,7 +3909,7 @@
         <v>1.4220969821832989</v>
       </c>
       <c r="M29">
-        <v>800.2168085106382</v>
+        <v>37610.19</v>
       </c>
       <c r="N29">
         <v>131.8084032963564</v>
@@ -3837,13 +3930,13 @@
         <v>0</v>
       </c>
       <c r="T29">
-        <v>798.22121562182349</v>
+        <v>37340.163773614542</v>
       </c>
       <c r="U29">
-        <v>1.995592888814713</v>
+        <v>270.0262263854529</v>
       </c>
       <c r="V29">
-        <v>0.25000499232034612</v>
+        <v>0.72315222831523829</v>
       </c>
       <c r="W29" t="s">
         <v>30</v>
@@ -3855,10 +3948,13 @@
         <v>111</v>
       </c>
       <c r="Z29" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AA29" t="s">
-        <v>208</v>
+        <v>209</v>
+      </c>
+      <c r="AB29">
+        <v>0</v>
       </c>
       <c r="AC29">
         <v>0</v>
@@ -3911,7 +4007,7 @@
         <v>1.489966456210964</v>
       </c>
       <c r="M30">
-        <v>829.50142857142839</v>
+        <v>40645.569999999992</v>
       </c>
       <c r="N30">
         <v>121.88595493964461</v>
@@ -3932,16 +4028,16 @@
         <v>0</v>
       </c>
       <c r="T30">
-        <v>790.77723143307549</v>
+        <v>41024.865235751036</v>
       </c>
       <c r="U30">
-        <v>38.724197138352913</v>
+        <v>379.29523575105122</v>
       </c>
       <c r="V30">
-        <v>4.8969792754623827</v>
+        <v>-0.92454962026423693</v>
       </c>
       <c r="W30" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X30" t="s">
         <v>62</v>
@@ -3950,22 +4046,25 @@
         <v>112</v>
       </c>
       <c r="Z30" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AA30" t="s">
-        <v>209</v>
+        <v>210</v>
+      </c>
+      <c r="AB30">
+        <v>0</v>
       </c>
       <c r="AC30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD30">
         <v>0</v>
       </c>
       <c r="AE30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF30" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.2">
@@ -4006,7 +4105,7 @@
         <v>1.5812402632504361</v>
       </c>
       <c r="M31">
-        <v>924.81</v>
+        <v>43466.07</v>
       </c>
       <c r="N31">
         <v>129.37215610516941</v>
@@ -4027,13 +4126,13 @@
         <v>0</v>
       </c>
       <c r="T31">
-        <v>868.43323086281384</v>
+        <v>42193.579248959257</v>
       </c>
       <c r="U31">
-        <v>56.376769137186102</v>
+        <v>1272.4907510407361</v>
       </c>
       <c r="V31">
-        <v>6.49177934856018</v>
+        <v>3.0158397881642678</v>
       </c>
       <c r="W31" t="s">
         <v>28</v>
@@ -4045,10 +4144,13 @@
         <v>113</v>
       </c>
       <c r="Z31" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AA31" t="s">
-        <v>210</v>
+        <v>211</v>
+      </c>
+      <c r="AB31">
+        <v>0</v>
       </c>
       <c r="AC31">
         <v>1</v>
@@ -4060,7 +4162,7 @@
         <v>0</v>
       </c>
       <c r="AF31" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.2">
@@ -4101,7 +4203,7 @@
         <v>1.3808061834359411</v>
       </c>
       <c r="M32">
-        <v>936.08660000000009</v>
+        <v>46804.33</v>
       </c>
       <c r="N32">
         <v>132.40123745331459</v>
@@ -4122,16 +4224,16 @@
         <v>0</v>
       </c>
       <c r="T32">
-        <v>901.76366041011761</v>
+        <v>46176.110479082039</v>
       </c>
       <c r="U32">
-        <v>34.322939589882481</v>
+        <v>628.21952091796265</v>
       </c>
       <c r="V32">
-        <v>3.806201236172301</v>
+        <v>1.360486005426006</v>
       </c>
       <c r="W32" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X32" t="s">
         <v>64</v>
@@ -4140,22 +4242,25 @@
         <v>114</v>
       </c>
       <c r="Z32" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AA32" t="s">
-        <v>211</v>
+        <v>212</v>
+      </c>
+      <c r="AB32">
+        <v>0</v>
       </c>
       <c r="AC32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD32">
         <v>0</v>
       </c>
       <c r="AE32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF32" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.2">
@@ -4196,7 +4301,7 @@
         <v>1.433169152353416</v>
       </c>
       <c r="M33">
-        <v>963.9997826086958</v>
+        <v>44343.990000000013</v>
       </c>
       <c r="N33">
         <v>126.123031419165</v>
@@ -4217,13 +4322,13 @@
         <v>0</v>
       </c>
       <c r="T33">
-        <v>934.51890862297739</v>
+        <v>43190.487210260151</v>
       </c>
       <c r="U33">
-        <v>29.4808739857184</v>
+        <v>1153.5027897398541</v>
       </c>
       <c r="V33">
-        <v>3.154657836635832</v>
+        <v>2.6707334513833239</v>
       </c>
       <c r="W33" t="s">
         <v>28</v>
@@ -4235,10 +4340,13 @@
         <v>115</v>
       </c>
       <c r="Z33" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AA33" t="s">
-        <v>212</v>
+        <v>213</v>
+      </c>
+      <c r="AB33">
+        <v>0</v>
       </c>
       <c r="AC33">
         <v>1</v>
@@ -4250,7 +4358,7 @@
         <v>0</v>
       </c>
       <c r="AF33" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.2">
@@ -4291,7 +4399,7 @@
         <v>1.1003059032470801</v>
       </c>
       <c r="M34">
-        <v>774.85739130434808</v>
+        <v>35643.44000000001</v>
       </c>
       <c r="N34">
         <v>131.2974445696461</v>
@@ -4312,13 +4420,13 @@
         <v>0</v>
       </c>
       <c r="T34">
-        <v>830.18990013976349</v>
+        <v>38152.536431429631</v>
       </c>
       <c r="U34">
-        <v>55.33250883541541</v>
+        <v>2509.096431429622</v>
       </c>
       <c r="V34">
-        <v>-6.6650423988656229</v>
+        <v>-6.5764865618807358</v>
       </c>
       <c r="W34" t="s">
         <v>29</v>
@@ -4330,10 +4438,13 @@
         <v>116</v>
       </c>
       <c r="Z34" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AA34" t="s">
-        <v>213</v>
+        <v>214</v>
+      </c>
+      <c r="AB34">
+        <v>0</v>
       </c>
       <c r="AC34">
         <v>0</v>
@@ -4345,7 +4456,7 @@
         <v>0</v>
       </c>
       <c r="AF34" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.2">
@@ -4386,7 +4497,7 @@
         <v>1.398052712623856</v>
       </c>
       <c r="M35">
-        <v>689.20877551020396</v>
+        <v>33771.230000000003</v>
       </c>
       <c r="N35">
         <v>129.33523095238101</v>
@@ -4407,16 +4518,16 @@
         <v>0</v>
       </c>
       <c r="T35">
-        <v>683.11230959206171</v>
+        <v>32776.518107042393</v>
       </c>
       <c r="U35">
-        <v>6.0964659181422576</v>
+        <v>994.71189295760269</v>
       </c>
       <c r="V35">
-        <v>0.89245440794104869</v>
+        <v>3.034830880171735</v>
       </c>
       <c r="W35" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X35" t="s">
         <v>67</v>
@@ -4425,22 +4536,25 @@
         <v>117</v>
       </c>
       <c r="Z35" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AA35" t="s">
-        <v>214</v>
+        <v>215</v>
+      </c>
+      <c r="AB35">
+        <v>0</v>
       </c>
       <c r="AC35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD35">
         <v>0</v>
       </c>
       <c r="AE35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF35" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.2">
@@ -4481,7 +4595,7 @@
         <v>1.0919104209282779</v>
       </c>
       <c r="M36">
-        <v>652.84040816326535</v>
+        <v>31989.18</v>
       </c>
       <c r="N36">
         <v>119.4754328453953</v>
@@ -4502,13 +4616,13 @@
         <v>0</v>
       </c>
       <c r="T36">
-        <v>659.43863895535731</v>
+        <v>32184.707484431619</v>
       </c>
       <c r="U36">
-        <v>6.5982307920919538</v>
+        <v>195.52748443161909</v>
       </c>
       <c r="V36">
-        <v>-1.000582981085923</v>
+        <v>-0.60751673609648182</v>
       </c>
       <c r="W36" t="s">
         <v>30</v>
@@ -4520,10 +4634,13 @@
         <v>118</v>
       </c>
       <c r="Z36" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AA36" t="s">
-        <v>215</v>
+        <v>216</v>
+      </c>
+      <c r="AB36">
+        <v>0</v>
       </c>
       <c r="AC36">
         <v>0</v>
@@ -4535,7 +4652,7 @@
         <v>1</v>
       </c>
       <c r="AF36" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:32" x14ac:dyDescent="0.2">
@@ -4576,7 +4693,7 @@
         <v>0.80705564455029088</v>
       </c>
       <c r="M37">
-        <v>602.83479999999997</v>
+        <v>30141.74</v>
       </c>
       <c r="N37">
         <v>133.4672717994271</v>
@@ -4597,16 +4714,16 @@
         <v>0</v>
       </c>
       <c r="T37">
-        <v>660.97949744635025</v>
+        <v>30586.349653224421</v>
       </c>
       <c r="U37">
-        <v>58.144697446350278</v>
+        <v>444.60965322442638</v>
       </c>
       <c r="V37">
-        <v>-8.7967475044216048</v>
+        <v>-1.4536211684795</v>
       </c>
       <c r="W37" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X37" t="s">
         <v>69</v>
@@ -4615,22 +4732,25 @@
         <v>119</v>
       </c>
       <c r="Z37" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AA37" t="s">
-        <v>216</v>
+        <v>217</v>
+      </c>
+      <c r="AB37">
+        <v>0</v>
       </c>
       <c r="AC37">
         <v>0</v>
       </c>
       <c r="AD37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF37" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.2">
@@ -4671,7 +4791,7 @@
         <v>0.78116826578056542</v>
       </c>
       <c r="M38">
-        <v>593.67538461538459</v>
+        <v>30871.119999999999</v>
       </c>
       <c r="N38">
         <v>125.80320453431371</v>
@@ -4692,16 +4812,16 @@
         <v>0</v>
       </c>
       <c r="T38">
-        <v>638.85803762125056</v>
+        <v>31407.50223745139</v>
       </c>
       <c r="U38">
-        <v>45.182653005865973</v>
+        <v>536.38223745139476</v>
       </c>
       <c r="V38">
-        <v>-7.0724089461409703</v>
+        <v>-1.70781564670811</v>
       </c>
       <c r="W38" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X38" t="s">
         <v>70</v>
@@ -4710,22 +4830,25 @@
         <v>120</v>
       </c>
       <c r="Z38" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AA38" t="s">
-        <v>217</v>
+        <v>218</v>
+      </c>
+      <c r="AB38">
+        <v>0</v>
       </c>
       <c r="AC38">
         <v>0</v>
       </c>
       <c r="AD38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF38" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:32" x14ac:dyDescent="0.2">
@@ -4766,7 +4889,7 @@
         <v>0.75050874540375134</v>
       </c>
       <c r="M39">
-        <v>637.61477272727268</v>
+        <v>28055.05</v>
       </c>
       <c r="N39">
         <v>121.97405311995399</v>
@@ -4787,13 +4910,13 @@
         <v>0</v>
       </c>
       <c r="T39">
-        <v>641.46614639548523</v>
+        <v>28554.15093705208</v>
       </c>
       <c r="U39">
-        <v>3.851373668212545</v>
+        <v>499.10093705208061</v>
       </c>
       <c r="V39">
-        <v>-0.60040170316923402</v>
+        <v>-1.747910271092822</v>
       </c>
       <c r="W39" t="s">
         <v>30</v>
@@ -4805,10 +4928,13 @@
         <v>121</v>
       </c>
       <c r="Z39" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AA39" t="s">
-        <v>218</v>
+        <v>219</v>
+      </c>
+      <c r="AB39">
+        <v>0</v>
       </c>
       <c r="AC39">
         <v>0</v>
@@ -4820,7 +4946,7 @@
         <v>1</v>
       </c>
       <c r="AF39" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:32" x14ac:dyDescent="0.2">
@@ -4861,7 +4987,7 @@
         <v>0.78448032551647395</v>
       </c>
       <c r="M40">
-        <v>547.64326923076919</v>
+        <v>28477.45</v>
       </c>
       <c r="N40">
         <v>118.8923114041113</v>
@@ -4882,16 +5008,16 @@
         <v>0</v>
       </c>
       <c r="T40">
-        <v>583.5023870701425</v>
+        <v>28216.379047717619</v>
       </c>
       <c r="U40">
-        <v>35.859117839373312</v>
+        <v>261.07095228237807</v>
       </c>
       <c r="V40">
-        <v>-6.1454963396855318</v>
+        <v>0.92524611978338067</v>
       </c>
       <c r="W40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X40" t="s">
         <v>72</v>
@@ -4900,22 +5026,25 @@
         <v>122</v>
       </c>
       <c r="Z40" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AA40" t="s">
-        <v>219</v>
+        <v>220</v>
+      </c>
+      <c r="AB40">
+        <v>0</v>
       </c>
       <c r="AC40">
         <v>0</v>
       </c>
       <c r="AD40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF40" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.2">
@@ -4956,7 +5085,7 @@
         <v>0.84139516557590044</v>
       </c>
       <c r="M41">
-        <v>609.58519999999999</v>
+        <v>30479.26</v>
       </c>
       <c r="N41">
         <v>129.8005284362103</v>
@@ -4977,13 +5106,13 @@
         <v>0</v>
       </c>
       <c r="T41">
-        <v>612.95471875887279</v>
+        <v>30268.937007555691</v>
       </c>
       <c r="U41">
-        <v>3.3695187588727999</v>
+        <v>210.32299244431491</v>
       </c>
       <c r="V41">
-        <v>-0.54971740256694535</v>
+        <v>0.69484763337349553</v>
       </c>
       <c r="W41" t="s">
         <v>30</v>
@@ -4995,10 +5124,13 @@
         <v>123</v>
       </c>
       <c r="Z41" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AA41" t="s">
-        <v>220</v>
+        <v>221</v>
+      </c>
+      <c r="AB41">
+        <v>0</v>
       </c>
       <c r="AC41">
         <v>0</v>
@@ -5010,7 +5142,7 @@
         <v>1</v>
       </c>
       <c r="AF41" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="1:32" x14ac:dyDescent="0.2">
@@ -5051,7 +5183,7 @@
         <v>0.98196703296703292</v>
       </c>
       <c r="M42">
-        <v>482.13404255319148</v>
+        <v>22660.3</v>
       </c>
       <c r="N42">
         <v>126.4523151587302</v>
@@ -5072,13 +5204,13 @@
         <v>0</v>
       </c>
       <c r="T42">
-        <v>541.93904152517803</v>
+        <v>23729.71013905355</v>
       </c>
       <c r="U42">
-        <v>59.804998971986549</v>
+        <v>1069.4101390535541</v>
       </c>
       <c r="V42">
-        <v>-11.03537379474958</v>
+        <v>-4.5066295912884131</v>
       </c>
       <c r="W42" t="s">
         <v>29</v>
@@ -5090,10 +5222,13 @@
         <v>124</v>
       </c>
       <c r="Z42" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AA42" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="AB42">
+        <v>0</v>
       </c>
       <c r="AC42">
         <v>0</v>
@@ -5105,7 +5240,7 @@
         <v>0</v>
       </c>
       <c r="AF42" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.2">
@@ -5146,7 +5281,7 @@
         <v>1.0177159916882159</v>
       </c>
       <c r="M43">
-        <v>747.84285714285716</v>
+        <v>36644.300000000003</v>
       </c>
       <c r="N43">
         <v>131.48980277429931</v>
@@ -5167,13 +5302,13 @@
         <v>1</v>
       </c>
       <c r="T43">
-        <v>759.8722049040822</v>
+        <v>35846.078485092417</v>
       </c>
       <c r="U43">
-        <v>12.02934776122504</v>
+        <v>798.22151490758552</v>
       </c>
       <c r="V43">
-        <v>-1.583075112313588</v>
+        <v>2.2268028990662061</v>
       </c>
       <c r="W43" t="s">
         <v>30</v>
@@ -5185,10 +5320,13 @@
         <v>125</v>
       </c>
       <c r="Z43" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AA43" t="s">
-        <v>222</v>
+        <v>223</v>
+      </c>
+      <c r="AB43">
+        <v>0</v>
       </c>
       <c r="AC43">
         <v>0</v>
@@ -5200,7 +5338,7 @@
         <v>1</v>
       </c>
       <c r="AF43" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.2">
@@ -5241,7 +5379,7 @@
         <v>0.84694928517251544</v>
       </c>
       <c r="M44">
-        <v>662.73450980392158</v>
+        <v>33799.46</v>
       </c>
       <c r="N44">
         <v>135.9959574857314</v>
@@ -5262,16 +5400,16 @@
         <v>0</v>
       </c>
       <c r="T44">
-        <v>684.11043506089743</v>
+        <v>34450.023029103912</v>
       </c>
       <c r="U44">
-        <v>21.375925256975851</v>
+        <v>650.56302910391241</v>
       </c>
       <c r="V44">
-        <v>-3.1246307849511208</v>
+        <v>-1.8884255274787669</v>
       </c>
       <c r="W44" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X44" t="s">
         <v>76</v>
@@ -5280,22 +5418,25 @@
         <v>126</v>
       </c>
       <c r="Z44" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AA44" t="s">
-        <v>223</v>
+        <v>224</v>
+      </c>
+      <c r="AB44">
+        <v>0</v>
       </c>
       <c r="AC44">
         <v>0</v>
       </c>
       <c r="AD44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF44" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.2">
@@ -5336,7 +5477,7 @@
         <v>1.1043983617877779</v>
       </c>
       <c r="M45">
-        <v>571.54083333333335</v>
+        <v>27433.96</v>
       </c>
       <c r="N45">
         <v>115.25504762490159</v>
@@ -5357,16 +5498,16 @@
         <v>0</v>
       </c>
       <c r="T45">
-        <v>533.31350448947137</v>
+        <v>26971.632663918779</v>
       </c>
       <c r="U45">
-        <v>38.227328843861983</v>
+        <v>462.32733608122362</v>
       </c>
       <c r="V45">
-        <v>7.167890653820236</v>
+        <v>1.714124398185582</v>
       </c>
       <c r="W45" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X45" t="s">
         <v>77</v>
@@ -5375,22 +5516,25 @@
         <v>127</v>
       </c>
       <c r="Z45" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AA45" t="s">
-        <v>224</v>
+        <v>225</v>
+      </c>
+      <c r="AB45">
+        <v>0</v>
       </c>
       <c r="AC45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD45">
         <v>0</v>
       </c>
       <c r="AE45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF45" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.2">
@@ -5431,7 +5575,7 @@
         <v>0.86826743872779688</v>
       </c>
       <c r="M46">
-        <v>711.24166666666656</v>
+        <v>29872.149999999991</v>
       </c>
       <c r="N46">
         <v>126.1720277724726</v>
@@ -5452,16 +5596,16 @@
         <v>1</v>
       </c>
       <c r="T46">
-        <v>684.26240212498772</v>
+        <v>29790.650007857661</v>
       </c>
       <c r="U46">
-        <v>26.979264541678841</v>
+        <v>81.499992142329575</v>
       </c>
       <c r="V46">
-        <v>3.942824340179194</v>
+        <v>0.27357574313025362</v>
       </c>
       <c r="W46" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X46" t="s">
         <v>78</v>
@@ -5470,22 +5614,25 @@
         <v>128</v>
       </c>
       <c r="Z46" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AA46" t="s">
-        <v>225</v>
+        <v>226</v>
+      </c>
+      <c r="AB46">
+        <v>0</v>
       </c>
       <c r="AC46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD46">
         <v>0</v>
       </c>
       <c r="AE46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF46" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.2">
@@ -5526,7 +5673,7 @@
         <v>1.1934800318728891</v>
       </c>
       <c r="M47">
-        <v>656.26604166666664</v>
+        <v>31500.77</v>
       </c>
       <c r="N47">
         <v>127.71092864635359</v>
@@ -5547,13 +5694,13 @@
         <v>0</v>
       </c>
       <c r="T47">
-        <v>604.84194149230359</v>
+        <v>30524.605354269039</v>
       </c>
       <c r="U47">
-        <v>51.424100174363048</v>
+        <v>976.164645730958</v>
       </c>
       <c r="V47">
-        <v>8.502072466649107</v>
+        <v>3.1979599225004751</v>
       </c>
       <c r="W47" t="s">
         <v>28</v>
@@ -5565,10 +5712,13 @@
         <v>129</v>
       </c>
       <c r="Z47" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AA47" t="s">
-        <v>226</v>
+        <v>227</v>
+      </c>
+      <c r="AB47">
+        <v>0</v>
       </c>
       <c r="AC47">
         <v>1</v>
@@ -5580,7 +5730,7 @@
         <v>0</v>
       </c>
       <c r="AF47" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.2">
@@ -5621,7 +5771,7 @@
         <v>1.028220732806618</v>
       </c>
       <c r="M48">
-        <v>657.98579999999993</v>
+        <v>32899.289999999994</v>
       </c>
       <c r="N48">
         <v>128.19902998366831</v>
@@ -5642,16 +5792,16 @@
         <v>1</v>
       </c>
       <c r="T48">
-        <v>676.64590362388924</v>
+        <v>32554.80563602992</v>
       </c>
       <c r="U48">
-        <v>18.660103623889309</v>
+        <v>344.48436397007032</v>
       </c>
       <c r="V48">
-        <v>-2.7577354010350219</v>
+        <v>1.058167472481585</v>
       </c>
       <c r="W48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X48" t="s">
         <v>80</v>
@@ -5660,25 +5810,28 @@
         <v>130</v>
       </c>
       <c r="Z48" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AA48" t="s">
-        <v>227</v>
+        <v>228</v>
+      </c>
+      <c r="AB48">
+        <v>0</v>
       </c>
       <c r="AC48">
         <v>0</v>
       </c>
       <c r="AD48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF48" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>33</v>
       </c>
@@ -5716,7 +5869,7 @@
         <v>1.0153909865644559</v>
       </c>
       <c r="M49">
-        <v>605.83739130434788</v>
+        <v>27868.52</v>
       </c>
       <c r="N49">
         <v>120.3165731768232</v>
@@ -5737,13 +5890,13 @@
         <v>0</v>
       </c>
       <c r="T49">
-        <v>555.71056737743709</v>
+        <v>27090.25865815402</v>
       </c>
       <c r="U49">
-        <v>50.126823926910788</v>
+        <v>778.26134184598413</v>
       </c>
       <c r="V49">
-        <v>9.0203114480032536</v>
+        <v>2.8728457401115728</v>
       </c>
       <c r="W49" t="s">
         <v>28</v>
@@ -5755,10 +5908,13 @@
         <v>131</v>
       </c>
       <c r="Z49" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="AA49" t="s">
-        <v>228</v>
+        <v>229</v>
+      </c>
+      <c r="AB49">
+        <v>0</v>
       </c>
       <c r="AC49">
         <v>1</v>
@@ -5769,8 +5925,11 @@
       <c r="AE49">
         <v>0</v>
       </c>
+      <c r="AF49" t="s">
+        <v>233</v>
+      </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>33</v>
       </c>
@@ -5808,7 +5967,7 @@
         <v>0.77387011432965125</v>
       </c>
       <c r="M50">
-        <v>732.28818181818178</v>
+        <v>32220.68</v>
       </c>
       <c r="N50">
         <v>129.1729718697479</v>
@@ -5829,16 +5988,16 @@
         <v>0</v>
       </c>
       <c r="T50">
-        <v>710.61262759001636</v>
+        <v>32035.369408812341</v>
       </c>
       <c r="U50">
-        <v>21.675554228165421</v>
+        <v>185.31059118765549</v>
       </c>
       <c r="V50">
-        <v>3.0502630246912812</v>
+        <v>0.57845623324287299</v>
       </c>
       <c r="W50" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X50" t="s">
         <v>82</v>
@@ -5847,22 +6006,28 @@
         <v>132</v>
       </c>
       <c r="Z50" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="AA50" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="AB50">
+        <v>0</v>
       </c>
       <c r="AC50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD50">
         <v>0</v>
       </c>
       <c r="AE50">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AF50" t="s">
+        <v>233</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>33</v>
       </c>
@@ -5900,7 +6065,7 @@
         <v>1.0371377640225059</v>
       </c>
       <c r="M51">
-        <v>627.00152173913034</v>
+        <v>28842.07</v>
       </c>
       <c r="N51">
         <v>117.5989579804254</v>
@@ -5921,16 +6086,16 @@
         <v>0</v>
       </c>
       <c r="T51">
-        <v>603.55014242148559</v>
+        <v>28796.79492842947</v>
       </c>
       <c r="U51">
-        <v>23.451379317644751</v>
+        <v>45.275071570522407</v>
       </c>
       <c r="V51">
-        <v>3.8855726590596391</v>
+        <v>0.15722260648467121</v>
       </c>
       <c r="W51" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X51" t="s">
         <v>83</v>
@@ -5939,19 +6104,25 @@
         <v>133</v>
       </c>
       <c r="Z51" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AA51" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="AB51">
+        <v>0</v>
       </c>
       <c r="AC51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD51">
         <v>0</v>
       </c>
       <c r="AE51">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AF51" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: update revenue-data.xlsx and revenue-data.json with latest source data
</commit_message>
<xml_diff>
--- a/data/revenue-data.xlsx
+++ b/data/revenue-data.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/Revenue_Performance_Analysis-2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBF62DE9-AD94-DF4E-A8BB-71BE738FAABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022A7EE7-A23A-8C47-92C7-19A524857A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="22460" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="760" windowWidth="27400" windowHeight="17060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AF$51</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -1091,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="S1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1254,7 +1257,7 @@
         <v>76.159937464899969</v>
       </c>
       <c r="J2">
-        <v>0.44318163325504012</v>
+        <v>0.44318163325504001</v>
       </c>
       <c r="K2">
         <v>0.43977253413911249</v>
@@ -6126,6 +6129,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AF51" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change source column for Missed/Gained Revenue chart from 'Missed Revenue (RF)' to 'Missed Revenue'
</commit_message>
<xml_diff>
--- a/data/revenue-data.xlsx
+++ b/data/revenue-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/Revenue_Performance_Analysis-2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2B67BA3-7C41-7640-9AF6-0E269E51C9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{719E12F6-5A35-5A43-B9DB-6F97609CF138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="760" windowWidth="25800" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="21340" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="286">
   <si>
     <t>Year</t>
   </si>
@@ -76,13 +76,13 @@
     <t>Payment Amount*</t>
   </si>
   <si>
-    <t>Expected Payments (RF)</t>
-  </si>
-  <si>
-    <t>Missed Revenue (RF)</t>
-  </si>
-  <si>
-    <t>% Error (RF)</t>
+    <t>Expected Payments</t>
+  </si>
+  <si>
+    <t>Missed Revenue</t>
+  </si>
+  <si>
+    <t>% Error</t>
   </si>
   <si>
     <t>Performance Diagnostic</t>
@@ -283,226 +283,226 @@
     <t>4-MEDICAID – Non E/M Code Visit Count increased from avg 1.08 to 2.00; 13-TRICARE – Existing E/M Code Procedure per Visit increased from avg 0.03 to 0.25; 15-UNITED HEALTHCARE – Existing E/M Code Procedure per Visit increased from avg 0.01 to 0.08; 3-MEDICARE – New E/M Code % of Visits w Radiology increased from avg 0.09 to 0.50; 17-AETNA – New E/M Code Procedure per Visit increased from avg 0.03 to 0.17; 4-MEDICAID – Non E/M Code Charge Amount increased from avg 76.92 to 231.00</t>
   </si>
   <si>
-    <t>12-HUMANA – New E/M Code Visit Count decreased from avg 2.13 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 3-MEDICARE – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 3-MEDICARE – New E/M Code Labs per Visit decreased from avg 0.75 to 0.00</t>
-  </si>
-  <si>
-    <t>12-HUMANA – New E/M Code Visit Count decreased from avg 2.13 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 4-MEDICAID – Existing E/M Code % of Visits w Radiology decreased from avg 0.08 to 0.00; 3-MEDICARE – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Non E/M Code Visit Count decreased from avg 13.04 to 3.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
-  </si>
-  <si>
-    <t>13-TRICARE – New E/M Code Visit Count decreased from avg 3.29 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 3-MEDICARE – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Non E/M Code Visit Count decreased from avg 13.04 to 6.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 3-MEDICARE – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – New E/M Code Visit Count decreased from avg 2.58 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code Labs per Visit decreased from avg 1.28 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Visit Count decreased from avg 3.24 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 4-MEDICAID – Non E/M Code Labs per Visit decreased from avg 0.23 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – New E/M Code Visit Count decreased from avg 17.98 to 9.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code Labs per Visit decreased from avg 1.28 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Visit Count decreased from avg 5.54 to 1.00; 5-COMMERCIAL – Non E/M Code Labs per Visit decreased from avg 0.33 to 0.00; 5-COMMERCIAL – Non E/M Code Charge Amount decreased from avg 83.67 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Visit Count decreased from avg 5.54 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code Labs per Visit decreased from avg 1.07 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 4-MEDICAID – Non E/M Code Labs per Visit decreased from avg 0.23 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Existing E/M Code Visit Count decreased from avg 6.16 to 1.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 3-MEDICARE – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 3-MEDICARE – Existing E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 18-CIGNA – Non E/M Code Labs per Visit decreased from avg 0.33 to 0.00; 18-CIGNA – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
-  </si>
-  <si>
-    <t>13-TRICARE – Existing E/M Code Visit Count decreased from avg 2.52 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 4-MEDICAID – Non E/M Code Labs per Visit decreased from avg 0.23 to 0.00; 4-MEDICAID – Non E/M Code Charge Amount decreased from avg 76.92 to 0.00</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Visit Count decreased from avg 4.48 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code Labs per Visit decreased from avg 1.28 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – Non E/M Code Charge Amount decreased from avg 76.92 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Visit Count decreased from avg 5.54 to 2.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Visit Count decreased from avg 5.54 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code Labs per Visit decreased from avg 1.28 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00</t>
-  </si>
-  <si>
-    <t>18-CIGNA – New E/M Code Visit Count decreased from avg 6.54 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – New E/M Code % of Visits w Radiology decreased from avg 0.08 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Visit Count decreased from avg 4.48 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – New E/M Code Visit Count decreased from avg 15.44 to 5.00; 5-COMMERCIAL – Non E/M Code Labs per Visit decreased from avg 0.33 to 0.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code Labs per Visit decreased from avg 1.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – New E/M Code Visit Count decreased from avg 8.71 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code Labs per Visit decreased from avg 1.28 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Visit Count decreased from avg 3.24 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – New E/M Code % of Visits w Radiology decreased from avg 0.08 to 0.00</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – New E/M Code Visit Count decreased from avg 15.44 to 6.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – New E/M Code % of Visits w Radiology decreased from avg 0.08 to 0.00; 4-MEDICAID – Existing E/M Code % of Visits w Radiology decreased from avg 0.08 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Visit Count decreased from avg 10.08 to 2.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code Labs per Visit decreased from avg 1.07 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 4-MEDICAID – Existing E/M Code % of Visits w Radiology decreased from avg 0.08 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – New E/M Code Visit Count decreased from avg 8.71 to 2.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 3-MEDICARE – New E/M Code % of Visits w Radiology decreased from avg 0.09 to 0.00; 3-MEDICARE – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – New E/M Code Visit Count decreased from avg 8.71 to 2.00; 5-COMMERCIAL – New E/M Code Labs per Visit decreased from avg 1.07 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 4-MEDICAID – Non E/M Code Labs per Visit decreased from avg 0.23 to 0.00; 4-MEDICAID – Non E/M Code Charge Amount decreased from avg 76.92 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Code Visit Count decreased from avg 11.12 to 2.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code Labs per Visit decreased from avg 1.07 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Visit Count decreased from avg 3.24 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – Non E/M Code Labs per Visit decreased from avg 0.23 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Existing E/M Code Visit Count decreased from avg 2.46 to 1.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – New E/M Code % of Visits w Radiology decreased from avg 0.08 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 3-MEDICARE – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – New E/M Code Visit Count decreased from avg 17.98 to 10.00; 5-COMMERCIAL – New E/M Code Labs per Visit decreased from avg 1.07 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – New E/M Code % of Visits w Radiology decreased from avg 0.08 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
-  </si>
-  <si>
-    <t>12-HUMANA – New E/M Code Visit Count decreased from avg 2.13 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 3-MEDICARE – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 3-MEDICARE – New E/M Code % of Visits w Radiology decreased from avg 0.09 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – New E/M Code Visit Count decreased from avg 2.45 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 4-MEDICAID – New E/M Code % of Visits w Radiology decreased from avg 0.08 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 3-MEDICARE – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 3-MEDICARE – New E/M Code % of Visits w Radiology decreased from avg 0.09 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Existing E/M Code Visit Count decreased from avg 2.46 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Existing E/M Code Visit Count decreased from avg 6.16 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code Labs per Visit decreased from avg 1.28 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Visit Count decreased from avg 3.24 to 1.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 4-MEDICAID – New E/M Code % of Visits w Radiology decreased from avg 0.08 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 3-MEDICARE – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 3-MEDICARE – New E/M Code % of Visits w Radiology decreased from avg 0.09 to 0.00</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – New E/M Code Visit Count decreased from avg 15.44 to 9.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Visit Count decreased from avg 3.24 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 4-MEDICAID – Non E/M Code Charge Amount decreased from avg 76.92 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 4-MEDICAID – Existing E/M Code % of Visits w Radiology decreased from avg 0.08 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – New E/M Code Visit Count decreased from avg 2.45 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code Labs per Visit decreased from avg 1.07 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code Labs per Visit decreased from avg 1.28 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00</t>
-  </si>
-  <si>
-    <t>12-HUMANA – New E/M Code Visit Count decreased from avg 2.13 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Visit Count decreased from avg 3.24 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 3-MEDICARE – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 3-MEDICARE – New E/M Code Labs per Visit decreased from avg 0.75 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – New E/M Code Visit Count decreased from avg 2.58 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code Labs per Visit decreased from avg 1.07 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – New E/M Code Visit Count decreased from avg 2.45 to 1.00; 99-NEEDS INFO – New E/M Code Labs per Visit decreased from avg 0.25 to 0.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code Labs per Visit decreased from avg 1.07 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Existing E/M Code Visit Count decreased from avg 6.16 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Existing E/M Code Visit Count decreased from avg 2.46 to 1.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code Labs per Visit decreased from avg 1.28 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Visit Count decreased from avg 3.24 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
-  </si>
-  <si>
-    <t>18-CIGNA – Existing E/M Code Visit Count decreased from avg 4.48 to 1.00; 99-NEEDS INFO – New E/M Code Labs per Visit decreased from avg 0.25 to 0.00; 5-COMMERCIAL – New E/M Code Labs per Visit decreased from avg 1.07 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00</t>
-  </si>
-  <si>
-    <t>13-TRICARE – Existing E/M Code Visit Count decreased from avg 2.52 to 1.00; 99-NEEDS INFO – New E/M Code Labs per Visit decreased from avg 0.25 to 0.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code Labs per Visit decreased from avg 1.28 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Existing E/M Code Visit Count decreased from avg 2.46 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Labs per Visit decreased from avg 1.28 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – New E/M Code Visit Count decreased from avg 2.58 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code Labs per Visit decreased from avg 1.07 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 5-COMMERCIAL – Existing E/M Code Procedure per Visit decreased from avg 0.07 to 0.00; 5-COMMERCIAL – Existing E/M Code % of Visits w Radiology decreased from avg 0.17 to 0.00</t>
-  </si>
-  <si>
-    <t>12-HUMANA – New E/M Code Visit Count decreased from avg 2.13 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 4-MEDICAID – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 4-MEDICAID – Existing E/M Code % of Visits w Radiology decreased from avg 0.08 to 0.00</t>
-  </si>
-  <si>
-    <t>12-HUMANA – Existing E/M Code Visit Count decreased from avg 2.31 to 1.00; 5-COMMERCIAL – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00; 5-COMMERCIAL – New E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00; 4-MEDICAID – Non E/M Code Labs per Visit decreased from avg 0.23 to 0.00; 4-MEDICAID – Existing E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 3-MEDICARE – New E/M Code Procedure per Visit decreased from avg 0.06 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Non E/M Code Payment Amount* increased from avg 100.27 to 397.43; 13-TRICARE – New E/M Code Payment Amount* increased from avg 420.79 to 1362.26; 2-BCBS – Non E/M Code NRV Zero Balance* increased from avg 69.98 to 198.72; 4-MEDICAID – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 89.83 to -23.77; 18-CIGNA – New E/M Code Payment Amount* increased from avg 1254.59 to 2640.14; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to 0.00; 5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 11.29 to 0.00; 5-COMMERCIAL – Existing E/M Code Denial % decreased from avg 0.13 to 0.00; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 53.03 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges decreased from avg -11.29 to -129.36; 2-BCBS – New E/M Code Charge Billed Balance decreased from avg 105.03 to -130.33; 13-TRICARE – New E/M Code Zero Balance - Collection * Charges decreased from avg 94.40 to -18.00; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Code Zero Balance - Collection * Charges decreased from avg 18.08 to -149.68; 5-COMMERCIAL – New E/M Code Payment Amount* increased from avg 474.23 to 1902.67; 15-UNITED HEALTHCARE – New E/M Code Charge Billed Balance decreased from avg 134.60 to -146.87; 12-HUMANA – Existing E/M Code Payment Amount* increased from avg 269.10 to 580.07; 5-COMMERCIAL – Existing E/M Code Payment Amount* increased from avg 397.12 to 819.06; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 11.29 to 0.00; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 53.03 to 0.00; 4-MEDICAID – New E/M Code Zero Balance - Collection * Charges decreased from avg 204.54 to 0.00; 4-MEDICAID – New E/M Code Charge Billed Balance decreased from avg 549.00 to 0.00; 4-MEDICAID – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 89.83 to 0.00; 4-MEDICAID – Existing E/M Code Charge Billed Balance decreased from avg 298.18 to 0.00</t>
+    <t>12-HUMANA – New E/M Code Visit Count decreased from avg 2.13 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00</t>
+  </si>
+  <si>
+    <t>12-HUMANA – New E/M Code Visit Count decreased from avg 2.13 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Non E/M Code Visit Count decreased from avg 13.04 to 3.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – Existing E/M Code % of Visits w Radiology decreased from avg 0.21 to 0.00</t>
+  </si>
+  <si>
+    <t>13-TRICARE – New E/M Code Visit Count decreased from avg 3.29 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 12-HUMANA – Existing E/M Code % of Visits w Radiology decreased from avg 0.21 to 0.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Non E/M Code Visit Count decreased from avg 13.04 to 6.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – New E/M Code Visit Count decreased from avg 2.58 to 1.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Visit Count decreased from avg 3.24 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – New E/M Code Visit Count decreased from avg 17.98 to 9.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Visit Count decreased from avg 5.54 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Visit Count decreased from avg 5.54 to 1.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 13-TRICARE – Existing E/M Code Procedure per Visit decreased from avg 0.03 to 0.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code Visit Count decreased from avg 6.16 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.87 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
+  </si>
+  <si>
+    <t>13-TRICARE – Existing E/M Code Visit Count decreased from avg 2.52 to 1.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 12-HUMANA – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 12-HUMANA – New E/M Code % of Visits w Radiology decreased from avg 0.20 to 0.00</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Visit Count decreased from avg 4.48 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.87 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Visit Count decreased from avg 5.54 to 2.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Visit Count decreased from avg 5.54 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.87 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00</t>
+  </si>
+  <si>
+    <t>18-CIGNA – New E/M Code Visit Count decreased from avg 6.54 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 13-TRICARE – Existing E/M Code Procedure per Visit decreased from avg 0.03 to 0.00</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Visit Count decreased from avg 4.48 to 1.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – New E/M Code Visit Count decreased from avg 15.44 to 5.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code Labs per Visit decreased from avg 0.59 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – New E/M Code Visit Count decreased from avg 8.71 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 13-TRICARE – Existing E/M Code Procedure per Visit decreased from avg 0.03 to 0.00; 13-TRICARE – Existing E/M Code Labs per Visit decreased from avg 0.73 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Visit Count decreased from avg 3.24 to 1.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 13-TRICARE – New E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 13-TRICARE – New E/M Code % of Visits w Radiology decreased from avg 0.09 to 0.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – New E/M Code Visit Count decreased from avg 15.44 to 6.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Visit Count decreased from avg 10.08 to 2.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 12-HUMANA – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – New E/M Code Visit Count decreased from avg 8.71 to 2.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 13-TRICARE – Existing E/M Code Procedure per Visit decreased from avg 0.03 to 0.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – New E/M Code Visit Count decreased from avg 8.71 to 2.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.87 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Code Visit Count decreased from avg 11.12 to 2.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 12-HUMANA – Existing E/M Code % of Visits w Radiology decreased from avg 0.21 to 0.00; 12-HUMANA – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Visit Count decreased from avg 3.24 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 13-TRICARE – Existing E/M Code Procedure per Visit decreased from avg 0.03 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Existing E/M Code Visit Count decreased from avg 2.46 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 13-TRICARE – Existing E/M Code Procedure per Visit decreased from avg 0.03 to 0.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – New E/M Code Visit Count decreased from avg 17.98 to 10.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
+  </si>
+  <si>
+    <t>12-HUMANA – New E/M Code Visit Count decreased from avg 2.13 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 12-HUMANA – Existing E/M Code % of Visits w Radiology decreased from avg 0.21 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – New E/M Code Visit Count decreased from avg 2.45 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.87 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Existing E/M Code Visit Count decreased from avg 2.46 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 12-HUMANA – Existing E/M Code % of Visits w Radiology decreased from avg 0.21 to 0.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code Visit Count decreased from avg 6.16 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.87 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Visit Count decreased from avg 3.24 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – New E/M Code Visit Count decreased from avg 15.44 to 9.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 12-HUMANA – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Visit Count decreased from avg 3.24 to 1.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 12-HUMANA – Existing E/M Code Labs per Visit decreased from avg 1.19 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – New E/M Code Visit Count decreased from avg 2.45 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 12-HUMANA – Existing E/M Code Labs per Visit decreased from avg 1.19 to 0.00</t>
+  </si>
+  <si>
+    <t>12-HUMANA – New E/M Code Visit Count decreased from avg 2.13 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 12-HUMANA – Existing E/M Code Labs per Visit decreased from avg 1.19 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Visit Count decreased from avg 3.24 to 1.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – New E/M Code Visit Count decreased from avg 2.58 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – New E/M Code Visit Count decreased from avg 2.45 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code Visit Count decreased from avg 6.16 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.87 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – Existing E/M Code Charge Amount decreased from avg 1018.36 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Existing E/M Code Visit Count decreased from avg 2.46 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Visit Count decreased from avg 3.24 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code % of Visits w Radiology decreased from avg 0.07 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
+  </si>
+  <si>
+    <t>18-CIGNA – Existing E/M Code Visit Count decreased from avg 4.48 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00</t>
+  </si>
+  <si>
+    <t>13-TRICARE – Existing E/M Code Visit Count decreased from avg 2.52 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 13-TRICARE – Existing E/M Code Procedure per Visit decreased from avg 0.03 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Existing E/M Code Visit Count decreased from avg 2.46 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 13-TRICARE – Existing E/M Code Procedure per Visit decreased from avg 0.03 to 0.00; 13-TRICARE – Existing E/M Code % of Visits w Radiology decreased from avg 0.11 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – New E/M Code Visit Count decreased from avg 2.58 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 12-HUMANA – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 12-HUMANA – New E/M Code Labs per Visit decreased from avg 0.72 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – New E/M Code Visit Count decreased from avg 2.58 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.87 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00</t>
+  </si>
+  <si>
+    <t>12-HUMANA – New E/M Code Visit Count decreased from avg 2.13 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 12-HUMANA – Existing E/M Code Procedure per Visit decreased from avg 0.02 to 0.00; 12-HUMANA – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00</t>
+  </si>
+  <si>
+    <t>12-HUMANA – Existing E/M Code Visit Count decreased from avg 2.31 to 1.00; 1-SELF PAY – Existing E/M Code Procedure per Visit decreased from avg 0.05 to 0.00; 1-SELF PAY – Existing E/M Code Labs per Visit decreased from avg 0.87 to 0.00; 1-SELF PAY – Existing E/M Code % of Visits w Radiology decreased from avg 0.04 to 0.00; 1-SELF PAY – New E/M Code Procedure per Visit decreased from avg 0.04 to 0.00; 1-SELF PAY – Non E/M Code Procedure per Visit decreased from avg 0.01 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Non E/M Code Payment Amount* increased from avg 100.27 to 397.43; 13-TRICARE – New E/M Code Payment Amount* increased from avg 420.79 to 1362.26; 2-BCBS – Non E/M Code NRV Zero Balance* increased from avg 69.98 to 198.72; 4-MEDICAID – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 89.83 to -23.77; 18-CIGNA – New E/M Code Payment Amount* increased from avg 1254.59 to 2640.14; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to 0.00; 1-SELF PAY – New E/M Code Charge Billed Balance decreased from avg 54.61 to 0.00; 1-SELF PAY – Non E/M Code Zero Balance - Collection * Charges increased from avg -0.60 to 0.00; 12-HUMANA – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 1.01 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges decreased from avg -11.29 to -129.36; 2-BCBS – New E/M Code Charge Billed Balance decreased from avg 105.03 to -130.33; 13-TRICARE – New E/M Code Zero Balance - Collection * Charges decreased from avg 94.40 to -18.00; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to 0.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Code Zero Balance - Collection * Charges decreased from avg 18.08 to -149.68; 5-COMMERCIAL – New E/M Code Payment Amount* increased from avg 474.23 to 1902.67; 15-UNITED HEALTHCARE – New E/M Code Charge Billed Balance decreased from avg 134.60 to -146.87; 12-HUMANA – Existing E/M Code Payment Amount* increased from avg 269.10 to 580.07; 5-COMMERCIAL – Existing E/M Code Payment Amount* increased from avg 397.12 to 819.06; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to 0.00; 1-SELF PAY – New E/M Code Charge Billed Balance decreased from avg 54.61 to 0.00; 1-SELF PAY – Non E/M Code Zero Balance - Collection * Charges increased from avg -0.60 to 0.00; 12-HUMANA – Existing E/M Code Denial % decreased from avg 0.26 to 0.00</t>
   </si>
   <si>
     <t>3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -3.80 to -177.08; 3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 3.38 to -122.59; 12-HUMANA – New E/M Code Payment Amount* increased from avg 367.16 to 1416.22; 3-MEDICARE – New E/M Code Zero Balance - Collection * Charges decreased from avg 17.77 to -32.18; 3-MEDICARE – New E/M Code Charge Billed Balance decreased from avg 53.90 to -31.51; 3-MEDICARE – Existing E/M Code Payment Amount* increased from avg 406.36 to 836.62</t>
   </si>
   <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg 36.48 to -53.44; 12-HUMANA – Existing E/M Code Payment Amount* increased from avg 269.10 to 566.88; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg 25.16 to -2.48; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – New E/M Code Charge Billed Balance decreased from avg 54.61 to -110.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to -110.00; 3-MEDICARE – Existing E/M Code Payment Amount* increased from avg 406.36 to 1138.29; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 11.29 to 0.00; 5-COMMERCIAL – Existing E/M Code Denial % decreased from avg 0.13 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 3.38 to -102.16; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -3.80 to -73.70; 3-MEDICARE – Existing E/M Code Payment Amount* increased from avg 406.36 to 854.10; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges decreased from avg -11.29 to -178.17; 2-BCBS – New E/M Code Charge Billed Balance decreased from avg 105.03 to -192.89; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to 0.00; 5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 11.29 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges decreased from avg -11.29 to -360.75; 13-TRICARE – Existing E/M Code Payment Amount* increased from avg 280.10 to 561.25; 4-MEDICAID – New E/M Code Zero Balance - Collection * Charges decreased from avg 204.54 to 0.00; 4-MEDICAID – New E/M Code Charge Billed Balance decreased from avg 549.00 to 0.00; 4-MEDICAID – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 89.83 to 0.00; 4-MEDICAID – Existing E/M Code Charge Billed Balance decreased from avg 298.18 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to 0.00; 5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 11.29 to 0.00; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 53.03 to 0.00; 4-MEDICAID – Non E/M Code Denial % decreased from avg 0.23 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -21.83 to -134.31; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg 36.48 to -60.44; 12-HUMANA – Existing E/M Code Payment Amount* increased from avg 269.10 to 546.89; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – New E/M Code Payment Amount* increased from avg 342.32 to 920.81; 13-TRICARE – Existing E/M Code Payment Amount* increased from avg 280.10 to 684.96; 4-MEDICAID – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 89.83 to -14.75; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg 36.48 to -1.60; 4-MEDICAID – Existing E/M Code Charge Billed Balance decreased from avg 298.18 to -4.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00</t>
-  </si>
-  <si>
-    <t>13-TRICARE – New E/M Code Payment Amount* increased from avg 420.79 to 1026.63; 4-MEDICAID – New E/M Code Zero Balance - Collection * Charges decreased from avg 204.54 to -8.21; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to 0.00; 5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 11.29 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -3.80 to -59.91; 3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 3.38 to -19.69; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to 0.00; 5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 11.29 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges decreased from avg -11.29 to -51.12; 2-BCBS – New E/M Code Charge Billed Balance decreased from avg 105.03 to -107.62; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to 0.00; 5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 11.29 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 3.38 to -20.77; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -3.80 to -20.84; 3-MEDICARE – New E/M Code Charge Billed Balance decreased from avg 53.90 to -29.54; 5-COMMERCIAL – Existing E/M Code Payment Amount* increased from avg 397.12 to 883.32; 1-SELF PAY – Existing E/M Code NRV Zero Balance* increased from avg 149.09 to 298.40; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -3.80 to -51.21; 3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 3.38 to -20.77; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to 0.00; 5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 11.29 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 3.38 to -20.77; 17-AETNA – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 93.97 to -29.70; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to 0.00; 5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 11.29 to 0.00</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – New E/M Code Zero Balance - Collection * Charges decreased from avg 204.54 to 0.00; 4-MEDICAID – New E/M Code Denial % decreased from avg 0.19 to 0.00; 4-MEDICAID – New E/M Code Charge Billed Balance decreased from avg 549.00 to 0.00; 3-MEDICARE – New E/M Code Zero Balance - Collection * Charges decreased from avg 17.77 to 0.00; 3-MEDICARE – New E/M Code Charge Billed Balance decreased from avg 53.90 to 0.00; 3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 3.38 to 0.00</t>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg 36.48 to -53.44; 12-HUMANA – Existing E/M Code Payment Amount* increased from avg 269.10 to 566.88; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg 25.16 to -2.48; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to 0.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – New E/M Code Charge Billed Balance decreased from avg 54.61 to -110.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to -110.00; 3-MEDICARE – Existing E/M Code Payment Amount* increased from avg 406.36 to 1138.29; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – Non E/M Code Zero Balance - Collection * Charges increased from avg -0.60 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 3.38 to -102.16; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -3.80 to -73.70; 3-MEDICARE – Existing E/M Code Payment Amount* increased from avg 406.36 to 854.10; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges decreased from avg -11.29 to -178.17; 2-BCBS – New E/M Code Charge Billed Balance decreased from avg 105.03 to -192.89; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to 0.00; 1-SELF PAY – New E/M Code Charge Billed Balance decreased from avg 54.61 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges decreased from avg -11.29 to -360.75; 13-TRICARE – Existing E/M Code Payment Amount* increased from avg 280.10 to 561.25; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – Non E/M Code Zero Balance - Collection * Charges increased from avg -0.60 to 0.00; 12-HUMANA – Existing E/M Code Denial % decreased from avg 0.26 to 0.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to 0.00; 1-SELF PAY – New E/M Code Charge Billed Balance decreased from avg 54.61 to 0.00; 1-SELF PAY – Non E/M Code Zero Balance - Collection * Charges increased from avg -0.60 to 0.00; 12-HUMANA – New E/M Code Denial % decreased from avg 0.18 to 0.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -21.83 to -134.31; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg 36.48 to -60.44; 12-HUMANA – Existing E/M Code Payment Amount* increased from avg 269.10 to 546.89; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – New E/M Code Payment Amount* increased from avg 342.32 to 920.81; 13-TRICARE – Existing E/M Code Payment Amount* increased from avg 280.10 to 684.96; 4-MEDICAID – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 89.83 to -14.75; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg 36.48 to -1.60; 4-MEDICAID – Existing E/M Code Charge Billed Balance decreased from avg 298.18 to -4.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to 0.00</t>
+  </si>
+  <si>
+    <t>13-TRICARE – New E/M Code Payment Amount* increased from avg 420.79 to 1026.63; 4-MEDICAID – New E/M Code Zero Balance - Collection * Charges decreased from avg 204.54 to -8.21; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – Non E/M Code Zero Balance - Collection * Charges increased from avg -0.60 to 0.00; 12-HUMANA – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 1.01 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -3.80 to -59.91; 3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 3.38 to -19.69; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to 0.00; 1-SELF PAY – New E/M Code Charge Billed Balance decreased from avg 54.61 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges decreased from avg -11.29 to -51.12; 2-BCBS – New E/M Code Charge Billed Balance decreased from avg 105.03 to -107.62; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to 0.00; 1-SELF PAY – New E/M Code Charge Billed Balance decreased from avg 54.61 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 3.38 to -20.77; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -3.80 to -20.84; 3-MEDICARE – New E/M Code Charge Billed Balance decreased from avg 53.90 to -29.54; 5-COMMERCIAL – Existing E/M Code Payment Amount* increased from avg 397.12 to 883.32; 1-SELF PAY – Existing E/M Code NRV Zero Balance* increased from avg 149.09 to 298.40; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -3.80 to -51.21; 3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 3.38 to -20.77; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – Non E/M Code Zero Balance - Collection * Charges increased from avg -0.60 to 0.00; 13-TRICARE – Existing E/M Code Denial % decreased from avg 0.03 to 0.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – Existing E/M Code Charge Billed Balance decreased from avg 3.38 to -20.77; 17-AETNA – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 93.97 to -29.70; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to 0.00; 1-SELF PAY – New E/M Code Charge Billed Balance decreased from avg 54.61 to 0.00</t>
   </si>
   <si>
     <t>13-TRICARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 48.87 to -239.43; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg 25.16 to -50.00; 2-BCBS – Non E/M Code Payment Amount* increased from avg 100.27 to 395.48; 2-BCBS – Non E/M Code NRV Zero Balance* increased from avg 69.98 to 197.74; 13-TRICARE – Existing E/M Code Charge Billed Balance decreased from avg 123.98 to -57.34; 2-BCBS – Non E/M Code Collection Rate* increased from avg 0.51 to 1.14</t>
   </si>
   <si>
-    <t>3-MEDICARE – New E/M Code Payment Amount* increased from avg 342.32 to 997.97; 5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 11.29 to 0.00; 5-COMMERCIAL – Existing E/M Code Denial % decreased from avg 0.13 to 0.00; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 53.03 to 0.00; 4-MEDICAID – New E/M Code Zero Balance - Collection * Charges decreased from avg 204.54 to 0.00; 4-MEDICAID – New E/M Code Charge Billed Balance decreased from avg 549.00 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – New E/M Code Charge Billed Balance decreased from avg 54.61 to -290.00; 15-UNITED HEALTHCARE – New E/M Code Charge Billed Balance decreased from avg 134.60 to -107.34; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to 0.00; 4-MEDICAID – Non E/M Code Denial % decreased from avg 0.23 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges decreased from avg -11.29 to -67.77; 2-BCBS – New E/M Code Charge Billed Balance decreased from avg 105.03 to -132.02; 5-COMMERCIAL – New E/M Code Collection Rate* increased from avg 0.42 to 0.96; 5-COMMERCIAL – New E/M Code Zero Balance Collection Rate increased from avg 0.47 to 0.96; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00</t>
+    <t>3-MEDICARE – New E/M Code Payment Amount* increased from avg 342.32 to 997.97; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to 0.00; 1-SELF PAY – New E/M Code Charge Billed Balance decreased from avg 54.61 to 0.00; 1-SELF PAY – Non E/M Code Zero Balance - Collection * Charges increased from avg -0.60 to 0.00</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – New E/M Code Charge Billed Balance decreased from avg 54.61 to -290.00; 15-UNITED HEALTHCARE – New E/M Code Charge Billed Balance decreased from avg 134.60 to -107.34; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – Non E/M Code Zero Balance - Collection * Charges increased from avg -0.60 to 0.00; 12-HUMANA – New E/M Code Zero Balance - Collection * Charges increased from avg -1.68 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges decreased from avg -11.29 to -67.77; 2-BCBS – New E/M Code Charge Billed Balance decreased from avg 105.03 to -132.02; 5-COMMERCIAL – New E/M Code Collection Rate* increased from avg 0.42 to 0.96; 5-COMMERCIAL – New E/M Code Zero Balance Collection Rate increased from avg 0.47 to 0.96; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to 0.00; 1-SELF PAY – New E/M Code Charge Billed Balance decreased from avg 54.61 to 0.00</t>
   </si>
   <si>
     <t>5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 11.29 to -287.00; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance decreased from avg 53.03 to -463.00; 18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg 7.58 to -33.96; 18-CIGNA – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -10.90 to -66.66; 5-COMMERCIAL – Existing E/M Code Collection Rate* increased from avg 0.44 to 1.45; 15-UNITED HEALTHCARE – New E/M Code Charge Billed Balance decreased from avg 134.60 to -116.80</t>
@@ -544,10 +544,10 @@
     <t>12-HUMANA – New E/M Code Zero Balance - Collection * Charges decreased from avg -1.68 to -134.82; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg 25.16 to -297.48; 12-HUMANA – New E/M Code Charge Billed Balance decreased from avg 10.70 to -105.00; 2-BCBS – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -32.45 to -163.11; 15-UNITED HEALTHCARE – New E/M Code Zero Balance - Collection * Charges decreased from avg 18.08 to -26.54; 15-UNITED HEALTHCARE – New E/M Code Charge Billed Balance decreased from avg 134.60 to -13.09</t>
   </si>
   <si>
-    <t>15-UNITED HEALTHCARE – New E/M Code Zero Balance - Collection * Charges decreased from avg 18.08 to -56.97; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg 25.16 to -13.16; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to -30.00; 15-UNITED HEALTHCARE – New E/M Code Charge Billed Balance decreased from avg 134.60 to -11.13; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -32.45 to -334.65; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg 25.16 to -184.83; 18-CIGNA – New E/M Code Zero Balance - Collection * Charges decreased from avg 12.06 to -23.48; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg 36.48 to -6.02; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00</t>
+    <t>15-UNITED HEALTHCARE – New E/M Code Zero Balance - Collection * Charges decreased from avg 18.08 to -56.97; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg 25.16 to -13.16; 5-COMMERCIAL – New E/M Code Charge Billed Balance decreased from avg 174.41 to -30.00; 15-UNITED HEALTHCARE – New E/M Code Charge Billed Balance decreased from avg 134.60 to -11.13; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -32.45 to -334.65; 2-BCBS – Existing E/M Code Charge Billed Balance decreased from avg 25.16 to -184.83; 18-CIGNA – New E/M Code Zero Balance - Collection * Charges decreased from avg 12.06 to -23.48; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg 36.48 to -6.02; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00</t>
   </si>
   <si>
     <t>18-CIGNA – New E/M Code Zero Balance - Collection * Charges decreased from avg 12.06 to -59.75; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to -50.00; 17-AETNA – New E/M Code Zero Balance - Collection * Charges decreased from avg 166.06 to -259.75; 4-MEDICAID – New E/M Code Zero Balance - Collection * Charges decreased from avg 204.54 to -256.62; 4-MEDICAID – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 89.83 to -71.65; 2-BCBS – New E/M Code Charge Billed Balance decreased from avg 105.03 to -65.54</t>
@@ -568,7 +568,7 @@
     <t>1-SELF PAY – New E/M Code Charge Billed Balance decreased from avg 54.61 to -100.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges decreased from avg 63.16 to -100.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -21.83 to -64.11; 4-MEDICAID – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 89.83 to -19.07; 4-MEDICAID – Existing E/M Code Charge Billed Balance decreased from avg 298.18 to -20.00; 4-MEDICAID – New E/M Code Zero Balance - Collection * Charges decreased from avg 204.54 to -13.40</t>
   </si>
   <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -21.83 to -208.08; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg 36.48 to -229.84; 2-BCBS – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -32.45 to -147.87; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges decreased from avg 76.36 to 0.00; 5-COMMERCIAL – New E/M Code Denial % decreased from avg 0.05 to 0.00; 5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 11.29 to 0.00</t>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -21.83 to -208.08; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance decreased from avg 36.48 to -229.84; 2-BCBS – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -32.45 to -147.87; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to 0.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance decreased from avg 20.99 to 0.00; 1-SELF PAY – Non E/M Code Zero Balance - Collection * Charges increased from avg -0.60 to 0.00</t>
   </si>
   <si>
     <t>2-BCBS – Non E/M Code Charge Billed Balance decreased from avg 0.67 to -35.00; 4-MEDICAID – Non E/M Code Charge Billed Balance decreased from avg 17.77 to -65.00; 2-BCBS – New E/M Code Zero Balance - Collection * Charges decreased from avg -11.29 to -34.82; 1-SELF PAY – Non E/M Code Payment Amount* increased from avg 930.90 to 2860.00; 18-CIGNA – Non E/M Code Charge Billed Balance decreased from avg -25.00 to -75.00; 4-MEDICAID – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 89.83 to -72.70</t>
@@ -580,43 +580,43 @@
     <t>4-MEDICAID – Non E/M Code Zero Balance - Collection * Charges decreased from avg -2.69 to -35.00; 18-CIGNA – New E/M Code Zero Balance - Collection * Charges decreased from avg 12.06 to -112.67; 15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges decreased from avg -21.83 to -139.69; 1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges decreased from avg 16.91 to -68.19; 18-CIGNA – Existing E/M Code Charge Billed Balance decreased from avg 7.58 to -21.83; 4-MEDICAID – Non E/M Code Charge Billed Balance decreased from avg 17.77 to -35.00</t>
   </si>
   <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg 36.48 to 518.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -21.83 to 156.26; 2-BCBS – Non E/M Code Denial % increased from avg 0.17 to 1.00; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.45; 13-TRICARE – New E/M Code Zero Balance - Collection * Charges increased from avg 94.40 to 206.00; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -3.80 to 0.00</t>
-  </si>
-  <si>
-    <t>18-CIGNA – New E/M Code Zero Balance - Collection * Charges increased from avg 12.06 to 97.48; 2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.46; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.40; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -3.80 to 0.00; 2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 0.00; 2-BCBS – Existing E/M Code Zero Balance - Collection * Charges increased from avg -32.45 to 0.00</t>
-  </si>
-  <si>
-    <t>3-MEDICARE – New E/M Code Denial % increased from avg 0.41 to 1.00; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.41; 2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.40; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -3.80 to 0.00; 2-BCBS – Existing E/M Code Zero Balance - Collection * Charges increased from avg -32.45 to 0.00; 18-CIGNA – Existing E/M Code Zero Balance - Collection * Charges increased from avg -10.90 to 0.00</t>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg 36.48 to 518.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -21.83 to 156.26; 2-BCBS – Non E/M Code Denial % increased from avg 0.17 to 1.00; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.45; 13-TRICARE – New E/M Code Zero Balance - Collection * Charges increased from avg 94.40 to 206.00; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00</t>
+  </si>
+  <si>
+    <t>18-CIGNA – New E/M Code Zero Balance - Collection * Charges increased from avg 12.06 to 97.48; 2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.46; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.40; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00; 2-BCBS – Non E/M Code Payment Amount* decreased from avg 100.27 to 25.00; 2-BCBS – Non E/M Code NRV Zero Balance* decreased from avg 69.98 to 25.00</t>
+  </si>
+  <si>
+    <t>3-MEDICARE – New E/M Code Denial % increased from avg 0.41 to 1.00; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.41; 2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.40; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00; 1-SELF PAY – Non E/M Code Payment Amount* decreased from avg 930.90 to 235.00; 5-COMMERCIAL – Existing E/M Code Collection Rate* decreased from avg 0.44 to 0.17</t>
   </si>
   <si>
     <t>2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.71; 15-UNITED HEALTHCARE – New E/M Code Denial % increased from avg 0.18 to 0.45; 12-HUMANA – Existing E/M Code Denial % increased from avg 0.26 to 0.67; 17-AETNA – New E/M Code Denial % increased from avg 0.08 to 0.20; 3-MEDICARE – New E/M Code Denial % increased from avg 0.41 to 1.00; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.45</t>
   </si>
   <si>
-    <t>15-UNITED HEALTHCARE – New E/M Code Zero Balance - Collection * Charges increased from avg 18.08 to 206.31; 13-TRICARE – New E/M Code Denial % increased from avg 0.06 to 0.50; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.45; 2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.41; 2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 0.00; 2-BCBS – Existing E/M Code Zero Balance - Collection * Charges increased from avg -32.45 to 0.00</t>
-  </si>
-  <si>
-    <t>13-TRICARE – Existing E/M Code Denial % increased from avg 0.03 to 0.33; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.51; 15-UNITED HEALTHCARE – Existing E/M Code Denial % increased from avg 0.15 to 0.38; 4-MEDICAID – New E/M Code Denial % increased from avg 0.19 to 0.46; 15-UNITED HEALTHCARE – New E/M Code Denial % increased from avg 0.18 to 0.42; 2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 0.00</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – Non E/M Code Denial % increased from avg 0.23 to 1.00; 2-BCBS – Existing E/M Code Zero Balance - Collection * Charges increased from avg -32.45 to 62.92; 15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -21.83 to 12.23; 2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.48; 4-MEDICAID – Non E/M Code Zero Balance - Collection * Charges increased from avg -2.69 to 0.00; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -3.80 to 0.00</t>
-  </si>
-  <si>
-    <t>12-HUMANA – Existing E/M Code Charge Billed Balance increased from avg 10.28 to 100.00; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges increased from avg 76.36 to 265.28; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.57; 2-BCBS – Non E/M Code Denial % increased from avg 0.17 to 0.50; 4-MEDICAID – Non E/M Code Zero Balance - Collection * Charges increased from avg -2.69 to 0.00; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -3.80 to 0.00</t>
-  </si>
-  <si>
-    <t>17-AETNA – Existing E/M Code Denial % increased from avg 0.08 to 1.00; 4-MEDICAID – Existing E/M Code Denial % increased from avg 0.14 to 0.44; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.53; 3-MEDICARE – New E/M Code Denial % increased from avg 0.41 to 1.00; 2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.43; 2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Existing E/M Code Denial % increased from avg 0.13 to 0.33; 15-UNITED HEALTHCARE – New E/M Code Denial % increased from avg 0.18 to 0.43; 2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.44; 4-MEDICAID – Non E/M Code Zero Balance - Collection * Charges increased from avg -2.69 to 0.00; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -3.80 to 0.00; 2-BCBS – Existing E/M Code Zero Balance - Collection * Charges increased from avg -32.45 to 0.00</t>
+    <t>15-UNITED HEALTHCARE – New E/M Code Zero Balance - Collection * Charges increased from avg 18.08 to 206.31; 13-TRICARE – New E/M Code Denial % increased from avg 0.06 to 0.50; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.45; 2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.41; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00; 5-COMMERCIAL – Existing E/M Code Denial % increased from avg 0.13 to 0.25</t>
+  </si>
+  <si>
+    <t>13-TRICARE – Existing E/M Code Denial % increased from avg 0.03 to 0.33; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.51; 15-UNITED HEALTHCARE – Existing E/M Code Denial % increased from avg 0.15 to 0.38; 4-MEDICAID – New E/M Code Denial % increased from avg 0.19 to 0.46; 15-UNITED HEALTHCARE – New E/M Code Denial % increased from avg 0.18 to 0.42; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – Non E/M Code Denial % increased from avg 0.23 to 1.00; 2-BCBS – Existing E/M Code Zero Balance - Collection * Charges increased from avg -32.45 to 62.92; 15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -21.83 to 12.23; 2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.48; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.36</t>
+  </si>
+  <si>
+    <t>12-HUMANA – Existing E/M Code Charge Billed Balance increased from avg 10.28 to 100.00; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges increased from avg 76.36 to 265.28; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.57; 2-BCBS – Non E/M Code Denial % increased from avg 0.17 to 0.50; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00; 5-COMMERCIAL – New E/M Code Charge Billed Balance increased from avg 174.41 to 336.00</t>
+  </si>
+  <si>
+    <t>17-AETNA – Existing E/M Code Denial % increased from avg 0.08 to 1.00; 4-MEDICAID – Existing E/M Code Denial % increased from avg 0.14 to 0.44; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.53; 3-MEDICARE – New E/M Code Denial % increased from avg 0.41 to 1.00; 2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.43; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Existing E/M Code Denial % increased from avg 0.13 to 0.33; 15-UNITED HEALTHCARE – New E/M Code Denial % increased from avg 0.18 to 0.43; 2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.44; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.36; 17-AETNA – Existing E/M Code Payment Amount* decreased from avg 1143.95 to 150.00</t>
   </si>
   <si>
     <t>1-SELF PAY – New E/M Code Charge Billed Balance increased from avg 54.61 to 1079.80; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges increased from avg 63.16 to 1125.65; 17-AETNA – Existing E/M Code Denial % increased from avg 0.08 to 0.25; 2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.50; 17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 146.99 to 341.00; 17-AETNA – Existing E/M Code Zero Balance - Collection * Charges increased from avg 93.97 to 198.93</t>
   </si>
   <si>
-    <t>2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.52; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.48; 5-COMMERCIAL – Existing E/M Code Denial % increased from avg 0.13 to 0.33; 4-MEDICAID – Non E/M Code Zero Balance - Collection * Charges increased from avg -2.69 to 0.00; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -3.80 to 0.00; 2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 0.00</t>
-  </si>
-  <si>
-    <t>4-MEDICAID – New E/M Code Denial % increased from avg 0.19 to 0.50; 3-MEDICARE – Existing E/M Code Denial % increased from avg 0.31 to 0.80; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.40; 4-MEDICAID – Non E/M Code Zero Balance - Collection * Charges increased from avg -2.69 to 0.00; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -3.80 to 0.00; 2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 0.00</t>
+    <t>2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.52; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.48; 5-COMMERCIAL – Existing E/M Code Denial % increased from avg 0.13 to 0.33; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00; 4-MEDICAID – Non E/M Code Payment Amount* decreased from avg 52.81 to 4.00; 4-MEDICAID – Non E/M Code NRV Zero Balance* decreased from avg 27.28 to 4.00</t>
+  </si>
+  <si>
+    <t>4-MEDICAID – New E/M Code Denial % increased from avg 0.19 to 0.50; 3-MEDICARE – Existing E/M Code Denial % increased from avg 0.31 to 0.80; 2-BCBS – New E/M Code Denial % increased from avg 0.19 to 0.40; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00; 12-HUMANA – Existing E/M Code Denial % increased from avg 0.26 to 0.50; 2-BCBS – Existing E/M Code Denial % increased from avg 0.19 to 0.36</t>
   </si>
   <si>
     <t>1-SELF PAY – Existing E/M Code Zero Balance - Collection * Charges increased from avg 16.91 to 621.00; 1-SELF PAY – Existing E/M Code Charge Billed Balance increased from avg 20.99 to 621.00; 2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 117.72; 18-CIGNA – New E/M Code Zero Balance - Collection * Charges increased from avg 12.06 to 71.51; 12-HUMANA – Existing E/M Code Denial % increased from avg 0.26 to 1.00; 5-COMMERCIAL – New E/M Code Zero Balance - Collection * Charges increased from avg 76.36 to 271.86</t>
@@ -625,25 +625,25 @@
     <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 323.65; 1-SELF PAY – New E/M Code Charge Billed Balance increased from avg 54.61 to 661.00; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges increased from avg 63.16 to 661.96; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg 25.16 to 160.00; 2-BCBS – Existing E/M Code Zero Balance - Collection * Charges increased from avg -32.45 to 65.81; 12-HUMANA – Existing E/M Code Denial % increased from avg 0.26 to 1.00</t>
   </si>
   <si>
-    <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 101.38; 17-AETNA – New E/M Code Denial % increased from avg 0.08 to 0.50; 15-UNITED HEALTHCARE – New E/M Code Denial % increased from avg 0.18 to 0.50; 2-BCBS – Existing E/M Code Zero Balance - Collection * Charges increased from avg -32.45 to 0.00; 18-CIGNA – Existing E/M Code Zero Balance - Collection * Charges increased from avg -10.90 to 0.00; 15-UNITED HEALTHCARE – Non E/M Code Charge Billed Balance increased from avg -51.04 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – New E/M Code Zero Balance - Collection * Charges increased from avg 18.08 to 218.26; 13-TRICARE – Existing E/M Code Denial % increased from avg 0.03 to 0.33; 18-CIGNA – New E/M Code Zero Balance - Collection * Charges increased from avg 12.06 to 69.94; 17-AETNA – Existing E/M Code Denial % increased from avg 0.08 to 0.20; 3-MEDICARE – New E/M Code Denial % increased from avg 0.41 to 1.00; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -3.80 to 0.00</t>
-  </si>
-  <si>
-    <t>15-UNITED HEALTHCARE – Existing E/M Code Denial % increased from avg 0.15 to 0.40; 4-MEDICAID – New E/M Code Denial % increased from avg 0.19 to 0.40; 2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 0.00; 2-BCBS – Existing E/M Code Zero Balance - Collection * Charges increased from avg -32.45 to 0.00; 18-CIGNA – Existing E/M Code Zero Balance - Collection * Charges increased from avg -10.90 to 0.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -21.83 to 0.00</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – New E/M Code Charge Billed Balance increased from avg 54.61 to 1151.92; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges increased from avg 63.16 to 1150.60; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg 36.48 to 205.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -21.83 to 41.68; 4-MEDICAID – Existing E/M Code Denial % increased from avg 0.14 to 0.38; 2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 0.00</t>
-  </si>
-  <si>
-    <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 18.17; 15-UNITED HEALTHCARE – Existing E/M Code Denial % increased from avg 0.15 to 0.50; 17-AETNA – Existing E/M Code Denial % increased from avg 0.08 to 0.25; 3-MEDICARE – New E/M Code Denial % increased from avg 0.41 to 1.00; 17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 146.99 to 336.00; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -3.80 to 0.00</t>
-  </si>
-  <si>
-    <t>5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges increased from avg 11.29 to 301.61; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 53.03 to 534.00; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -3.80 to 0.00; 2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 0.00; 2-BCBS – Existing E/M Code Zero Balance - Collection * Charges increased from avg -32.45 to 0.00; 18-CIGNA – Existing E/M Code Zero Balance - Collection * Charges increased from avg -10.90 to 0.00</t>
-  </si>
-  <si>
-    <t>13-TRICARE – Existing E/M Code Denial % increased from avg 0.03 to 0.67; 15-UNITED HEALTHCARE – New E/M Code Zero Balance - Collection * Charges increased from avg 18.08 to 130.27; 17-AETNA – Non E/M Code Denial % increased from avg 0.25 to 1.00; 17-AETNA – Existing E/M Code Denial % increased from avg 0.08 to 0.29; 15-UNITED HEALTHCARE – New E/M Code Charge Billed Balance increased from avg 134.60 to 399.00; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -3.80 to 0.00</t>
+    <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 101.38; 17-AETNA – New E/M Code Denial % increased from avg 0.08 to 0.50; 15-UNITED HEALTHCARE – New E/M Code Denial % increased from avg 0.18 to 0.50; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00; 15-UNITED HEALTHCARE – Non E/M Code Charge Billed Balance increased from avg -51.04 to 0.00; 15-UNITED HEALTHCARE – Non E/M Code Payment Amount* decreased from avg 158.61 to 29.04</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – New E/M Code Zero Balance - Collection * Charges increased from avg 18.08 to 218.26; 13-TRICARE – Existing E/M Code Denial % increased from avg 0.03 to 0.33; 18-CIGNA – New E/M Code Zero Balance - Collection * Charges increased from avg 12.06 to 69.94; 17-AETNA – Existing E/M Code Denial % increased from avg 0.08 to 0.20; 3-MEDICARE – New E/M Code Denial % increased from avg 0.41 to 1.00; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00</t>
+  </si>
+  <si>
+    <t>15-UNITED HEALTHCARE – Existing E/M Code Denial % increased from avg 0.15 to 0.40; 4-MEDICAID – New E/M Code Denial % increased from avg 0.19 to 0.40; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00; 4-MEDICAID – New E/M Code Payment Amount* decreased from avg 2274.18 to 690.14; 1-SELF PAY – Non E/M Code Payment Amount* decreased from avg 930.90 to 395.00; 13-TRICARE – New E/M Code Payment Amount* decreased from avg 420.79 to 211.21</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – New E/M Code Charge Billed Balance increased from avg 54.61 to 1151.92; 1-SELF PAY – New E/M Code Zero Balance - Collection * Charges increased from avg 63.16 to 1150.60; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg 36.48 to 205.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -21.83 to 41.68; 4-MEDICAID – Existing E/M Code Denial % increased from avg 0.14 to 0.38; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00</t>
+  </si>
+  <si>
+    <t>2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 18.17; 15-UNITED HEALTHCARE – Existing E/M Code Denial % increased from avg 0.15 to 0.50; 17-AETNA – Existing E/M Code Denial % increased from avg 0.08 to 0.25; 3-MEDICARE – New E/M Code Denial % increased from avg 0.41 to 1.00; 17-AETNA – Existing E/M Code Charge Billed Balance increased from avg 146.99 to 336.00; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00</t>
+  </si>
+  <si>
+    <t>5-COMMERCIAL – Existing E/M Code Zero Balance - Collection * Charges increased from avg 11.29 to 301.61; 5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 53.03 to 534.00; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00; 5-COMMERCIAL – Existing E/M Code Denial % increased from avg 0.13 to 0.25; 4-MEDICAID – Existing E/M Code Denial % increased from avg 0.14 to 0.28; 12-HUMANA – Existing E/M Code Payment Amount* decreased from avg 269.10 to 46.79</t>
+  </si>
+  <si>
+    <t>13-TRICARE – Existing E/M Code Denial % increased from avg 0.03 to 0.67; 15-UNITED HEALTHCARE – New E/M Code Zero Balance - Collection * Charges increased from avg 18.08 to 130.27; 17-AETNA – Non E/M Code Denial % increased from avg 0.25 to 1.00; 17-AETNA – Existing E/M Code Denial % increased from avg 0.08 to 0.29; 15-UNITED HEALTHCARE – New E/M Code Charge Billed Balance increased from avg 134.60 to 399.00; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00</t>
   </si>
   <si>
     <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg 7.58 to 160.00; 13-TRICARE – New E/M Code Denial % increased from avg 0.06 to 1.00; 18-CIGNA – Existing E/M Code Denial % increased from avg 0.01 to 0.12; 18-CIGNA – Existing E/M Code Zero Balance - Collection * Charges increased from avg -10.90 to 72.93; 2-BCBS – Existing E/M Code Zero Balance - Collection * Charges increased from avg -32.45 to 126.83; 12-HUMANA – Existing E/M Code Charge Billed Balance increased from avg 10.28 to 25.00</t>
@@ -706,7 +706,7 @@
     <t>15-UNITED HEALTHCARE – New E/M Code Zero Balance - Collection * Charges increased from avg 18.08 to 583.15; 18-CIGNA – Existing E/M Code Denial % increased from avg 0.01 to 0.33; 15-UNITED HEALTHCARE – New E/M Code Charge Billed Balance increased from avg 134.60 to 1395.45; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg 36.48 to 315.00; 5-COMMERCIAL – Existing E/M Code Denial % increased from avg 0.13 to 1.00; 13-TRICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg 48.87 to 295.92</t>
   </si>
   <si>
-    <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg 7.58 to 83.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -21.83 to 89.43; 3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 3.38 to 20.27; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg 36.48 to 208.87; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -3.80 to 0.00; 12-HUMANA – New E/M Code Zero Balance - Collection * Charges increased from avg -1.68 to 0.00</t>
+    <t>18-CIGNA – Existing E/M Code Charge Billed Balance increased from avg 7.58 to 83.00; 15-UNITED HEALTHCARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -21.83 to 89.43; 3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 3.38 to 20.27; 15-UNITED HEALTHCARE – Existing E/M Code Charge Billed Balance increased from avg 36.48 to 208.87; 1-SELF PAY – Non E/M Code Charge Billed Balance increased from avg -1.90 to 0.00; 3-MEDICARE – Existing E/M Code Payment Amount* decreased from avg 406.36 to 81.67</t>
   </si>
   <si>
     <t>5-COMMERCIAL – Existing E/M Code Charge Billed Balance increased from avg 53.03 to 641.00; 3-MEDICARE – Existing E/M Code Zero Balance - Collection * Charges increased from avg -3.80 to 20.46; 3-MEDICARE – Existing E/M Code Charge Billed Balance increased from avg 3.38 to 20.27; 3-MEDICARE – New E/M Code Zero Balance - Collection * Charges increased from avg 17.77 to 103.19; 17-AETNA – New E/M Code Denial % increased from avg 0.08 to 0.33; 3-MEDICARE – New E/M Code Charge Billed Balance increased from avg 53.90 to 132.14</t>
@@ -730,10 +730,154 @@
     <t>2-BCBS – Non E/M Code Charge Billed Balance increased from avg 0.67 to 45.00; 2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 510.99; 12-HUMANA – New E/M Code Charge Billed Balance increased from avg 10.70 to 263.00; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg 25.16 to 381.01; 13-TRICARE – New E/M Code Denial % increased from avg 0.06 to 0.67; 15-UNITED HEALTHCARE – New E/M Code Zero Balance - Collection * Charges increased from avg 18.08 to 181.28</t>
   </si>
   <si>
-    <t>Charges Collection Declined</t>
-  </si>
-  <si>
-    <t>Improved Charges Collections</t>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – High zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – High zero-balance collection vs baseline; 2-BCBS – Normal range; 3-MEDICARE – High zero-balance collection vs baseline; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Unusually high zero-balance vs total collection</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Low zero-balance collection vs baseline; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Low zero-balance collection vs baseline; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – High zero-balance collection vs baseline; 2-BCBS – Normal range; 3-MEDICARE – High zero-balance collection vs baseline; 3-MEDICARE – Low zero-balance collection vs baseline; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range; 5-COMMERCIAL – Very low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Low zero-balance collection vs baseline; 1-SELF PAY – Normal range; 12-HUMANA – Low zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Collection data incomplete; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Very low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Low zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – High zero-balance collection vs baseline; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Low zero-balance collection vs baseline; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – High zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Collection data incomplete; 12-HUMANA – Low zero-balance collection vs baseline; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Low zero-balance collection vs baseline; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 2-BCBS – Very low zero-balance collection vs baseline; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 1-SELF PAY – Unusually high zero-balance vs total collection; 12-HUMANA – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Collection data incomplete; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Low zero-balance collection vs baseline; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete; 5-COMMERCIAL – Low zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 13-TRICARE – Collection data incomplete; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – High zero-balance collection vs baseline; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 1-SELF PAY – Very low zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Low zero-balance collection vs baseline; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Low zero-balance collection vs baseline; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 12-HUMANA – Unusually high zero-balance vs total collection; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range; 5-COMMERCIAL – Unusually high zero-balance vs total collection</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Collection data incomplete; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Low zero-balance collection vs baseline; 4-MEDICAID – Normal range; 5-COMMERCIAL – Low zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 13-TRICARE – Low zero-balance collection vs baseline; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Low zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Low zero-balance collection vs baseline; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range; 5-COMMERCIAL – Very low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – High zero-balance collection vs baseline; 1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – High zero-balance collection vs baseline; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – High zero-balance collection vs baseline; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – High zero-balance collection vs baseline; 1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Low zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Low zero-balance collection vs baseline; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Collection data incomplete; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Low zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Low zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 15-UNITED HEALTHCARE – Unusually high zero-balance vs total collection; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Low zero-balance collection vs baseline; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – High zero-balance collection vs baseline; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Low zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – High zero-balance collection vs baseline; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – High zero-balance collection vs baseline; 1-SELF PAY – Normal range; 12-HUMANA – Collection data incomplete; 13-TRICARE – Low zero-balance collection vs baseline; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 15-UNITED HEALTHCARE – Unusually high zero-balance vs total collection; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Collection data incomplete; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 3-MEDICARE – Unusually high zero-balance vs total collection; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – Low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 12-HUMANA – Unusually high zero-balance vs total collection; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – High zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Low zero-balance collection vs baseline; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – High zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 18-CIGNA – Very low zero-balance collection vs baseline; 2-BCBS – Normal range; 2-BCBS – Very low zero-balance collection vs baseline; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Low zero-balance collection vs baseline; 1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 17-AETNA – Normal range; 18-CIGNA – Low zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Low zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Collection data incomplete; 12-HUMANA – Normal range; 13-TRICARE – High zero-balance collection vs baseline; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 3-MEDICARE – Unusually high zero-balance vs total collection; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete; 5-COMMERCIAL – High zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – High zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Collection data incomplete; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – High zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Low zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – High zero-balance collection vs baseline; 1-SELF PAY – Normal range; 12-HUMANA – Collection data incomplete; 12-HUMANA – High zero-balance collection vs baseline; 12-HUMANA – Unusually high zero-balance vs total collection; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Collection data incomplete; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Low zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Collection data incomplete; 2-BCBS – Normal range; 2-BCBS – Unusually high zero-balance vs total collection; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Low zero-balance collection vs baseline; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Unusually high zero-balance vs total collection; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Low zero-balance collection vs baseline; 4-MEDICAID – Normal range; 4-MEDICAID – Unusually high zero-balance vs total collection; 5-COMMERCIAL – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – High zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete; 99-NEEDS INFO – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Collection data incomplete; 1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 15-UNITED HEALTHCARE – Unusually high zero-balance vs total collection; 17-AETNA – Low zero-balance collection vs baseline; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 4-MEDICAID – Very low zero-balance collection vs baseline; 5-COMMERCIAL – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Collection data incomplete; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Collection data incomplete; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 3-MEDICARE – Unusually high zero-balance vs total collection; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Collection data incomplete; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – High zero-balance collection vs baseline; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete; 5-COMMERCIAL – Normal range; 7-PPO – Collection data incomplete; 99-NEEDS INFO – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 15-UNITED HEALTHCARE – Unusually high zero-balance vs total collection; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Collection data incomplete; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 4-MEDICAID – Unusually high zero-balance vs total collection; 5-COMMERCIAL – Collection data incomplete; 5-COMMERCIAL – Unusually high zero-balance vs total collection; 99-NEEDS INFO – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Low zero-balance collection vs baseline; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 4-MEDICAID – Normal range; 4-MEDICAID – Unusually high zero-balance vs total collection; 5-COMMERCIAL – Collection data incomplete; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Low zero-balance collection vs baseline; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – High zero-balance collection vs baseline; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – High zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Collection data incomplete; 18-CIGNA – Normal range; 2-BCBS – Collection data incomplete; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 3-MEDICARE – Unusually high zero-balance vs total collection; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Unusually high zero-balance vs total collection; 5-COMMERCIAL – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 12-HUMANA – Unusually high zero-balance vs total collection; 13-TRICARE – Collection data incomplete; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Collection data incomplete; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – High zero-balance collection vs baseline; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete; 99-NEEDS INFO – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Low zero-balance collection vs baseline; 1-SELF PAY – Normal range; 12-HUMANA – Collection data incomplete; 12-HUMANA – Normal range; 13-TRICARE – Collection data incomplete; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Normal range; 2-BCBS – Collection data incomplete; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – High zero-balance collection vs baseline; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
   </si>
 </sst>
 </file>
@@ -1103,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1127,8 +1271,8 @@
     <col min="16" max="16" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="26" width="255.83203125" bestFit="1" customWidth="1"/>
@@ -1136,7 +1280,7 @@
     <col min="28" max="28" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="18" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="255.83203125" bestFit="1" customWidth="1"/>
     <col min="32" max="33" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="19" bestFit="1" customWidth="1"/>
@@ -1305,16 +1449,16 @@
         <v>47000.029999999992</v>
       </c>
       <c r="S2">
-        <v>45155.99419999995</v>
+        <v>47789.018236151467</v>
       </c>
       <c r="T2">
-        <v>-1844.035800000041</v>
+        <v>-788.98823615147558</v>
       </c>
       <c r="U2">
-        <v>4.0837010294417206</v>
+        <v>-1.650982307802719</v>
       </c>
       <c r="V2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="W2" t="s">
         <v>37</v>
@@ -1323,22 +1467,22 @@
         <v>87</v>
       </c>
       <c r="Y2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Z2" t="s">
         <v>186</v>
       </c>
       <c r="AA2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB2">
         <v>0</v>
       </c>
       <c r="AC2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE2" t="s">
         <v>236</v>
@@ -1412,16 +1556,16 @@
         <v>31610.29</v>
       </c>
       <c r="S3">
-        <v>32769.370200000027</v>
+        <v>32136.761600700389</v>
       </c>
       <c r="T3">
-        <v>1159.080200000026</v>
+        <v>-526.47160070038808</v>
       </c>
       <c r="U3">
-        <v>-3.5370841518340339</v>
+        <v>-1.6382223176118469</v>
       </c>
       <c r="V3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W3" t="s">
         <v>38</v>
@@ -1430,7 +1574,7 @@
         <v>88</v>
       </c>
       <c r="Y3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="Z3" t="s">
         <v>187</v>
@@ -1439,16 +1583,16 @@
         <v>0</v>
       </c>
       <c r="AB3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD3">
         <v>0</v>
       </c>
       <c r="AE3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AF3">
         <v>0.33532467532467081</v>
@@ -1519,16 +1663,16 @@
         <v>29340.77</v>
       </c>
       <c r="S4">
-        <v>29272.011500000011</v>
+        <v>30773.153628044231</v>
       </c>
       <c r="T4">
-        <v>-68.758499999988999</v>
+        <v>-1432.383628044234</v>
       </c>
       <c r="U4">
-        <v>0.2348950293354079</v>
+        <v>-4.6546533558356913</v>
       </c>
       <c r="V4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W4" t="s">
         <v>39</v>
@@ -1537,7 +1681,7 @@
         <v>89</v>
       </c>
       <c r="Y4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Z4" t="s">
         <v>188</v>
@@ -1546,16 +1690,16 @@
         <v>0</v>
       </c>
       <c r="AB4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD4">
         <v>0</v>
       </c>
       <c r="AE4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AF4">
         <v>2.3166924066924248</v>
@@ -1626,16 +1770,16 @@
         <v>37248.69</v>
       </c>
       <c r="S5">
-        <v>37272.826399999984</v>
+        <v>39626.067251179011</v>
       </c>
       <c r="T5">
-        <v>24.136399999981219</v>
+        <v>-2377.3772511790162</v>
       </c>
       <c r="U5">
-        <v>-6.4756022902468263E-2</v>
+        <v>-5.9995286337891143</v>
       </c>
       <c r="V5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W5" t="s">
         <v>40</v>
@@ -1644,7 +1788,7 @@
         <v>90</v>
       </c>
       <c r="Y5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="Z5" t="s">
         <v>189</v>
@@ -1653,16 +1797,16 @@
         <v>0</v>
       </c>
       <c r="AB5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE5" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="AF5">
         <v>-0.61822510822514687</v>
@@ -1733,13 +1877,13 @@
         <v>35962.169999999991</v>
       </c>
       <c r="S6">
-        <v>36199.009899999983</v>
+        <v>35733.778245693909</v>
       </c>
       <c r="T6">
-        <v>236.83989999998451</v>
+        <v>228.39175430608159</v>
       </c>
       <c r="U6">
-        <v>-0.65427176227818495</v>
+        <v>0.63914807086934289</v>
       </c>
       <c r="V6" t="s">
         <v>28</v>
@@ -1751,7 +1895,7 @@
         <v>91</v>
       </c>
       <c r="Y6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="Z6" t="s">
         <v>190</v>
@@ -1766,10 +1910,10 @@
         <v>1</v>
       </c>
       <c r="AD6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE6" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="AF6">
         <v>1.311991071428565</v>
@@ -1840,16 +1984,16 @@
         <v>35947.040000000008</v>
       </c>
       <c r="S7">
-        <v>36230.01320000003</v>
+        <v>34116.917226724298</v>
       </c>
       <c r="T7">
-        <v>282.97320000002219</v>
+        <v>1830.1227732757029</v>
       </c>
       <c r="U7">
-        <v>-0.78104636186006671</v>
+        <v>5.3642677065855766</v>
       </c>
       <c r="V7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="W7" t="s">
         <v>42</v>
@@ -1858,25 +2002,25 @@
         <v>92</v>
       </c>
       <c r="Y7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="Z7" t="s">
         <v>191</v>
       </c>
       <c r="AA7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB7">
         <v>0</v>
       </c>
       <c r="AC7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD7">
         <v>0</v>
       </c>
       <c r="AE7" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="AF7">
         <v>-2.946746031746017</v>
@@ -1947,16 +2091,16 @@
         <v>35708.599999999991</v>
       </c>
       <c r="S8">
-        <v>35793.95590000003</v>
+        <v>34212.216513640968</v>
       </c>
       <c r="T8">
-        <v>85.355900000038673</v>
+        <v>1496.3834863590239</v>
       </c>
       <c r="U8">
-        <v>-0.23846456155475851</v>
+        <v>4.3738279446536046</v>
       </c>
       <c r="V8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="W8" t="s">
         <v>43</v>
@@ -1965,25 +2109,25 @@
         <v>93</v>
       </c>
       <c r="Y8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Z8" t="s">
         <v>192</v>
       </c>
       <c r="AA8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB8">
         <v>0</v>
       </c>
       <c r="AC8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD8">
         <v>0</v>
       </c>
       <c r="AE8" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="AF8">
         <v>-0.11908000364897479</v>
@@ -2054,16 +2198,16 @@
         <v>36416.249999999993</v>
       </c>
       <c r="S9">
-        <v>36718.599300000002</v>
+        <v>37937.584943763402</v>
       </c>
       <c r="T9">
-        <v>302.34930000000901</v>
+        <v>-1521.334943763402</v>
       </c>
       <c r="U9">
-        <v>-0.82342274967991214</v>
+        <v>-4.0100996044385706</v>
       </c>
       <c r="V9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W9" t="s">
         <v>44</v>
@@ -2072,7 +2216,7 @@
         <v>94</v>
       </c>
       <c r="Y9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Z9" t="s">
         <v>193</v>
@@ -2081,16 +2225,16 @@
         <v>0</v>
       </c>
       <c r="AB9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE9" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AF9">
         <v>15.71094836307773</v>
@@ -2161,13 +2305,13 @@
         <v>29620.74</v>
       </c>
       <c r="S10">
-        <v>29422.669900000041</v>
+        <v>29000.648103349191</v>
       </c>
       <c r="T10">
-        <v>-198.07009999995719</v>
+        <v>620.09189665080703</v>
       </c>
       <c r="U10">
-        <v>0.67318873736865348</v>
+        <v>2.138200134152155</v>
       </c>
       <c r="V10" t="s">
         <v>28</v>
@@ -2179,7 +2323,7 @@
         <v>95</v>
       </c>
       <c r="Y10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="Z10" t="s">
         <v>194</v>
@@ -2197,7 +2341,7 @@
         <v>0</v>
       </c>
       <c r="AE10" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="AF10">
         <v>-0.86457142857142344</v>
@@ -2268,16 +2412,16 @@
         <v>24459.74</v>
       </c>
       <c r="S11">
-        <v>24665.326200000029</v>
+        <v>23386.952036875318</v>
       </c>
       <c r="T11">
-        <v>205.58620000003069</v>
+        <v>1072.787963124676</v>
       </c>
       <c r="U11">
-        <v>-0.83350286281650887</v>
+        <v>4.5871217482002793</v>
       </c>
       <c r="V11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="W11" t="s">
         <v>46</v>
@@ -2286,25 +2430,25 @@
         <v>96</v>
       </c>
       <c r="Y11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="Z11" t="s">
         <v>195</v>
       </c>
       <c r="AA11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB11">
         <v>0</v>
       </c>
       <c r="AC11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD11">
         <v>0</v>
       </c>
       <c r="AE11" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="AF11">
         <v>0.6351407268170135</v>
@@ -2375,13 +2519,13 @@
         <v>27164.76</v>
       </c>
       <c r="S12">
-        <v>27025.52929999998</v>
+        <v>27032.04397191677</v>
       </c>
       <c r="T12">
-        <v>-139.2307000000219</v>
+        <v>132.7160280832322</v>
       </c>
       <c r="U12">
-        <v>0.51518213928199363</v>
+        <v>0.49095816883513932</v>
       </c>
       <c r="V12" t="s">
         <v>28</v>
@@ -2393,7 +2537,7 @@
         <v>97</v>
       </c>
       <c r="Y12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="Z12" t="s">
         <v>196</v>
@@ -2411,7 +2555,7 @@
         <v>0</v>
       </c>
       <c r="AE12" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="AF12">
         <v>3.6189800809212609</v>
@@ -2482,13 +2626,13 @@
         <v>27476.09</v>
       </c>
       <c r="S13">
-        <v>28617.79510000001</v>
+        <v>28324.43300887608</v>
       </c>
       <c r="T13">
-        <v>1141.705100000006</v>
+        <v>-848.34300887608333</v>
       </c>
       <c r="U13">
-        <v>-3.989493586107919</v>
+        <v>-2.995092641784697</v>
       </c>
       <c r="V13" t="s">
         <v>27</v>
@@ -2500,7 +2644,7 @@
         <v>98</v>
       </c>
       <c r="Y13" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="Z13" t="s">
         <v>197</v>
@@ -2518,7 +2662,7 @@
         <v>0</v>
       </c>
       <c r="AE13" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="AF13">
         <v>0</v>
@@ -2589,16 +2733,16 @@
         <v>20575.77</v>
       </c>
       <c r="S14">
-        <v>21184.46450000002</v>
+        <v>18963.27566946932</v>
       </c>
       <c r="T14">
-        <v>608.69450000001962</v>
+        <v>1612.494330530684</v>
       </c>
       <c r="U14">
-        <v>-2.873306049345826</v>
+        <v>8.5032478493511761</v>
       </c>
       <c r="V14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W14" t="s">
         <v>49</v>
@@ -2607,16 +2751,16 @@
         <v>99</v>
       </c>
       <c r="Y14" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="Z14" t="s">
         <v>198</v>
       </c>
       <c r="AA14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC14">
         <v>0</v>
@@ -2625,7 +2769,7 @@
         <v>0</v>
       </c>
       <c r="AE14" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="AF14">
         <v>-0.55211904761904407</v>
@@ -2696,16 +2840,16 @@
         <v>26750.36</v>
       </c>
       <c r="S15">
-        <v>27083.624000000011</v>
+        <v>28032.695772201219</v>
       </c>
       <c r="T15">
-        <v>333.26400000001013</v>
+        <v>-1282.335772201219</v>
       </c>
       <c r="U15">
-        <v>-1.2305000246643869</v>
+        <v>-4.5744290260976399</v>
       </c>
       <c r="V15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W15" t="s">
         <v>50</v>
@@ -2714,7 +2858,7 @@
         <v>100</v>
       </c>
       <c r="Y15" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Z15" t="s">
         <v>199</v>
@@ -2723,16 +2867,16 @@
         <v>0</v>
       </c>
       <c r="AB15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD15">
         <v>0</v>
       </c>
       <c r="AE15" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="AF15">
         <v>7.1093506493506311</v>
@@ -2803,16 +2947,16 @@
         <v>27416.39</v>
       </c>
       <c r="S16">
-        <v>27202.994400000011</v>
+        <v>26457.496659794819</v>
       </c>
       <c r="T16">
-        <v>-213.39559999998161</v>
+        <v>958.89334020518072</v>
       </c>
       <c r="U16">
-        <v>0.78445628765038289</v>
+        <v>3.6242784135444248</v>
       </c>
       <c r="V16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="W16" t="s">
         <v>51</v>
@@ -2821,25 +2965,25 @@
         <v>101</v>
       </c>
       <c r="Y16" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="Z16" t="s">
         <v>200</v>
       </c>
       <c r="AA16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB16">
         <v>0</v>
       </c>
       <c r="AC16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD16">
         <v>0</v>
       </c>
       <c r="AE16" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="AF16">
         <v>1.693639152298857</v>
@@ -2910,16 +3054,16 @@
         <v>21838.43</v>
       </c>
       <c r="S17">
-        <v>22035.3269</v>
+        <v>18797.238821588991</v>
       </c>
       <c r="T17">
-        <v>196.89689999999251</v>
+        <v>3041.1911784110162</v>
       </c>
       <c r="U17">
-        <v>-0.89355107320868687</v>
+        <v>16.178925039342211</v>
       </c>
       <c r="V17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="W17" t="s">
         <v>52</v>
@@ -2928,25 +3072,25 @@
         <v>102</v>
       </c>
       <c r="Y17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Z17" t="s">
         <v>201</v>
       </c>
       <c r="AA17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB17">
         <v>0</v>
       </c>
       <c r="AC17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD17">
         <v>0</v>
       </c>
       <c r="AE17" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="AF17">
         <v>1.6387116666666941</v>
@@ -3017,16 +3161,16 @@
         <v>25951.37000000001</v>
       </c>
       <c r="S18">
-        <v>26573.272900000029</v>
+        <v>26658.838347964262</v>
       </c>
       <c r="T18">
-        <v>621.90290000002642</v>
+        <v>-707.46834796425173</v>
       </c>
       <c r="U18">
-        <v>-2.3403323419751789</v>
+        <v>-2.6537853552732762</v>
       </c>
       <c r="V18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W18" t="s">
         <v>53</v>
@@ -3035,7 +3179,7 @@
         <v>103</v>
       </c>
       <c r="Y18" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="Z18" t="s">
         <v>202</v>
@@ -3044,16 +3188,16 @@
         <v>0</v>
       </c>
       <c r="AB18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD18">
         <v>0</v>
       </c>
       <c r="AE18" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="AF18">
         <v>3.2588543859648951</v>
@@ -3124,16 +3268,16 @@
         <v>24325.55</v>
       </c>
       <c r="S19">
-        <v>24002.058900000011</v>
+        <v>23006.64065070586</v>
       </c>
       <c r="T19">
-        <v>-323.49109999998842</v>
+        <v>1318.9093492941361</v>
       </c>
       <c r="U19">
-        <v>1.3477639620323909</v>
+        <v>5.7327332978257743</v>
       </c>
       <c r="V19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="W19" t="s">
         <v>54</v>
@@ -3142,25 +3286,25 @@
         <v>104</v>
       </c>
       <c r="Y19" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="Z19" t="s">
         <v>203</v>
       </c>
       <c r="AA19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB19">
         <v>0</v>
       </c>
       <c r="AC19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD19">
         <v>0</v>
       </c>
       <c r="AE19" t="s">
-        <v>236</v>
+        <v>253</v>
       </c>
       <c r="AF19">
         <v>-0.94814847478158981</v>
@@ -3231,16 +3375,16 @@
         <v>24475.18</v>
       </c>
       <c r="S20">
-        <v>24691.878100000009</v>
+        <v>22755.248176811911</v>
       </c>
       <c r="T20">
-        <v>216.69810000001229</v>
+        <v>1719.9318231880859</v>
       </c>
       <c r="U20">
-        <v>-0.87760881988159611</v>
+        <v>7.5583962425895841</v>
       </c>
       <c r="V20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="W20" t="s">
         <v>55</v>
@@ -3249,25 +3393,25 @@
         <v>105</v>
       </c>
       <c r="Y20" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="Z20" t="s">
         <v>204</v>
       </c>
       <c r="AA20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB20">
         <v>0</v>
       </c>
       <c r="AC20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD20">
         <v>0</v>
       </c>
       <c r="AE20" t="s">
-        <v>237</v>
+        <v>254</v>
       </c>
       <c r="AF20">
         <v>0.76327487837241392</v>
@@ -3338,13 +3482,13 @@
         <v>24504.18</v>
       </c>
       <c r="S21">
-        <v>24615.227400000011</v>
+        <v>24958.317397889092</v>
       </c>
       <c r="T21">
-        <v>111.0474000000104</v>
+        <v>-454.13739788909152</v>
       </c>
       <c r="U21">
-        <v>-0.4511329438297626</v>
+        <v>-1.8195833903751111</v>
       </c>
       <c r="V21" t="s">
         <v>28</v>
@@ -3356,7 +3500,7 @@
         <v>106</v>
       </c>
       <c r="Y21" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="Z21" t="s">
         <v>205</v>
@@ -3374,7 +3518,7 @@
         <v>0</v>
       </c>
       <c r="AE21" t="s">
-        <v>236</v>
+        <v>255</v>
       </c>
       <c r="AF21">
         <v>0.50504165580537119</v>
@@ -3445,16 +3589,16 @@
         <v>24780.58</v>
       </c>
       <c r="S22">
-        <v>24970.64080000003</v>
+        <v>24042.921800131699</v>
       </c>
       <c r="T22">
-        <v>190.0608000000357</v>
+        <v>737.65819986829956</v>
       </c>
       <c r="U22">
-        <v>-0.76113705500114925</v>
+        <v>3.068088837124026</v>
       </c>
       <c r="V22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="W22" t="s">
         <v>57</v>
@@ -3463,25 +3607,25 @@
         <v>107</v>
       </c>
       <c r="Y22" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="Z22" t="s">
         <v>206</v>
       </c>
       <c r="AA22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB22">
         <v>0</v>
       </c>
       <c r="AC22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD22">
         <v>0</v>
       </c>
       <c r="AE22" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="AF22">
         <v>1.939806892453944</v>
@@ -3552,16 +3696,16 @@
         <v>23883.61</v>
       </c>
       <c r="S23">
-        <v>23456.290000000041</v>
+        <v>23080.448721431949</v>
       </c>
       <c r="T23">
-        <v>-427.31999999995969</v>
+        <v>803.16127856805178</v>
       </c>
       <c r="U23">
-        <v>1.821771473664245</v>
+        <v>3.4798338986462412</v>
       </c>
       <c r="V23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="W23" t="s">
         <v>58</v>
@@ -3576,19 +3720,19 @@
         <v>207</v>
       </c>
       <c r="AA23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB23">
         <v>0</v>
       </c>
       <c r="AC23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD23">
         <v>0</v>
       </c>
       <c r="AE23" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="AF23">
         <v>-3.403746320346329</v>
@@ -3659,13 +3803,13 @@
         <v>23209.87</v>
       </c>
       <c r="S24">
-        <v>23053.442900000038</v>
+        <v>23291.301253957681</v>
       </c>
       <c r="T24">
-        <v>-156.42709999995711</v>
+        <v>-81.431253957682202</v>
       </c>
       <c r="U24">
-        <v>0.67854116488586114</v>
+        <v>-0.34962088665546459</v>
       </c>
       <c r="V24" t="s">
         <v>28</v>
@@ -3695,7 +3839,7 @@
         <v>0</v>
       </c>
       <c r="AE24" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="AF24">
         <v>2.0056517723261038</v>
@@ -3766,16 +3910,16 @@
         <v>21325.839999999989</v>
       </c>
       <c r="S25">
-        <v>22054.152200000019</v>
+        <v>20984.844264244519</v>
       </c>
       <c r="T25">
-        <v>728.31220000002941</v>
+        <v>340.99573575547038</v>
       </c>
       <c r="U25">
-        <v>-3.3023813084958609</v>
+        <v>1.6249619556933439</v>
       </c>
       <c r="V25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W25" t="s">
         <v>60</v>
@@ -3793,16 +3937,16 @@
         <v>0</v>
       </c>
       <c r="AB25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD25">
         <v>0</v>
       </c>
       <c r="AE25" t="s">
-        <v>236</v>
+        <v>259</v>
       </c>
       <c r="AF25">
         <v>2.7551066477382449</v>
@@ -3873,13 +4017,13 @@
         <v>22153.67</v>
       </c>
       <c r="S26">
-        <v>22148.29949999999</v>
+        <v>22343.987824663269</v>
       </c>
       <c r="T26">
-        <v>-5.3705000000118162</v>
+        <v>-190.31782466326689</v>
       </c>
       <c r="U26">
-        <v>2.4247911222312211E-2</v>
+        <v>-0.85176301632779428</v>
       </c>
       <c r="V26" t="s">
         <v>28</v>
@@ -3909,7 +4053,7 @@
         <v>0</v>
       </c>
       <c r="AE26" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="AF26">
         <v>-0.12155373281689209</v>
@@ -3980,13 +4124,13 @@
         <v>21992.31</v>
       </c>
       <c r="S27">
-        <v>22136.33780000003</v>
+        <v>22159.57776456916</v>
       </c>
       <c r="T27">
-        <v>144.02780000002889</v>
+        <v>-167.26776456916559</v>
       </c>
       <c r="U27">
-        <v>-0.65063969162970026</v>
+        <v>-0.75483281471458896</v>
       </c>
       <c r="V27" t="s">
         <v>28</v>
@@ -4016,7 +4160,7 @@
         <v>0</v>
       </c>
       <c r="AE27" t="s">
-        <v>236</v>
+        <v>261</v>
       </c>
       <c r="AF27">
         <v>0.71355183632155672</v>
@@ -4087,13 +4231,13 @@
         <v>38653.370000000003</v>
       </c>
       <c r="S28">
-        <v>38641.450800000057</v>
+        <v>38586.831512639452</v>
       </c>
       <c r="T28">
-        <v>-11.91919999993843</v>
+        <v>66.538487360543513</v>
       </c>
       <c r="U28">
-        <v>3.0845632741973581E-2</v>
+        <v>0.17243832870482839</v>
       </c>
       <c r="V28" t="s">
         <v>28</v>
@@ -4120,10 +4264,10 @@
         <v>1</v>
       </c>
       <c r="AD28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE28" t="s">
-        <v>237</v>
+        <v>262</v>
       </c>
       <c r="AF28">
         <v>3.553447639809292</v>
@@ -4194,16 +4338,16 @@
         <v>37746.199999999997</v>
       </c>
       <c r="S29">
-        <v>37561.591900000058</v>
+        <v>36511.659854305421</v>
       </c>
       <c r="T29">
-        <v>-184.60809999994669</v>
+        <v>1234.540145694584</v>
       </c>
       <c r="U29">
-        <v>0.49148103331570042</v>
+        <v>3.3812216443208571</v>
       </c>
       <c r="V29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="W29" t="s">
         <v>64</v>
@@ -4218,19 +4362,19 @@
         <v>213</v>
       </c>
       <c r="AA29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB29">
         <v>0</v>
       </c>
       <c r="AC29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD29">
         <v>0</v>
       </c>
       <c r="AE29" t="s">
-        <v>236</v>
+        <v>263</v>
       </c>
       <c r="AF29">
         <v>9.5750860660608055</v>
@@ -4301,16 +4445,16 @@
         <v>40645.57</v>
       </c>
       <c r="S30">
-        <v>41582.728899999936</v>
+        <v>41699.624448423543</v>
       </c>
       <c r="T30">
-        <v>937.15889999993669</v>
+        <v>-1054.0544484235429</v>
       </c>
       <c r="U30">
-        <v>-2.2537214963781231</v>
+        <v>-2.5277312742402689</v>
       </c>
       <c r="V30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W30" t="s">
         <v>65</v>
@@ -4328,16 +4472,16 @@
         <v>0</v>
       </c>
       <c r="AB30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE30" t="s">
-        <v>236</v>
+        <v>264</v>
       </c>
       <c r="AF30">
         <v>0.61735166644967876</v>
@@ -4408,13 +4552,13 @@
         <v>43466.070000000007</v>
       </c>
       <c r="S31">
-        <v>42519.616999999962</v>
+        <v>42467.61941022965</v>
       </c>
       <c r="T31">
-        <v>-946.45300000004499</v>
+        <v>998.4505897703566</v>
       </c>
       <c r="U31">
-        <v>2.22592080262634</v>
+        <v>2.3510867895030829</v>
       </c>
       <c r="V31" t="s">
         <v>28</v>
@@ -4441,10 +4585,10 @@
         <v>1</v>
       </c>
       <c r="AD31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE31" t="s">
-        <v>236</v>
+        <v>265</v>
       </c>
       <c r="AF31">
         <v>12.036249347518041</v>
@@ -4515,16 +4659,16 @@
         <v>46804.329999999987</v>
       </c>
       <c r="S32">
-        <v>45365.440800000011</v>
+        <v>47437.503366886856</v>
       </c>
       <c r="T32">
-        <v>-1438.889199999983</v>
+        <v>-633.17336688686919</v>
       </c>
       <c r="U32">
-        <v>3.1717738759412271</v>
+        <v>-1.334752720837429</v>
       </c>
       <c r="V32" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="W32" t="s">
         <v>67</v>
@@ -4539,19 +4683,19 @@
         <v>216</v>
       </c>
       <c r="AA32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB32">
         <v>0</v>
       </c>
       <c r="AC32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE32" t="s">
-        <v>236</v>
+        <v>266</v>
       </c>
       <c r="AF32">
         <v>-0.8823864926537226</v>
@@ -4622,13 +4766,13 @@
         <v>44343.990000000013</v>
       </c>
       <c r="S33">
-        <v>43511.807200000047</v>
+        <v>43599.284159958697</v>
       </c>
       <c r="T33">
-        <v>-832.18279999995138</v>
+        <v>744.70584004130069</v>
       </c>
       <c r="U33">
-        <v>1.9125447862343681</v>
+        <v>1.708068961199215</v>
       </c>
       <c r="V33" t="s">
         <v>28</v>
@@ -4655,10 +4799,10 @@
         <v>1</v>
       </c>
       <c r="AD33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE33" t="s">
-        <v>237</v>
+        <v>267</v>
       </c>
       <c r="AF33">
         <v>13.77526714304136</v>
@@ -4729,16 +4873,16 @@
         <v>35643.440000000002</v>
       </c>
       <c r="S34">
-        <v>35989.726099999978</v>
+        <v>36666.322945301239</v>
       </c>
       <c r="T34">
-        <v>346.2860999999757</v>
+        <v>-1022.882945301237</v>
       </c>
       <c r="U34">
-        <v>-0.96218042626330502</v>
+        <v>-2.7897069112361552</v>
       </c>
       <c r="V34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W34" t="s">
         <v>69</v>
@@ -4756,16 +4900,16 @@
         <v>0</v>
       </c>
       <c r="AB34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE34" t="s">
-        <v>237</v>
+        <v>268</v>
       </c>
       <c r="AF34">
         <v>21.92631690998633</v>
@@ -4836,16 +4980,16 @@
         <v>33771.230000000003</v>
       </c>
       <c r="S35">
-        <v>32589.036599999989</v>
+        <v>33425.336621711038</v>
       </c>
       <c r="T35">
-        <v>-1182.1934000000069</v>
+        <v>345.89337828895799</v>
       </c>
       <c r="U35">
-        <v>3.6275800801058589</v>
+        <v>1.034823918764328</v>
       </c>
       <c r="V35" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="W35" t="s">
         <v>70</v>
@@ -4860,19 +5004,19 @@
         <v>219</v>
       </c>
       <c r="AA35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB35">
         <v>0</v>
       </c>
       <c r="AC35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE35" t="s">
-        <v>237</v>
+        <v>269</v>
       </c>
       <c r="AF35">
         <v>10.68619155201125</v>
@@ -4943,13 +5087,13 @@
         <v>31989.18</v>
       </c>
       <c r="S36">
-        <v>31836.583800000029</v>
+        <v>32554.75627354861</v>
       </c>
       <c r="T36">
-        <v>-152.59619999997449</v>
+        <v>-565.57627354860597</v>
       </c>
       <c r="U36">
-        <v>0.4793108486720688</v>
+        <v>-1.737307657278172</v>
       </c>
       <c r="V36" t="s">
         <v>28</v>
@@ -4976,10 +5120,10 @@
         <v>1</v>
       </c>
       <c r="AD36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE36" t="s">
-        <v>237</v>
+        <v>270</v>
       </c>
       <c r="AF36">
         <v>13.76297085222623</v>
@@ -5050,16 +5194,16 @@
         <v>30141.740000000009</v>
       </c>
       <c r="S37">
-        <v>29801.953500000011</v>
+        <v>29290.38707478793</v>
       </c>
       <c r="T37">
-        <v>-339.78649999999112</v>
+        <v>851.35292521207157</v>
       </c>
       <c r="U37">
-        <v>1.1401484134252839</v>
+        <v>2.9065949966393041</v>
       </c>
       <c r="V37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="W37" t="s">
         <v>72</v>
@@ -5074,19 +5218,19 @@
         <v>221</v>
       </c>
       <c r="AA37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB37">
         <v>0</v>
       </c>
       <c r="AC37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD37">
         <v>0</v>
       </c>
       <c r="AE37" t="s">
-        <v>237</v>
+        <v>271</v>
       </c>
       <c r="AF37">
         <v>16.407750688113989</v>
@@ -5157,13 +5301,13 @@
         <v>30767.510000000009</v>
       </c>
       <c r="S38">
-        <v>30633.56719999995</v>
+        <v>31192.872794961881</v>
       </c>
       <c r="T38">
-        <v>-133.94280000005159</v>
+        <v>-425.36279496187848</v>
       </c>
       <c r="U38">
-        <v>0.43724192852098481</v>
+        <v>-1.3636537992441049</v>
       </c>
       <c r="V38" t="s">
         <v>28</v>
@@ -5190,10 +5334,10 @@
         <v>1</v>
       </c>
       <c r="AD38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE38" t="s">
-        <v>237</v>
+        <v>272</v>
       </c>
       <c r="AF38">
         <v>17.88151088985714</v>
@@ -5264,16 +5408,16 @@
         <v>28055.05</v>
       </c>
       <c r="S39">
-        <v>28816.955399999981</v>
+        <v>28102.647018959069</v>
       </c>
       <c r="T39">
-        <v>761.90539999997782</v>
+        <v>-47.59701895906619</v>
       </c>
       <c r="U39">
-        <v>-2.6439482916365908</v>
+        <v>-0.1693684546048474</v>
       </c>
       <c r="V39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W39" t="s">
         <v>74</v>
@@ -5291,16 +5435,16 @@
         <v>0</v>
       </c>
       <c r="AB39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD39">
         <v>1</v>
       </c>
       <c r="AE39" t="s">
-        <v>237</v>
+        <v>273</v>
       </c>
       <c r="AF39">
         <v>16.816307286585101</v>
@@ -5371,13 +5515,13 @@
         <v>28477.45</v>
       </c>
       <c r="S40">
-        <v>29077.56600000001</v>
+        <v>28663.008546367659</v>
       </c>
       <c r="T40">
-        <v>600.11600000001272</v>
+        <v>-185.55854636765801</v>
       </c>
       <c r="U40">
-        <v>-2.063845371376726</v>
+        <v>-0.64737986616960708</v>
       </c>
       <c r="V40" t="s">
         <v>28</v>
@@ -5407,7 +5551,7 @@
         <v>1</v>
       </c>
       <c r="AE40" t="s">
-        <v>237</v>
+        <v>274</v>
       </c>
       <c r="AF40">
         <v>10.81563372972778</v>
@@ -5478,13 +5622,13 @@
         <v>30479.26</v>
       </c>
       <c r="S41">
-        <v>30439.032599999959</v>
+        <v>30865.725663167821</v>
       </c>
       <c r="T41">
-        <v>-40.227400000039779</v>
+        <v>-386.46566316782258</v>
       </c>
       <c r="U41">
-        <v>0.13215728807373411</v>
+        <v>-1.252086755987057</v>
       </c>
       <c r="V41" t="s">
         <v>28</v>
@@ -5514,7 +5658,7 @@
         <v>0</v>
       </c>
       <c r="AE41" t="s">
-        <v>236</v>
+        <v>275</v>
       </c>
       <c r="AF41">
         <v>6.3477748521019919</v>
@@ -5585,13 +5729,13 @@
         <v>22660.3</v>
       </c>
       <c r="S42">
-        <v>23148.664500000021</v>
+        <v>22742.66776422512</v>
       </c>
       <c r="T42">
-        <v>488.36450000002151</v>
+        <v>-82.36776422512412</v>
       </c>
       <c r="U42">
-        <v>-2.1096875804650459</v>
+        <v>-0.36217283336782058</v>
       </c>
       <c r="V42" t="s">
         <v>28</v>
@@ -5621,7 +5765,7 @@
         <v>0</v>
       </c>
       <c r="AE42" t="s">
-        <v>236</v>
+        <v>276</v>
       </c>
       <c r="AF42">
         <v>14.62110951066416</v>
@@ -5692,13 +5836,13 @@
         <v>36839.19</v>
       </c>
       <c r="S43">
-        <v>37061.884199999957</v>
+        <v>36768.243552007501</v>
       </c>
       <c r="T43">
-        <v>222.69419999996171</v>
+        <v>70.946447992500907</v>
       </c>
       <c r="U43">
-        <v>-0.60087123147387611</v>
+        <v>0.19295577144485959</v>
       </c>
       <c r="V43" t="s">
         <v>28</v>
@@ -5725,10 +5869,10 @@
         <v>1</v>
       </c>
       <c r="AD43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE43" t="s">
-        <v>236</v>
+        <v>277</v>
       </c>
       <c r="AF43">
         <v>-2.076115794737603</v>
@@ -5799,13 +5943,13 @@
         <v>33799.46</v>
       </c>
       <c r="S44">
-        <v>33032.208299999969</v>
+        <v>34340.085234858903</v>
       </c>
       <c r="T44">
-        <v>-767.25170000002981</v>
+        <v>-540.62523485890415</v>
       </c>
       <c r="U44">
-        <v>2.3227381379767769</v>
+        <v>-1.5743270034464301</v>
       </c>
       <c r="V44" t="s">
         <v>28</v>
@@ -5832,10 +5976,10 @@
         <v>1</v>
       </c>
       <c r="AD44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE44" t="s">
-        <v>236</v>
+        <v>278</v>
       </c>
       <c r="AF44">
         <v>6.9110867305562644</v>
@@ -5906,13 +6050,13 @@
         <v>28060.400000000001</v>
       </c>
       <c r="S45">
-        <v>28337.257599999979</v>
+        <v>28749.554497169989</v>
       </c>
       <c r="T45">
-        <v>276.85759999997748</v>
+        <v>-689.15449716999137</v>
       </c>
       <c r="U45">
-        <v>-0.97700915137242406</v>
+        <v>-2.397096265397189</v>
       </c>
       <c r="V45" t="s">
         <v>28</v>
@@ -5942,7 +6086,7 @@
         <v>0</v>
       </c>
       <c r="AE45" t="s">
-        <v>236</v>
+        <v>279</v>
       </c>
       <c r="AF45">
         <v>17.663115194893241</v>
@@ -6013,13 +6157,13 @@
         <v>29911.54</v>
       </c>
       <c r="S46">
-        <v>29592.82440000002</v>
+        <v>30175.13838829696</v>
       </c>
       <c r="T46">
-        <v>-318.71559999998141</v>
+        <v>-263.59838829695951</v>
       </c>
       <c r="U46">
-        <v>1.0770029777893759</v>
+        <v>-0.87356148927950805</v>
       </c>
       <c r="V46" t="s">
         <v>28</v>
@@ -6049,7 +6193,7 @@
         <v>1</v>
       </c>
       <c r="AE46" t="s">
-        <v>236</v>
+        <v>280</v>
       </c>
       <c r="AF46">
         <v>12.53114547980249</v>
@@ -6120,13 +6264,13 @@
         <v>31787.919999999998</v>
       </c>
       <c r="S47">
-        <v>31112.967499999981</v>
+        <v>31516.558738070111</v>
       </c>
       <c r="T47">
-        <v>-674.95250000002125</v>
+        <v>271.36126192988741</v>
       </c>
       <c r="U47">
-        <v>2.1693607335912972</v>
+        <v>0.86101171192303849</v>
       </c>
       <c r="V47" t="s">
         <v>28</v>
@@ -6153,10 +6297,10 @@
         <v>1</v>
       </c>
       <c r="AD47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE47" t="s">
-        <v>236</v>
+        <v>281</v>
       </c>
       <c r="AF47">
         <v>10.34083217511764</v>
@@ -6227,13 +6371,13 @@
         <v>33038.649999999987</v>
       </c>
       <c r="S48">
-        <v>32051.739199999971</v>
+        <v>31714.723093803372</v>
       </c>
       <c r="T48">
-        <v>-986.91080000002694</v>
+        <v>1323.9269061966261</v>
       </c>
       <c r="U48">
-        <v>3.079117778420049</v>
+        <v>4.1744867274445907</v>
       </c>
       <c r="V48" t="s">
         <v>26</v>
@@ -6263,7 +6407,7 @@
         <v>0</v>
       </c>
       <c r="AE48" t="s">
-        <v>237</v>
+        <v>282</v>
       </c>
       <c r="AF48">
         <v>-0.91124050874225304</v>
@@ -6334,13 +6478,13 @@
         <v>28112.5</v>
       </c>
       <c r="S49">
-        <v>27469.167399999998</v>
+        <v>27759.11763710195</v>
       </c>
       <c r="T49">
-        <v>-643.33260000000155</v>
+        <v>353.38236289805349</v>
       </c>
       <c r="U49">
-        <v>2.3420171082433381</v>
+        <v>1.273031684644522</v>
       </c>
       <c r="V49" t="s">
         <v>28</v>
@@ -6349,7 +6493,7 @@
         <v>84</v>
       </c>
       <c r="X49" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Y49" t="s">
         <v>183</v>
@@ -6370,7 +6514,7 @@
         <v>1</v>
       </c>
       <c r="AE49" t="s">
-        <v>237</v>
+        <v>283</v>
       </c>
       <c r="AF49">
         <v>13.86040041370083</v>
@@ -6441,13 +6585,13 @@
         <v>32412.29</v>
       </c>
       <c r="S50">
-        <v>31925.7991</v>
+        <v>33037.944833113077</v>
       </c>
       <c r="T50">
-        <v>-486.49090000000427</v>
+        <v>-625.65483311307253</v>
       </c>
       <c r="U50">
-        <v>1.523817457085997</v>
+        <v>-1.8937462250557271</v>
       </c>
       <c r="V50" t="s">
         <v>28</v>
@@ -6456,7 +6600,7 @@
         <v>85</v>
       </c>
       <c r="X50" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Y50" t="s">
         <v>184</v>
@@ -6474,10 +6618,10 @@
         <v>1</v>
       </c>
       <c r="AD50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE50" t="s">
-        <v>237</v>
+        <v>284</v>
       </c>
       <c r="AF50">
         <v>18.92693910201638</v>
@@ -6548,13 +6692,13 @@
         <v>29321.21</v>
       </c>
       <c r="S51">
-        <v>29775.13689999998</v>
+        <v>28892.968805534791</v>
       </c>
       <c r="T51">
-        <v>453.92689999997668</v>
+        <v>428.24119446521217</v>
       </c>
       <c r="U51">
-        <v>-1.524516584170523</v>
+        <v>1.482164042565185</v>
       </c>
       <c r="V51" t="s">
         <v>28</v>
@@ -6563,7 +6707,7 @@
         <v>86</v>
       </c>
       <c r="X51" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Y51" t="s">
         <v>185</v>
@@ -6584,7 +6728,7 @@
         <v>1</v>
       </c>
       <c r="AE51" t="s">
-        <v>237</v>
+        <v>285</v>
       </c>
       <c r="AF51">
         <v>30.98293225544802</v>

</xml_diff>

<commit_message>
Update chart titles: change / to & and restructure titles with subtitles
</commit_message>
<xml_diff>
--- a/data/revenue-data.xlsx
+++ b/data/revenue-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/Revenue_Performance_Analysis-2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{719E12F6-5A35-5A43-B9DB-6F97609CF138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2199225C-0203-244F-92C3-95CE51A13BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="21340" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1460" yWindow="760" windowWidth="25980" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -730,154 +730,154 @@
     <t>2-BCBS – Non E/M Code Charge Billed Balance increased from avg 0.67 to 45.00; 2-BCBS – New E/M Code Zero Balance - Collection * Charges increased from avg -11.29 to 510.99; 12-HUMANA – New E/M Code Charge Billed Balance increased from avg 10.70 to 263.00; 2-BCBS – Existing E/M Code Charge Billed Balance increased from avg 25.16 to 381.01; 13-TRICARE – New E/M Code Denial % increased from avg 0.06 to 0.67; 15-UNITED HEALTHCARE – New E/M Code Zero Balance - Collection * Charges increased from avg 18.08 to 181.28</t>
   </si>
   <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – High zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – High zero-balance collection vs baseline; 2-BCBS – Normal range; 3-MEDICARE – High zero-balance collection vs baseline; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Unusually high zero-balance vs total collection</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Low zero-balance collection vs baseline; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Low zero-balance collection vs baseline; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – High zero-balance collection vs baseline; 2-BCBS – Normal range; 3-MEDICARE – High zero-balance collection vs baseline; 3-MEDICARE – Low zero-balance collection vs baseline; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range; 5-COMMERCIAL – Very low zero-balance collection vs baseline</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Low zero-balance collection vs baseline; 1-SELF PAY – Normal range; 12-HUMANA – Low zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Collection data incomplete; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Very low zero-balance collection vs baseline</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Low zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – High zero-balance collection vs baseline; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Low zero-balance collection vs baseline; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – High zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Collection data incomplete; 12-HUMANA – Low zero-balance collection vs baseline; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Low zero-balance collection vs baseline; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 2-BCBS – Very low zero-balance collection vs baseline; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 1-SELF PAY – Unusually high zero-balance vs total collection; 12-HUMANA – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Collection data incomplete; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Low zero-balance collection vs baseline; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete; 5-COMMERCIAL – Low zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 13-TRICARE – Collection data incomplete; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – High zero-balance collection vs baseline; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 1-SELF PAY – Very low zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Low zero-balance collection vs baseline; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Low zero-balance collection vs baseline; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 12-HUMANA – Unusually high zero-balance vs total collection; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range; 5-COMMERCIAL – Unusually high zero-balance vs total collection</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Collection data incomplete; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Low zero-balance collection vs baseline; 4-MEDICAID – Normal range; 5-COMMERCIAL – Low zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 13-TRICARE – Low zero-balance collection vs baseline; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Low zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Low zero-balance collection vs baseline; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range; 5-COMMERCIAL – Very low zero-balance collection vs baseline</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – High zero-balance collection vs baseline; 1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – High zero-balance collection vs baseline; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – High zero-balance collection vs baseline; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Low zero-balance collection vs baseline</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – High zero-balance collection vs baseline; 1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Low zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Low zero-balance collection vs baseline; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Collection data incomplete; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Low zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Low zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 15-UNITED HEALTHCARE – Unusually high zero-balance vs total collection; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Low zero-balance collection vs baseline; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – High zero-balance collection vs baseline; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Low zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – High zero-balance collection vs baseline; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – High zero-balance collection vs baseline; 1-SELF PAY – Normal range; 12-HUMANA – Collection data incomplete; 13-TRICARE – Low zero-balance collection vs baseline; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 15-UNITED HEALTHCARE – Unusually high zero-balance vs total collection; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Collection data incomplete; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 3-MEDICARE – Unusually high zero-balance vs total collection; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – Low zero-balance collection vs baseline</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 12-HUMANA – Unusually high zero-balance vs total collection; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – High zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Low zero-balance collection vs baseline; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – High zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 18-CIGNA – Very low zero-balance collection vs baseline; 2-BCBS – Normal range; 2-BCBS – Very low zero-balance collection vs baseline; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Low zero-balance collection vs baseline; 1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 17-AETNA – Normal range; 18-CIGNA – Low zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Low zero-balance collection vs baseline</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Low zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Collection data incomplete; 12-HUMANA – Normal range; 13-TRICARE – High zero-balance collection vs baseline; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 3-MEDICARE – Unusually high zero-balance vs total collection; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete; 5-COMMERCIAL – High zero-balance collection vs baseline</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – High zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Collection data incomplete; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – High zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Low zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – High zero-balance collection vs baseline; 1-SELF PAY – Normal range; 12-HUMANA – Collection data incomplete; 12-HUMANA – High zero-balance collection vs baseline; 12-HUMANA – Unusually high zero-balance vs total collection; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Collection data incomplete; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Low zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Collection data incomplete; 2-BCBS – Normal range; 2-BCBS – Unusually high zero-balance vs total collection; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – High zero-balance collection vs baseline; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Low zero-balance collection vs baseline; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – High zero-balance collection vs baseline; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Unusually high zero-balance vs total collection; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Low zero-balance collection vs baseline; 4-MEDICAID – Normal range; 4-MEDICAID – Unusually high zero-balance vs total collection; 5-COMMERCIAL – Collection data incomplete</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – High zero-balance collection vs baseline; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete; 99-NEEDS INFO – Collection data incomplete</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Collection data incomplete; 1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 15-UNITED HEALTHCARE – Unusually high zero-balance vs total collection; 17-AETNA – Low zero-balance collection vs baseline; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 4-MEDICAID – Very low zero-balance collection vs baseline; 5-COMMERCIAL – Collection data incomplete</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Collection data incomplete; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Collection data incomplete; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 3-MEDICARE – Unusually high zero-balance vs total collection; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Collection data incomplete; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – High zero-balance collection vs baseline; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete; 5-COMMERCIAL – Normal range; 7-PPO – Collection data incomplete; 99-NEEDS INFO – Collection data incomplete</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 15-UNITED HEALTHCARE – Unusually high zero-balance vs total collection; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Collection data incomplete; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 4-MEDICAID – Unusually high zero-balance vs total collection; 5-COMMERCIAL – Collection data incomplete; 5-COMMERCIAL – Unusually high zero-balance vs total collection; 99-NEEDS INFO – Collection data incomplete</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Low zero-balance collection vs baseline; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 4-MEDICAID – Normal range; 4-MEDICAID – Unusually high zero-balance vs total collection; 5-COMMERCIAL – Collection data incomplete; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 13-TRICARE – Low zero-balance collection vs baseline; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – High zero-balance collection vs baseline; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – High zero-balance collection vs baseline; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – High zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Collection data incomplete; 18-CIGNA – Normal range; 2-BCBS – Collection data incomplete; 2-BCBS – Normal range; 3-MEDICARE – Normal range; 3-MEDICARE – Unusually high zero-balance vs total collection; 4-MEDICAID – Collection data incomplete; 4-MEDICAID – Unusually high zero-balance vs total collection; 5-COMMERCIAL – Normal range</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Normal range; 12-HUMANA – Normal range; 12-HUMANA – Unusually high zero-balance vs total collection; 13-TRICARE – Collection data incomplete; 13-TRICARE – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 18-CIGNA – Collection data incomplete; 18-CIGNA – Normal range; 2-BCBS – Normal range; 3-MEDICARE – High zero-balance collection vs baseline; 4-MEDICAID – Normal range; 5-COMMERCIAL – Collection data incomplete; 99-NEEDS INFO – Collection data incomplete</t>
-  </si>
-  <si>
-    <t>1-SELF PAY – Low zero-balance collection vs baseline; 1-SELF PAY – Normal range; 12-HUMANA – Collection data incomplete; 12-HUMANA – Normal range; 13-TRICARE – Collection data incomplete; 13-TRICARE – Normal range; 15-UNITED HEALTHCARE – Normal range; 17-AETNA – Normal range; 17-AETNA – Unusually high zero-balance vs total collection; 18-CIGNA – Normal range; 2-BCBS – Collection data incomplete; 2-BCBS – Normal range; 3-MEDICARE – Collection data incomplete; 3-MEDICARE – Normal range; 4-MEDICAID – High zero-balance collection vs baseline; 4-MEDICAID – Normal range; 5-COMMERCIAL – Normal range</t>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 12-HUMANA – New E/M Code – High zero-balance collection vs baseline; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 2-BCBS – Non E/M Code – High zero-balance collection vs baseline; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – High zero-balance collection vs baseline; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Unusually high zero-balance vs total collection</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Low zero-balance collection vs baseline; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Low zero-balance collection vs baseline; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 2-BCBS – Non E/M Code – High zero-balance collection vs baseline; 3-MEDICARE – Existing E/M Code – High zero-balance collection vs baseline; 3-MEDICARE – New E/M Code – Low zero-balance collection vs baseline; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Very low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Low zero-balance collection vs baseline; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Low zero-balance collection vs baseline; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 17-AETNA – Non E/M Code – Collection data incomplete; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Very low zero-balance collection vs baseline; 5-COMMERCIAL – New E/M Code – Very low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 12-HUMANA – New E/M Code – Low zero-balance collection vs baseline; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – High zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – High zero-balance collection vs baseline; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 2-BCBS – Non E/M Code – Low zero-balance collection vs baseline; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – High zero-balance collection vs baseline; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 4-MEDICAID – Non E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Collection data incomplete; 12-HUMANA – New E/M Code – Low zero-balance collection vs baseline; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Low zero-balance collection vs baseline; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 2-BCBS – Non E/M Code – Very low zero-balance collection vs baseline; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 4-MEDICAID – Non E/M Code – Collection data incomplete; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – High zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Unusually high zero-balance vs total collection; 12-HUMANA – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 17-AETNA – Non E/M Code – Collection data incomplete; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 2-BCBS – Non E/M Code – Low zero-balance collection vs baseline; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Low zero-balance collection vs baseline; 5-COMMERCIAL – Non E/M Code – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 13-TRICARE – Non E/M Code – Collection data incomplete; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 4-MEDICAID – Non E/M Code – Collection data incomplete; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 13-TRICARE – Existing E/M Code – High zero-balance collection vs baseline; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 18-CIGNA – Non E/M Code – High zero-balance collection vs baseline; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Very low zero-balance collection vs baseline; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Low zero-balance collection vs baseline; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 2-BCBS – Non E/M Code – Low zero-balance collection vs baseline; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 4-MEDICAID – Non E/M Code – Collection data incomplete; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Unusually high zero-balance vs total collection; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Unusually high zero-balance vs total collection; 13-TRICARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 4-MEDICAID – Non E/M Code – Collection data incomplete; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Unusually high zero-balance vs total collection</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – High zero-balance collection vs baseline; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Non E/M Code – Collection data incomplete; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Low zero-balance collection vs baseline; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Low zero-balance collection vs baseline; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Low zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Non E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Low zero-balance collection vs baseline; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Very low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – High zero-balance collection vs baseline; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 13-TRICARE – Existing E/M Code – High zero-balance collection vs baseline; 13-TRICARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – High zero-balance collection vs baseline; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Low zero-balance collection vs baseline; 5-COMMERCIAL – New E/M Code – Low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – High zero-balance collection vs baseline; 12-HUMANA – Existing E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Normal range; 13-TRICARE – Non E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Collection data incomplete; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Normal range; 5-COMMERCIAL – Non E/M Code – Low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Non E/M Code – Normal range; 17-AETNA – Existing E/M Code – Low zero-balance collection vs baseline; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Non E/M Code – Collection data incomplete; 13-TRICARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Collection data incomplete; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Low zero-balance collection vs baseline; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Unusually high zero-balance vs total collection; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 17-AETNA – Non E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 2-BCBS – Non E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Low zero-balance collection vs baseline; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – New E/M Code – High zero-balance collection vs baseline; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 17-AETNA – Non E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Low zero-balance collection vs baseline; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 2-BCBS – Non E/M Code – High zero-balance collection vs baseline; 3-MEDICARE – Existing E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – High zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – High zero-balance collection vs baseline; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Collection data incomplete; 13-TRICARE – Existing E/M Code – Low zero-balance collection vs baseline; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 2-BCBS – Non E/M Code – Collection data incomplete; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Unusually high zero-balance vs total collection; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – High zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 3-MEDICARE – Non E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 4-MEDICAID – Non E/M Code – Collection data incomplete; 5-COMMERCIAL – New E/M Code – Low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 12-HUMANA – New E/M Code – Unusually high zero-balance vs total collection; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – High zero-balance collection vs baseline; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Low zero-balance collection vs baseline; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 2-BCBS – Non E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 4-MEDICAID – Non E/M Code – Collection data incomplete; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – High zero-balance collection vs baseline; 5-COMMERCIAL – Non E/M Code – High zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 4-MEDICAID – Non E/M Code – Collection data incomplete; 5-COMMERCIAL – Existing E/M Code – High zero-balance collection vs baseline; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Unusually high zero-balance vs total collection; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – High zero-balance collection vs baseline; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – High zero-balance collection vs baseline; 17-AETNA – New E/M Code – High zero-balance collection vs baseline; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 18-CIGNA – Non E/M Code – Very low zero-balance collection vs baseline; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 2-BCBS – Non E/M Code – Very low zero-balance collection vs baseline; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Collection data incomplete; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Low zero-balance collection vs baseline; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – High zero-balance collection vs baseline; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Low zero-balance collection vs baseline; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Low zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Unusually high zero-balance vs total collection; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Low zero-balance collection vs baseline; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Collection data incomplete; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 12-HUMANA – New E/M Code – Collection data incomplete; 13-TRICARE – Existing E/M Code – High zero-balance collection vs baseline; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Unusually high zero-balance vs total collection; 17-AETNA – New E/M Code – Unusually high zero-balance vs total collection; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Unusually high zero-balance vs total collection; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Collection data incomplete; 5-COMMERCIAL – New E/M Code – High zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Unusually high zero-balance vs total collection; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – High zero-balance collection vs baseline; 17-AETNA – Existing E/M Code – High zero-balance collection vs baseline; 17-AETNA – New E/M Code – High zero-balance collection vs baseline; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Collection data incomplete; 5-COMMERCIAL – New E/M Code – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Non E/M Code – Collection data incomplete; 17-AETNA – Existing E/M Code – High zero-balance collection vs baseline; 17-AETNA – New E/M Code – High zero-balance collection vs baseline; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – High zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – High zero-balance collection vs baseline; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – High zero-balance collection vs baseline; 17-AETNA – New E/M Code – High zero-balance collection vs baseline; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Low zero-balance collection vs baseline; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Unusually high zero-balance vs total collection; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 4-MEDICAID – Non E/M Code – Collection data incomplete; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – High zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – High zero-balance collection vs baseline; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Unusually high zero-balance vs total collection; 12-HUMANA – New E/M Code – High zero-balance collection vs baseline; 12-HUMANA – Non E/M Code – Collection data incomplete; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – High zero-balance collection vs baseline; 17-AETNA – New E/M Code – Unusually high zero-balance vs total collection; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 4-MEDICAID – Non E/M Code – Collection data incomplete; 5-COMMERCIAL – Existing E/M Code – Collection data incomplete; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Non E/M Code – Collection data incomplete; 17-AETNA – Existing E/M Code – Unusually high zero-balance vs total collection; 17-AETNA – New E/M Code – High zero-balance collection vs baseline; 18-CIGNA – Existing E/M Code – Low zero-balance collection vs baseline; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Unusually high zero-balance vs total collection; 2-BCBS – Non E/M Code – Collection data incomplete; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – High zero-balance collection vs baseline</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Low zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Unusually high zero-balance vs total collection; 17-AETNA – New E/M Code – High zero-balance collection vs baseline; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Collection data incomplete; 3-MEDICARE – New E/M Code – Unusually high zero-balance vs total collection; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – New E/M Code – Low zero-balance collection vs baseline; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Unusually high zero-balance vs total collection; 5-COMMERCIAL – New E/M Code – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – High zero-balance collection vs baseline; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Collection data incomplete; 99-NEEDS INFO – New E/M Code – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Collection data incomplete; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Unusually high zero-balance vs total collection; 17-AETNA – Existing E/M Code – Low zero-balance collection vs baseline; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Collection data incomplete; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 4-MEDICAID – Non E/M Code – Very low zero-balance collection vs baseline; 5-COMMERCIAL – Existing E/M Code – Collection data incomplete; 5-COMMERCIAL – New E/M Code – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Unusually high zero-balance vs total collection; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 13-TRICARE – Non E/M Code – Collection data incomplete; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Unusually high zero-balance vs total collection; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Collection data incomplete; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Unusually high zero-balance vs total collection; 3-MEDICARE – Non E/M Code – Collection data incomplete; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Collection data incomplete; 5-COMMERCIAL – New E/M Code – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Unusually high zero-balance vs total collection; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Non E/M Code – Collection data incomplete; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Collection data incomplete; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Collection data incomplete; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – High zero-balance collection vs baseline; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Unusually high zero-balance vs total collection; 17-AETNA – New E/M Code – Unusually high zero-balance vs total collection; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Collection data incomplete; 5-COMMERCIAL – New E/M Code – Normal range; 7-PPO – Existing E/M Code – Collection data incomplete; 99-NEEDS INFO – New E/M Code – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Unusually high zero-balance vs total collection; 13-TRICARE – New E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – Existing E/M Code – Unusually high zero-balance vs total collection; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 2-BCBS – Non E/M Code – Collection data incomplete; 3-MEDICARE – Existing E/M Code – Collection data incomplete; 3-MEDICARE – New E/M Code – Normal range; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Unusually high zero-balance vs total collection; 5-COMMERCIAL – Existing E/M Code – Collection data incomplete; 5-COMMERCIAL – New E/M Code – Unusually high zero-balance vs total collection; 99-NEEDS INFO – New E/M Code – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – New E/M Code – Low zero-balance collection vs baseline; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Collection data incomplete; 3-MEDICARE – New E/M Code – Collection data incomplete; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Unusually high zero-balance vs total collection; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Low zero-balance collection vs baseline; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – High zero-balance collection vs baseline; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Collection data incomplete; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – Existing E/M Code – Collection data incomplete; 5-COMMERCIAL – Medicare Wellness E/M – Collection data incomplete; 5-COMMERCIAL – New E/M Code – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – High zero-balance collection vs baseline; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Normal range; 15-UNITED HEALTHCARE – Existing E/M Code – High zero-balance collection vs baseline; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – Medicare Wellness E/M – Normal range; 18-CIGNA – New E/M Code – Normal range; 18-CIGNA – Non E/M Code – Collection data incomplete; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 2-BCBS – Non E/M Code – Collection data incomplete; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Unusually high zero-balance vs total collection; 4-MEDICAID – Existing E/M Code – Unusually high zero-balance vs total collection; 4-MEDICAID – New E/M Code – Unusually high zero-balance vs total collection; 4-MEDICAID – Non E/M Code – Collection data incomplete; 5-COMMERCIAL – Existing E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Normal range</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Normal range; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Unusually high zero-balance vs total collection; 12-HUMANA – New E/M Code – Normal range; 13-TRICARE – Existing E/M Code – Unusually high zero-balance vs total collection; 13-TRICARE – New E/M Code – Collection data incomplete; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Normal range; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Collection data incomplete; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 3-MEDICARE – New E/M Code – High zero-balance collection vs baseline; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 5-COMMERCIAL – New E/M Code – Collection data incomplete; 99-NEEDS INFO – New E/M Code – Collection data incomplete</t>
+  </si>
+  <si>
+    <t>1-SELF PAY – Existing E/M Code – Low zero-balance collection vs baseline; 1-SELF PAY – New E/M Code – Normal range; 1-SELF PAY – Non E/M Code – Normal range; 12-HUMANA – Existing E/M Code – Normal range; 12-HUMANA – New E/M Code – Collection data incomplete; 13-TRICARE – Existing E/M Code – Normal range; 13-TRICARE – New E/M Code – Collection data incomplete; 13-TRICARE – Non E/M Code – Collection data incomplete; 15-UNITED HEALTHCARE – Existing E/M Code – Normal range; 15-UNITED HEALTHCARE – New E/M Code – Normal range; 17-AETNA – Existing E/M Code – Unusually high zero-balance vs total collection; 17-AETNA – New E/M Code – Normal range; 18-CIGNA – Existing E/M Code – Normal range; 18-CIGNA – New E/M Code – Normal range; 2-BCBS – Existing E/M Code – Normal range; 2-BCBS – New E/M Code – Normal range; 2-BCBS – Non E/M Code – Collection data incomplete; 3-MEDICARE – Existing E/M Code – Normal range; 3-MEDICARE – New E/M Code – Collection data incomplete; 4-MEDICAID – Existing E/M Code – Normal range; 4-MEDICAID – New E/M Code – Normal range; 4-MEDICAID – Non E/M Code – High zero-balance collection vs baseline; 5-COMMERCIAL – New E/M Code – Normal range</t>
   </si>
 </sst>
 </file>
@@ -936,10 +936,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1247,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AE12" sqref="AE12"/>
+    <sheetView tabSelected="1" topLeftCell="AD43" workbookViewId="0">
+      <selection activeCell="AE71" sqref="AE71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1280,13 +1286,13 @@
     <col min="28" max="28" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="18" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="255.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="32" max="33" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1377,7 +1383,7 @@
       <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="3" t="s">
         <v>30</v>
       </c>
       <c r="AF1" s="1" t="s">

</xml_diff>